<commit_message>
Build test cases directly from the dataframe, removing need for csv file.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00538DC-63D5-4397-B963-B806683CA93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E3FECD-8C5A-4AAB-8D5A-E02D59C51403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30765" yWindow="390" windowWidth="25410" windowHeight="15510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capture_test_data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="163">
   <si>
     <t>setup</t>
   </si>
@@ -520,6 +520,9 @@
   <si>
     <t>match no capt, mult, in opp dir</t>
   </si>
+  <si>
+    <t>[]</t>
+  </si>
 </sst>
 </file>
 
@@ -1002,7 +1005,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1213,7 +1216,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1550,9 +1552,9 @@
   <dimension ref="A1:AMK224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C190" sqref="C190"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2656,13 +2658,13 @@
         <v>8</v>
       </c>
       <c r="T2" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="U2" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="V2" s="49" t="s">
-        <v>8</v>
+        <v>162</v>
+      </c>
+      <c r="U2" s="49">
+        <v>0</v>
+      </c>
+      <c r="V2" s="49">
+        <v>0</v>
       </c>
       <c r="W2" s="49" t="s">
         <v>8</v>
@@ -2670,14 +2672,18 @@
       <c r="X2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z2" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
+      <c r="Y2" s="49">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="49">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="49">
+        <v>0</v>
+      </c>
       <c r="AC2" s="49"/>
       <c r="AD2" s="49">
         <v>0</v>
@@ -27002,10 +27008,10 @@
     </row>
     <row r="190" spans="1:302" x14ac:dyDescent="0.2">
       <c r="A190" s="41"/>
-      <c r="B190" s="114">
-        <v>2</v>
-      </c>
-      <c r="C190" s="114">
+      <c r="B190" s="33">
+        <v>2</v>
+      </c>
+      <c r="C190" s="33">
         <v>2</v>
       </c>
       <c r="D190" s="33">

</xml_diff>

<commit_message>
Bug fixes for capt_dir both. Added Qelat II and Raja Pasu.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6D743F-0486-411D-B9E4-333FD489EDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B781EFC3-1B2F-4B06-A70F-8E90D7B859E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="179">
   <si>
     <t>setup</t>
   </si>
@@ -565,6 +565,12 @@
   <si>
     <t>capt both with limited multi and mopp</t>
   </si>
+  <si>
+    <t>capt both with limited multi, no capt first</t>
+  </si>
+  <si>
+    <t>initial capture is not required</t>
+  </si>
 </sst>
 </file>
 
@@ -1041,7 +1047,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1213,8 +1219,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1222,6 +1226,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1555,12 +1560,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AMK244"/>
+  <dimension ref="A1:AMK248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="U243" sqref="U243"/>
+      <selection pane="bottomLeft" activeCell="AQ247" sqref="AQ247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -42559,16 +42564,16 @@
       <c r="A233" s="40">
         <v>106</v>
       </c>
-      <c r="B233" s="91">
-        <v>3</v>
-      </c>
-      <c r="C233" s="91">
-        <v>3</v>
-      </c>
-      <c r="D233" s="91">
-        <v>3</v>
-      </c>
-      <c r="E233" s="91">
+      <c r="B233">
+        <v>3</v>
+      </c>
+      <c r="C233">
+        <v>3</v>
+      </c>
+      <c r="D233">
+        <v>3</v>
+      </c>
+      <c r="E233">
         <v>3</v>
       </c>
       <c r="N233">
@@ -42595,16 +42600,16 @@
       <c r="W233" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="AH233" s="91">
-        <v>0</v>
-      </c>
-      <c r="AI233" s="91">
-        <v>0</v>
-      </c>
-      <c r="AJ233" s="91">
-        <v>0</v>
-      </c>
-      <c r="AK233" s="91">
+      <c r="AH233">
+        <v>0</v>
+      </c>
+      <c r="AI233">
+        <v>0</v>
+      </c>
+      <c r="AJ233">
+        <v>0</v>
+      </c>
+      <c r="AK233">
         <v>3</v>
       </c>
       <c r="AP233">
@@ -42621,28 +42626,28 @@
       </c>
     </row>
     <row r="234" spans="1:302" x14ac:dyDescent="0.2">
-      <c r="B234" s="91">
-        <v>3</v>
-      </c>
-      <c r="C234" s="91">
-        <v>3</v>
-      </c>
-      <c r="D234" s="91">
-        <v>3</v>
-      </c>
-      <c r="E234" s="91">
-        <v>0</v>
-      </c>
-      <c r="AH234" s="91">
-        <v>3</v>
-      </c>
-      <c r="AI234" s="91">
-        <v>3</v>
-      </c>
-      <c r="AJ234" s="91">
-        <v>3</v>
-      </c>
-      <c r="AK234" s="91">
+      <c r="B234">
+        <v>3</v>
+      </c>
+      <c r="C234">
+        <v>3</v>
+      </c>
+      <c r="D234">
+        <v>3</v>
+      </c>
+      <c r="E234">
+        <v>0</v>
+      </c>
+      <c r="AH234">
+        <v>3</v>
+      </c>
+      <c r="AI234">
+        <v>3</v>
+      </c>
+      <c r="AJ234">
+        <v>3</v>
+      </c>
+      <c r="AK234">
         <v>0</v>
       </c>
     </row>
@@ -42650,16 +42655,16 @@
       <c r="A235" s="46">
         <v>107</v>
       </c>
-      <c r="B235" s="92">
-        <v>3</v>
-      </c>
-      <c r="C235" s="92">
-        <v>3</v>
-      </c>
-      <c r="D235" s="92">
-        <v>3</v>
-      </c>
-      <c r="E235" s="92">
+      <c r="B235" s="29">
+        <v>3</v>
+      </c>
+      <c r="C235" s="29">
+        <v>3</v>
+      </c>
+      <c r="D235" s="29">
+        <v>3</v>
+      </c>
+      <c r="E235" s="29">
         <v>3</v>
       </c>
       <c r="F235" s="28"/>
@@ -42701,17 +42706,17 @@
       <c r="AD235" s="65"/>
       <c r="AE235" s="65"/>
       <c r="AF235" s="65"/>
-      <c r="AG235" s="93"/>
-      <c r="AH235" s="92">
-        <v>0</v>
-      </c>
-      <c r="AI235" s="92">
-        <v>0</v>
-      </c>
-      <c r="AJ235" s="92">
-        <v>0</v>
-      </c>
-      <c r="AK235" s="92">
+      <c r="AG235" s="91"/>
+      <c r="AH235" s="29">
+        <v>0</v>
+      </c>
+      <c r="AI235" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ235" s="29">
+        <v>0</v>
+      </c>
+      <c r="AK235" s="29">
         <v>0</v>
       </c>
       <c r="AP235" s="29">
@@ -42720,293 +42725,293 @@
       <c r="AQ235" s="29">
         <v>3</v>
       </c>
-      <c r="AR235" s="94" t="b">
+      <c r="AR235" s="92" t="b">
         <v>1</v>
       </c>
       <c r="AS235" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="AT235" s="95"/>
-      <c r="AU235" s="95"/>
-      <c r="AV235" s="95"/>
-      <c r="AW235" s="95"/>
-      <c r="AX235" s="95"/>
-      <c r="AY235" s="95"/>
-      <c r="AZ235" s="95"/>
-      <c r="BA235" s="95"/>
-      <c r="BB235" s="95"/>
-      <c r="BC235" s="95"/>
-      <c r="BD235" s="95"/>
-      <c r="BE235" s="95"/>
-      <c r="BF235" s="95"/>
-      <c r="BG235" s="95"/>
-      <c r="BH235" s="95"/>
-      <c r="BI235" s="95"/>
-      <c r="BJ235" s="95"/>
-      <c r="BK235" s="95"/>
-      <c r="BL235" s="95"/>
-      <c r="BM235" s="95"/>
-      <c r="BN235" s="95"/>
-      <c r="BO235" s="95"/>
-      <c r="BP235" s="95"/>
-      <c r="BQ235" s="95"/>
-      <c r="BR235" s="95"/>
-      <c r="BS235" s="95"/>
-      <c r="BT235" s="95"/>
-      <c r="BU235" s="95"/>
-      <c r="BV235" s="95"/>
-      <c r="BW235" s="95"/>
-      <c r="BX235" s="95"/>
-      <c r="BY235" s="95"/>
-      <c r="BZ235" s="95"/>
-      <c r="CA235" s="95"/>
-      <c r="CB235" s="95"/>
-      <c r="CC235" s="95"/>
-      <c r="CD235" s="95"/>
-      <c r="CE235" s="95"/>
-      <c r="CF235" s="95"/>
-      <c r="CG235" s="95"/>
-      <c r="CH235" s="95"/>
-      <c r="CI235" s="95"/>
-      <c r="CJ235" s="95"/>
-      <c r="CK235" s="95"/>
-      <c r="CL235" s="95"/>
-      <c r="CM235" s="95"/>
-      <c r="CN235" s="95"/>
-      <c r="CO235" s="95"/>
-      <c r="CP235" s="95"/>
-      <c r="CQ235" s="95"/>
-      <c r="CR235" s="95"/>
-      <c r="CS235" s="95"/>
-      <c r="CT235" s="95"/>
-      <c r="CU235" s="95"/>
-      <c r="CV235" s="95"/>
-      <c r="CW235" s="95"/>
-      <c r="CX235" s="95"/>
-      <c r="CY235" s="95"/>
-      <c r="CZ235" s="95"/>
-      <c r="DA235" s="95"/>
-      <c r="DB235" s="95"/>
-      <c r="DC235" s="95"/>
-      <c r="DD235" s="95"/>
-      <c r="DE235" s="95"/>
-      <c r="DF235" s="95"/>
-      <c r="DG235" s="95"/>
-      <c r="DH235" s="95"/>
-      <c r="DI235" s="95"/>
-      <c r="DJ235" s="95"/>
-      <c r="DK235" s="95"/>
-      <c r="DL235" s="95"/>
-      <c r="DM235" s="95"/>
-      <c r="DN235" s="95"/>
-      <c r="DO235" s="95"/>
-      <c r="DP235" s="95"/>
-      <c r="DQ235" s="95"/>
-      <c r="DR235" s="95"/>
-      <c r="DS235" s="95"/>
-      <c r="DT235" s="95"/>
-      <c r="DU235" s="95"/>
-      <c r="DV235" s="95"/>
-      <c r="DW235" s="95"/>
-      <c r="DX235" s="95"/>
-      <c r="DY235" s="95"/>
-      <c r="DZ235" s="95"/>
-      <c r="EA235" s="95"/>
-      <c r="EB235" s="95"/>
-      <c r="EC235" s="95"/>
-      <c r="ED235" s="95"/>
-      <c r="EE235" s="95"/>
-      <c r="EF235" s="95"/>
-      <c r="EG235" s="95"/>
-      <c r="EH235" s="95"/>
-      <c r="EI235" s="95"/>
-      <c r="EJ235" s="95"/>
-      <c r="EK235" s="95"/>
-      <c r="EL235" s="95"/>
-      <c r="EM235" s="95"/>
-      <c r="EN235" s="95"/>
-      <c r="EO235" s="95"/>
-      <c r="EP235" s="95"/>
-      <c r="EQ235" s="95"/>
-      <c r="ER235" s="95"/>
-      <c r="ES235" s="95"/>
-      <c r="ET235" s="95"/>
-      <c r="EU235" s="95"/>
-      <c r="EV235" s="95"/>
-      <c r="EW235" s="95"/>
-      <c r="EX235" s="95"/>
-      <c r="EY235" s="95"/>
-      <c r="EZ235" s="95"/>
-      <c r="FA235" s="95"/>
-      <c r="FB235" s="95"/>
-      <c r="FC235" s="95"/>
-      <c r="FD235" s="95"/>
-      <c r="FE235" s="95"/>
-      <c r="FF235" s="95"/>
-      <c r="FG235" s="95"/>
-      <c r="FH235" s="95"/>
-      <c r="FI235" s="95"/>
-      <c r="FJ235" s="95"/>
-      <c r="FK235" s="95"/>
-      <c r="FL235" s="95"/>
-      <c r="FM235" s="95"/>
-      <c r="FN235" s="95"/>
-      <c r="FO235" s="95"/>
-      <c r="FP235" s="95"/>
-      <c r="FQ235" s="95"/>
-      <c r="FR235" s="95"/>
-      <c r="FS235" s="95"/>
-      <c r="FT235" s="95"/>
-      <c r="FU235" s="95"/>
-      <c r="FV235" s="95"/>
-      <c r="FW235" s="95"/>
-      <c r="FX235" s="95"/>
-      <c r="FY235" s="95"/>
-      <c r="FZ235" s="95"/>
-      <c r="GA235" s="95"/>
-      <c r="GB235" s="95"/>
-      <c r="GC235" s="95"/>
-      <c r="GD235" s="95"/>
-      <c r="GE235" s="95"/>
-      <c r="GF235" s="95"/>
-      <c r="GG235" s="95"/>
-      <c r="GH235" s="95"/>
-      <c r="GI235" s="95"/>
-      <c r="GJ235" s="95"/>
-      <c r="GK235" s="95"/>
-      <c r="GL235" s="95"/>
-      <c r="GM235" s="95"/>
-      <c r="GN235" s="95"/>
-      <c r="GO235" s="95"/>
-      <c r="GP235" s="95"/>
-      <c r="GQ235" s="95"/>
-      <c r="GR235" s="95"/>
-      <c r="GS235" s="95"/>
-      <c r="GT235" s="95"/>
-      <c r="GU235" s="95"/>
-      <c r="GV235" s="95"/>
-      <c r="GW235" s="95"/>
-      <c r="GX235" s="95"/>
-      <c r="GY235" s="95"/>
-      <c r="GZ235" s="95"/>
-      <c r="HA235" s="95"/>
-      <c r="HB235" s="95"/>
-      <c r="HC235" s="95"/>
-      <c r="HD235" s="95"/>
-      <c r="HE235" s="95"/>
-      <c r="HF235" s="95"/>
-      <c r="HG235" s="95"/>
-      <c r="HH235" s="95"/>
-      <c r="HI235" s="95"/>
-      <c r="HJ235" s="95"/>
-      <c r="HK235" s="95"/>
-      <c r="HL235" s="95"/>
-      <c r="HM235" s="95"/>
-      <c r="HN235" s="95"/>
-      <c r="HO235" s="95"/>
-      <c r="HP235" s="95"/>
-      <c r="HQ235" s="95"/>
-      <c r="HR235" s="95"/>
-      <c r="HS235" s="95"/>
-      <c r="HT235" s="95"/>
-      <c r="HU235" s="95"/>
-      <c r="HV235" s="95"/>
-      <c r="HW235" s="95"/>
-      <c r="HX235" s="95"/>
-      <c r="HY235" s="95"/>
-      <c r="HZ235" s="95"/>
-      <c r="IA235" s="95"/>
-      <c r="IB235" s="95"/>
-      <c r="IC235" s="95"/>
-      <c r="ID235" s="95"/>
-      <c r="IE235" s="95"/>
-      <c r="IF235" s="95"/>
-      <c r="IG235" s="95"/>
-      <c r="IH235" s="95"/>
-      <c r="II235" s="95"/>
-      <c r="IJ235" s="95"/>
-      <c r="IK235" s="95"/>
-      <c r="IL235" s="95"/>
-      <c r="IM235" s="95"/>
-      <c r="IN235" s="95"/>
-      <c r="IO235" s="95"/>
-      <c r="IP235" s="95"/>
-      <c r="IQ235" s="95"/>
-      <c r="IR235" s="95"/>
-      <c r="IS235" s="95"/>
-      <c r="IT235" s="95"/>
-      <c r="IU235" s="95"/>
-      <c r="IV235" s="95"/>
-      <c r="IW235" s="95"/>
-      <c r="IX235" s="95"/>
-      <c r="IY235" s="95"/>
-      <c r="IZ235" s="95"/>
-      <c r="JA235" s="95"/>
-      <c r="JB235" s="95"/>
-      <c r="JC235" s="95"/>
-      <c r="JD235" s="95"/>
-      <c r="JE235" s="95"/>
-      <c r="JF235" s="95"/>
-      <c r="JG235" s="95"/>
-      <c r="JH235" s="95"/>
-      <c r="JI235" s="95"/>
-      <c r="JJ235" s="95"/>
-      <c r="JK235" s="95"/>
-      <c r="JL235" s="95"/>
-      <c r="JM235" s="95"/>
-      <c r="JN235" s="95"/>
-      <c r="JO235" s="95"/>
-      <c r="JP235" s="95"/>
-      <c r="JQ235" s="95"/>
-      <c r="JR235" s="95"/>
-      <c r="JS235" s="95"/>
-      <c r="JT235" s="95"/>
-      <c r="JU235" s="95"/>
-      <c r="JV235" s="95"/>
-      <c r="JW235" s="95"/>
-      <c r="JX235" s="95"/>
-      <c r="JY235" s="95"/>
-      <c r="JZ235" s="95"/>
-      <c r="KA235" s="95"/>
-      <c r="KB235" s="95"/>
-      <c r="KC235" s="95"/>
-      <c r="KD235" s="95"/>
-      <c r="KE235" s="95"/>
-      <c r="KF235" s="95"/>
-      <c r="KG235" s="95"/>
-      <c r="KH235" s="95"/>
-      <c r="KI235" s="95"/>
-      <c r="KJ235" s="95"/>
-      <c r="KK235" s="95"/>
-      <c r="KL235" s="95"/>
-      <c r="KM235" s="95"/>
-      <c r="KN235" s="95"/>
-      <c r="KO235" s="95"/>
-      <c r="KP235" s="95"/>
+      <c r="AT235" s="93"/>
+      <c r="AU235" s="93"/>
+      <c r="AV235" s="93"/>
+      <c r="AW235" s="93"/>
+      <c r="AX235" s="93"/>
+      <c r="AY235" s="93"/>
+      <c r="AZ235" s="93"/>
+      <c r="BA235" s="93"/>
+      <c r="BB235" s="93"/>
+      <c r="BC235" s="93"/>
+      <c r="BD235" s="93"/>
+      <c r="BE235" s="93"/>
+      <c r="BF235" s="93"/>
+      <c r="BG235" s="93"/>
+      <c r="BH235" s="93"/>
+      <c r="BI235" s="93"/>
+      <c r="BJ235" s="93"/>
+      <c r="BK235" s="93"/>
+      <c r="BL235" s="93"/>
+      <c r="BM235" s="93"/>
+      <c r="BN235" s="93"/>
+      <c r="BO235" s="93"/>
+      <c r="BP235" s="93"/>
+      <c r="BQ235" s="93"/>
+      <c r="BR235" s="93"/>
+      <c r="BS235" s="93"/>
+      <c r="BT235" s="93"/>
+      <c r="BU235" s="93"/>
+      <c r="BV235" s="93"/>
+      <c r="BW235" s="93"/>
+      <c r="BX235" s="93"/>
+      <c r="BY235" s="93"/>
+      <c r="BZ235" s="93"/>
+      <c r="CA235" s="93"/>
+      <c r="CB235" s="93"/>
+      <c r="CC235" s="93"/>
+      <c r="CD235" s="93"/>
+      <c r="CE235" s="93"/>
+      <c r="CF235" s="93"/>
+      <c r="CG235" s="93"/>
+      <c r="CH235" s="93"/>
+      <c r="CI235" s="93"/>
+      <c r="CJ235" s="93"/>
+      <c r="CK235" s="93"/>
+      <c r="CL235" s="93"/>
+      <c r="CM235" s="93"/>
+      <c r="CN235" s="93"/>
+      <c r="CO235" s="93"/>
+      <c r="CP235" s="93"/>
+      <c r="CQ235" s="93"/>
+      <c r="CR235" s="93"/>
+      <c r="CS235" s="93"/>
+      <c r="CT235" s="93"/>
+      <c r="CU235" s="93"/>
+      <c r="CV235" s="93"/>
+      <c r="CW235" s="93"/>
+      <c r="CX235" s="93"/>
+      <c r="CY235" s="93"/>
+      <c r="CZ235" s="93"/>
+      <c r="DA235" s="93"/>
+      <c r="DB235" s="93"/>
+      <c r="DC235" s="93"/>
+      <c r="DD235" s="93"/>
+      <c r="DE235" s="93"/>
+      <c r="DF235" s="93"/>
+      <c r="DG235" s="93"/>
+      <c r="DH235" s="93"/>
+      <c r="DI235" s="93"/>
+      <c r="DJ235" s="93"/>
+      <c r="DK235" s="93"/>
+      <c r="DL235" s="93"/>
+      <c r="DM235" s="93"/>
+      <c r="DN235" s="93"/>
+      <c r="DO235" s="93"/>
+      <c r="DP235" s="93"/>
+      <c r="DQ235" s="93"/>
+      <c r="DR235" s="93"/>
+      <c r="DS235" s="93"/>
+      <c r="DT235" s="93"/>
+      <c r="DU235" s="93"/>
+      <c r="DV235" s="93"/>
+      <c r="DW235" s="93"/>
+      <c r="DX235" s="93"/>
+      <c r="DY235" s="93"/>
+      <c r="DZ235" s="93"/>
+      <c r="EA235" s="93"/>
+      <c r="EB235" s="93"/>
+      <c r="EC235" s="93"/>
+      <c r="ED235" s="93"/>
+      <c r="EE235" s="93"/>
+      <c r="EF235" s="93"/>
+      <c r="EG235" s="93"/>
+      <c r="EH235" s="93"/>
+      <c r="EI235" s="93"/>
+      <c r="EJ235" s="93"/>
+      <c r="EK235" s="93"/>
+      <c r="EL235" s="93"/>
+      <c r="EM235" s="93"/>
+      <c r="EN235" s="93"/>
+      <c r="EO235" s="93"/>
+      <c r="EP235" s="93"/>
+      <c r="EQ235" s="93"/>
+      <c r="ER235" s="93"/>
+      <c r="ES235" s="93"/>
+      <c r="ET235" s="93"/>
+      <c r="EU235" s="93"/>
+      <c r="EV235" s="93"/>
+      <c r="EW235" s="93"/>
+      <c r="EX235" s="93"/>
+      <c r="EY235" s="93"/>
+      <c r="EZ235" s="93"/>
+      <c r="FA235" s="93"/>
+      <c r="FB235" s="93"/>
+      <c r="FC235" s="93"/>
+      <c r="FD235" s="93"/>
+      <c r="FE235" s="93"/>
+      <c r="FF235" s="93"/>
+      <c r="FG235" s="93"/>
+      <c r="FH235" s="93"/>
+      <c r="FI235" s="93"/>
+      <c r="FJ235" s="93"/>
+      <c r="FK235" s="93"/>
+      <c r="FL235" s="93"/>
+      <c r="FM235" s="93"/>
+      <c r="FN235" s="93"/>
+      <c r="FO235" s="93"/>
+      <c r="FP235" s="93"/>
+      <c r="FQ235" s="93"/>
+      <c r="FR235" s="93"/>
+      <c r="FS235" s="93"/>
+      <c r="FT235" s="93"/>
+      <c r="FU235" s="93"/>
+      <c r="FV235" s="93"/>
+      <c r="FW235" s="93"/>
+      <c r="FX235" s="93"/>
+      <c r="FY235" s="93"/>
+      <c r="FZ235" s="93"/>
+      <c r="GA235" s="93"/>
+      <c r="GB235" s="93"/>
+      <c r="GC235" s="93"/>
+      <c r="GD235" s="93"/>
+      <c r="GE235" s="93"/>
+      <c r="GF235" s="93"/>
+      <c r="GG235" s="93"/>
+      <c r="GH235" s="93"/>
+      <c r="GI235" s="93"/>
+      <c r="GJ235" s="93"/>
+      <c r="GK235" s="93"/>
+      <c r="GL235" s="93"/>
+      <c r="GM235" s="93"/>
+      <c r="GN235" s="93"/>
+      <c r="GO235" s="93"/>
+      <c r="GP235" s="93"/>
+      <c r="GQ235" s="93"/>
+      <c r="GR235" s="93"/>
+      <c r="GS235" s="93"/>
+      <c r="GT235" s="93"/>
+      <c r="GU235" s="93"/>
+      <c r="GV235" s="93"/>
+      <c r="GW235" s="93"/>
+      <c r="GX235" s="93"/>
+      <c r="GY235" s="93"/>
+      <c r="GZ235" s="93"/>
+      <c r="HA235" s="93"/>
+      <c r="HB235" s="93"/>
+      <c r="HC235" s="93"/>
+      <c r="HD235" s="93"/>
+      <c r="HE235" s="93"/>
+      <c r="HF235" s="93"/>
+      <c r="HG235" s="93"/>
+      <c r="HH235" s="93"/>
+      <c r="HI235" s="93"/>
+      <c r="HJ235" s="93"/>
+      <c r="HK235" s="93"/>
+      <c r="HL235" s="93"/>
+      <c r="HM235" s="93"/>
+      <c r="HN235" s="93"/>
+      <c r="HO235" s="93"/>
+      <c r="HP235" s="93"/>
+      <c r="HQ235" s="93"/>
+      <c r="HR235" s="93"/>
+      <c r="HS235" s="93"/>
+      <c r="HT235" s="93"/>
+      <c r="HU235" s="93"/>
+      <c r="HV235" s="93"/>
+      <c r="HW235" s="93"/>
+      <c r="HX235" s="93"/>
+      <c r="HY235" s="93"/>
+      <c r="HZ235" s="93"/>
+      <c r="IA235" s="93"/>
+      <c r="IB235" s="93"/>
+      <c r="IC235" s="93"/>
+      <c r="ID235" s="93"/>
+      <c r="IE235" s="93"/>
+      <c r="IF235" s="93"/>
+      <c r="IG235" s="93"/>
+      <c r="IH235" s="93"/>
+      <c r="II235" s="93"/>
+      <c r="IJ235" s="93"/>
+      <c r="IK235" s="93"/>
+      <c r="IL235" s="93"/>
+      <c r="IM235" s="93"/>
+      <c r="IN235" s="93"/>
+      <c r="IO235" s="93"/>
+      <c r="IP235" s="93"/>
+      <c r="IQ235" s="93"/>
+      <c r="IR235" s="93"/>
+      <c r="IS235" s="93"/>
+      <c r="IT235" s="93"/>
+      <c r="IU235" s="93"/>
+      <c r="IV235" s="93"/>
+      <c r="IW235" s="93"/>
+      <c r="IX235" s="93"/>
+      <c r="IY235" s="93"/>
+      <c r="IZ235" s="93"/>
+      <c r="JA235" s="93"/>
+      <c r="JB235" s="93"/>
+      <c r="JC235" s="93"/>
+      <c r="JD235" s="93"/>
+      <c r="JE235" s="93"/>
+      <c r="JF235" s="93"/>
+      <c r="JG235" s="93"/>
+      <c r="JH235" s="93"/>
+      <c r="JI235" s="93"/>
+      <c r="JJ235" s="93"/>
+      <c r="JK235" s="93"/>
+      <c r="JL235" s="93"/>
+      <c r="JM235" s="93"/>
+      <c r="JN235" s="93"/>
+      <c r="JO235" s="93"/>
+      <c r="JP235" s="93"/>
+      <c r="JQ235" s="93"/>
+      <c r="JR235" s="93"/>
+      <c r="JS235" s="93"/>
+      <c r="JT235" s="93"/>
+      <c r="JU235" s="93"/>
+      <c r="JV235" s="93"/>
+      <c r="JW235" s="93"/>
+      <c r="JX235" s="93"/>
+      <c r="JY235" s="93"/>
+      <c r="JZ235" s="93"/>
+      <c r="KA235" s="93"/>
+      <c r="KB235" s="93"/>
+      <c r="KC235" s="93"/>
+      <c r="KD235" s="93"/>
+      <c r="KE235" s="93"/>
+      <c r="KF235" s="93"/>
+      <c r="KG235" s="93"/>
+      <c r="KH235" s="93"/>
+      <c r="KI235" s="93"/>
+      <c r="KJ235" s="93"/>
+      <c r="KK235" s="93"/>
+      <c r="KL235" s="93"/>
+      <c r="KM235" s="93"/>
+      <c r="KN235" s="93"/>
+      <c r="KO235" s="93"/>
+      <c r="KP235" s="93"/>
     </row>
     <row r="236" spans="1:302" x14ac:dyDescent="0.2">
-      <c r="B236" s="91">
-        <v>3</v>
-      </c>
-      <c r="C236" s="91">
-        <v>3</v>
-      </c>
-      <c r="D236" s="91">
-        <v>3</v>
-      </c>
-      <c r="E236" s="91">
-        <v>0</v>
-      </c>
-      <c r="AH236" s="91">
-        <v>0</v>
-      </c>
-      <c r="AI236" s="91">
-        <v>0</v>
-      </c>
-      <c r="AJ236" s="91">
-        <v>0</v>
-      </c>
-      <c r="AK236" s="91">
+      <c r="B236">
+        <v>3</v>
+      </c>
+      <c r="C236">
+        <v>3</v>
+      </c>
+      <c r="D236">
+        <v>3</v>
+      </c>
+      <c r="E236">
+        <v>0</v>
+      </c>
+      <c r="AH236">
+        <v>0</v>
+      </c>
+      <c r="AI236">
+        <v>0</v>
+      </c>
+      <c r="AJ236">
+        <v>0</v>
+      </c>
+      <c r="AK236">
         <v>0</v>
       </c>
     </row>
@@ -43014,16 +43019,16 @@
       <c r="A237" s="46">
         <v>108</v>
       </c>
-      <c r="B237" s="92">
-        <v>3</v>
-      </c>
-      <c r="C237" s="92">
-        <v>3</v>
-      </c>
-      <c r="D237" s="92">
-        <v>3</v>
-      </c>
-      <c r="E237" s="92">
+      <c r="B237" s="29">
+        <v>3</v>
+      </c>
+      <c r="C237" s="29">
+        <v>3</v>
+      </c>
+      <c r="D237" s="29">
+        <v>3</v>
+      </c>
+      <c r="E237" s="29">
         <v>3</v>
       </c>
       <c r="F237" s="28"/>
@@ -43065,17 +43070,17 @@
       <c r="AD237" s="65"/>
       <c r="AE237" s="65"/>
       <c r="AF237" s="65"/>
-      <c r="AG237" s="93"/>
-      <c r="AH237" s="92">
-        <v>3</v>
-      </c>
-      <c r="AI237" s="92">
-        <v>3</v>
-      </c>
-      <c r="AJ237" s="92">
-        <v>3</v>
-      </c>
-      <c r="AK237" s="92">
+      <c r="AG237" s="91"/>
+      <c r="AH237" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI237" s="29">
+        <v>3</v>
+      </c>
+      <c r="AJ237" s="29">
+        <v>3</v>
+      </c>
+      <c r="AK237" s="29">
         <v>3</v>
       </c>
       <c r="AP237" s="29">
@@ -43084,293 +43089,293 @@
       <c r="AQ237" s="29">
         <v>0</v>
       </c>
-      <c r="AR237" s="94" t="b">
+      <c r="AR237" s="92" t="b">
         <v>0</v>
       </c>
       <c r="AS237" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AT237" s="95"/>
-      <c r="AU237" s="95"/>
-      <c r="AV237" s="95"/>
-      <c r="AW237" s="95"/>
-      <c r="AX237" s="95"/>
-      <c r="AY237" s="95"/>
-      <c r="AZ237" s="95"/>
-      <c r="BA237" s="95"/>
-      <c r="BB237" s="95"/>
-      <c r="BC237" s="95"/>
-      <c r="BD237" s="95"/>
-      <c r="BE237" s="95"/>
-      <c r="BF237" s="95"/>
-      <c r="BG237" s="95"/>
-      <c r="BH237" s="95"/>
-      <c r="BI237" s="95"/>
-      <c r="BJ237" s="95"/>
-      <c r="BK237" s="95"/>
-      <c r="BL237" s="95"/>
-      <c r="BM237" s="95"/>
-      <c r="BN237" s="95"/>
-      <c r="BO237" s="95"/>
-      <c r="BP237" s="95"/>
-      <c r="BQ237" s="95"/>
-      <c r="BR237" s="95"/>
-      <c r="BS237" s="95"/>
-      <c r="BT237" s="95"/>
-      <c r="BU237" s="95"/>
-      <c r="BV237" s="95"/>
-      <c r="BW237" s="95"/>
-      <c r="BX237" s="95"/>
-      <c r="BY237" s="95"/>
-      <c r="BZ237" s="95"/>
-      <c r="CA237" s="95"/>
-      <c r="CB237" s="95"/>
-      <c r="CC237" s="95"/>
-      <c r="CD237" s="95"/>
-      <c r="CE237" s="95"/>
-      <c r="CF237" s="95"/>
-      <c r="CG237" s="95"/>
-      <c r="CH237" s="95"/>
-      <c r="CI237" s="95"/>
-      <c r="CJ237" s="95"/>
-      <c r="CK237" s="95"/>
-      <c r="CL237" s="95"/>
-      <c r="CM237" s="95"/>
-      <c r="CN237" s="95"/>
-      <c r="CO237" s="95"/>
-      <c r="CP237" s="95"/>
-      <c r="CQ237" s="95"/>
-      <c r="CR237" s="95"/>
-      <c r="CS237" s="95"/>
-      <c r="CT237" s="95"/>
-      <c r="CU237" s="95"/>
-      <c r="CV237" s="95"/>
-      <c r="CW237" s="95"/>
-      <c r="CX237" s="95"/>
-      <c r="CY237" s="95"/>
-      <c r="CZ237" s="95"/>
-      <c r="DA237" s="95"/>
-      <c r="DB237" s="95"/>
-      <c r="DC237" s="95"/>
-      <c r="DD237" s="95"/>
-      <c r="DE237" s="95"/>
-      <c r="DF237" s="95"/>
-      <c r="DG237" s="95"/>
-      <c r="DH237" s="95"/>
-      <c r="DI237" s="95"/>
-      <c r="DJ237" s="95"/>
-      <c r="DK237" s="95"/>
-      <c r="DL237" s="95"/>
-      <c r="DM237" s="95"/>
-      <c r="DN237" s="95"/>
-      <c r="DO237" s="95"/>
-      <c r="DP237" s="95"/>
-      <c r="DQ237" s="95"/>
-      <c r="DR237" s="95"/>
-      <c r="DS237" s="95"/>
-      <c r="DT237" s="95"/>
-      <c r="DU237" s="95"/>
-      <c r="DV237" s="95"/>
-      <c r="DW237" s="95"/>
-      <c r="DX237" s="95"/>
-      <c r="DY237" s="95"/>
-      <c r="DZ237" s="95"/>
-      <c r="EA237" s="95"/>
-      <c r="EB237" s="95"/>
-      <c r="EC237" s="95"/>
-      <c r="ED237" s="95"/>
-      <c r="EE237" s="95"/>
-      <c r="EF237" s="95"/>
-      <c r="EG237" s="95"/>
-      <c r="EH237" s="95"/>
-      <c r="EI237" s="95"/>
-      <c r="EJ237" s="95"/>
-      <c r="EK237" s="95"/>
-      <c r="EL237" s="95"/>
-      <c r="EM237" s="95"/>
-      <c r="EN237" s="95"/>
-      <c r="EO237" s="95"/>
-      <c r="EP237" s="95"/>
-      <c r="EQ237" s="95"/>
-      <c r="ER237" s="95"/>
-      <c r="ES237" s="95"/>
-      <c r="ET237" s="95"/>
-      <c r="EU237" s="95"/>
-      <c r="EV237" s="95"/>
-      <c r="EW237" s="95"/>
-      <c r="EX237" s="95"/>
-      <c r="EY237" s="95"/>
-      <c r="EZ237" s="95"/>
-      <c r="FA237" s="95"/>
-      <c r="FB237" s="95"/>
-      <c r="FC237" s="95"/>
-      <c r="FD237" s="95"/>
-      <c r="FE237" s="95"/>
-      <c r="FF237" s="95"/>
-      <c r="FG237" s="95"/>
-      <c r="FH237" s="95"/>
-      <c r="FI237" s="95"/>
-      <c r="FJ237" s="95"/>
-      <c r="FK237" s="95"/>
-      <c r="FL237" s="95"/>
-      <c r="FM237" s="95"/>
-      <c r="FN237" s="95"/>
-      <c r="FO237" s="95"/>
-      <c r="FP237" s="95"/>
-      <c r="FQ237" s="95"/>
-      <c r="FR237" s="95"/>
-      <c r="FS237" s="95"/>
-      <c r="FT237" s="95"/>
-      <c r="FU237" s="95"/>
-      <c r="FV237" s="95"/>
-      <c r="FW237" s="95"/>
-      <c r="FX237" s="95"/>
-      <c r="FY237" s="95"/>
-      <c r="FZ237" s="95"/>
-      <c r="GA237" s="95"/>
-      <c r="GB237" s="95"/>
-      <c r="GC237" s="95"/>
-      <c r="GD237" s="95"/>
-      <c r="GE237" s="95"/>
-      <c r="GF237" s="95"/>
-      <c r="GG237" s="95"/>
-      <c r="GH237" s="95"/>
-      <c r="GI237" s="95"/>
-      <c r="GJ237" s="95"/>
-      <c r="GK237" s="95"/>
-      <c r="GL237" s="95"/>
-      <c r="GM237" s="95"/>
-      <c r="GN237" s="95"/>
-      <c r="GO237" s="95"/>
-      <c r="GP237" s="95"/>
-      <c r="GQ237" s="95"/>
-      <c r="GR237" s="95"/>
-      <c r="GS237" s="95"/>
-      <c r="GT237" s="95"/>
-      <c r="GU237" s="95"/>
-      <c r="GV237" s="95"/>
-      <c r="GW237" s="95"/>
-      <c r="GX237" s="95"/>
-      <c r="GY237" s="95"/>
-      <c r="GZ237" s="95"/>
-      <c r="HA237" s="95"/>
-      <c r="HB237" s="95"/>
-      <c r="HC237" s="95"/>
-      <c r="HD237" s="95"/>
-      <c r="HE237" s="95"/>
-      <c r="HF237" s="95"/>
-      <c r="HG237" s="95"/>
-      <c r="HH237" s="95"/>
-      <c r="HI237" s="95"/>
-      <c r="HJ237" s="95"/>
-      <c r="HK237" s="95"/>
-      <c r="HL237" s="95"/>
-      <c r="HM237" s="95"/>
-      <c r="HN237" s="95"/>
-      <c r="HO237" s="95"/>
-      <c r="HP237" s="95"/>
-      <c r="HQ237" s="95"/>
-      <c r="HR237" s="95"/>
-      <c r="HS237" s="95"/>
-      <c r="HT237" s="95"/>
-      <c r="HU237" s="95"/>
-      <c r="HV237" s="95"/>
-      <c r="HW237" s="95"/>
-      <c r="HX237" s="95"/>
-      <c r="HY237" s="95"/>
-      <c r="HZ237" s="95"/>
-      <c r="IA237" s="95"/>
-      <c r="IB237" s="95"/>
-      <c r="IC237" s="95"/>
-      <c r="ID237" s="95"/>
-      <c r="IE237" s="95"/>
-      <c r="IF237" s="95"/>
-      <c r="IG237" s="95"/>
-      <c r="IH237" s="95"/>
-      <c r="II237" s="95"/>
-      <c r="IJ237" s="95"/>
-      <c r="IK237" s="95"/>
-      <c r="IL237" s="95"/>
-      <c r="IM237" s="95"/>
-      <c r="IN237" s="95"/>
-      <c r="IO237" s="95"/>
-      <c r="IP237" s="95"/>
-      <c r="IQ237" s="95"/>
-      <c r="IR237" s="95"/>
-      <c r="IS237" s="95"/>
-      <c r="IT237" s="95"/>
-      <c r="IU237" s="95"/>
-      <c r="IV237" s="95"/>
-      <c r="IW237" s="95"/>
-      <c r="IX237" s="95"/>
-      <c r="IY237" s="95"/>
-      <c r="IZ237" s="95"/>
-      <c r="JA237" s="95"/>
-      <c r="JB237" s="95"/>
-      <c r="JC237" s="95"/>
-      <c r="JD237" s="95"/>
-      <c r="JE237" s="95"/>
-      <c r="JF237" s="95"/>
-      <c r="JG237" s="95"/>
-      <c r="JH237" s="95"/>
-      <c r="JI237" s="95"/>
-      <c r="JJ237" s="95"/>
-      <c r="JK237" s="95"/>
-      <c r="JL237" s="95"/>
-      <c r="JM237" s="95"/>
-      <c r="JN237" s="95"/>
-      <c r="JO237" s="95"/>
-      <c r="JP237" s="95"/>
-      <c r="JQ237" s="95"/>
-      <c r="JR237" s="95"/>
-      <c r="JS237" s="95"/>
-      <c r="JT237" s="95"/>
-      <c r="JU237" s="95"/>
-      <c r="JV237" s="95"/>
-      <c r="JW237" s="95"/>
-      <c r="JX237" s="95"/>
-      <c r="JY237" s="95"/>
-      <c r="JZ237" s="95"/>
-      <c r="KA237" s="95"/>
-      <c r="KB237" s="95"/>
-      <c r="KC237" s="95"/>
-      <c r="KD237" s="95"/>
-      <c r="KE237" s="95"/>
-      <c r="KF237" s="95"/>
-      <c r="KG237" s="95"/>
-      <c r="KH237" s="95"/>
-      <c r="KI237" s="95"/>
-      <c r="KJ237" s="95"/>
-      <c r="KK237" s="95"/>
-      <c r="KL237" s="95"/>
-      <c r="KM237" s="95"/>
-      <c r="KN237" s="95"/>
-      <c r="KO237" s="95"/>
-      <c r="KP237" s="95"/>
+      <c r="AT237" s="93"/>
+      <c r="AU237" s="93"/>
+      <c r="AV237" s="93"/>
+      <c r="AW237" s="93"/>
+      <c r="AX237" s="93"/>
+      <c r="AY237" s="93"/>
+      <c r="AZ237" s="93"/>
+      <c r="BA237" s="93"/>
+      <c r="BB237" s="93"/>
+      <c r="BC237" s="93"/>
+      <c r="BD237" s="93"/>
+      <c r="BE237" s="93"/>
+      <c r="BF237" s="93"/>
+      <c r="BG237" s="93"/>
+      <c r="BH237" s="93"/>
+      <c r="BI237" s="93"/>
+      <c r="BJ237" s="93"/>
+      <c r="BK237" s="93"/>
+      <c r="BL237" s="93"/>
+      <c r="BM237" s="93"/>
+      <c r="BN237" s="93"/>
+      <c r="BO237" s="93"/>
+      <c r="BP237" s="93"/>
+      <c r="BQ237" s="93"/>
+      <c r="BR237" s="93"/>
+      <c r="BS237" s="93"/>
+      <c r="BT237" s="93"/>
+      <c r="BU237" s="93"/>
+      <c r="BV237" s="93"/>
+      <c r="BW237" s="93"/>
+      <c r="BX237" s="93"/>
+      <c r="BY237" s="93"/>
+      <c r="BZ237" s="93"/>
+      <c r="CA237" s="93"/>
+      <c r="CB237" s="93"/>
+      <c r="CC237" s="93"/>
+      <c r="CD237" s="93"/>
+      <c r="CE237" s="93"/>
+      <c r="CF237" s="93"/>
+      <c r="CG237" s="93"/>
+      <c r="CH237" s="93"/>
+      <c r="CI237" s="93"/>
+      <c r="CJ237" s="93"/>
+      <c r="CK237" s="93"/>
+      <c r="CL237" s="93"/>
+      <c r="CM237" s="93"/>
+      <c r="CN237" s="93"/>
+      <c r="CO237" s="93"/>
+      <c r="CP237" s="93"/>
+      <c r="CQ237" s="93"/>
+      <c r="CR237" s="93"/>
+      <c r="CS237" s="93"/>
+      <c r="CT237" s="93"/>
+      <c r="CU237" s="93"/>
+      <c r="CV237" s="93"/>
+      <c r="CW237" s="93"/>
+      <c r="CX237" s="93"/>
+      <c r="CY237" s="93"/>
+      <c r="CZ237" s="93"/>
+      <c r="DA237" s="93"/>
+      <c r="DB237" s="93"/>
+      <c r="DC237" s="93"/>
+      <c r="DD237" s="93"/>
+      <c r="DE237" s="93"/>
+      <c r="DF237" s="93"/>
+      <c r="DG237" s="93"/>
+      <c r="DH237" s="93"/>
+      <c r="DI237" s="93"/>
+      <c r="DJ237" s="93"/>
+      <c r="DK237" s="93"/>
+      <c r="DL237" s="93"/>
+      <c r="DM237" s="93"/>
+      <c r="DN237" s="93"/>
+      <c r="DO237" s="93"/>
+      <c r="DP237" s="93"/>
+      <c r="DQ237" s="93"/>
+      <c r="DR237" s="93"/>
+      <c r="DS237" s="93"/>
+      <c r="DT237" s="93"/>
+      <c r="DU237" s="93"/>
+      <c r="DV237" s="93"/>
+      <c r="DW237" s="93"/>
+      <c r="DX237" s="93"/>
+      <c r="DY237" s="93"/>
+      <c r="DZ237" s="93"/>
+      <c r="EA237" s="93"/>
+      <c r="EB237" s="93"/>
+      <c r="EC237" s="93"/>
+      <c r="ED237" s="93"/>
+      <c r="EE237" s="93"/>
+      <c r="EF237" s="93"/>
+      <c r="EG237" s="93"/>
+      <c r="EH237" s="93"/>
+      <c r="EI237" s="93"/>
+      <c r="EJ237" s="93"/>
+      <c r="EK237" s="93"/>
+      <c r="EL237" s="93"/>
+      <c r="EM237" s="93"/>
+      <c r="EN237" s="93"/>
+      <c r="EO237" s="93"/>
+      <c r="EP237" s="93"/>
+      <c r="EQ237" s="93"/>
+      <c r="ER237" s="93"/>
+      <c r="ES237" s="93"/>
+      <c r="ET237" s="93"/>
+      <c r="EU237" s="93"/>
+      <c r="EV237" s="93"/>
+      <c r="EW237" s="93"/>
+      <c r="EX237" s="93"/>
+      <c r="EY237" s="93"/>
+      <c r="EZ237" s="93"/>
+      <c r="FA237" s="93"/>
+      <c r="FB237" s="93"/>
+      <c r="FC237" s="93"/>
+      <c r="FD237" s="93"/>
+      <c r="FE237" s="93"/>
+      <c r="FF237" s="93"/>
+      <c r="FG237" s="93"/>
+      <c r="FH237" s="93"/>
+      <c r="FI237" s="93"/>
+      <c r="FJ237" s="93"/>
+      <c r="FK237" s="93"/>
+      <c r="FL237" s="93"/>
+      <c r="FM237" s="93"/>
+      <c r="FN237" s="93"/>
+      <c r="FO237" s="93"/>
+      <c r="FP237" s="93"/>
+      <c r="FQ237" s="93"/>
+      <c r="FR237" s="93"/>
+      <c r="FS237" s="93"/>
+      <c r="FT237" s="93"/>
+      <c r="FU237" s="93"/>
+      <c r="FV237" s="93"/>
+      <c r="FW237" s="93"/>
+      <c r="FX237" s="93"/>
+      <c r="FY237" s="93"/>
+      <c r="FZ237" s="93"/>
+      <c r="GA237" s="93"/>
+      <c r="GB237" s="93"/>
+      <c r="GC237" s="93"/>
+      <c r="GD237" s="93"/>
+      <c r="GE237" s="93"/>
+      <c r="GF237" s="93"/>
+      <c r="GG237" s="93"/>
+      <c r="GH237" s="93"/>
+      <c r="GI237" s="93"/>
+      <c r="GJ237" s="93"/>
+      <c r="GK237" s="93"/>
+      <c r="GL237" s="93"/>
+      <c r="GM237" s="93"/>
+      <c r="GN237" s="93"/>
+      <c r="GO237" s="93"/>
+      <c r="GP237" s="93"/>
+      <c r="GQ237" s="93"/>
+      <c r="GR237" s="93"/>
+      <c r="GS237" s="93"/>
+      <c r="GT237" s="93"/>
+      <c r="GU237" s="93"/>
+      <c r="GV237" s="93"/>
+      <c r="GW237" s="93"/>
+      <c r="GX237" s="93"/>
+      <c r="GY237" s="93"/>
+      <c r="GZ237" s="93"/>
+      <c r="HA237" s="93"/>
+      <c r="HB237" s="93"/>
+      <c r="HC237" s="93"/>
+      <c r="HD237" s="93"/>
+      <c r="HE237" s="93"/>
+      <c r="HF237" s="93"/>
+      <c r="HG237" s="93"/>
+      <c r="HH237" s="93"/>
+      <c r="HI237" s="93"/>
+      <c r="HJ237" s="93"/>
+      <c r="HK237" s="93"/>
+      <c r="HL237" s="93"/>
+      <c r="HM237" s="93"/>
+      <c r="HN237" s="93"/>
+      <c r="HO237" s="93"/>
+      <c r="HP237" s="93"/>
+      <c r="HQ237" s="93"/>
+      <c r="HR237" s="93"/>
+      <c r="HS237" s="93"/>
+      <c r="HT237" s="93"/>
+      <c r="HU237" s="93"/>
+      <c r="HV237" s="93"/>
+      <c r="HW237" s="93"/>
+      <c r="HX237" s="93"/>
+      <c r="HY237" s="93"/>
+      <c r="HZ237" s="93"/>
+      <c r="IA237" s="93"/>
+      <c r="IB237" s="93"/>
+      <c r="IC237" s="93"/>
+      <c r="ID237" s="93"/>
+      <c r="IE237" s="93"/>
+      <c r="IF237" s="93"/>
+      <c r="IG237" s="93"/>
+      <c r="IH237" s="93"/>
+      <c r="II237" s="93"/>
+      <c r="IJ237" s="93"/>
+      <c r="IK237" s="93"/>
+      <c r="IL237" s="93"/>
+      <c r="IM237" s="93"/>
+      <c r="IN237" s="93"/>
+      <c r="IO237" s="93"/>
+      <c r="IP237" s="93"/>
+      <c r="IQ237" s="93"/>
+      <c r="IR237" s="93"/>
+      <c r="IS237" s="93"/>
+      <c r="IT237" s="93"/>
+      <c r="IU237" s="93"/>
+      <c r="IV237" s="93"/>
+      <c r="IW237" s="93"/>
+      <c r="IX237" s="93"/>
+      <c r="IY237" s="93"/>
+      <c r="IZ237" s="93"/>
+      <c r="JA237" s="93"/>
+      <c r="JB237" s="93"/>
+      <c r="JC237" s="93"/>
+      <c r="JD237" s="93"/>
+      <c r="JE237" s="93"/>
+      <c r="JF237" s="93"/>
+      <c r="JG237" s="93"/>
+      <c r="JH237" s="93"/>
+      <c r="JI237" s="93"/>
+      <c r="JJ237" s="93"/>
+      <c r="JK237" s="93"/>
+      <c r="JL237" s="93"/>
+      <c r="JM237" s="93"/>
+      <c r="JN237" s="93"/>
+      <c r="JO237" s="93"/>
+      <c r="JP237" s="93"/>
+      <c r="JQ237" s="93"/>
+      <c r="JR237" s="93"/>
+      <c r="JS237" s="93"/>
+      <c r="JT237" s="93"/>
+      <c r="JU237" s="93"/>
+      <c r="JV237" s="93"/>
+      <c r="JW237" s="93"/>
+      <c r="JX237" s="93"/>
+      <c r="JY237" s="93"/>
+      <c r="JZ237" s="93"/>
+      <c r="KA237" s="93"/>
+      <c r="KB237" s="93"/>
+      <c r="KC237" s="93"/>
+      <c r="KD237" s="93"/>
+      <c r="KE237" s="93"/>
+      <c r="KF237" s="93"/>
+      <c r="KG237" s="93"/>
+      <c r="KH237" s="93"/>
+      <c r="KI237" s="93"/>
+      <c r="KJ237" s="93"/>
+      <c r="KK237" s="93"/>
+      <c r="KL237" s="93"/>
+      <c r="KM237" s="93"/>
+      <c r="KN237" s="93"/>
+      <c r="KO237" s="93"/>
+      <c r="KP237" s="93"/>
     </row>
     <row r="238" spans="1:302" x14ac:dyDescent="0.2">
-      <c r="B238" s="91">
-        <v>3</v>
-      </c>
-      <c r="C238" s="91">
-        <v>3</v>
-      </c>
-      <c r="D238" s="91">
-        <v>3</v>
-      </c>
-      <c r="E238" s="91">
-        <v>3</v>
-      </c>
-      <c r="AH238" s="91">
-        <v>3</v>
-      </c>
-      <c r="AI238" s="91">
-        <v>3</v>
-      </c>
-      <c r="AJ238" s="91">
-        <v>3</v>
-      </c>
-      <c r="AK238" s="91">
+      <c r="B238">
+        <v>3</v>
+      </c>
+      <c r="C238">
+        <v>3</v>
+      </c>
+      <c r="D238">
+        <v>3</v>
+      </c>
+      <c r="E238">
+        <v>3</v>
+      </c>
+      <c r="AH238">
+        <v>3</v>
+      </c>
+      <c r="AI238">
+        <v>3</v>
+      </c>
+      <c r="AJ238">
+        <v>3</v>
+      </c>
+      <c r="AK238">
         <v>3</v>
       </c>
     </row>
@@ -43378,16 +43383,16 @@
       <c r="A239" s="46">
         <v>109</v>
       </c>
-      <c r="B239" s="92">
-        <v>3</v>
-      </c>
-      <c r="C239" s="92">
-        <v>3</v>
-      </c>
-      <c r="D239" s="92">
-        <v>2</v>
-      </c>
-      <c r="E239" s="92">
+      <c r="B239" s="29">
+        <v>3</v>
+      </c>
+      <c r="C239" s="29">
+        <v>3</v>
+      </c>
+      <c r="D239" s="29">
+        <v>2</v>
+      </c>
+      <c r="E239" s="29">
         <v>4</v>
       </c>
       <c r="F239" s="28"/>
@@ -43429,17 +43434,17 @@
       <c r="AD239" s="65"/>
       <c r="AE239" s="65"/>
       <c r="AF239" s="65"/>
-      <c r="AG239" s="93"/>
-      <c r="AH239" s="92">
-        <v>3</v>
-      </c>
-      <c r="AI239" s="92">
-        <v>3</v>
-      </c>
-      <c r="AJ239" s="92">
-        <v>2</v>
-      </c>
-      <c r="AK239" s="92">
+      <c r="AG239" s="91"/>
+      <c r="AH239" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI239" s="29">
+        <v>3</v>
+      </c>
+      <c r="AJ239" s="29">
+        <v>2</v>
+      </c>
+      <c r="AK239" s="29">
         <v>4</v>
       </c>
       <c r="AP239" s="29">
@@ -43448,293 +43453,293 @@
       <c r="AQ239" s="29">
         <v>12</v>
       </c>
-      <c r="AR239" s="94" t="b">
+      <c r="AR239" s="92" t="b">
         <v>1</v>
       </c>
       <c r="AS239" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="AT239" s="95"/>
-      <c r="AU239" s="95"/>
-      <c r="AV239" s="95"/>
-      <c r="AW239" s="95"/>
-      <c r="AX239" s="95"/>
-      <c r="AY239" s="95"/>
-      <c r="AZ239" s="95"/>
-      <c r="BA239" s="95"/>
-      <c r="BB239" s="95"/>
-      <c r="BC239" s="95"/>
-      <c r="BD239" s="95"/>
-      <c r="BE239" s="95"/>
-      <c r="BF239" s="95"/>
-      <c r="BG239" s="95"/>
-      <c r="BH239" s="95"/>
-      <c r="BI239" s="95"/>
-      <c r="BJ239" s="95"/>
-      <c r="BK239" s="95"/>
-      <c r="BL239" s="95"/>
-      <c r="BM239" s="95"/>
-      <c r="BN239" s="95"/>
-      <c r="BO239" s="95"/>
-      <c r="BP239" s="95"/>
-      <c r="BQ239" s="95"/>
-      <c r="BR239" s="95"/>
-      <c r="BS239" s="95"/>
-      <c r="BT239" s="95"/>
-      <c r="BU239" s="95"/>
-      <c r="BV239" s="95"/>
-      <c r="BW239" s="95"/>
-      <c r="BX239" s="95"/>
-      <c r="BY239" s="95"/>
-      <c r="BZ239" s="95"/>
-      <c r="CA239" s="95"/>
-      <c r="CB239" s="95"/>
-      <c r="CC239" s="95"/>
-      <c r="CD239" s="95"/>
-      <c r="CE239" s="95"/>
-      <c r="CF239" s="95"/>
-      <c r="CG239" s="95"/>
-      <c r="CH239" s="95"/>
-      <c r="CI239" s="95"/>
-      <c r="CJ239" s="95"/>
-      <c r="CK239" s="95"/>
-      <c r="CL239" s="95"/>
-      <c r="CM239" s="95"/>
-      <c r="CN239" s="95"/>
-      <c r="CO239" s="95"/>
-      <c r="CP239" s="95"/>
-      <c r="CQ239" s="95"/>
-      <c r="CR239" s="95"/>
-      <c r="CS239" s="95"/>
-      <c r="CT239" s="95"/>
-      <c r="CU239" s="95"/>
-      <c r="CV239" s="95"/>
-      <c r="CW239" s="95"/>
-      <c r="CX239" s="95"/>
-      <c r="CY239" s="95"/>
-      <c r="CZ239" s="95"/>
-      <c r="DA239" s="95"/>
-      <c r="DB239" s="95"/>
-      <c r="DC239" s="95"/>
-      <c r="DD239" s="95"/>
-      <c r="DE239" s="95"/>
-      <c r="DF239" s="95"/>
-      <c r="DG239" s="95"/>
-      <c r="DH239" s="95"/>
-      <c r="DI239" s="95"/>
-      <c r="DJ239" s="95"/>
-      <c r="DK239" s="95"/>
-      <c r="DL239" s="95"/>
-      <c r="DM239" s="95"/>
-      <c r="DN239" s="95"/>
-      <c r="DO239" s="95"/>
-      <c r="DP239" s="95"/>
-      <c r="DQ239" s="95"/>
-      <c r="DR239" s="95"/>
-      <c r="DS239" s="95"/>
-      <c r="DT239" s="95"/>
-      <c r="DU239" s="95"/>
-      <c r="DV239" s="95"/>
-      <c r="DW239" s="95"/>
-      <c r="DX239" s="95"/>
-      <c r="DY239" s="95"/>
-      <c r="DZ239" s="95"/>
-      <c r="EA239" s="95"/>
-      <c r="EB239" s="95"/>
-      <c r="EC239" s="95"/>
-      <c r="ED239" s="95"/>
-      <c r="EE239" s="95"/>
-      <c r="EF239" s="95"/>
-      <c r="EG239" s="95"/>
-      <c r="EH239" s="95"/>
-      <c r="EI239" s="95"/>
-      <c r="EJ239" s="95"/>
-      <c r="EK239" s="95"/>
-      <c r="EL239" s="95"/>
-      <c r="EM239" s="95"/>
-      <c r="EN239" s="95"/>
-      <c r="EO239" s="95"/>
-      <c r="EP239" s="95"/>
-      <c r="EQ239" s="95"/>
-      <c r="ER239" s="95"/>
-      <c r="ES239" s="95"/>
-      <c r="ET239" s="95"/>
-      <c r="EU239" s="95"/>
-      <c r="EV239" s="95"/>
-      <c r="EW239" s="95"/>
-      <c r="EX239" s="95"/>
-      <c r="EY239" s="95"/>
-      <c r="EZ239" s="95"/>
-      <c r="FA239" s="95"/>
-      <c r="FB239" s="95"/>
-      <c r="FC239" s="95"/>
-      <c r="FD239" s="95"/>
-      <c r="FE239" s="95"/>
-      <c r="FF239" s="95"/>
-      <c r="FG239" s="95"/>
-      <c r="FH239" s="95"/>
-      <c r="FI239" s="95"/>
-      <c r="FJ239" s="95"/>
-      <c r="FK239" s="95"/>
-      <c r="FL239" s="95"/>
-      <c r="FM239" s="95"/>
-      <c r="FN239" s="95"/>
-      <c r="FO239" s="95"/>
-      <c r="FP239" s="95"/>
-      <c r="FQ239" s="95"/>
-      <c r="FR239" s="95"/>
-      <c r="FS239" s="95"/>
-      <c r="FT239" s="95"/>
-      <c r="FU239" s="95"/>
-      <c r="FV239" s="95"/>
-      <c r="FW239" s="95"/>
-      <c r="FX239" s="95"/>
-      <c r="FY239" s="95"/>
-      <c r="FZ239" s="95"/>
-      <c r="GA239" s="95"/>
-      <c r="GB239" s="95"/>
-      <c r="GC239" s="95"/>
-      <c r="GD239" s="95"/>
-      <c r="GE239" s="95"/>
-      <c r="GF239" s="95"/>
-      <c r="GG239" s="95"/>
-      <c r="GH239" s="95"/>
-      <c r="GI239" s="95"/>
-      <c r="GJ239" s="95"/>
-      <c r="GK239" s="95"/>
-      <c r="GL239" s="95"/>
-      <c r="GM239" s="95"/>
-      <c r="GN239" s="95"/>
-      <c r="GO239" s="95"/>
-      <c r="GP239" s="95"/>
-      <c r="GQ239" s="95"/>
-      <c r="GR239" s="95"/>
-      <c r="GS239" s="95"/>
-      <c r="GT239" s="95"/>
-      <c r="GU239" s="95"/>
-      <c r="GV239" s="95"/>
-      <c r="GW239" s="95"/>
-      <c r="GX239" s="95"/>
-      <c r="GY239" s="95"/>
-      <c r="GZ239" s="95"/>
-      <c r="HA239" s="95"/>
-      <c r="HB239" s="95"/>
-      <c r="HC239" s="95"/>
-      <c r="HD239" s="95"/>
-      <c r="HE239" s="95"/>
-      <c r="HF239" s="95"/>
-      <c r="HG239" s="95"/>
-      <c r="HH239" s="95"/>
-      <c r="HI239" s="95"/>
-      <c r="HJ239" s="95"/>
-      <c r="HK239" s="95"/>
-      <c r="HL239" s="95"/>
-      <c r="HM239" s="95"/>
-      <c r="HN239" s="95"/>
-      <c r="HO239" s="95"/>
-      <c r="HP239" s="95"/>
-      <c r="HQ239" s="95"/>
-      <c r="HR239" s="95"/>
-      <c r="HS239" s="95"/>
-      <c r="HT239" s="95"/>
-      <c r="HU239" s="95"/>
-      <c r="HV239" s="95"/>
-      <c r="HW239" s="95"/>
-      <c r="HX239" s="95"/>
-      <c r="HY239" s="95"/>
-      <c r="HZ239" s="95"/>
-      <c r="IA239" s="95"/>
-      <c r="IB239" s="95"/>
-      <c r="IC239" s="95"/>
-      <c r="ID239" s="95"/>
-      <c r="IE239" s="95"/>
-      <c r="IF239" s="95"/>
-      <c r="IG239" s="95"/>
-      <c r="IH239" s="95"/>
-      <c r="II239" s="95"/>
-      <c r="IJ239" s="95"/>
-      <c r="IK239" s="95"/>
-      <c r="IL239" s="95"/>
-      <c r="IM239" s="95"/>
-      <c r="IN239" s="95"/>
-      <c r="IO239" s="95"/>
-      <c r="IP239" s="95"/>
-      <c r="IQ239" s="95"/>
-      <c r="IR239" s="95"/>
-      <c r="IS239" s="95"/>
-      <c r="IT239" s="95"/>
-      <c r="IU239" s="95"/>
-      <c r="IV239" s="95"/>
-      <c r="IW239" s="95"/>
-      <c r="IX239" s="95"/>
-      <c r="IY239" s="95"/>
-      <c r="IZ239" s="95"/>
-      <c r="JA239" s="95"/>
-      <c r="JB239" s="95"/>
-      <c r="JC239" s="95"/>
-      <c r="JD239" s="95"/>
-      <c r="JE239" s="95"/>
-      <c r="JF239" s="95"/>
-      <c r="JG239" s="95"/>
-      <c r="JH239" s="95"/>
-      <c r="JI239" s="95"/>
-      <c r="JJ239" s="95"/>
-      <c r="JK239" s="95"/>
-      <c r="JL239" s="95"/>
-      <c r="JM239" s="95"/>
-      <c r="JN239" s="95"/>
-      <c r="JO239" s="95"/>
-      <c r="JP239" s="95"/>
-      <c r="JQ239" s="95"/>
-      <c r="JR239" s="95"/>
-      <c r="JS239" s="95"/>
-      <c r="JT239" s="95"/>
-      <c r="JU239" s="95"/>
-      <c r="JV239" s="95"/>
-      <c r="JW239" s="95"/>
-      <c r="JX239" s="95"/>
-      <c r="JY239" s="95"/>
-      <c r="JZ239" s="95"/>
-      <c r="KA239" s="95"/>
-      <c r="KB239" s="95"/>
-      <c r="KC239" s="95"/>
-      <c r="KD239" s="95"/>
-      <c r="KE239" s="95"/>
-      <c r="KF239" s="95"/>
-      <c r="KG239" s="95"/>
-      <c r="KH239" s="95"/>
-      <c r="KI239" s="95"/>
-      <c r="KJ239" s="95"/>
-      <c r="KK239" s="95"/>
-      <c r="KL239" s="95"/>
-      <c r="KM239" s="95"/>
-      <c r="KN239" s="95"/>
-      <c r="KO239" s="95"/>
-      <c r="KP239" s="95"/>
+      <c r="AT239" s="93"/>
+      <c r="AU239" s="93"/>
+      <c r="AV239" s="93"/>
+      <c r="AW239" s="93"/>
+      <c r="AX239" s="93"/>
+      <c r="AY239" s="93"/>
+      <c r="AZ239" s="93"/>
+      <c r="BA239" s="93"/>
+      <c r="BB239" s="93"/>
+      <c r="BC239" s="93"/>
+      <c r="BD239" s="93"/>
+      <c r="BE239" s="93"/>
+      <c r="BF239" s="93"/>
+      <c r="BG239" s="93"/>
+      <c r="BH239" s="93"/>
+      <c r="BI239" s="93"/>
+      <c r="BJ239" s="93"/>
+      <c r="BK239" s="93"/>
+      <c r="BL239" s="93"/>
+      <c r="BM239" s="93"/>
+      <c r="BN239" s="93"/>
+      <c r="BO239" s="93"/>
+      <c r="BP239" s="93"/>
+      <c r="BQ239" s="93"/>
+      <c r="BR239" s="93"/>
+      <c r="BS239" s="93"/>
+      <c r="BT239" s="93"/>
+      <c r="BU239" s="93"/>
+      <c r="BV239" s="93"/>
+      <c r="BW239" s="93"/>
+      <c r="BX239" s="93"/>
+      <c r="BY239" s="93"/>
+      <c r="BZ239" s="93"/>
+      <c r="CA239" s="93"/>
+      <c r="CB239" s="93"/>
+      <c r="CC239" s="93"/>
+      <c r="CD239" s="93"/>
+      <c r="CE239" s="93"/>
+      <c r="CF239" s="93"/>
+      <c r="CG239" s="93"/>
+      <c r="CH239" s="93"/>
+      <c r="CI239" s="93"/>
+      <c r="CJ239" s="93"/>
+      <c r="CK239" s="93"/>
+      <c r="CL239" s="93"/>
+      <c r="CM239" s="93"/>
+      <c r="CN239" s="93"/>
+      <c r="CO239" s="93"/>
+      <c r="CP239" s="93"/>
+      <c r="CQ239" s="93"/>
+      <c r="CR239" s="93"/>
+      <c r="CS239" s="93"/>
+      <c r="CT239" s="93"/>
+      <c r="CU239" s="93"/>
+      <c r="CV239" s="93"/>
+      <c r="CW239" s="93"/>
+      <c r="CX239" s="93"/>
+      <c r="CY239" s="93"/>
+      <c r="CZ239" s="93"/>
+      <c r="DA239" s="93"/>
+      <c r="DB239" s="93"/>
+      <c r="DC239" s="93"/>
+      <c r="DD239" s="93"/>
+      <c r="DE239" s="93"/>
+      <c r="DF239" s="93"/>
+      <c r="DG239" s="93"/>
+      <c r="DH239" s="93"/>
+      <c r="DI239" s="93"/>
+      <c r="DJ239" s="93"/>
+      <c r="DK239" s="93"/>
+      <c r="DL239" s="93"/>
+      <c r="DM239" s="93"/>
+      <c r="DN239" s="93"/>
+      <c r="DO239" s="93"/>
+      <c r="DP239" s="93"/>
+      <c r="DQ239" s="93"/>
+      <c r="DR239" s="93"/>
+      <c r="DS239" s="93"/>
+      <c r="DT239" s="93"/>
+      <c r="DU239" s="93"/>
+      <c r="DV239" s="93"/>
+      <c r="DW239" s="93"/>
+      <c r="DX239" s="93"/>
+      <c r="DY239" s="93"/>
+      <c r="DZ239" s="93"/>
+      <c r="EA239" s="93"/>
+      <c r="EB239" s="93"/>
+      <c r="EC239" s="93"/>
+      <c r="ED239" s="93"/>
+      <c r="EE239" s="93"/>
+      <c r="EF239" s="93"/>
+      <c r="EG239" s="93"/>
+      <c r="EH239" s="93"/>
+      <c r="EI239" s="93"/>
+      <c r="EJ239" s="93"/>
+      <c r="EK239" s="93"/>
+      <c r="EL239" s="93"/>
+      <c r="EM239" s="93"/>
+      <c r="EN239" s="93"/>
+      <c r="EO239" s="93"/>
+      <c r="EP239" s="93"/>
+      <c r="EQ239" s="93"/>
+      <c r="ER239" s="93"/>
+      <c r="ES239" s="93"/>
+      <c r="ET239" s="93"/>
+      <c r="EU239" s="93"/>
+      <c r="EV239" s="93"/>
+      <c r="EW239" s="93"/>
+      <c r="EX239" s="93"/>
+      <c r="EY239" s="93"/>
+      <c r="EZ239" s="93"/>
+      <c r="FA239" s="93"/>
+      <c r="FB239" s="93"/>
+      <c r="FC239" s="93"/>
+      <c r="FD239" s="93"/>
+      <c r="FE239" s="93"/>
+      <c r="FF239" s="93"/>
+      <c r="FG239" s="93"/>
+      <c r="FH239" s="93"/>
+      <c r="FI239" s="93"/>
+      <c r="FJ239" s="93"/>
+      <c r="FK239" s="93"/>
+      <c r="FL239" s="93"/>
+      <c r="FM239" s="93"/>
+      <c r="FN239" s="93"/>
+      <c r="FO239" s="93"/>
+      <c r="FP239" s="93"/>
+      <c r="FQ239" s="93"/>
+      <c r="FR239" s="93"/>
+      <c r="FS239" s="93"/>
+      <c r="FT239" s="93"/>
+      <c r="FU239" s="93"/>
+      <c r="FV239" s="93"/>
+      <c r="FW239" s="93"/>
+      <c r="FX239" s="93"/>
+      <c r="FY239" s="93"/>
+      <c r="FZ239" s="93"/>
+      <c r="GA239" s="93"/>
+      <c r="GB239" s="93"/>
+      <c r="GC239" s="93"/>
+      <c r="GD239" s="93"/>
+      <c r="GE239" s="93"/>
+      <c r="GF239" s="93"/>
+      <c r="GG239" s="93"/>
+      <c r="GH239" s="93"/>
+      <c r="GI239" s="93"/>
+      <c r="GJ239" s="93"/>
+      <c r="GK239" s="93"/>
+      <c r="GL239" s="93"/>
+      <c r="GM239" s="93"/>
+      <c r="GN239" s="93"/>
+      <c r="GO239" s="93"/>
+      <c r="GP239" s="93"/>
+      <c r="GQ239" s="93"/>
+      <c r="GR239" s="93"/>
+      <c r="GS239" s="93"/>
+      <c r="GT239" s="93"/>
+      <c r="GU239" s="93"/>
+      <c r="GV239" s="93"/>
+      <c r="GW239" s="93"/>
+      <c r="GX239" s="93"/>
+      <c r="GY239" s="93"/>
+      <c r="GZ239" s="93"/>
+      <c r="HA239" s="93"/>
+      <c r="HB239" s="93"/>
+      <c r="HC239" s="93"/>
+      <c r="HD239" s="93"/>
+      <c r="HE239" s="93"/>
+      <c r="HF239" s="93"/>
+      <c r="HG239" s="93"/>
+      <c r="HH239" s="93"/>
+      <c r="HI239" s="93"/>
+      <c r="HJ239" s="93"/>
+      <c r="HK239" s="93"/>
+      <c r="HL239" s="93"/>
+      <c r="HM239" s="93"/>
+      <c r="HN239" s="93"/>
+      <c r="HO239" s="93"/>
+      <c r="HP239" s="93"/>
+      <c r="HQ239" s="93"/>
+      <c r="HR239" s="93"/>
+      <c r="HS239" s="93"/>
+      <c r="HT239" s="93"/>
+      <c r="HU239" s="93"/>
+      <c r="HV239" s="93"/>
+      <c r="HW239" s="93"/>
+      <c r="HX239" s="93"/>
+      <c r="HY239" s="93"/>
+      <c r="HZ239" s="93"/>
+      <c r="IA239" s="93"/>
+      <c r="IB239" s="93"/>
+      <c r="IC239" s="93"/>
+      <c r="ID239" s="93"/>
+      <c r="IE239" s="93"/>
+      <c r="IF239" s="93"/>
+      <c r="IG239" s="93"/>
+      <c r="IH239" s="93"/>
+      <c r="II239" s="93"/>
+      <c r="IJ239" s="93"/>
+      <c r="IK239" s="93"/>
+      <c r="IL239" s="93"/>
+      <c r="IM239" s="93"/>
+      <c r="IN239" s="93"/>
+      <c r="IO239" s="93"/>
+      <c r="IP239" s="93"/>
+      <c r="IQ239" s="93"/>
+      <c r="IR239" s="93"/>
+      <c r="IS239" s="93"/>
+      <c r="IT239" s="93"/>
+      <c r="IU239" s="93"/>
+      <c r="IV239" s="93"/>
+      <c r="IW239" s="93"/>
+      <c r="IX239" s="93"/>
+      <c r="IY239" s="93"/>
+      <c r="IZ239" s="93"/>
+      <c r="JA239" s="93"/>
+      <c r="JB239" s="93"/>
+      <c r="JC239" s="93"/>
+      <c r="JD239" s="93"/>
+      <c r="JE239" s="93"/>
+      <c r="JF239" s="93"/>
+      <c r="JG239" s="93"/>
+      <c r="JH239" s="93"/>
+      <c r="JI239" s="93"/>
+      <c r="JJ239" s="93"/>
+      <c r="JK239" s="93"/>
+      <c r="JL239" s="93"/>
+      <c r="JM239" s="93"/>
+      <c r="JN239" s="93"/>
+      <c r="JO239" s="93"/>
+      <c r="JP239" s="93"/>
+      <c r="JQ239" s="93"/>
+      <c r="JR239" s="93"/>
+      <c r="JS239" s="93"/>
+      <c r="JT239" s="93"/>
+      <c r="JU239" s="93"/>
+      <c r="JV239" s="93"/>
+      <c r="JW239" s="93"/>
+      <c r="JX239" s="93"/>
+      <c r="JY239" s="93"/>
+      <c r="JZ239" s="93"/>
+      <c r="KA239" s="93"/>
+      <c r="KB239" s="93"/>
+      <c r="KC239" s="93"/>
+      <c r="KD239" s="93"/>
+      <c r="KE239" s="93"/>
+      <c r="KF239" s="93"/>
+      <c r="KG239" s="93"/>
+      <c r="KH239" s="93"/>
+      <c r="KI239" s="93"/>
+      <c r="KJ239" s="93"/>
+      <c r="KK239" s="93"/>
+      <c r="KL239" s="93"/>
+      <c r="KM239" s="93"/>
+      <c r="KN239" s="93"/>
+      <c r="KO239" s="93"/>
+      <c r="KP239" s="93"/>
     </row>
     <row r="240" spans="1:302" x14ac:dyDescent="0.2">
-      <c r="B240" s="91">
-        <v>3</v>
-      </c>
-      <c r="C240" s="91">
-        <v>3</v>
-      </c>
-      <c r="D240" s="91">
-        <v>3</v>
-      </c>
-      <c r="E240" s="91">
-        <v>3</v>
-      </c>
-      <c r="AH240" s="91">
-        <v>0</v>
-      </c>
-      <c r="AI240" s="91">
-        <v>0</v>
-      </c>
-      <c r="AJ240" s="91">
-        <v>0</v>
-      </c>
-      <c r="AK240" s="91">
+      <c r="B240">
+        <v>3</v>
+      </c>
+      <c r="C240">
+        <v>3</v>
+      </c>
+      <c r="D240" s="86">
+        <v>3</v>
+      </c>
+      <c r="E240">
+        <v>3</v>
+      </c>
+      <c r="AH240">
+        <v>0</v>
+      </c>
+      <c r="AI240">
+        <v>0</v>
+      </c>
+      <c r="AJ240">
+        <v>0</v>
+      </c>
+      <c r="AK240">
         <v>0</v>
       </c>
     </row>
@@ -43742,16 +43747,16 @@
       <c r="A241" s="46">
         <v>110</v>
       </c>
-      <c r="B241" s="92">
-        <v>3</v>
-      </c>
-      <c r="C241" s="92">
-        <v>3</v>
-      </c>
-      <c r="D241" s="92">
-        <v>2</v>
-      </c>
-      <c r="E241" s="92">
+      <c r="B241" s="29">
+        <v>3</v>
+      </c>
+      <c r="C241" s="29">
+        <v>3</v>
+      </c>
+      <c r="D241" s="29">
+        <v>2</v>
+      </c>
+      <c r="E241" s="29">
         <v>4</v>
       </c>
       <c r="F241" s="28"/>
@@ -43795,312 +43800,312 @@
       <c r="AD241" s="65"/>
       <c r="AE241" s="65"/>
       <c r="AF241" s="65"/>
-      <c r="AG241" s="93"/>
-      <c r="AH241" s="92">
-        <v>3</v>
-      </c>
-      <c r="AI241" s="92">
-        <v>3</v>
-      </c>
-      <c r="AJ241" s="92">
-        <v>2</v>
-      </c>
-      <c r="AK241" s="92">
+      <c r="AG241" s="91"/>
+      <c r="AH241" s="29">
+        <v>0</v>
+      </c>
+      <c r="AI241" s="29">
+        <v>3</v>
+      </c>
+      <c r="AJ241" s="29">
+        <v>2</v>
+      </c>
+      <c r="AK241" s="29">
         <v>4</v>
       </c>
       <c r="AP241" s="29">
         <v>0</v>
       </c>
       <c r="AQ241" s="29">
-        <v>9</v>
-      </c>
-      <c r="AR241" s="94" t="b">
+        <v>12</v>
+      </c>
+      <c r="AR241" s="92" t="b">
         <v>1</v>
       </c>
       <c r="AS241" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="AT241" s="95"/>
-      <c r="AU241" s="95"/>
-      <c r="AV241" s="95"/>
-      <c r="AW241" s="95"/>
-      <c r="AX241" s="95"/>
-      <c r="AY241" s="95"/>
-      <c r="AZ241" s="95"/>
-      <c r="BA241" s="95"/>
-      <c r="BB241" s="95"/>
-      <c r="BC241" s="95"/>
-      <c r="BD241" s="95"/>
-      <c r="BE241" s="95"/>
-      <c r="BF241" s="95"/>
-      <c r="BG241" s="95"/>
-      <c r="BH241" s="95"/>
-      <c r="BI241" s="95"/>
-      <c r="BJ241" s="95"/>
-      <c r="BK241" s="95"/>
-      <c r="BL241" s="95"/>
-      <c r="BM241" s="95"/>
-      <c r="BN241" s="95"/>
-      <c r="BO241" s="95"/>
-      <c r="BP241" s="95"/>
-      <c r="BQ241" s="95"/>
-      <c r="BR241" s="95"/>
-      <c r="BS241" s="95"/>
-      <c r="BT241" s="95"/>
-      <c r="BU241" s="95"/>
-      <c r="BV241" s="95"/>
-      <c r="BW241" s="95"/>
-      <c r="BX241" s="95"/>
-      <c r="BY241" s="95"/>
-      <c r="BZ241" s="95"/>
-      <c r="CA241" s="95"/>
-      <c r="CB241" s="95"/>
-      <c r="CC241" s="95"/>
-      <c r="CD241" s="95"/>
-      <c r="CE241" s="95"/>
-      <c r="CF241" s="95"/>
-      <c r="CG241" s="95"/>
-      <c r="CH241" s="95"/>
-      <c r="CI241" s="95"/>
-      <c r="CJ241" s="95"/>
-      <c r="CK241" s="95"/>
-      <c r="CL241" s="95"/>
-      <c r="CM241" s="95"/>
-      <c r="CN241" s="95"/>
-      <c r="CO241" s="95"/>
-      <c r="CP241" s="95"/>
-      <c r="CQ241" s="95"/>
-      <c r="CR241" s="95"/>
-      <c r="CS241" s="95"/>
-      <c r="CT241" s="95"/>
-      <c r="CU241" s="95"/>
-      <c r="CV241" s="95"/>
-      <c r="CW241" s="95"/>
-      <c r="CX241" s="95"/>
-      <c r="CY241" s="95"/>
-      <c r="CZ241" s="95"/>
-      <c r="DA241" s="95"/>
-      <c r="DB241" s="95"/>
-      <c r="DC241" s="95"/>
-      <c r="DD241" s="95"/>
-      <c r="DE241" s="95"/>
-      <c r="DF241" s="95"/>
-      <c r="DG241" s="95"/>
-      <c r="DH241" s="95"/>
-      <c r="DI241" s="95"/>
-      <c r="DJ241" s="95"/>
-      <c r="DK241" s="95"/>
-      <c r="DL241" s="95"/>
-      <c r="DM241" s="95"/>
-      <c r="DN241" s="95"/>
-      <c r="DO241" s="95"/>
-      <c r="DP241" s="95"/>
-      <c r="DQ241" s="95"/>
-      <c r="DR241" s="95"/>
-      <c r="DS241" s="95"/>
-      <c r="DT241" s="95"/>
-      <c r="DU241" s="95"/>
-      <c r="DV241" s="95"/>
-      <c r="DW241" s="95"/>
-      <c r="DX241" s="95"/>
-      <c r="DY241" s="95"/>
-      <c r="DZ241" s="95"/>
-      <c r="EA241" s="95"/>
-      <c r="EB241" s="95"/>
-      <c r="EC241" s="95"/>
-      <c r="ED241" s="95"/>
-      <c r="EE241" s="95"/>
-      <c r="EF241" s="95"/>
-      <c r="EG241" s="95"/>
-      <c r="EH241" s="95"/>
-      <c r="EI241" s="95"/>
-      <c r="EJ241" s="95"/>
-      <c r="EK241" s="95"/>
-      <c r="EL241" s="95"/>
-      <c r="EM241" s="95"/>
-      <c r="EN241" s="95"/>
-      <c r="EO241" s="95"/>
-      <c r="EP241" s="95"/>
-      <c r="EQ241" s="95"/>
-      <c r="ER241" s="95"/>
-      <c r="ES241" s="95"/>
-      <c r="ET241" s="95"/>
-      <c r="EU241" s="95"/>
-      <c r="EV241" s="95"/>
-      <c r="EW241" s="95"/>
-      <c r="EX241" s="95"/>
-      <c r="EY241" s="95"/>
-      <c r="EZ241" s="95"/>
-      <c r="FA241" s="95"/>
-      <c r="FB241" s="95"/>
-      <c r="FC241" s="95"/>
-      <c r="FD241" s="95"/>
-      <c r="FE241" s="95"/>
-      <c r="FF241" s="95"/>
-      <c r="FG241" s="95"/>
-      <c r="FH241" s="95"/>
-      <c r="FI241" s="95"/>
-      <c r="FJ241" s="95"/>
-      <c r="FK241" s="95"/>
-      <c r="FL241" s="95"/>
-      <c r="FM241" s="95"/>
-      <c r="FN241" s="95"/>
-      <c r="FO241" s="95"/>
-      <c r="FP241" s="95"/>
-      <c r="FQ241" s="95"/>
-      <c r="FR241" s="95"/>
-      <c r="FS241" s="95"/>
-      <c r="FT241" s="95"/>
-      <c r="FU241" s="95"/>
-      <c r="FV241" s="95"/>
-      <c r="FW241" s="95"/>
-      <c r="FX241" s="95"/>
-      <c r="FY241" s="95"/>
-      <c r="FZ241" s="95"/>
-      <c r="GA241" s="95"/>
-      <c r="GB241" s="95"/>
-      <c r="GC241" s="95"/>
-      <c r="GD241" s="95"/>
-      <c r="GE241" s="95"/>
-      <c r="GF241" s="95"/>
-      <c r="GG241" s="95"/>
-      <c r="GH241" s="95"/>
-      <c r="GI241" s="95"/>
-      <c r="GJ241" s="95"/>
-      <c r="GK241" s="95"/>
-      <c r="GL241" s="95"/>
-      <c r="GM241" s="95"/>
-      <c r="GN241" s="95"/>
-      <c r="GO241" s="95"/>
-      <c r="GP241" s="95"/>
-      <c r="GQ241" s="95"/>
-      <c r="GR241" s="95"/>
-      <c r="GS241" s="95"/>
-      <c r="GT241" s="95"/>
-      <c r="GU241" s="95"/>
-      <c r="GV241" s="95"/>
-      <c r="GW241" s="95"/>
-      <c r="GX241" s="95"/>
-      <c r="GY241" s="95"/>
-      <c r="GZ241" s="95"/>
-      <c r="HA241" s="95"/>
-      <c r="HB241" s="95"/>
-      <c r="HC241" s="95"/>
-      <c r="HD241" s="95"/>
-      <c r="HE241" s="95"/>
-      <c r="HF241" s="95"/>
-      <c r="HG241" s="95"/>
-      <c r="HH241" s="95"/>
-      <c r="HI241" s="95"/>
-      <c r="HJ241" s="95"/>
-      <c r="HK241" s="95"/>
-      <c r="HL241" s="95"/>
-      <c r="HM241" s="95"/>
-      <c r="HN241" s="95"/>
-      <c r="HO241" s="95"/>
-      <c r="HP241" s="95"/>
-      <c r="HQ241" s="95"/>
-      <c r="HR241" s="95"/>
-      <c r="HS241" s="95"/>
-      <c r="HT241" s="95"/>
-      <c r="HU241" s="95"/>
-      <c r="HV241" s="95"/>
-      <c r="HW241" s="95"/>
-      <c r="HX241" s="95"/>
-      <c r="HY241" s="95"/>
-      <c r="HZ241" s="95"/>
-      <c r="IA241" s="95"/>
-      <c r="IB241" s="95"/>
-      <c r="IC241" s="95"/>
-      <c r="ID241" s="95"/>
-      <c r="IE241" s="95"/>
-      <c r="IF241" s="95"/>
-      <c r="IG241" s="95"/>
-      <c r="IH241" s="95"/>
-      <c r="II241" s="95"/>
-      <c r="IJ241" s="95"/>
-      <c r="IK241" s="95"/>
-      <c r="IL241" s="95"/>
-      <c r="IM241" s="95"/>
-      <c r="IN241" s="95"/>
-      <c r="IO241" s="95"/>
-      <c r="IP241" s="95"/>
-      <c r="IQ241" s="95"/>
-      <c r="IR241" s="95"/>
-      <c r="IS241" s="95"/>
-      <c r="IT241" s="95"/>
-      <c r="IU241" s="95"/>
-      <c r="IV241" s="95"/>
-      <c r="IW241" s="95"/>
-      <c r="IX241" s="95"/>
-      <c r="IY241" s="95"/>
-      <c r="IZ241" s="95"/>
-      <c r="JA241" s="95"/>
-      <c r="JB241" s="95"/>
-      <c r="JC241" s="95"/>
-      <c r="JD241" s="95"/>
-      <c r="JE241" s="95"/>
-      <c r="JF241" s="95"/>
-      <c r="JG241" s="95"/>
-      <c r="JH241" s="95"/>
-      <c r="JI241" s="95"/>
-      <c r="JJ241" s="95"/>
-      <c r="JK241" s="95"/>
-      <c r="JL241" s="95"/>
-      <c r="JM241" s="95"/>
-      <c r="JN241" s="95"/>
-      <c r="JO241" s="95"/>
-      <c r="JP241" s="95"/>
-      <c r="JQ241" s="95"/>
-      <c r="JR241" s="95"/>
-      <c r="JS241" s="95"/>
-      <c r="JT241" s="95"/>
-      <c r="JU241" s="95"/>
-      <c r="JV241" s="95"/>
-      <c r="JW241" s="95"/>
-      <c r="JX241" s="95"/>
-      <c r="JY241" s="95"/>
-      <c r="JZ241" s="95"/>
-      <c r="KA241" s="95"/>
-      <c r="KB241" s="95"/>
-      <c r="KC241" s="95"/>
-      <c r="KD241" s="95"/>
-      <c r="KE241" s="95"/>
-      <c r="KF241" s="95"/>
-      <c r="KG241" s="95"/>
-      <c r="KH241" s="95"/>
-      <c r="KI241" s="95"/>
-      <c r="KJ241" s="95"/>
-      <c r="KK241" s="95"/>
-      <c r="KL241" s="95"/>
-      <c r="KM241" s="95"/>
-      <c r="KN241" s="95"/>
-      <c r="KO241" s="95"/>
-      <c r="KP241" s="95"/>
+      <c r="AT241" s="93"/>
+      <c r="AU241" s="93"/>
+      <c r="AV241" s="93"/>
+      <c r="AW241" s="93"/>
+      <c r="AX241" s="93"/>
+      <c r="AY241" s="93"/>
+      <c r="AZ241" s="93"/>
+      <c r="BA241" s="93"/>
+      <c r="BB241" s="93"/>
+      <c r="BC241" s="93"/>
+      <c r="BD241" s="93"/>
+      <c r="BE241" s="93"/>
+      <c r="BF241" s="93"/>
+      <c r="BG241" s="93"/>
+      <c r="BH241" s="93"/>
+      <c r="BI241" s="93"/>
+      <c r="BJ241" s="93"/>
+      <c r="BK241" s="93"/>
+      <c r="BL241" s="93"/>
+      <c r="BM241" s="93"/>
+      <c r="BN241" s="93"/>
+      <c r="BO241" s="93"/>
+      <c r="BP241" s="93"/>
+      <c r="BQ241" s="93"/>
+      <c r="BR241" s="93"/>
+      <c r="BS241" s="93"/>
+      <c r="BT241" s="93"/>
+      <c r="BU241" s="93"/>
+      <c r="BV241" s="93"/>
+      <c r="BW241" s="93"/>
+      <c r="BX241" s="93"/>
+      <c r="BY241" s="93"/>
+      <c r="BZ241" s="93"/>
+      <c r="CA241" s="93"/>
+      <c r="CB241" s="93"/>
+      <c r="CC241" s="93"/>
+      <c r="CD241" s="93"/>
+      <c r="CE241" s="93"/>
+      <c r="CF241" s="93"/>
+      <c r="CG241" s="93"/>
+      <c r="CH241" s="93"/>
+      <c r="CI241" s="93"/>
+      <c r="CJ241" s="93"/>
+      <c r="CK241" s="93"/>
+      <c r="CL241" s="93"/>
+      <c r="CM241" s="93"/>
+      <c r="CN241" s="93"/>
+      <c r="CO241" s="93"/>
+      <c r="CP241" s="93"/>
+      <c r="CQ241" s="93"/>
+      <c r="CR241" s="93"/>
+      <c r="CS241" s="93"/>
+      <c r="CT241" s="93"/>
+      <c r="CU241" s="93"/>
+      <c r="CV241" s="93"/>
+      <c r="CW241" s="93"/>
+      <c r="CX241" s="93"/>
+      <c r="CY241" s="93"/>
+      <c r="CZ241" s="93"/>
+      <c r="DA241" s="93"/>
+      <c r="DB241" s="93"/>
+      <c r="DC241" s="93"/>
+      <c r="DD241" s="93"/>
+      <c r="DE241" s="93"/>
+      <c r="DF241" s="93"/>
+      <c r="DG241" s="93"/>
+      <c r="DH241" s="93"/>
+      <c r="DI241" s="93"/>
+      <c r="DJ241" s="93"/>
+      <c r="DK241" s="93"/>
+      <c r="DL241" s="93"/>
+      <c r="DM241" s="93"/>
+      <c r="DN241" s="93"/>
+      <c r="DO241" s="93"/>
+      <c r="DP241" s="93"/>
+      <c r="DQ241" s="93"/>
+      <c r="DR241" s="93"/>
+      <c r="DS241" s="93"/>
+      <c r="DT241" s="93"/>
+      <c r="DU241" s="93"/>
+      <c r="DV241" s="93"/>
+      <c r="DW241" s="93"/>
+      <c r="DX241" s="93"/>
+      <c r="DY241" s="93"/>
+      <c r="DZ241" s="93"/>
+      <c r="EA241" s="93"/>
+      <c r="EB241" s="93"/>
+      <c r="EC241" s="93"/>
+      <c r="ED241" s="93"/>
+      <c r="EE241" s="93"/>
+      <c r="EF241" s="93"/>
+      <c r="EG241" s="93"/>
+      <c r="EH241" s="93"/>
+      <c r="EI241" s="93"/>
+      <c r="EJ241" s="93"/>
+      <c r="EK241" s="93"/>
+      <c r="EL241" s="93"/>
+      <c r="EM241" s="93"/>
+      <c r="EN241" s="93"/>
+      <c r="EO241" s="93"/>
+      <c r="EP241" s="93"/>
+      <c r="EQ241" s="93"/>
+      <c r="ER241" s="93"/>
+      <c r="ES241" s="93"/>
+      <c r="ET241" s="93"/>
+      <c r="EU241" s="93"/>
+      <c r="EV241" s="93"/>
+      <c r="EW241" s="93"/>
+      <c r="EX241" s="93"/>
+      <c r="EY241" s="93"/>
+      <c r="EZ241" s="93"/>
+      <c r="FA241" s="93"/>
+      <c r="FB241" s="93"/>
+      <c r="FC241" s="93"/>
+      <c r="FD241" s="93"/>
+      <c r="FE241" s="93"/>
+      <c r="FF241" s="93"/>
+      <c r="FG241" s="93"/>
+      <c r="FH241" s="93"/>
+      <c r="FI241" s="93"/>
+      <c r="FJ241" s="93"/>
+      <c r="FK241" s="93"/>
+      <c r="FL241" s="93"/>
+      <c r="FM241" s="93"/>
+      <c r="FN241" s="93"/>
+      <c r="FO241" s="93"/>
+      <c r="FP241" s="93"/>
+      <c r="FQ241" s="93"/>
+      <c r="FR241" s="93"/>
+      <c r="FS241" s="93"/>
+      <c r="FT241" s="93"/>
+      <c r="FU241" s="93"/>
+      <c r="FV241" s="93"/>
+      <c r="FW241" s="93"/>
+      <c r="FX241" s="93"/>
+      <c r="FY241" s="93"/>
+      <c r="FZ241" s="93"/>
+      <c r="GA241" s="93"/>
+      <c r="GB241" s="93"/>
+      <c r="GC241" s="93"/>
+      <c r="GD241" s="93"/>
+      <c r="GE241" s="93"/>
+      <c r="GF241" s="93"/>
+      <c r="GG241" s="93"/>
+      <c r="GH241" s="93"/>
+      <c r="GI241" s="93"/>
+      <c r="GJ241" s="93"/>
+      <c r="GK241" s="93"/>
+      <c r="GL241" s="93"/>
+      <c r="GM241" s="93"/>
+      <c r="GN241" s="93"/>
+      <c r="GO241" s="93"/>
+      <c r="GP241" s="93"/>
+      <c r="GQ241" s="93"/>
+      <c r="GR241" s="93"/>
+      <c r="GS241" s="93"/>
+      <c r="GT241" s="93"/>
+      <c r="GU241" s="93"/>
+      <c r="GV241" s="93"/>
+      <c r="GW241" s="93"/>
+      <c r="GX241" s="93"/>
+      <c r="GY241" s="93"/>
+      <c r="GZ241" s="93"/>
+      <c r="HA241" s="93"/>
+      <c r="HB241" s="93"/>
+      <c r="HC241" s="93"/>
+      <c r="HD241" s="93"/>
+      <c r="HE241" s="93"/>
+      <c r="HF241" s="93"/>
+      <c r="HG241" s="93"/>
+      <c r="HH241" s="93"/>
+      <c r="HI241" s="93"/>
+      <c r="HJ241" s="93"/>
+      <c r="HK241" s="93"/>
+      <c r="HL241" s="93"/>
+      <c r="HM241" s="93"/>
+      <c r="HN241" s="93"/>
+      <c r="HO241" s="93"/>
+      <c r="HP241" s="93"/>
+      <c r="HQ241" s="93"/>
+      <c r="HR241" s="93"/>
+      <c r="HS241" s="93"/>
+      <c r="HT241" s="93"/>
+      <c r="HU241" s="93"/>
+      <c r="HV241" s="93"/>
+      <c r="HW241" s="93"/>
+      <c r="HX241" s="93"/>
+      <c r="HY241" s="93"/>
+      <c r="HZ241" s="93"/>
+      <c r="IA241" s="93"/>
+      <c r="IB241" s="93"/>
+      <c r="IC241" s="93"/>
+      <c r="ID241" s="93"/>
+      <c r="IE241" s="93"/>
+      <c r="IF241" s="93"/>
+      <c r="IG241" s="93"/>
+      <c r="IH241" s="93"/>
+      <c r="II241" s="93"/>
+      <c r="IJ241" s="93"/>
+      <c r="IK241" s="93"/>
+      <c r="IL241" s="93"/>
+      <c r="IM241" s="93"/>
+      <c r="IN241" s="93"/>
+      <c r="IO241" s="93"/>
+      <c r="IP241" s="93"/>
+      <c r="IQ241" s="93"/>
+      <c r="IR241" s="93"/>
+      <c r="IS241" s="93"/>
+      <c r="IT241" s="93"/>
+      <c r="IU241" s="93"/>
+      <c r="IV241" s="93"/>
+      <c r="IW241" s="93"/>
+      <c r="IX241" s="93"/>
+      <c r="IY241" s="93"/>
+      <c r="IZ241" s="93"/>
+      <c r="JA241" s="93"/>
+      <c r="JB241" s="93"/>
+      <c r="JC241" s="93"/>
+      <c r="JD241" s="93"/>
+      <c r="JE241" s="93"/>
+      <c r="JF241" s="93"/>
+      <c r="JG241" s="93"/>
+      <c r="JH241" s="93"/>
+      <c r="JI241" s="93"/>
+      <c r="JJ241" s="93"/>
+      <c r="JK241" s="93"/>
+      <c r="JL241" s="93"/>
+      <c r="JM241" s="93"/>
+      <c r="JN241" s="93"/>
+      <c r="JO241" s="93"/>
+      <c r="JP241" s="93"/>
+      <c r="JQ241" s="93"/>
+      <c r="JR241" s="93"/>
+      <c r="JS241" s="93"/>
+      <c r="JT241" s="93"/>
+      <c r="JU241" s="93"/>
+      <c r="JV241" s="93"/>
+      <c r="JW241" s="93"/>
+      <c r="JX241" s="93"/>
+      <c r="JY241" s="93"/>
+      <c r="JZ241" s="93"/>
+      <c r="KA241" s="93"/>
+      <c r="KB241" s="93"/>
+      <c r="KC241" s="93"/>
+      <c r="KD241" s="93"/>
+      <c r="KE241" s="93"/>
+      <c r="KF241" s="93"/>
+      <c r="KG241" s="93"/>
+      <c r="KH241" s="93"/>
+      <c r="KI241" s="93"/>
+      <c r="KJ241" s="93"/>
+      <c r="KK241" s="93"/>
+      <c r="KL241" s="93"/>
+      <c r="KM241" s="93"/>
+      <c r="KN241" s="93"/>
+      <c r="KO241" s="93"/>
+      <c r="KP241" s="93"/>
     </row>
     <row r="242" spans="1:302" x14ac:dyDescent="0.2">
-      <c r="B242" s="91">
-        <v>3</v>
-      </c>
-      <c r="C242" s="91">
-        <v>3</v>
-      </c>
-      <c r="D242" s="91">
-        <v>3</v>
-      </c>
-      <c r="E242" s="91">
-        <v>3</v>
-      </c>
-      <c r="AH242" s="91">
-        <v>0</v>
-      </c>
-      <c r="AI242" s="91">
-        <v>0</v>
-      </c>
-      <c r="AJ242" s="91">
-        <v>3</v>
-      </c>
-      <c r="AK242" s="91">
+      <c r="B242">
+        <v>3</v>
+      </c>
+      <c r="C242">
+        <v>3</v>
+      </c>
+      <c r="D242" s="86">
+        <v>3</v>
+      </c>
+      <c r="E242">
+        <v>3</v>
+      </c>
+      <c r="AH242">
+        <v>0</v>
+      </c>
+      <c r="AI242">
+        <v>0</v>
+      </c>
+      <c r="AJ242">
+        <v>3</v>
+      </c>
+      <c r="AK242">
         <v>0</v>
       </c>
     </row>
@@ -44108,16 +44113,16 @@
       <c r="A243" s="46">
         <v>111</v>
       </c>
-      <c r="B243" s="92">
-        <v>2</v>
-      </c>
-      <c r="C243" s="92">
-        <v>3</v>
-      </c>
-      <c r="D243" s="92">
-        <v>3</v>
-      </c>
-      <c r="E243" s="92">
+      <c r="B243" s="29">
+        <v>2</v>
+      </c>
+      <c r="C243" s="29">
+        <v>3</v>
+      </c>
+      <c r="D243" s="29">
+        <v>3</v>
+      </c>
+      <c r="E243" s="29">
         <v>4</v>
       </c>
       <c r="F243" s="28"/>
@@ -44161,17 +44166,17 @@
       <c r="AD243" s="65"/>
       <c r="AE243" s="65"/>
       <c r="AF243" s="65"/>
-      <c r="AG243" s="93"/>
-      <c r="AH243" s="92">
-        <v>2</v>
-      </c>
-      <c r="AI243" s="92">
-        <v>0</v>
-      </c>
-      <c r="AJ243" s="92">
-        <v>0</v>
-      </c>
-      <c r="AK243" s="92">
+      <c r="AG243" s="91"/>
+      <c r="AH243" s="29">
+        <v>2</v>
+      </c>
+      <c r="AI243" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ243" s="29">
+        <v>0</v>
+      </c>
+      <c r="AK243" s="29">
         <v>4</v>
       </c>
       <c r="AP243" s="29">
@@ -44180,294 +44185,1027 @@
       <c r="AQ243" s="29">
         <v>12</v>
       </c>
-      <c r="AR243" s="94" t="b">
+      <c r="AR243" s="92" t="b">
         <v>1</v>
       </c>
       <c r="AS243" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="AT243" s="95"/>
-      <c r="AU243" s="95"/>
-      <c r="AV243" s="95"/>
-      <c r="AW243" s="95"/>
-      <c r="AX243" s="95"/>
-      <c r="AY243" s="95"/>
-      <c r="AZ243" s="95"/>
-      <c r="BA243" s="95"/>
-      <c r="BB243" s="95"/>
-      <c r="BC243" s="95"/>
-      <c r="BD243" s="95"/>
-      <c r="BE243" s="95"/>
-      <c r="BF243" s="95"/>
-      <c r="BG243" s="95"/>
-      <c r="BH243" s="95"/>
-      <c r="BI243" s="95"/>
-      <c r="BJ243" s="95"/>
-      <c r="BK243" s="95"/>
-      <c r="BL243" s="95"/>
-      <c r="BM243" s="95"/>
-      <c r="BN243" s="95"/>
-      <c r="BO243" s="95"/>
-      <c r="BP243" s="95"/>
-      <c r="BQ243" s="95"/>
-      <c r="BR243" s="95"/>
-      <c r="BS243" s="95"/>
-      <c r="BT243" s="95"/>
-      <c r="BU243" s="95"/>
-      <c r="BV243" s="95"/>
-      <c r="BW243" s="95"/>
-      <c r="BX243" s="95"/>
-      <c r="BY243" s="95"/>
-      <c r="BZ243" s="95"/>
-      <c r="CA243" s="95"/>
-      <c r="CB243" s="95"/>
-      <c r="CC243" s="95"/>
-      <c r="CD243" s="95"/>
-      <c r="CE243" s="95"/>
-      <c r="CF243" s="95"/>
-      <c r="CG243" s="95"/>
-      <c r="CH243" s="95"/>
-      <c r="CI243" s="95"/>
-      <c r="CJ243" s="95"/>
-      <c r="CK243" s="95"/>
-      <c r="CL243" s="95"/>
-      <c r="CM243" s="95"/>
-      <c r="CN243" s="95"/>
-      <c r="CO243" s="95"/>
-      <c r="CP243" s="95"/>
-      <c r="CQ243" s="95"/>
-      <c r="CR243" s="95"/>
-      <c r="CS243" s="95"/>
-      <c r="CT243" s="95"/>
-      <c r="CU243" s="95"/>
-      <c r="CV243" s="95"/>
-      <c r="CW243" s="95"/>
-      <c r="CX243" s="95"/>
-      <c r="CY243" s="95"/>
-      <c r="CZ243" s="95"/>
-      <c r="DA243" s="95"/>
-      <c r="DB243" s="95"/>
-      <c r="DC243" s="95"/>
-      <c r="DD243" s="95"/>
-      <c r="DE243" s="95"/>
-      <c r="DF243" s="95"/>
-      <c r="DG243" s="95"/>
-      <c r="DH243" s="95"/>
-      <c r="DI243" s="95"/>
-      <c r="DJ243" s="95"/>
-      <c r="DK243" s="95"/>
-      <c r="DL243" s="95"/>
-      <c r="DM243" s="95"/>
-      <c r="DN243" s="95"/>
-      <c r="DO243" s="95"/>
-      <c r="DP243" s="95"/>
-      <c r="DQ243" s="95"/>
-      <c r="DR243" s="95"/>
-      <c r="DS243" s="95"/>
-      <c r="DT243" s="95"/>
-      <c r="DU243" s="95"/>
-      <c r="DV243" s="95"/>
-      <c r="DW243" s="95"/>
-      <c r="DX243" s="95"/>
-      <c r="DY243" s="95"/>
-      <c r="DZ243" s="95"/>
-      <c r="EA243" s="95"/>
-      <c r="EB243" s="95"/>
-      <c r="EC243" s="95"/>
-      <c r="ED243" s="95"/>
-      <c r="EE243" s="95"/>
-      <c r="EF243" s="95"/>
-      <c r="EG243" s="95"/>
-      <c r="EH243" s="95"/>
-      <c r="EI243" s="95"/>
-      <c r="EJ243" s="95"/>
-      <c r="EK243" s="95"/>
-      <c r="EL243" s="95"/>
-      <c r="EM243" s="95"/>
-      <c r="EN243" s="95"/>
-      <c r="EO243" s="95"/>
-      <c r="EP243" s="95"/>
-      <c r="EQ243" s="95"/>
-      <c r="ER243" s="95"/>
-      <c r="ES243" s="95"/>
-      <c r="ET243" s="95"/>
-      <c r="EU243" s="95"/>
-      <c r="EV243" s="95"/>
-      <c r="EW243" s="95"/>
-      <c r="EX243" s="95"/>
-      <c r="EY243" s="95"/>
-      <c r="EZ243" s="95"/>
-      <c r="FA243" s="95"/>
-      <c r="FB243" s="95"/>
-      <c r="FC243" s="95"/>
-      <c r="FD243" s="95"/>
-      <c r="FE243" s="95"/>
-      <c r="FF243" s="95"/>
-      <c r="FG243" s="95"/>
-      <c r="FH243" s="95"/>
-      <c r="FI243" s="95"/>
-      <c r="FJ243" s="95"/>
-      <c r="FK243" s="95"/>
-      <c r="FL243" s="95"/>
-      <c r="FM243" s="95"/>
-      <c r="FN243" s="95"/>
-      <c r="FO243" s="95"/>
-      <c r="FP243" s="95"/>
-      <c r="FQ243" s="95"/>
-      <c r="FR243" s="95"/>
-      <c r="FS243" s="95"/>
-      <c r="FT243" s="95"/>
-      <c r="FU243" s="95"/>
-      <c r="FV243" s="95"/>
-      <c r="FW243" s="95"/>
-      <c r="FX243" s="95"/>
-      <c r="FY243" s="95"/>
-      <c r="FZ243" s="95"/>
-      <c r="GA243" s="95"/>
-      <c r="GB243" s="95"/>
-      <c r="GC243" s="95"/>
-      <c r="GD243" s="95"/>
-      <c r="GE243" s="95"/>
-      <c r="GF243" s="95"/>
-      <c r="GG243" s="95"/>
-      <c r="GH243" s="95"/>
-      <c r="GI243" s="95"/>
-      <c r="GJ243" s="95"/>
-      <c r="GK243" s="95"/>
-      <c r="GL243" s="95"/>
-      <c r="GM243" s="95"/>
-      <c r="GN243" s="95"/>
-      <c r="GO243" s="95"/>
-      <c r="GP243" s="95"/>
-      <c r="GQ243" s="95"/>
-      <c r="GR243" s="95"/>
-      <c r="GS243" s="95"/>
-      <c r="GT243" s="95"/>
-      <c r="GU243" s="95"/>
-      <c r="GV243" s="95"/>
-      <c r="GW243" s="95"/>
-      <c r="GX243" s="95"/>
-      <c r="GY243" s="95"/>
-      <c r="GZ243" s="95"/>
-      <c r="HA243" s="95"/>
-      <c r="HB243" s="95"/>
-      <c r="HC243" s="95"/>
-      <c r="HD243" s="95"/>
-      <c r="HE243" s="95"/>
-      <c r="HF243" s="95"/>
-      <c r="HG243" s="95"/>
-      <c r="HH243" s="95"/>
-      <c r="HI243" s="95"/>
-      <c r="HJ243" s="95"/>
-      <c r="HK243" s="95"/>
-      <c r="HL243" s="95"/>
-      <c r="HM243" s="95"/>
-      <c r="HN243" s="95"/>
-      <c r="HO243" s="95"/>
-      <c r="HP243" s="95"/>
-      <c r="HQ243" s="95"/>
-      <c r="HR243" s="95"/>
-      <c r="HS243" s="95"/>
-      <c r="HT243" s="95"/>
-      <c r="HU243" s="95"/>
-      <c r="HV243" s="95"/>
-      <c r="HW243" s="95"/>
-      <c r="HX243" s="95"/>
-      <c r="HY243" s="95"/>
-      <c r="HZ243" s="95"/>
-      <c r="IA243" s="95"/>
-      <c r="IB243" s="95"/>
-      <c r="IC243" s="95"/>
-      <c r="ID243" s="95"/>
-      <c r="IE243" s="95"/>
-      <c r="IF243" s="95"/>
-      <c r="IG243" s="95"/>
-      <c r="IH243" s="95"/>
-      <c r="II243" s="95"/>
-      <c r="IJ243" s="95"/>
-      <c r="IK243" s="95"/>
-      <c r="IL243" s="95"/>
-      <c r="IM243" s="95"/>
-      <c r="IN243" s="95"/>
-      <c r="IO243" s="95"/>
-      <c r="IP243" s="95"/>
-      <c r="IQ243" s="95"/>
-      <c r="IR243" s="95"/>
-      <c r="IS243" s="95"/>
-      <c r="IT243" s="95"/>
-      <c r="IU243" s="95"/>
-      <c r="IV243" s="95"/>
-      <c r="IW243" s="95"/>
-      <c r="IX243" s="95"/>
-      <c r="IY243" s="95"/>
-      <c r="IZ243" s="95"/>
-      <c r="JA243" s="95"/>
-      <c r="JB243" s="95"/>
-      <c r="JC243" s="95"/>
-      <c r="JD243" s="95"/>
-      <c r="JE243" s="95"/>
-      <c r="JF243" s="95"/>
-      <c r="JG243" s="95"/>
-      <c r="JH243" s="95"/>
-      <c r="JI243" s="95"/>
-      <c r="JJ243" s="95"/>
-      <c r="JK243" s="95"/>
-      <c r="JL243" s="95"/>
-      <c r="JM243" s="95"/>
-      <c r="JN243" s="95"/>
-      <c r="JO243" s="95"/>
-      <c r="JP243" s="95"/>
-      <c r="JQ243" s="95"/>
-      <c r="JR243" s="95"/>
-      <c r="JS243" s="95"/>
-      <c r="JT243" s="95"/>
-      <c r="JU243" s="95"/>
-      <c r="JV243" s="95"/>
-      <c r="JW243" s="95"/>
-      <c r="JX243" s="95"/>
-      <c r="JY243" s="95"/>
-      <c r="JZ243" s="95"/>
-      <c r="KA243" s="95"/>
-      <c r="KB243" s="95"/>
-      <c r="KC243" s="95"/>
-      <c r="KD243" s="95"/>
-      <c r="KE243" s="95"/>
-      <c r="KF243" s="95"/>
-      <c r="KG243" s="95"/>
-      <c r="KH243" s="95"/>
-      <c r="KI243" s="95"/>
-      <c r="KJ243" s="95"/>
-      <c r="KK243" s="95"/>
-      <c r="KL243" s="95"/>
-      <c r="KM243" s="95"/>
-      <c r="KN243" s="95"/>
-      <c r="KO243" s="95"/>
-      <c r="KP243" s="95"/>
+      <c r="AT243" s="93"/>
+      <c r="AU243" s="93"/>
+      <c r="AV243" s="93"/>
+      <c r="AW243" s="93"/>
+      <c r="AX243" s="93"/>
+      <c r="AY243" s="93"/>
+      <c r="AZ243" s="93"/>
+      <c r="BA243" s="93"/>
+      <c r="BB243" s="93"/>
+      <c r="BC243" s="93"/>
+      <c r="BD243" s="93"/>
+      <c r="BE243" s="93"/>
+      <c r="BF243" s="93"/>
+      <c r="BG243" s="93"/>
+      <c r="BH243" s="93"/>
+      <c r="BI243" s="93"/>
+      <c r="BJ243" s="93"/>
+      <c r="BK243" s="93"/>
+      <c r="BL243" s="93"/>
+      <c r="BM243" s="93"/>
+      <c r="BN243" s="93"/>
+      <c r="BO243" s="93"/>
+      <c r="BP243" s="93"/>
+      <c r="BQ243" s="93"/>
+      <c r="BR243" s="93"/>
+      <c r="BS243" s="93"/>
+      <c r="BT243" s="93"/>
+      <c r="BU243" s="93"/>
+      <c r="BV243" s="93"/>
+      <c r="BW243" s="93"/>
+      <c r="BX243" s="93"/>
+      <c r="BY243" s="93"/>
+      <c r="BZ243" s="93"/>
+      <c r="CA243" s="93"/>
+      <c r="CB243" s="93"/>
+      <c r="CC243" s="93"/>
+      <c r="CD243" s="93"/>
+      <c r="CE243" s="93"/>
+      <c r="CF243" s="93"/>
+      <c r="CG243" s="93"/>
+      <c r="CH243" s="93"/>
+      <c r="CI243" s="93"/>
+      <c r="CJ243" s="93"/>
+      <c r="CK243" s="93"/>
+      <c r="CL243" s="93"/>
+      <c r="CM243" s="93"/>
+      <c r="CN243" s="93"/>
+      <c r="CO243" s="93"/>
+      <c r="CP243" s="93"/>
+      <c r="CQ243" s="93"/>
+      <c r="CR243" s="93"/>
+      <c r="CS243" s="93"/>
+      <c r="CT243" s="93"/>
+      <c r="CU243" s="93"/>
+      <c r="CV243" s="93"/>
+      <c r="CW243" s="93"/>
+      <c r="CX243" s="93"/>
+      <c r="CY243" s="93"/>
+      <c r="CZ243" s="93"/>
+      <c r="DA243" s="93"/>
+      <c r="DB243" s="93"/>
+      <c r="DC243" s="93"/>
+      <c r="DD243" s="93"/>
+      <c r="DE243" s="93"/>
+      <c r="DF243" s="93"/>
+      <c r="DG243" s="93"/>
+      <c r="DH243" s="93"/>
+      <c r="DI243" s="93"/>
+      <c r="DJ243" s="93"/>
+      <c r="DK243" s="93"/>
+      <c r="DL243" s="93"/>
+      <c r="DM243" s="93"/>
+      <c r="DN243" s="93"/>
+      <c r="DO243" s="93"/>
+      <c r="DP243" s="93"/>
+      <c r="DQ243" s="93"/>
+      <c r="DR243" s="93"/>
+      <c r="DS243" s="93"/>
+      <c r="DT243" s="93"/>
+      <c r="DU243" s="93"/>
+      <c r="DV243" s="93"/>
+      <c r="DW243" s="93"/>
+      <c r="DX243" s="93"/>
+      <c r="DY243" s="93"/>
+      <c r="DZ243" s="93"/>
+      <c r="EA243" s="93"/>
+      <c r="EB243" s="93"/>
+      <c r="EC243" s="93"/>
+      <c r="ED243" s="93"/>
+      <c r="EE243" s="93"/>
+      <c r="EF243" s="93"/>
+      <c r="EG243" s="93"/>
+      <c r="EH243" s="93"/>
+      <c r="EI243" s="93"/>
+      <c r="EJ243" s="93"/>
+      <c r="EK243" s="93"/>
+      <c r="EL243" s="93"/>
+      <c r="EM243" s="93"/>
+      <c r="EN243" s="93"/>
+      <c r="EO243" s="93"/>
+      <c r="EP243" s="93"/>
+      <c r="EQ243" s="93"/>
+      <c r="ER243" s="93"/>
+      <c r="ES243" s="93"/>
+      <c r="ET243" s="93"/>
+      <c r="EU243" s="93"/>
+      <c r="EV243" s="93"/>
+      <c r="EW243" s="93"/>
+      <c r="EX243" s="93"/>
+      <c r="EY243" s="93"/>
+      <c r="EZ243" s="93"/>
+      <c r="FA243" s="93"/>
+      <c r="FB243" s="93"/>
+      <c r="FC243" s="93"/>
+      <c r="FD243" s="93"/>
+      <c r="FE243" s="93"/>
+      <c r="FF243" s="93"/>
+      <c r="FG243" s="93"/>
+      <c r="FH243" s="93"/>
+      <c r="FI243" s="93"/>
+      <c r="FJ243" s="93"/>
+      <c r="FK243" s="93"/>
+      <c r="FL243" s="93"/>
+      <c r="FM243" s="93"/>
+      <c r="FN243" s="93"/>
+      <c r="FO243" s="93"/>
+      <c r="FP243" s="93"/>
+      <c r="FQ243" s="93"/>
+      <c r="FR243" s="93"/>
+      <c r="FS243" s="93"/>
+      <c r="FT243" s="93"/>
+      <c r="FU243" s="93"/>
+      <c r="FV243" s="93"/>
+      <c r="FW243" s="93"/>
+      <c r="FX243" s="93"/>
+      <c r="FY243" s="93"/>
+      <c r="FZ243" s="93"/>
+      <c r="GA243" s="93"/>
+      <c r="GB243" s="93"/>
+      <c r="GC243" s="93"/>
+      <c r="GD243" s="93"/>
+      <c r="GE243" s="93"/>
+      <c r="GF243" s="93"/>
+      <c r="GG243" s="93"/>
+      <c r="GH243" s="93"/>
+      <c r="GI243" s="93"/>
+      <c r="GJ243" s="93"/>
+      <c r="GK243" s="93"/>
+      <c r="GL243" s="93"/>
+      <c r="GM243" s="93"/>
+      <c r="GN243" s="93"/>
+      <c r="GO243" s="93"/>
+      <c r="GP243" s="93"/>
+      <c r="GQ243" s="93"/>
+      <c r="GR243" s="93"/>
+      <c r="GS243" s="93"/>
+      <c r="GT243" s="93"/>
+      <c r="GU243" s="93"/>
+      <c r="GV243" s="93"/>
+      <c r="GW243" s="93"/>
+      <c r="GX243" s="93"/>
+      <c r="GY243" s="93"/>
+      <c r="GZ243" s="93"/>
+      <c r="HA243" s="93"/>
+      <c r="HB243" s="93"/>
+      <c r="HC243" s="93"/>
+      <c r="HD243" s="93"/>
+      <c r="HE243" s="93"/>
+      <c r="HF243" s="93"/>
+      <c r="HG243" s="93"/>
+      <c r="HH243" s="93"/>
+      <c r="HI243" s="93"/>
+      <c r="HJ243" s="93"/>
+      <c r="HK243" s="93"/>
+      <c r="HL243" s="93"/>
+      <c r="HM243" s="93"/>
+      <c r="HN243" s="93"/>
+      <c r="HO243" s="93"/>
+      <c r="HP243" s="93"/>
+      <c r="HQ243" s="93"/>
+      <c r="HR243" s="93"/>
+      <c r="HS243" s="93"/>
+      <c r="HT243" s="93"/>
+      <c r="HU243" s="93"/>
+      <c r="HV243" s="93"/>
+      <c r="HW243" s="93"/>
+      <c r="HX243" s="93"/>
+      <c r="HY243" s="93"/>
+      <c r="HZ243" s="93"/>
+      <c r="IA243" s="93"/>
+      <c r="IB243" s="93"/>
+      <c r="IC243" s="93"/>
+      <c r="ID243" s="93"/>
+      <c r="IE243" s="93"/>
+      <c r="IF243" s="93"/>
+      <c r="IG243" s="93"/>
+      <c r="IH243" s="93"/>
+      <c r="II243" s="93"/>
+      <c r="IJ243" s="93"/>
+      <c r="IK243" s="93"/>
+      <c r="IL243" s="93"/>
+      <c r="IM243" s="93"/>
+      <c r="IN243" s="93"/>
+      <c r="IO243" s="93"/>
+      <c r="IP243" s="93"/>
+      <c r="IQ243" s="93"/>
+      <c r="IR243" s="93"/>
+      <c r="IS243" s="93"/>
+      <c r="IT243" s="93"/>
+      <c r="IU243" s="93"/>
+      <c r="IV243" s="93"/>
+      <c r="IW243" s="93"/>
+      <c r="IX243" s="93"/>
+      <c r="IY243" s="93"/>
+      <c r="IZ243" s="93"/>
+      <c r="JA243" s="93"/>
+      <c r="JB243" s="93"/>
+      <c r="JC243" s="93"/>
+      <c r="JD243" s="93"/>
+      <c r="JE243" s="93"/>
+      <c r="JF243" s="93"/>
+      <c r="JG243" s="93"/>
+      <c r="JH243" s="93"/>
+      <c r="JI243" s="93"/>
+      <c r="JJ243" s="93"/>
+      <c r="JK243" s="93"/>
+      <c r="JL243" s="93"/>
+      <c r="JM243" s="93"/>
+      <c r="JN243" s="93"/>
+      <c r="JO243" s="93"/>
+      <c r="JP243" s="93"/>
+      <c r="JQ243" s="93"/>
+      <c r="JR243" s="93"/>
+      <c r="JS243" s="93"/>
+      <c r="JT243" s="93"/>
+      <c r="JU243" s="93"/>
+      <c r="JV243" s="93"/>
+      <c r="JW243" s="93"/>
+      <c r="JX243" s="93"/>
+      <c r="JY243" s="93"/>
+      <c r="JZ243" s="93"/>
+      <c r="KA243" s="93"/>
+      <c r="KB243" s="93"/>
+      <c r="KC243" s="93"/>
+      <c r="KD243" s="93"/>
+      <c r="KE243" s="93"/>
+      <c r="KF243" s="93"/>
+      <c r="KG243" s="93"/>
+      <c r="KH243" s="93"/>
+      <c r="KI243" s="93"/>
+      <c r="KJ243" s="93"/>
+      <c r="KK243" s="93"/>
+      <c r="KL243" s="93"/>
+      <c r="KM243" s="93"/>
+      <c r="KN243" s="93"/>
+      <c r="KO243" s="93"/>
+      <c r="KP243" s="93"/>
     </row>
     <row r="244" spans="1:302" x14ac:dyDescent="0.2">
-      <c r="B244" s="91">
-        <v>3</v>
-      </c>
-      <c r="C244" s="91">
-        <v>3</v>
-      </c>
-      <c r="D244" s="91">
-        <v>3</v>
-      </c>
-      <c r="E244" s="91">
-        <v>3</v>
-      </c>
-      <c r="AH244" s="91">
-        <v>3</v>
-      </c>
-      <c r="AI244" s="91">
-        <v>0</v>
-      </c>
-      <c r="AJ244" s="91">
-        <v>0</v>
-      </c>
-      <c r="AK244" s="91">
-        <v>3</v>
+      <c r="B244">
+        <v>3</v>
+      </c>
+      <c r="C244">
+        <v>3</v>
+      </c>
+      <c r="D244" s="86">
+        <v>3</v>
+      </c>
+      <c r="E244">
+        <v>3</v>
+      </c>
+      <c r="AH244">
+        <v>3</v>
+      </c>
+      <c r="AI244">
+        <v>0</v>
+      </c>
+      <c r="AJ244">
+        <v>0</v>
+      </c>
+      <c r="AK244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="46">
+        <v>112</v>
+      </c>
+      <c r="B245" s="29">
+        <v>3</v>
+      </c>
+      <c r="C245" s="87">
+        <v>4</v>
+      </c>
+      <c r="D245" s="29">
+        <v>3</v>
+      </c>
+      <c r="E245" s="29">
+        <v>3</v>
+      </c>
+      <c r="F245" s="28"/>
+      <c r="I245" s="30"/>
+      <c r="J245" s="28"/>
+      <c r="M245" s="30"/>
+      <c r="N245" s="29">
+        <v>0</v>
+      </c>
+      <c r="O245" s="29">
+        <v>3</v>
+      </c>
+      <c r="P245" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q245" s="28">
+        <v>6</v>
+      </c>
+      <c r="R245" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S245" s="65"/>
+      <c r="T245" s="65">
+        <v>3</v>
+      </c>
+      <c r="U245" s="65">
+        <v>-1</v>
+      </c>
+      <c r="V245" s="65"/>
+      <c r="W245" s="65" t="s">
+        <v>170</v>
+      </c>
+      <c r="X245" s="65"/>
+      <c r="Y245" s="65"/>
+      <c r="Z245" s="65"/>
+      <c r="AA245" s="65"/>
+      <c r="AB245" s="65"/>
+      <c r="AC245" s="65"/>
+      <c r="AD245" s="65"/>
+      <c r="AE245" s="65"/>
+      <c r="AF245" s="65"/>
+      <c r="AG245" s="91"/>
+      <c r="AH245" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI245" s="29">
+        <v>4</v>
+      </c>
+      <c r="AJ245" s="29">
+        <v>3</v>
+      </c>
+      <c r="AK245" s="29">
+        <v>3</v>
+      </c>
+      <c r="AP245" s="29">
+        <v>0</v>
+      </c>
+      <c r="AQ245" s="29">
+        <v>3</v>
+      </c>
+      <c r="AR245" s="92" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS245" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="AT245" s="93"/>
+      <c r="AU245" s="93"/>
+      <c r="AV245" s="93"/>
+      <c r="AW245" s="93"/>
+      <c r="AX245" s="93"/>
+      <c r="AY245" s="93"/>
+      <c r="AZ245" s="93"/>
+      <c r="BA245" s="93"/>
+      <c r="BB245" s="93"/>
+      <c r="BC245" s="93"/>
+      <c r="BD245" s="93"/>
+      <c r="BE245" s="93"/>
+      <c r="BF245" s="93"/>
+      <c r="BG245" s="93"/>
+      <c r="BH245" s="93"/>
+      <c r="BI245" s="93"/>
+      <c r="BJ245" s="93"/>
+      <c r="BK245" s="93"/>
+      <c r="BL245" s="93"/>
+      <c r="BM245" s="93"/>
+      <c r="BN245" s="93"/>
+      <c r="BO245" s="93"/>
+      <c r="BP245" s="93"/>
+      <c r="BQ245" s="93"/>
+      <c r="BR245" s="93"/>
+      <c r="BS245" s="93"/>
+      <c r="BT245" s="93"/>
+      <c r="BU245" s="93"/>
+      <c r="BV245" s="93"/>
+      <c r="BW245" s="93"/>
+      <c r="BX245" s="93"/>
+      <c r="BY245" s="93"/>
+      <c r="BZ245" s="93"/>
+      <c r="CA245" s="93"/>
+      <c r="CB245" s="93"/>
+      <c r="CC245" s="93"/>
+      <c r="CD245" s="93"/>
+      <c r="CE245" s="93"/>
+      <c r="CF245" s="93"/>
+      <c r="CG245" s="93"/>
+      <c r="CH245" s="93"/>
+      <c r="CI245" s="93"/>
+      <c r="CJ245" s="93"/>
+      <c r="CK245" s="93"/>
+      <c r="CL245" s="93"/>
+      <c r="CM245" s="93"/>
+      <c r="CN245" s="93"/>
+      <c r="CO245" s="93"/>
+      <c r="CP245" s="93"/>
+      <c r="CQ245" s="93"/>
+      <c r="CR245" s="93"/>
+      <c r="CS245" s="93"/>
+      <c r="CT245" s="93"/>
+      <c r="CU245" s="93"/>
+      <c r="CV245" s="93"/>
+      <c r="CW245" s="93"/>
+      <c r="CX245" s="93"/>
+      <c r="CY245" s="93"/>
+      <c r="CZ245" s="93"/>
+      <c r="DA245" s="93"/>
+      <c r="DB245" s="93"/>
+      <c r="DC245" s="93"/>
+      <c r="DD245" s="93"/>
+      <c r="DE245" s="93"/>
+      <c r="DF245" s="93"/>
+      <c r="DG245" s="93"/>
+      <c r="DH245" s="93"/>
+      <c r="DI245" s="93"/>
+      <c r="DJ245" s="93"/>
+      <c r="DK245" s="93"/>
+      <c r="DL245" s="93"/>
+      <c r="DM245" s="93"/>
+      <c r="DN245" s="93"/>
+      <c r="DO245" s="93"/>
+      <c r="DP245" s="93"/>
+      <c r="DQ245" s="93"/>
+      <c r="DR245" s="93"/>
+      <c r="DS245" s="93"/>
+      <c r="DT245" s="93"/>
+      <c r="DU245" s="93"/>
+      <c r="DV245" s="93"/>
+      <c r="DW245" s="93"/>
+      <c r="DX245" s="93"/>
+      <c r="DY245" s="93"/>
+      <c r="DZ245" s="93"/>
+      <c r="EA245" s="93"/>
+      <c r="EB245" s="93"/>
+      <c r="EC245" s="93"/>
+      <c r="ED245" s="93"/>
+      <c r="EE245" s="93"/>
+      <c r="EF245" s="93"/>
+      <c r="EG245" s="93"/>
+      <c r="EH245" s="93"/>
+      <c r="EI245" s="93"/>
+      <c r="EJ245" s="93"/>
+      <c r="EK245" s="93"/>
+      <c r="EL245" s="93"/>
+      <c r="EM245" s="93"/>
+      <c r="EN245" s="93"/>
+      <c r="EO245" s="93"/>
+      <c r="EP245" s="93"/>
+      <c r="EQ245" s="93"/>
+      <c r="ER245" s="93"/>
+      <c r="ES245" s="93"/>
+      <c r="ET245" s="93"/>
+      <c r="EU245" s="93"/>
+      <c r="EV245" s="93"/>
+      <c r="EW245" s="93"/>
+      <c r="EX245" s="93"/>
+      <c r="EY245" s="93"/>
+      <c r="EZ245" s="93"/>
+      <c r="FA245" s="93"/>
+      <c r="FB245" s="93"/>
+      <c r="FC245" s="93"/>
+      <c r="FD245" s="93"/>
+      <c r="FE245" s="93"/>
+      <c r="FF245" s="93"/>
+      <c r="FG245" s="93"/>
+      <c r="FH245" s="93"/>
+      <c r="FI245" s="93"/>
+      <c r="FJ245" s="93"/>
+      <c r="FK245" s="93"/>
+      <c r="FL245" s="93"/>
+      <c r="FM245" s="93"/>
+      <c r="FN245" s="93"/>
+      <c r="FO245" s="93"/>
+      <c r="FP245" s="93"/>
+      <c r="FQ245" s="93"/>
+      <c r="FR245" s="93"/>
+      <c r="FS245" s="93"/>
+      <c r="FT245" s="93"/>
+      <c r="FU245" s="93"/>
+      <c r="FV245" s="93"/>
+      <c r="FW245" s="93"/>
+      <c r="FX245" s="93"/>
+      <c r="FY245" s="93"/>
+      <c r="FZ245" s="93"/>
+      <c r="GA245" s="93"/>
+      <c r="GB245" s="93"/>
+      <c r="GC245" s="93"/>
+      <c r="GD245" s="93"/>
+      <c r="GE245" s="93"/>
+      <c r="GF245" s="93"/>
+      <c r="GG245" s="93"/>
+      <c r="GH245" s="93"/>
+      <c r="GI245" s="93"/>
+      <c r="GJ245" s="93"/>
+      <c r="GK245" s="93"/>
+      <c r="GL245" s="93"/>
+      <c r="GM245" s="93"/>
+      <c r="GN245" s="93"/>
+      <c r="GO245" s="93"/>
+      <c r="GP245" s="93"/>
+      <c r="GQ245" s="93"/>
+      <c r="GR245" s="93"/>
+      <c r="GS245" s="93"/>
+      <c r="GT245" s="93"/>
+      <c r="GU245" s="93"/>
+      <c r="GV245" s="93"/>
+      <c r="GW245" s="93"/>
+      <c r="GX245" s="93"/>
+      <c r="GY245" s="93"/>
+      <c r="GZ245" s="93"/>
+      <c r="HA245" s="93"/>
+      <c r="HB245" s="93"/>
+      <c r="HC245" s="93"/>
+      <c r="HD245" s="93"/>
+      <c r="HE245" s="93"/>
+      <c r="HF245" s="93"/>
+      <c r="HG245" s="93"/>
+      <c r="HH245" s="93"/>
+      <c r="HI245" s="93"/>
+      <c r="HJ245" s="93"/>
+      <c r="HK245" s="93"/>
+      <c r="HL245" s="93"/>
+      <c r="HM245" s="93"/>
+      <c r="HN245" s="93"/>
+      <c r="HO245" s="93"/>
+      <c r="HP245" s="93"/>
+      <c r="HQ245" s="93"/>
+      <c r="HR245" s="93"/>
+      <c r="HS245" s="93"/>
+      <c r="HT245" s="93"/>
+      <c r="HU245" s="93"/>
+      <c r="HV245" s="93"/>
+      <c r="HW245" s="93"/>
+      <c r="HX245" s="93"/>
+      <c r="HY245" s="93"/>
+      <c r="HZ245" s="93"/>
+      <c r="IA245" s="93"/>
+      <c r="IB245" s="93"/>
+      <c r="IC245" s="93"/>
+      <c r="ID245" s="93"/>
+      <c r="IE245" s="93"/>
+      <c r="IF245" s="93"/>
+      <c r="IG245" s="93"/>
+      <c r="IH245" s="93"/>
+      <c r="II245" s="93"/>
+      <c r="IJ245" s="93"/>
+      <c r="IK245" s="93"/>
+      <c r="IL245" s="93"/>
+      <c r="IM245" s="93"/>
+      <c r="IN245" s="93"/>
+      <c r="IO245" s="93"/>
+      <c r="IP245" s="93"/>
+      <c r="IQ245" s="93"/>
+      <c r="IR245" s="93"/>
+      <c r="IS245" s="93"/>
+      <c r="IT245" s="93"/>
+      <c r="IU245" s="93"/>
+      <c r="IV245" s="93"/>
+      <c r="IW245" s="93"/>
+      <c r="IX245" s="93"/>
+      <c r="IY245" s="93"/>
+      <c r="IZ245" s="93"/>
+      <c r="JA245" s="93"/>
+      <c r="JB245" s="93"/>
+      <c r="JC245" s="93"/>
+      <c r="JD245" s="93"/>
+      <c r="JE245" s="93"/>
+      <c r="JF245" s="93"/>
+      <c r="JG245" s="93"/>
+      <c r="JH245" s="93"/>
+      <c r="JI245" s="93"/>
+      <c r="JJ245" s="93"/>
+      <c r="JK245" s="93"/>
+      <c r="JL245" s="93"/>
+      <c r="JM245" s="93"/>
+      <c r="JN245" s="93"/>
+      <c r="JO245" s="93"/>
+      <c r="JP245" s="93"/>
+      <c r="JQ245" s="93"/>
+      <c r="JR245" s="93"/>
+      <c r="JS245" s="93"/>
+      <c r="JT245" s="93"/>
+      <c r="JU245" s="93"/>
+      <c r="JV245" s="93"/>
+      <c r="JW245" s="93"/>
+      <c r="JX245" s="93"/>
+      <c r="JY245" s="93"/>
+      <c r="JZ245" s="93"/>
+      <c r="KA245" s="93"/>
+      <c r="KB245" s="93"/>
+      <c r="KC245" s="93"/>
+      <c r="KD245" s="93"/>
+      <c r="KE245" s="93"/>
+      <c r="KF245" s="93"/>
+      <c r="KG245" s="93"/>
+      <c r="KH245" s="93"/>
+      <c r="KI245" s="93"/>
+      <c r="KJ245" s="93"/>
+      <c r="KK245" s="93"/>
+      <c r="KL245" s="93"/>
+      <c r="KM245" s="93"/>
+      <c r="KN245" s="93"/>
+      <c r="KO245" s="93"/>
+      <c r="KP245" s="93"/>
+    </row>
+    <row r="246" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B246">
+        <v>3</v>
+      </c>
+      <c r="C246">
+        <v>2</v>
+      </c>
+      <c r="D246">
+        <v>3</v>
+      </c>
+      <c r="E246">
+        <v>0</v>
+      </c>
+      <c r="AH246">
+        <v>3</v>
+      </c>
+      <c r="AI246">
+        <v>2</v>
+      </c>
+      <c r="AJ246">
+        <v>3</v>
+      </c>
+      <c r="AK246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="46">
+        <v>113</v>
+      </c>
+      <c r="B247" s="29">
+        <v>3</v>
+      </c>
+      <c r="C247" s="29">
+        <v>2</v>
+      </c>
+      <c r="D247" s="29">
+        <v>2</v>
+      </c>
+      <c r="E247" s="29">
+        <v>3</v>
+      </c>
+      <c r="F247" s="28"/>
+      <c r="I247" s="30"/>
+      <c r="J247" s="28"/>
+      <c r="M247" s="30"/>
+      <c r="N247" s="29">
+        <v>0</v>
+      </c>
+      <c r="O247" s="29">
+        <v>0</v>
+      </c>
+      <c r="P247" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q247" s="28">
+        <v>2</v>
+      </c>
+      <c r="R247" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S247" s="65"/>
+      <c r="T247" s="65">
+        <v>3</v>
+      </c>
+      <c r="U247" s="65">
+        <v>3</v>
+      </c>
+      <c r="V247" s="65"/>
+      <c r="W247" s="65" t="s">
+        <v>170</v>
+      </c>
+      <c r="X247" s="65"/>
+      <c r="Y247" s="65"/>
+      <c r="Z247" s="65"/>
+      <c r="AA247" s="65"/>
+      <c r="AB247" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC247" s="65"/>
+      <c r="AD247" s="65"/>
+      <c r="AE247" s="65"/>
+      <c r="AF247" s="65"/>
+      <c r="AG247" s="91"/>
+      <c r="AH247" s="29">
+        <v>0</v>
+      </c>
+      <c r="AI247" s="29">
+        <v>2</v>
+      </c>
+      <c r="AJ247" s="29">
+        <v>2</v>
+      </c>
+      <c r="AK247" s="29">
+        <v>3</v>
+      </c>
+      <c r="AP247" s="29">
+        <v>0</v>
+      </c>
+      <c r="AQ247" s="29">
+        <v>9</v>
+      </c>
+      <c r="AR247" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS247" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="AT247" s="93"/>
+      <c r="AU247" s="93"/>
+      <c r="AV247" s="93"/>
+      <c r="AW247" s="93"/>
+      <c r="AX247" s="93"/>
+      <c r="AY247" s="93"/>
+      <c r="AZ247" s="93"/>
+      <c r="BA247" s="93"/>
+      <c r="BB247" s="93"/>
+      <c r="BC247" s="93"/>
+      <c r="BD247" s="93"/>
+      <c r="BE247" s="93"/>
+      <c r="BF247" s="93"/>
+      <c r="BG247" s="93"/>
+      <c r="BH247" s="93"/>
+      <c r="BI247" s="93"/>
+      <c r="BJ247" s="93"/>
+      <c r="BK247" s="93"/>
+      <c r="BL247" s="93"/>
+      <c r="BM247" s="93"/>
+      <c r="BN247" s="93"/>
+      <c r="BO247" s="93"/>
+      <c r="BP247" s="93"/>
+      <c r="BQ247" s="93"/>
+      <c r="BR247" s="93"/>
+      <c r="BS247" s="93"/>
+      <c r="BT247" s="93"/>
+      <c r="BU247" s="93"/>
+      <c r="BV247" s="93"/>
+      <c r="BW247" s="93"/>
+      <c r="BX247" s="93"/>
+      <c r="BY247" s="93"/>
+      <c r="BZ247" s="93"/>
+      <c r="CA247" s="93"/>
+      <c r="CB247" s="93"/>
+      <c r="CC247" s="93"/>
+      <c r="CD247" s="93"/>
+      <c r="CE247" s="93"/>
+      <c r="CF247" s="93"/>
+      <c r="CG247" s="93"/>
+      <c r="CH247" s="93"/>
+      <c r="CI247" s="93"/>
+      <c r="CJ247" s="93"/>
+      <c r="CK247" s="93"/>
+      <c r="CL247" s="93"/>
+      <c r="CM247" s="93"/>
+      <c r="CN247" s="93"/>
+      <c r="CO247" s="93"/>
+      <c r="CP247" s="93"/>
+      <c r="CQ247" s="93"/>
+      <c r="CR247" s="93"/>
+      <c r="CS247" s="93"/>
+      <c r="CT247" s="93"/>
+      <c r="CU247" s="93"/>
+      <c r="CV247" s="93"/>
+      <c r="CW247" s="93"/>
+      <c r="CX247" s="93"/>
+      <c r="CY247" s="93"/>
+      <c r="CZ247" s="93"/>
+      <c r="DA247" s="93"/>
+      <c r="DB247" s="93"/>
+      <c r="DC247" s="93"/>
+      <c r="DD247" s="93"/>
+      <c r="DE247" s="93"/>
+      <c r="DF247" s="93"/>
+      <c r="DG247" s="93"/>
+      <c r="DH247" s="93"/>
+      <c r="DI247" s="93"/>
+      <c r="DJ247" s="93"/>
+      <c r="DK247" s="93"/>
+      <c r="DL247" s="93"/>
+      <c r="DM247" s="93"/>
+      <c r="DN247" s="93"/>
+      <c r="DO247" s="93"/>
+      <c r="DP247" s="93"/>
+      <c r="DQ247" s="93"/>
+      <c r="DR247" s="93"/>
+      <c r="DS247" s="93"/>
+      <c r="DT247" s="93"/>
+      <c r="DU247" s="93"/>
+      <c r="DV247" s="93"/>
+      <c r="DW247" s="93"/>
+      <c r="DX247" s="93"/>
+      <c r="DY247" s="93"/>
+      <c r="DZ247" s="93"/>
+      <c r="EA247" s="93"/>
+      <c r="EB247" s="93"/>
+      <c r="EC247" s="93"/>
+      <c r="ED247" s="93"/>
+      <c r="EE247" s="93"/>
+      <c r="EF247" s="93"/>
+      <c r="EG247" s="93"/>
+      <c r="EH247" s="93"/>
+      <c r="EI247" s="93"/>
+      <c r="EJ247" s="93"/>
+      <c r="EK247" s="93"/>
+      <c r="EL247" s="93"/>
+      <c r="EM247" s="93"/>
+      <c r="EN247" s="93"/>
+      <c r="EO247" s="93"/>
+      <c r="EP247" s="93"/>
+      <c r="EQ247" s="93"/>
+      <c r="ER247" s="93"/>
+      <c r="ES247" s="93"/>
+      <c r="ET247" s="93"/>
+      <c r="EU247" s="93"/>
+      <c r="EV247" s="93"/>
+      <c r="EW247" s="93"/>
+      <c r="EX247" s="93"/>
+      <c r="EY247" s="93"/>
+      <c r="EZ247" s="93"/>
+      <c r="FA247" s="93"/>
+      <c r="FB247" s="93"/>
+      <c r="FC247" s="93"/>
+      <c r="FD247" s="93"/>
+      <c r="FE247" s="93"/>
+      <c r="FF247" s="93"/>
+      <c r="FG247" s="93"/>
+      <c r="FH247" s="93"/>
+      <c r="FI247" s="93"/>
+      <c r="FJ247" s="93"/>
+      <c r="FK247" s="93"/>
+      <c r="FL247" s="93"/>
+      <c r="FM247" s="93"/>
+      <c r="FN247" s="93"/>
+      <c r="FO247" s="93"/>
+      <c r="FP247" s="93"/>
+      <c r="FQ247" s="93"/>
+      <c r="FR247" s="93"/>
+      <c r="FS247" s="93"/>
+      <c r="FT247" s="93"/>
+      <c r="FU247" s="93"/>
+      <c r="FV247" s="93"/>
+      <c r="FW247" s="93"/>
+      <c r="FX247" s="93"/>
+      <c r="FY247" s="93"/>
+      <c r="FZ247" s="93"/>
+      <c r="GA247" s="93"/>
+      <c r="GB247" s="93"/>
+      <c r="GC247" s="93"/>
+      <c r="GD247" s="93"/>
+      <c r="GE247" s="93"/>
+      <c r="GF247" s="93"/>
+      <c r="GG247" s="93"/>
+      <c r="GH247" s="93"/>
+      <c r="GI247" s="93"/>
+      <c r="GJ247" s="93"/>
+      <c r="GK247" s="93"/>
+      <c r="GL247" s="93"/>
+      <c r="GM247" s="93"/>
+      <c r="GN247" s="93"/>
+      <c r="GO247" s="93"/>
+      <c r="GP247" s="93"/>
+      <c r="GQ247" s="93"/>
+      <c r="GR247" s="93"/>
+      <c r="GS247" s="93"/>
+      <c r="GT247" s="93"/>
+      <c r="GU247" s="93"/>
+      <c r="GV247" s="93"/>
+      <c r="GW247" s="93"/>
+      <c r="GX247" s="93"/>
+      <c r="GY247" s="93"/>
+      <c r="GZ247" s="93"/>
+      <c r="HA247" s="93"/>
+      <c r="HB247" s="93"/>
+      <c r="HC247" s="93"/>
+      <c r="HD247" s="93"/>
+      <c r="HE247" s="93"/>
+      <c r="HF247" s="93"/>
+      <c r="HG247" s="93"/>
+      <c r="HH247" s="93"/>
+      <c r="HI247" s="93"/>
+      <c r="HJ247" s="93"/>
+      <c r="HK247" s="93"/>
+      <c r="HL247" s="93"/>
+      <c r="HM247" s="93"/>
+      <c r="HN247" s="93"/>
+      <c r="HO247" s="93"/>
+      <c r="HP247" s="93"/>
+      <c r="HQ247" s="93"/>
+      <c r="HR247" s="93"/>
+      <c r="HS247" s="93"/>
+      <c r="HT247" s="93"/>
+      <c r="HU247" s="93"/>
+      <c r="HV247" s="93"/>
+      <c r="HW247" s="93"/>
+      <c r="HX247" s="93"/>
+      <c r="HY247" s="93"/>
+      <c r="HZ247" s="93"/>
+      <c r="IA247" s="93"/>
+      <c r="IB247" s="93"/>
+      <c r="IC247" s="93"/>
+      <c r="ID247" s="93"/>
+      <c r="IE247" s="93"/>
+      <c r="IF247" s="93"/>
+      <c r="IG247" s="93"/>
+      <c r="IH247" s="93"/>
+      <c r="II247" s="93"/>
+      <c r="IJ247" s="93"/>
+      <c r="IK247" s="93"/>
+      <c r="IL247" s="93"/>
+      <c r="IM247" s="93"/>
+      <c r="IN247" s="93"/>
+      <c r="IO247" s="93"/>
+      <c r="IP247" s="93"/>
+      <c r="IQ247" s="93"/>
+      <c r="IR247" s="93"/>
+      <c r="IS247" s="93"/>
+      <c r="IT247" s="93"/>
+      <c r="IU247" s="93"/>
+      <c r="IV247" s="93"/>
+      <c r="IW247" s="93"/>
+      <c r="IX247" s="93"/>
+      <c r="IY247" s="93"/>
+      <c r="IZ247" s="93"/>
+      <c r="JA247" s="93"/>
+      <c r="JB247" s="93"/>
+      <c r="JC247" s="93"/>
+      <c r="JD247" s="93"/>
+      <c r="JE247" s="93"/>
+      <c r="JF247" s="93"/>
+      <c r="JG247" s="93"/>
+      <c r="JH247" s="93"/>
+      <c r="JI247" s="93"/>
+      <c r="JJ247" s="93"/>
+      <c r="JK247" s="93"/>
+      <c r="JL247" s="93"/>
+      <c r="JM247" s="93"/>
+      <c r="JN247" s="93"/>
+      <c r="JO247" s="93"/>
+      <c r="JP247" s="93"/>
+      <c r="JQ247" s="93"/>
+      <c r="JR247" s="93"/>
+      <c r="JS247" s="93"/>
+      <c r="JT247" s="93"/>
+      <c r="JU247" s="93"/>
+      <c r="JV247" s="93"/>
+      <c r="JW247" s="93"/>
+      <c r="JX247" s="93"/>
+      <c r="JY247" s="93"/>
+      <c r="JZ247" s="93"/>
+      <c r="KA247" s="93"/>
+      <c r="KB247" s="93"/>
+      <c r="KC247" s="93"/>
+      <c r="KD247" s="93"/>
+      <c r="KE247" s="93"/>
+      <c r="KF247" s="93"/>
+      <c r="KG247" s="93"/>
+      <c r="KH247" s="93"/>
+      <c r="KI247" s="93"/>
+      <c r="KJ247" s="93"/>
+      <c r="KK247" s="93"/>
+      <c r="KL247" s="93"/>
+      <c r="KM247" s="93"/>
+      <c r="KN247" s="93"/>
+      <c r="KO247" s="93"/>
+      <c r="KP247" s="93"/>
+    </row>
+    <row r="248" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B248">
+        <v>3</v>
+      </c>
+      <c r="C248">
+        <v>3</v>
+      </c>
+      <c r="D248" s="86">
+        <v>4</v>
+      </c>
+      <c r="E248">
+        <v>4</v>
+      </c>
+      <c r="AH248">
+        <v>0</v>
+      </c>
+      <c r="AI248">
+        <v>0</v>
+      </c>
+      <c r="AJ248">
+        <v>4</v>
+      </c>
+      <c r="AK248">
+        <v>4</v>
+      </c>
+      <c r="AS248" s="94" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected OWN/OPP_CONT by adding capt_start to MoveData as a property that sets both a hidden attribute and capt_loc. The checks for OWN/OPP_CONT now use capt_start which is not changed during the capturer. Disallowed the combination of LAPPER, CaptDir.BOTH, and CaptType.NEXT because the capture behavior is odd.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710C710E-7FFF-4F64-8296-CAC7A75AF9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377A4C32-D003-44C7-9222-D8FF6DEEE178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capture_test_data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="184">
   <si>
     <t>setup</t>
   </si>
@@ -574,6 +574,18 @@
   <si>
     <t>capt both/next - center needs to stay</t>
   </si>
+  <si>
+    <t>113b</t>
+  </si>
+  <si>
+    <t>only tested without LAPPER</t>
+  </si>
+  <si>
+    <t>OPP_CONT capture</t>
+  </si>
+  <si>
+    <t>OWN_CONT capture</t>
+  </si>
 </sst>
 </file>
 
@@ -797,7 +809,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1028,6 +1040,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1050,7 +1073,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1229,8 +1252,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1564,12 +1588,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AMK251"/>
+  <dimension ref="A1:AMK258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A251" sqref="A251"/>
+      <selection pane="bottomLeft" activeCell="AK256" sqref="AK256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -43829,7 +43853,9 @@
       <c r="AS241" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="AT241" s="93"/>
+      <c r="AT241" s="93" t="s">
+        <v>181</v>
+      </c>
       <c r="AU241" s="93"/>
       <c r="AV241" s="93"/>
       <c r="AW241" s="93"/>
@@ -44925,7 +44951,9 @@
       <c r="AS247" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="AT247" s="93"/>
+      <c r="AT247" s="93" t="s">
+        <v>181</v>
+      </c>
       <c r="AU247" s="93"/>
       <c r="AV247" s="93"/>
       <c r="AW247" s="93"/>
@@ -45213,46 +45241,46 @@
       </c>
     </row>
     <row r="249" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A249" s="46">
-        <v>114</v>
+      <c r="A249" s="46" t="s">
+        <v>180</v>
       </c>
       <c r="B249" s="29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C249" s="29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D249" s="29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E249" s="29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F249" s="28"/>
       <c r="I249" s="30"/>
       <c r="J249" s="28"/>
       <c r="M249" s="30"/>
       <c r="N249" s="29">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="O249" s="29">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P249" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q249" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R249" s="30" t="s">
         <v>32</v>
       </c>
       <c r="S249" s="65"/>
       <c r="T249" s="65">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U249" s="65">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="V249" s="65"/>
       <c r="W249" s="65" t="s">
@@ -45274,27 +45302,29 @@
         <v>0</v>
       </c>
       <c r="AI249" s="29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ249" s="29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK249" s="29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP249" s="29">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AQ249" s="29">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AR249" s="92" t="b">
         <v>1</v>
       </c>
       <c r="AS249" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="AT249" s="93"/>
+        <v>175</v>
+      </c>
+      <c r="AT249" s="93" t="s">
+        <v>181</v>
+      </c>
       <c r="AU249" s="93"/>
       <c r="AV249" s="93"/>
       <c r="AW249" s="93"/>
@@ -45553,56 +45583,119 @@
       <c r="KP249" s="93"/>
     </row>
     <row r="250" spans="1:302" x14ac:dyDescent="0.2">
-      <c r="B250" s="94">
-        <v>0</v>
-      </c>
-      <c r="C250" s="95">
-        <v>1</v>
-      </c>
-      <c r="D250" s="94">
-        <v>1</v>
-      </c>
-      <c r="E250" s="94">
+      <c r="B250">
+        <v>3</v>
+      </c>
+      <c r="C250">
+        <v>3</v>
+      </c>
+      <c r="D250" s="86">
+        <v>3</v>
+      </c>
+      <c r="E250">
         <v>4</v>
       </c>
-      <c r="AH250" s="94">
-        <v>0</v>
-      </c>
-      <c r="AI250" s="94">
-        <v>1</v>
-      </c>
-      <c r="AJ250" s="94">
-        <v>0</v>
-      </c>
-      <c r="AK250" s="94">
+      <c r="AH250">
+        <v>0</v>
+      </c>
+      <c r="AI250">
+        <v>0</v>
+      </c>
+      <c r="AJ250">
+        <v>3</v>
+      </c>
+      <c r="AK250">
         <v>4</v>
+      </c>
+      <c r="AS250" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="251" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A251" s="46"/>
+      <c r="A251" s="46">
+        <v>114</v>
+      </c>
+      <c r="B251" s="29">
+        <v>0</v>
+      </c>
+      <c r="C251" s="29">
+        <v>0</v>
+      </c>
+      <c r="D251" s="29">
+        <v>4</v>
+      </c>
+      <c r="E251" s="29">
+        <v>0</v>
+      </c>
       <c r="F251" s="28"/>
       <c r="I251" s="30"/>
       <c r="J251" s="28"/>
       <c r="M251" s="30"/>
-      <c r="Q251" s="28"/>
-      <c r="R251" s="30"/>
+      <c r="N251" s="29">
+        <v>7</v>
+      </c>
+      <c r="O251" s="29">
+        <v>7</v>
+      </c>
+      <c r="P251" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q251" s="28">
+        <v>1</v>
+      </c>
+      <c r="R251" s="30" t="s">
+        <v>32</v>
+      </c>
       <c r="S251" s="65"/>
-      <c r="T251" s="65"/>
-      <c r="U251" s="65"/>
+      <c r="T251" s="65">
+        <v>1</v>
+      </c>
+      <c r="U251" s="65">
+        <v>-1</v>
+      </c>
       <c r="V251" s="65"/>
-      <c r="W251" s="65"/>
+      <c r="W251" s="65" t="s">
+        <v>170</v>
+      </c>
       <c r="X251" s="65"/>
       <c r="Y251" s="65"/>
       <c r="Z251" s="65"/>
       <c r="AA251" s="65"/>
-      <c r="AB251" s="65"/>
+      <c r="AB251" s="65" t="s">
+        <v>141</v>
+      </c>
       <c r="AC251" s="65"/>
       <c r="AD251" s="65"/>
       <c r="AE251" s="65"/>
       <c r="AF251" s="65"/>
       <c r="AG251" s="91"/>
-      <c r="AR251" s="92"/>
-      <c r="AT251" s="93"/>
+      <c r="AH251" s="29">
+        <v>0</v>
+      </c>
+      <c r="AI251" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ251" s="29">
+        <v>4</v>
+      </c>
+      <c r="AK251" s="29">
+        <v>0</v>
+      </c>
+      <c r="AP251" s="29">
+        <v>8</v>
+      </c>
+      <c r="AQ251" s="29">
+        <v>7</v>
+      </c>
+      <c r="AR251" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS251" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="AT251" s="93" t="s">
+        <v>181</v>
+      </c>
       <c r="AU251" s="93"/>
       <c r="AV251" s="93"/>
       <c r="AW251" s="93"/>
@@ -45860,6 +45953,1420 @@
       <c r="KO251" s="93"/>
       <c r="KP251" s="93"/>
     </row>
+    <row r="252" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B252">
+        <v>0</v>
+      </c>
+      <c r="C252" s="86">
+        <v>1</v>
+      </c>
+      <c r="D252">
+        <v>1</v>
+      </c>
+      <c r="E252">
+        <v>4</v>
+      </c>
+      <c r="AH252">
+        <v>0</v>
+      </c>
+      <c r="AI252">
+        <v>1</v>
+      </c>
+      <c r="AJ252">
+        <v>0</v>
+      </c>
+      <c r="AK252">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="46">
+        <v>115</v>
+      </c>
+      <c r="B253" s="29">
+        <v>1</v>
+      </c>
+      <c r="C253" s="29">
+        <v>0</v>
+      </c>
+      <c r="D253" s="29">
+        <v>4</v>
+      </c>
+      <c r="E253" s="29">
+        <v>0</v>
+      </c>
+      <c r="F253" s="28"/>
+      <c r="I253" s="30"/>
+      <c r="J253" s="28"/>
+      <c r="M253" s="30"/>
+      <c r="N253" s="29">
+        <v>6</v>
+      </c>
+      <c r="O253" s="29">
+        <v>7</v>
+      </c>
+      <c r="P253" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q253" s="28">
+        <v>1</v>
+      </c>
+      <c r="R253" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S253" s="65"/>
+      <c r="T253" s="65">
+        <v>1</v>
+      </c>
+      <c r="U253" s="65">
+        <v>-1</v>
+      </c>
+      <c r="V253" s="65"/>
+      <c r="W253" s="65" t="s">
+        <v>170</v>
+      </c>
+      <c r="X253" s="65"/>
+      <c r="Y253" s="65"/>
+      <c r="Z253" s="65"/>
+      <c r="AA253" s="65"/>
+      <c r="AB253" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC253" s="65"/>
+      <c r="AD253" s="65"/>
+      <c r="AE253" s="65"/>
+      <c r="AF253" s="65"/>
+      <c r="AG253" s="91"/>
+      <c r="AH253" s="94">
+        <v>1</v>
+      </c>
+      <c r="AI253" s="95">
+        <v>0</v>
+      </c>
+      <c r="AJ253" s="95">
+        <v>4</v>
+      </c>
+      <c r="AK253" s="95">
+        <v>0</v>
+      </c>
+      <c r="AP253" s="29">
+        <v>7</v>
+      </c>
+      <c r="AQ253" s="29">
+        <v>7</v>
+      </c>
+      <c r="AR253" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS253" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="AT253" s="93" t="s">
+        <v>181</v>
+      </c>
+      <c r="AU253" s="93"/>
+      <c r="AV253" s="93"/>
+      <c r="AW253" s="93"/>
+      <c r="AX253" s="93"/>
+      <c r="AY253" s="93"/>
+      <c r="AZ253" s="93"/>
+      <c r="BA253" s="93"/>
+      <c r="BB253" s="93"/>
+      <c r="BC253" s="93"/>
+      <c r="BD253" s="93"/>
+      <c r="BE253" s="93"/>
+      <c r="BF253" s="93"/>
+      <c r="BG253" s="93"/>
+      <c r="BH253" s="93"/>
+      <c r="BI253" s="93"/>
+      <c r="BJ253" s="93"/>
+      <c r="BK253" s="93"/>
+      <c r="BL253" s="93"/>
+      <c r="BM253" s="93"/>
+      <c r="BN253" s="93"/>
+      <c r="BO253" s="93"/>
+      <c r="BP253" s="93"/>
+      <c r="BQ253" s="93"/>
+      <c r="BR253" s="93"/>
+      <c r="BS253" s="93"/>
+      <c r="BT253" s="93"/>
+      <c r="BU253" s="93"/>
+      <c r="BV253" s="93"/>
+      <c r="BW253" s="93"/>
+      <c r="BX253" s="93"/>
+      <c r="BY253" s="93"/>
+      <c r="BZ253" s="93"/>
+      <c r="CA253" s="93"/>
+      <c r="CB253" s="93"/>
+      <c r="CC253" s="93"/>
+      <c r="CD253" s="93"/>
+      <c r="CE253" s="93"/>
+      <c r="CF253" s="93"/>
+      <c r="CG253" s="93"/>
+      <c r="CH253" s="93"/>
+      <c r="CI253" s="93"/>
+      <c r="CJ253" s="93"/>
+      <c r="CK253" s="93"/>
+      <c r="CL253" s="93"/>
+      <c r="CM253" s="93"/>
+      <c r="CN253" s="93"/>
+      <c r="CO253" s="93"/>
+      <c r="CP253" s="93"/>
+      <c r="CQ253" s="93"/>
+      <c r="CR253" s="93"/>
+      <c r="CS253" s="93"/>
+      <c r="CT253" s="93"/>
+      <c r="CU253" s="93"/>
+      <c r="CV253" s="93"/>
+      <c r="CW253" s="93"/>
+      <c r="CX253" s="93"/>
+      <c r="CY253" s="93"/>
+      <c r="CZ253" s="93"/>
+      <c r="DA253" s="93"/>
+      <c r="DB253" s="93"/>
+      <c r="DC253" s="93"/>
+      <c r="DD253" s="93"/>
+      <c r="DE253" s="93"/>
+      <c r="DF253" s="93"/>
+      <c r="DG253" s="93"/>
+      <c r="DH253" s="93"/>
+      <c r="DI253" s="93"/>
+      <c r="DJ253" s="93"/>
+      <c r="DK253" s="93"/>
+      <c r="DL253" s="93"/>
+      <c r="DM253" s="93"/>
+      <c r="DN253" s="93"/>
+      <c r="DO253" s="93"/>
+      <c r="DP253" s="93"/>
+      <c r="DQ253" s="93"/>
+      <c r="DR253" s="93"/>
+      <c r="DS253" s="93"/>
+      <c r="DT253" s="93"/>
+      <c r="DU253" s="93"/>
+      <c r="DV253" s="93"/>
+      <c r="DW253" s="93"/>
+      <c r="DX253" s="93"/>
+      <c r="DY253" s="93"/>
+      <c r="DZ253" s="93"/>
+      <c r="EA253" s="93"/>
+      <c r="EB253" s="93"/>
+      <c r="EC253" s="93"/>
+      <c r="ED253" s="93"/>
+      <c r="EE253" s="93"/>
+      <c r="EF253" s="93"/>
+      <c r="EG253" s="93"/>
+      <c r="EH253" s="93"/>
+      <c r="EI253" s="93"/>
+      <c r="EJ253" s="93"/>
+      <c r="EK253" s="93"/>
+      <c r="EL253" s="93"/>
+      <c r="EM253" s="93"/>
+      <c r="EN253" s="93"/>
+      <c r="EO253" s="93"/>
+      <c r="EP253" s="93"/>
+      <c r="EQ253" s="93"/>
+      <c r="ER253" s="93"/>
+      <c r="ES253" s="93"/>
+      <c r="ET253" s="93"/>
+      <c r="EU253" s="93"/>
+      <c r="EV253" s="93"/>
+      <c r="EW253" s="93"/>
+      <c r="EX253" s="93"/>
+      <c r="EY253" s="93"/>
+      <c r="EZ253" s="93"/>
+      <c r="FA253" s="93"/>
+      <c r="FB253" s="93"/>
+      <c r="FC253" s="93"/>
+      <c r="FD253" s="93"/>
+      <c r="FE253" s="93"/>
+      <c r="FF253" s="93"/>
+      <c r="FG253" s="93"/>
+      <c r="FH253" s="93"/>
+      <c r="FI253" s="93"/>
+      <c r="FJ253" s="93"/>
+      <c r="FK253" s="93"/>
+      <c r="FL253" s="93"/>
+      <c r="FM253" s="93"/>
+      <c r="FN253" s="93"/>
+      <c r="FO253" s="93"/>
+      <c r="FP253" s="93"/>
+      <c r="FQ253" s="93"/>
+      <c r="FR253" s="93"/>
+      <c r="FS253" s="93"/>
+      <c r="FT253" s="93"/>
+      <c r="FU253" s="93"/>
+      <c r="FV253" s="93"/>
+      <c r="FW253" s="93"/>
+      <c r="FX253" s="93"/>
+      <c r="FY253" s="93"/>
+      <c r="FZ253" s="93"/>
+      <c r="GA253" s="93"/>
+      <c r="GB253" s="93"/>
+      <c r="GC253" s="93"/>
+      <c r="GD253" s="93"/>
+      <c r="GE253" s="93"/>
+      <c r="GF253" s="93"/>
+      <c r="GG253" s="93"/>
+      <c r="GH253" s="93"/>
+      <c r="GI253" s="93"/>
+      <c r="GJ253" s="93"/>
+      <c r="GK253" s="93"/>
+      <c r="GL253" s="93"/>
+      <c r="GM253" s="93"/>
+      <c r="GN253" s="93"/>
+      <c r="GO253" s="93"/>
+      <c r="GP253" s="93"/>
+      <c r="GQ253" s="93"/>
+      <c r="GR253" s="93"/>
+      <c r="GS253" s="93"/>
+      <c r="GT253" s="93"/>
+      <c r="GU253" s="93"/>
+      <c r="GV253" s="93"/>
+      <c r="GW253" s="93"/>
+      <c r="GX253" s="93"/>
+      <c r="GY253" s="93"/>
+      <c r="GZ253" s="93"/>
+      <c r="HA253" s="93"/>
+      <c r="HB253" s="93"/>
+      <c r="HC253" s="93"/>
+      <c r="HD253" s="93"/>
+      <c r="HE253" s="93"/>
+      <c r="HF253" s="93"/>
+      <c r="HG253" s="93"/>
+      <c r="HH253" s="93"/>
+      <c r="HI253" s="93"/>
+      <c r="HJ253" s="93"/>
+      <c r="HK253" s="93"/>
+      <c r="HL253" s="93"/>
+      <c r="HM253" s="93"/>
+      <c r="HN253" s="93"/>
+      <c r="HO253" s="93"/>
+      <c r="HP253" s="93"/>
+      <c r="HQ253" s="93"/>
+      <c r="HR253" s="93"/>
+      <c r="HS253" s="93"/>
+      <c r="HT253" s="93"/>
+      <c r="HU253" s="93"/>
+      <c r="HV253" s="93"/>
+      <c r="HW253" s="93"/>
+      <c r="HX253" s="93"/>
+      <c r="HY253" s="93"/>
+      <c r="HZ253" s="93"/>
+      <c r="IA253" s="93"/>
+      <c r="IB253" s="93"/>
+      <c r="IC253" s="93"/>
+      <c r="ID253" s="93"/>
+      <c r="IE253" s="93"/>
+      <c r="IF253" s="93"/>
+      <c r="IG253" s="93"/>
+      <c r="IH253" s="93"/>
+      <c r="II253" s="93"/>
+      <c r="IJ253" s="93"/>
+      <c r="IK253" s="93"/>
+      <c r="IL253" s="93"/>
+      <c r="IM253" s="93"/>
+      <c r="IN253" s="93"/>
+      <c r="IO253" s="93"/>
+      <c r="IP253" s="93"/>
+      <c r="IQ253" s="93"/>
+      <c r="IR253" s="93"/>
+      <c r="IS253" s="93"/>
+      <c r="IT253" s="93"/>
+      <c r="IU253" s="93"/>
+      <c r="IV253" s="93"/>
+      <c r="IW253" s="93"/>
+      <c r="IX253" s="93"/>
+      <c r="IY253" s="93"/>
+      <c r="IZ253" s="93"/>
+      <c r="JA253" s="93"/>
+      <c r="JB253" s="93"/>
+      <c r="JC253" s="93"/>
+      <c r="JD253" s="93"/>
+      <c r="JE253" s="93"/>
+      <c r="JF253" s="93"/>
+      <c r="JG253" s="93"/>
+      <c r="JH253" s="93"/>
+      <c r="JI253" s="93"/>
+      <c r="JJ253" s="93"/>
+      <c r="JK253" s="93"/>
+      <c r="JL253" s="93"/>
+      <c r="JM253" s="93"/>
+      <c r="JN253" s="93"/>
+      <c r="JO253" s="93"/>
+      <c r="JP253" s="93"/>
+      <c r="JQ253" s="93"/>
+      <c r="JR253" s="93"/>
+      <c r="JS253" s="93"/>
+      <c r="JT253" s="93"/>
+      <c r="JU253" s="93"/>
+      <c r="JV253" s="93"/>
+      <c r="JW253" s="93"/>
+      <c r="JX253" s="93"/>
+      <c r="JY253" s="93"/>
+      <c r="JZ253" s="93"/>
+      <c r="KA253" s="93"/>
+      <c r="KB253" s="93"/>
+      <c r="KC253" s="93"/>
+      <c r="KD253" s="93"/>
+      <c r="KE253" s="93"/>
+      <c r="KF253" s="93"/>
+      <c r="KG253" s="93"/>
+      <c r="KH253" s="93"/>
+      <c r="KI253" s="93"/>
+      <c r="KJ253" s="93"/>
+      <c r="KK253" s="93"/>
+      <c r="KL253" s="93"/>
+      <c r="KM253" s="93"/>
+      <c r="KN253" s="93"/>
+      <c r="KO253" s="93"/>
+      <c r="KP253" s="93"/>
+    </row>
+    <row r="254" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A254" s="41"/>
+      <c r="B254" s="33">
+        <v>0</v>
+      </c>
+      <c r="C254" s="85">
+        <v>1</v>
+      </c>
+      <c r="D254" s="33">
+        <v>1</v>
+      </c>
+      <c r="E254" s="33">
+        <v>4</v>
+      </c>
+      <c r="F254" s="32"/>
+      <c r="I254" s="34"/>
+      <c r="J254" s="32"/>
+      <c r="M254" s="34"/>
+      <c r="Q254" s="32"/>
+      <c r="R254" s="34"/>
+      <c r="S254" s="67"/>
+      <c r="T254" s="67"/>
+      <c r="U254" s="67"/>
+      <c r="V254" s="67"/>
+      <c r="W254" s="67"/>
+      <c r="X254" s="67"/>
+      <c r="Y254" s="67"/>
+      <c r="Z254" s="67"/>
+      <c r="AA254" s="67"/>
+      <c r="AB254" s="67"/>
+      <c r="AC254" s="67"/>
+      <c r="AD254" s="67"/>
+      <c r="AE254" s="67"/>
+      <c r="AF254" s="67"/>
+      <c r="AG254" s="68"/>
+      <c r="AH254" s="90">
+        <v>0</v>
+      </c>
+      <c r="AI254" s="90">
+        <v>1</v>
+      </c>
+      <c r="AJ254" s="96">
+        <v>0</v>
+      </c>
+      <c r="AK254" s="90">
+        <v>4</v>
+      </c>
+      <c r="AR254" s="83"/>
+      <c r="AT254" s="84"/>
+      <c r="AU254" s="84"/>
+      <c r="AV254" s="84"/>
+      <c r="AW254" s="84"/>
+      <c r="AX254" s="84"/>
+      <c r="AY254" s="84"/>
+      <c r="AZ254" s="84"/>
+      <c r="BA254" s="84"/>
+      <c r="BB254" s="84"/>
+      <c r="BC254" s="84"/>
+      <c r="BD254" s="84"/>
+      <c r="BE254" s="84"/>
+      <c r="BF254" s="84"/>
+      <c r="BG254" s="84"/>
+      <c r="BH254" s="84"/>
+      <c r="BI254" s="84"/>
+      <c r="BJ254" s="84"/>
+      <c r="BK254" s="84"/>
+      <c r="BL254" s="84"/>
+      <c r="BM254" s="84"/>
+      <c r="BN254" s="84"/>
+      <c r="BO254" s="84"/>
+      <c r="BP254" s="84"/>
+      <c r="BQ254" s="84"/>
+      <c r="BR254" s="84"/>
+      <c r="BS254" s="84"/>
+      <c r="BT254" s="84"/>
+      <c r="BU254" s="84"/>
+      <c r="BV254" s="84"/>
+      <c r="BW254" s="84"/>
+      <c r="BX254" s="84"/>
+      <c r="BY254" s="84"/>
+      <c r="BZ254" s="84"/>
+      <c r="CA254" s="84"/>
+      <c r="CB254" s="84"/>
+      <c r="CC254" s="84"/>
+      <c r="CD254" s="84"/>
+      <c r="CE254" s="84"/>
+      <c r="CF254" s="84"/>
+      <c r="CG254" s="84"/>
+      <c r="CH254" s="84"/>
+      <c r="CI254" s="84"/>
+      <c r="CJ254" s="84"/>
+      <c r="CK254" s="84"/>
+      <c r="CL254" s="84"/>
+      <c r="CM254" s="84"/>
+      <c r="CN254" s="84"/>
+      <c r="CO254" s="84"/>
+      <c r="CP254" s="84"/>
+      <c r="CQ254" s="84"/>
+      <c r="CR254" s="84"/>
+      <c r="CS254" s="84"/>
+      <c r="CT254" s="84"/>
+      <c r="CU254" s="84"/>
+      <c r="CV254" s="84"/>
+      <c r="CW254" s="84"/>
+      <c r="CX254" s="84"/>
+      <c r="CY254" s="84"/>
+      <c r="CZ254" s="84"/>
+      <c r="DA254" s="84"/>
+      <c r="DB254" s="84"/>
+      <c r="DC254" s="84"/>
+      <c r="DD254" s="84"/>
+      <c r="DE254" s="84"/>
+      <c r="DF254" s="84"/>
+      <c r="DG254" s="84"/>
+      <c r="DH254" s="84"/>
+      <c r="DI254" s="84"/>
+      <c r="DJ254" s="84"/>
+      <c r="DK254" s="84"/>
+      <c r="DL254" s="84"/>
+      <c r="DM254" s="84"/>
+      <c r="DN254" s="84"/>
+      <c r="DO254" s="84"/>
+      <c r="DP254" s="84"/>
+      <c r="DQ254" s="84"/>
+      <c r="DR254" s="84"/>
+      <c r="DS254" s="84"/>
+      <c r="DT254" s="84"/>
+      <c r="DU254" s="84"/>
+      <c r="DV254" s="84"/>
+      <c r="DW254" s="84"/>
+      <c r="DX254" s="84"/>
+      <c r="DY254" s="84"/>
+      <c r="DZ254" s="84"/>
+      <c r="EA254" s="84"/>
+      <c r="EB254" s="84"/>
+      <c r="EC254" s="84"/>
+      <c r="ED254" s="84"/>
+      <c r="EE254" s="84"/>
+      <c r="EF254" s="84"/>
+      <c r="EG254" s="84"/>
+      <c r="EH254" s="84"/>
+      <c r="EI254" s="84"/>
+      <c r="EJ254" s="84"/>
+      <c r="EK254" s="84"/>
+      <c r="EL254" s="84"/>
+      <c r="EM254" s="84"/>
+      <c r="EN254" s="84"/>
+      <c r="EO254" s="84"/>
+      <c r="EP254" s="84"/>
+      <c r="EQ254" s="84"/>
+      <c r="ER254" s="84"/>
+      <c r="ES254" s="84"/>
+      <c r="ET254" s="84"/>
+      <c r="EU254" s="84"/>
+      <c r="EV254" s="84"/>
+      <c r="EW254" s="84"/>
+      <c r="EX254" s="84"/>
+      <c r="EY254" s="84"/>
+      <c r="EZ254" s="84"/>
+      <c r="FA254" s="84"/>
+      <c r="FB254" s="84"/>
+      <c r="FC254" s="84"/>
+      <c r="FD254" s="84"/>
+      <c r="FE254" s="84"/>
+      <c r="FF254" s="84"/>
+      <c r="FG254" s="84"/>
+      <c r="FH254" s="84"/>
+      <c r="FI254" s="84"/>
+      <c r="FJ254" s="84"/>
+      <c r="FK254" s="84"/>
+      <c r="FL254" s="84"/>
+      <c r="FM254" s="84"/>
+      <c r="FN254" s="84"/>
+      <c r="FO254" s="84"/>
+      <c r="FP254" s="84"/>
+      <c r="FQ254" s="84"/>
+      <c r="FR254" s="84"/>
+      <c r="FS254" s="84"/>
+      <c r="FT254" s="84"/>
+      <c r="FU254" s="84"/>
+      <c r="FV254" s="84"/>
+      <c r="FW254" s="84"/>
+      <c r="FX254" s="84"/>
+      <c r="FY254" s="84"/>
+      <c r="FZ254" s="84"/>
+      <c r="GA254" s="84"/>
+      <c r="GB254" s="84"/>
+      <c r="GC254" s="84"/>
+      <c r="GD254" s="84"/>
+      <c r="GE254" s="84"/>
+      <c r="GF254" s="84"/>
+      <c r="GG254" s="84"/>
+      <c r="GH254" s="84"/>
+      <c r="GI254" s="84"/>
+      <c r="GJ254" s="84"/>
+      <c r="GK254" s="84"/>
+      <c r="GL254" s="84"/>
+      <c r="GM254" s="84"/>
+      <c r="GN254" s="84"/>
+      <c r="GO254" s="84"/>
+      <c r="GP254" s="84"/>
+      <c r="GQ254" s="84"/>
+      <c r="GR254" s="84"/>
+      <c r="GS254" s="84"/>
+      <c r="GT254" s="84"/>
+      <c r="GU254" s="84"/>
+      <c r="GV254" s="84"/>
+      <c r="GW254" s="84"/>
+      <c r="GX254" s="84"/>
+      <c r="GY254" s="84"/>
+      <c r="GZ254" s="84"/>
+      <c r="HA254" s="84"/>
+      <c r="HB254" s="84"/>
+      <c r="HC254" s="84"/>
+      <c r="HD254" s="84"/>
+      <c r="HE254" s="84"/>
+      <c r="HF254" s="84"/>
+      <c r="HG254" s="84"/>
+      <c r="HH254" s="84"/>
+      <c r="HI254" s="84"/>
+      <c r="HJ254" s="84"/>
+      <c r="HK254" s="84"/>
+      <c r="HL254" s="84"/>
+      <c r="HM254" s="84"/>
+      <c r="HN254" s="84"/>
+      <c r="HO254" s="84"/>
+      <c r="HP254" s="84"/>
+      <c r="HQ254" s="84"/>
+      <c r="HR254" s="84"/>
+      <c r="HS254" s="84"/>
+      <c r="HT254" s="84"/>
+      <c r="HU254" s="84"/>
+      <c r="HV254" s="84"/>
+      <c r="HW254" s="84"/>
+      <c r="HX254" s="84"/>
+      <c r="HY254" s="84"/>
+      <c r="HZ254" s="84"/>
+      <c r="IA254" s="84"/>
+      <c r="IB254" s="84"/>
+      <c r="IC254" s="84"/>
+      <c r="ID254" s="84"/>
+      <c r="IE254" s="84"/>
+      <c r="IF254" s="84"/>
+      <c r="IG254" s="84"/>
+      <c r="IH254" s="84"/>
+      <c r="II254" s="84"/>
+      <c r="IJ254" s="84"/>
+      <c r="IK254" s="84"/>
+      <c r="IL254" s="84"/>
+      <c r="IM254" s="84"/>
+      <c r="IN254" s="84"/>
+      <c r="IO254" s="84"/>
+      <c r="IP254" s="84"/>
+      <c r="IQ254" s="84"/>
+      <c r="IR254" s="84"/>
+      <c r="IS254" s="84"/>
+      <c r="IT254" s="84"/>
+      <c r="IU254" s="84"/>
+      <c r="IV254" s="84"/>
+      <c r="IW254" s="84"/>
+      <c r="IX254" s="84"/>
+      <c r="IY254" s="84"/>
+      <c r="IZ254" s="84"/>
+      <c r="JA254" s="84"/>
+      <c r="JB254" s="84"/>
+      <c r="JC254" s="84"/>
+      <c r="JD254" s="84"/>
+      <c r="JE254" s="84"/>
+      <c r="JF254" s="84"/>
+      <c r="JG254" s="84"/>
+      <c r="JH254" s="84"/>
+      <c r="JI254" s="84"/>
+      <c r="JJ254" s="84"/>
+      <c r="JK254" s="84"/>
+      <c r="JL254" s="84"/>
+      <c r="JM254" s="84"/>
+      <c r="JN254" s="84"/>
+      <c r="JO254" s="84"/>
+      <c r="JP254" s="84"/>
+      <c r="JQ254" s="84"/>
+      <c r="JR254" s="84"/>
+      <c r="JS254" s="84"/>
+      <c r="JT254" s="84"/>
+      <c r="JU254" s="84"/>
+      <c r="JV254" s="84"/>
+      <c r="JW254" s="84"/>
+      <c r="JX254" s="84"/>
+      <c r="JY254" s="84"/>
+      <c r="JZ254" s="84"/>
+      <c r="KA254" s="84"/>
+      <c r="KB254" s="84"/>
+      <c r="KC254" s="84"/>
+      <c r="KD254" s="84"/>
+      <c r="KE254" s="84"/>
+      <c r="KF254" s="84"/>
+      <c r="KG254" s="84"/>
+      <c r="KH254" s="84"/>
+      <c r="KI254" s="84"/>
+      <c r="KJ254" s="84"/>
+      <c r="KK254" s="84"/>
+      <c r="KL254" s="84"/>
+      <c r="KM254" s="84"/>
+      <c r="KN254" s="84"/>
+      <c r="KO254" s="84"/>
+      <c r="KP254" s="84"/>
+    </row>
+    <row r="255" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="A255" s="40">
+        <v>116</v>
+      </c>
+      <c r="B255" s="86">
+        <v>2</v>
+      </c>
+      <c r="C255">
+        <v>4</v>
+      </c>
+      <c r="D255">
+        <v>3</v>
+      </c>
+      <c r="E255">
+        <v>2</v>
+      </c>
+      <c r="N255">
+        <v>0</v>
+      </c>
+      <c r="O255">
+        <v>0</v>
+      </c>
+      <c r="P255" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q255" s="23">
+        <v>7</v>
+      </c>
+      <c r="R255" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="S255" s="60" t="b">
+        <v>1</v>
+      </c>
+      <c r="U255" s="60">
+        <v>-1</v>
+      </c>
+      <c r="V255" s="60">
+        <v>3</v>
+      </c>
+      <c r="W255" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="AH255">
+        <v>0</v>
+      </c>
+      <c r="AI255">
+        <v>4</v>
+      </c>
+      <c r="AJ255">
+        <v>3</v>
+      </c>
+      <c r="AK255">
+        <v>2</v>
+      </c>
+      <c r="AP255">
+        <v>10</v>
+      </c>
+      <c r="AQ255">
+        <v>0</v>
+      </c>
+      <c r="AR255" s="80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS255" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="256" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B256">
+        <v>2</v>
+      </c>
+      <c r="C256">
+        <v>6</v>
+      </c>
+      <c r="D256">
+        <v>5</v>
+      </c>
+      <c r="E256">
+        <v>0</v>
+      </c>
+      <c r="AH256">
+        <v>0</v>
+      </c>
+      <c r="AI256">
+        <v>0</v>
+      </c>
+      <c r="AJ256">
+        <v>5</v>
+      </c>
+      <c r="AK256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="46">
+        <v>117</v>
+      </c>
+      <c r="B257" s="29">
+        <v>2</v>
+      </c>
+      <c r="C257" s="29">
+        <v>3</v>
+      </c>
+      <c r="D257" s="29">
+        <v>3</v>
+      </c>
+      <c r="E257" s="29">
+        <v>2</v>
+      </c>
+      <c r="F257" s="28"/>
+      <c r="I257" s="30"/>
+      <c r="J257" s="28"/>
+      <c r="M257" s="30"/>
+      <c r="N257" s="29">
+        <v>0</v>
+      </c>
+      <c r="O257" s="29">
+        <v>0</v>
+      </c>
+      <c r="P257" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q257" s="28">
+        <v>2</v>
+      </c>
+      <c r="R257" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S257" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="T257" s="65"/>
+      <c r="U257" s="65">
+        <v>-1</v>
+      </c>
+      <c r="V257" s="65">
+        <v>4</v>
+      </c>
+      <c r="W257" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="X257" s="65"/>
+      <c r="Y257" s="65"/>
+      <c r="Z257" s="65"/>
+      <c r="AA257" s="65"/>
+      <c r="AB257" s="65"/>
+      <c r="AC257" s="65"/>
+      <c r="AD257" s="65"/>
+      <c r="AE257" s="65"/>
+      <c r="AF257" s="65"/>
+      <c r="AG257" s="91"/>
+      <c r="AH257" s="29">
+        <v>2</v>
+      </c>
+      <c r="AI257" s="29">
+        <v>3</v>
+      </c>
+      <c r="AJ257" s="29">
+        <v>3</v>
+      </c>
+      <c r="AK257" s="29">
+        <v>0</v>
+      </c>
+      <c r="AP257" s="29">
+        <v>10</v>
+      </c>
+      <c r="AQ257" s="29">
+        <v>0</v>
+      </c>
+      <c r="AR257" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS257" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="AT257" s="93"/>
+      <c r="AU257" s="93"/>
+      <c r="AV257" s="93"/>
+      <c r="AW257" s="93"/>
+      <c r="AX257" s="93"/>
+      <c r="AY257" s="93"/>
+      <c r="AZ257" s="93"/>
+      <c r="BA257" s="93"/>
+      <c r="BB257" s="93"/>
+      <c r="BC257" s="93"/>
+      <c r="BD257" s="93"/>
+      <c r="BE257" s="93"/>
+      <c r="BF257" s="93"/>
+      <c r="BG257" s="93"/>
+      <c r="BH257" s="93"/>
+      <c r="BI257" s="93"/>
+      <c r="BJ257" s="93"/>
+      <c r="BK257" s="93"/>
+      <c r="BL257" s="93"/>
+      <c r="BM257" s="93"/>
+      <c r="BN257" s="93"/>
+      <c r="BO257" s="93"/>
+      <c r="BP257" s="93"/>
+      <c r="BQ257" s="93"/>
+      <c r="BR257" s="93"/>
+      <c r="BS257" s="93"/>
+      <c r="BT257" s="93"/>
+      <c r="BU257" s="93"/>
+      <c r="BV257" s="93"/>
+      <c r="BW257" s="93"/>
+      <c r="BX257" s="93"/>
+      <c r="BY257" s="93"/>
+      <c r="BZ257" s="93"/>
+      <c r="CA257" s="93"/>
+      <c r="CB257" s="93"/>
+      <c r="CC257" s="93"/>
+      <c r="CD257" s="93"/>
+      <c r="CE257" s="93"/>
+      <c r="CF257" s="93"/>
+      <c r="CG257" s="93"/>
+      <c r="CH257" s="93"/>
+      <c r="CI257" s="93"/>
+      <c r="CJ257" s="93"/>
+      <c r="CK257" s="93"/>
+      <c r="CL257" s="93"/>
+      <c r="CM257" s="93"/>
+      <c r="CN257" s="93"/>
+      <c r="CO257" s="93"/>
+      <c r="CP257" s="93"/>
+      <c r="CQ257" s="93"/>
+      <c r="CR257" s="93"/>
+      <c r="CS257" s="93"/>
+      <c r="CT257" s="93"/>
+      <c r="CU257" s="93"/>
+      <c r="CV257" s="93"/>
+      <c r="CW257" s="93"/>
+      <c r="CX257" s="93"/>
+      <c r="CY257" s="93"/>
+      <c r="CZ257" s="93"/>
+      <c r="DA257" s="93"/>
+      <c r="DB257" s="93"/>
+      <c r="DC257" s="93"/>
+      <c r="DD257" s="93"/>
+      <c r="DE257" s="93"/>
+      <c r="DF257" s="93"/>
+      <c r="DG257" s="93"/>
+      <c r="DH257" s="93"/>
+      <c r="DI257" s="93"/>
+      <c r="DJ257" s="93"/>
+      <c r="DK257" s="93"/>
+      <c r="DL257" s="93"/>
+      <c r="DM257" s="93"/>
+      <c r="DN257" s="93"/>
+      <c r="DO257" s="93"/>
+      <c r="DP257" s="93"/>
+      <c r="DQ257" s="93"/>
+      <c r="DR257" s="93"/>
+      <c r="DS257" s="93"/>
+      <c r="DT257" s="93"/>
+      <c r="DU257" s="93"/>
+      <c r="DV257" s="93"/>
+      <c r="DW257" s="93"/>
+      <c r="DX257" s="93"/>
+      <c r="DY257" s="93"/>
+      <c r="DZ257" s="93"/>
+      <c r="EA257" s="93"/>
+      <c r="EB257" s="93"/>
+      <c r="EC257" s="93"/>
+      <c r="ED257" s="93"/>
+      <c r="EE257" s="93"/>
+      <c r="EF257" s="93"/>
+      <c r="EG257" s="93"/>
+      <c r="EH257" s="93"/>
+      <c r="EI257" s="93"/>
+      <c r="EJ257" s="93"/>
+      <c r="EK257" s="93"/>
+      <c r="EL257" s="93"/>
+      <c r="EM257" s="93"/>
+      <c r="EN257" s="93"/>
+      <c r="EO257" s="93"/>
+      <c r="EP257" s="93"/>
+      <c r="EQ257" s="93"/>
+      <c r="ER257" s="93"/>
+      <c r="ES257" s="93"/>
+      <c r="ET257" s="93"/>
+      <c r="EU257" s="93"/>
+      <c r="EV257" s="93"/>
+      <c r="EW257" s="93"/>
+      <c r="EX257" s="93"/>
+      <c r="EY257" s="93"/>
+      <c r="EZ257" s="93"/>
+      <c r="FA257" s="93"/>
+      <c r="FB257" s="93"/>
+      <c r="FC257" s="93"/>
+      <c r="FD257" s="93"/>
+      <c r="FE257" s="93"/>
+      <c r="FF257" s="93"/>
+      <c r="FG257" s="93"/>
+      <c r="FH257" s="93"/>
+      <c r="FI257" s="93"/>
+      <c r="FJ257" s="93"/>
+      <c r="FK257" s="93"/>
+      <c r="FL257" s="93"/>
+      <c r="FM257" s="93"/>
+      <c r="FN257" s="93"/>
+      <c r="FO257" s="93"/>
+      <c r="FP257" s="93"/>
+      <c r="FQ257" s="93"/>
+      <c r="FR257" s="93"/>
+      <c r="FS257" s="93"/>
+      <c r="FT257" s="93"/>
+      <c r="FU257" s="93"/>
+      <c r="FV257" s="93"/>
+      <c r="FW257" s="93"/>
+      <c r="FX257" s="93"/>
+      <c r="FY257" s="93"/>
+      <c r="FZ257" s="93"/>
+      <c r="GA257" s="93"/>
+      <c r="GB257" s="93"/>
+      <c r="GC257" s="93"/>
+      <c r="GD257" s="93"/>
+      <c r="GE257" s="93"/>
+      <c r="GF257" s="93"/>
+      <c r="GG257" s="93"/>
+      <c r="GH257" s="93"/>
+      <c r="GI257" s="93"/>
+      <c r="GJ257" s="93"/>
+      <c r="GK257" s="93"/>
+      <c r="GL257" s="93"/>
+      <c r="GM257" s="93"/>
+      <c r="GN257" s="93"/>
+      <c r="GO257" s="93"/>
+      <c r="GP257" s="93"/>
+      <c r="GQ257" s="93"/>
+      <c r="GR257" s="93"/>
+      <c r="GS257" s="93"/>
+      <c r="GT257" s="93"/>
+      <c r="GU257" s="93"/>
+      <c r="GV257" s="93"/>
+      <c r="GW257" s="93"/>
+      <c r="GX257" s="93"/>
+      <c r="GY257" s="93"/>
+      <c r="GZ257" s="93"/>
+      <c r="HA257" s="93"/>
+      <c r="HB257" s="93"/>
+      <c r="HC257" s="93"/>
+      <c r="HD257" s="93"/>
+      <c r="HE257" s="93"/>
+      <c r="HF257" s="93"/>
+      <c r="HG257" s="93"/>
+      <c r="HH257" s="93"/>
+      <c r="HI257" s="93"/>
+      <c r="HJ257" s="93"/>
+      <c r="HK257" s="93"/>
+      <c r="HL257" s="93"/>
+      <c r="HM257" s="93"/>
+      <c r="HN257" s="93"/>
+      <c r="HO257" s="93"/>
+      <c r="HP257" s="93"/>
+      <c r="HQ257" s="93"/>
+      <c r="HR257" s="93"/>
+      <c r="HS257" s="93"/>
+      <c r="HT257" s="93"/>
+      <c r="HU257" s="93"/>
+      <c r="HV257" s="93"/>
+      <c r="HW257" s="93"/>
+      <c r="HX257" s="93"/>
+      <c r="HY257" s="93"/>
+      <c r="HZ257" s="93"/>
+      <c r="IA257" s="93"/>
+      <c r="IB257" s="93"/>
+      <c r="IC257" s="93"/>
+      <c r="ID257" s="93"/>
+      <c r="IE257" s="93"/>
+      <c r="IF257" s="93"/>
+      <c r="IG257" s="93"/>
+      <c r="IH257" s="93"/>
+      <c r="II257" s="93"/>
+      <c r="IJ257" s="93"/>
+      <c r="IK257" s="93"/>
+      <c r="IL257" s="93"/>
+      <c r="IM257" s="93"/>
+      <c r="IN257" s="93"/>
+      <c r="IO257" s="93"/>
+      <c r="IP257" s="93"/>
+      <c r="IQ257" s="93"/>
+      <c r="IR257" s="93"/>
+      <c r="IS257" s="93"/>
+      <c r="IT257" s="93"/>
+      <c r="IU257" s="93"/>
+      <c r="IV257" s="93"/>
+      <c r="IW257" s="93"/>
+      <c r="IX257" s="93"/>
+      <c r="IY257" s="93"/>
+      <c r="IZ257" s="93"/>
+      <c r="JA257" s="93"/>
+      <c r="JB257" s="93"/>
+      <c r="JC257" s="93"/>
+      <c r="JD257" s="93"/>
+      <c r="JE257" s="93"/>
+      <c r="JF257" s="93"/>
+      <c r="JG257" s="93"/>
+      <c r="JH257" s="93"/>
+      <c r="JI257" s="93"/>
+      <c r="JJ257" s="93"/>
+      <c r="JK257" s="93"/>
+      <c r="JL257" s="93"/>
+      <c r="JM257" s="93"/>
+      <c r="JN257" s="93"/>
+      <c r="JO257" s="93"/>
+      <c r="JP257" s="93"/>
+      <c r="JQ257" s="93"/>
+      <c r="JR257" s="93"/>
+      <c r="JS257" s="93"/>
+      <c r="JT257" s="93"/>
+      <c r="JU257" s="93"/>
+      <c r="JV257" s="93"/>
+      <c r="JW257" s="93"/>
+      <c r="JX257" s="93"/>
+      <c r="JY257" s="93"/>
+      <c r="JZ257" s="93"/>
+      <c r="KA257" s="93"/>
+      <c r="KB257" s="93"/>
+      <c r="KC257" s="93"/>
+      <c r="KD257" s="93"/>
+      <c r="KE257" s="93"/>
+      <c r="KF257" s="93"/>
+      <c r="KG257" s="93"/>
+      <c r="KH257" s="93"/>
+      <c r="KI257" s="93"/>
+      <c r="KJ257" s="93"/>
+      <c r="KK257" s="93"/>
+      <c r="KL257" s="93"/>
+      <c r="KM257" s="93"/>
+      <c r="KN257" s="93"/>
+      <c r="KO257" s="93"/>
+      <c r="KP257" s="93"/>
+    </row>
+    <row r="258" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="41"/>
+      <c r="B258" s="33">
+        <v>2</v>
+      </c>
+      <c r="C258" s="33">
+        <v>4</v>
+      </c>
+      <c r="D258" s="85">
+        <v>6</v>
+      </c>
+      <c r="E258" s="33">
+        <v>2</v>
+      </c>
+      <c r="F258" s="32"/>
+      <c r="I258" s="34"/>
+      <c r="J258" s="32"/>
+      <c r="M258" s="34"/>
+      <c r="Q258" s="32"/>
+      <c r="R258" s="34"/>
+      <c r="S258" s="67"/>
+      <c r="T258" s="67"/>
+      <c r="U258" s="67"/>
+      <c r="V258" s="67"/>
+      <c r="W258" s="67"/>
+      <c r="X258" s="67"/>
+      <c r="Y258" s="67"/>
+      <c r="Z258" s="67"/>
+      <c r="AA258" s="67"/>
+      <c r="AB258" s="67"/>
+      <c r="AC258" s="67"/>
+      <c r="AD258" s="67"/>
+      <c r="AE258" s="67"/>
+      <c r="AF258" s="67"/>
+      <c r="AG258" s="68"/>
+      <c r="AH258" s="33">
+        <v>2</v>
+      </c>
+      <c r="AI258" s="33">
+        <v>4</v>
+      </c>
+      <c r="AJ258" s="33">
+        <v>0</v>
+      </c>
+      <c r="AK258" s="33">
+        <v>0</v>
+      </c>
+      <c r="AR258" s="83"/>
+      <c r="AT258" s="84"/>
+      <c r="AU258" s="84"/>
+      <c r="AV258" s="84"/>
+      <c r="AW258" s="84"/>
+      <c r="AX258" s="84"/>
+      <c r="AY258" s="84"/>
+      <c r="AZ258" s="84"/>
+      <c r="BA258" s="84"/>
+      <c r="BB258" s="84"/>
+      <c r="BC258" s="84"/>
+      <c r="BD258" s="84"/>
+      <c r="BE258" s="84"/>
+      <c r="BF258" s="84"/>
+      <c r="BG258" s="84"/>
+      <c r="BH258" s="84"/>
+      <c r="BI258" s="84"/>
+      <c r="BJ258" s="84"/>
+      <c r="BK258" s="84"/>
+      <c r="BL258" s="84"/>
+      <c r="BM258" s="84"/>
+      <c r="BN258" s="84"/>
+      <c r="BO258" s="84"/>
+      <c r="BP258" s="84"/>
+      <c r="BQ258" s="84"/>
+      <c r="BR258" s="84"/>
+      <c r="BS258" s="84"/>
+      <c r="BT258" s="84"/>
+      <c r="BU258" s="84"/>
+      <c r="BV258" s="84"/>
+      <c r="BW258" s="84"/>
+      <c r="BX258" s="84"/>
+      <c r="BY258" s="84"/>
+      <c r="BZ258" s="84"/>
+      <c r="CA258" s="84"/>
+      <c r="CB258" s="84"/>
+      <c r="CC258" s="84"/>
+      <c r="CD258" s="84"/>
+      <c r="CE258" s="84"/>
+      <c r="CF258" s="84"/>
+      <c r="CG258" s="84"/>
+      <c r="CH258" s="84"/>
+      <c r="CI258" s="84"/>
+      <c r="CJ258" s="84"/>
+      <c r="CK258" s="84"/>
+      <c r="CL258" s="84"/>
+      <c r="CM258" s="84"/>
+      <c r="CN258" s="84"/>
+      <c r="CO258" s="84"/>
+      <c r="CP258" s="84"/>
+      <c r="CQ258" s="84"/>
+      <c r="CR258" s="84"/>
+      <c r="CS258" s="84"/>
+      <c r="CT258" s="84"/>
+      <c r="CU258" s="84"/>
+      <c r="CV258" s="84"/>
+      <c r="CW258" s="84"/>
+      <c r="CX258" s="84"/>
+      <c r="CY258" s="84"/>
+      <c r="CZ258" s="84"/>
+      <c r="DA258" s="84"/>
+      <c r="DB258" s="84"/>
+      <c r="DC258" s="84"/>
+      <c r="DD258" s="84"/>
+      <c r="DE258" s="84"/>
+      <c r="DF258" s="84"/>
+      <c r="DG258" s="84"/>
+      <c r="DH258" s="84"/>
+      <c r="DI258" s="84"/>
+      <c r="DJ258" s="84"/>
+      <c r="DK258" s="84"/>
+      <c r="DL258" s="84"/>
+      <c r="DM258" s="84"/>
+      <c r="DN258" s="84"/>
+      <c r="DO258" s="84"/>
+      <c r="DP258" s="84"/>
+      <c r="DQ258" s="84"/>
+      <c r="DR258" s="84"/>
+      <c r="DS258" s="84"/>
+      <c r="DT258" s="84"/>
+      <c r="DU258" s="84"/>
+      <c r="DV258" s="84"/>
+      <c r="DW258" s="84"/>
+      <c r="DX258" s="84"/>
+      <c r="DY258" s="84"/>
+      <c r="DZ258" s="84"/>
+      <c r="EA258" s="84"/>
+      <c r="EB258" s="84"/>
+      <c r="EC258" s="84"/>
+      <c r="ED258" s="84"/>
+      <c r="EE258" s="84"/>
+      <c r="EF258" s="84"/>
+      <c r="EG258" s="84"/>
+      <c r="EH258" s="84"/>
+      <c r="EI258" s="84"/>
+      <c r="EJ258" s="84"/>
+      <c r="EK258" s="84"/>
+      <c r="EL258" s="84"/>
+      <c r="EM258" s="84"/>
+      <c r="EN258" s="84"/>
+      <c r="EO258" s="84"/>
+      <c r="EP258" s="84"/>
+      <c r="EQ258" s="84"/>
+      <c r="ER258" s="84"/>
+      <c r="ES258" s="84"/>
+      <c r="ET258" s="84"/>
+      <c r="EU258" s="84"/>
+      <c r="EV258" s="84"/>
+      <c r="EW258" s="84"/>
+      <c r="EX258" s="84"/>
+      <c r="EY258" s="84"/>
+      <c r="EZ258" s="84"/>
+      <c r="FA258" s="84"/>
+      <c r="FB258" s="84"/>
+      <c r="FC258" s="84"/>
+      <c r="FD258" s="84"/>
+      <c r="FE258" s="84"/>
+      <c r="FF258" s="84"/>
+      <c r="FG258" s="84"/>
+      <c r="FH258" s="84"/>
+      <c r="FI258" s="84"/>
+      <c r="FJ258" s="84"/>
+      <c r="FK258" s="84"/>
+      <c r="FL258" s="84"/>
+      <c r="FM258" s="84"/>
+      <c r="FN258" s="84"/>
+      <c r="FO258" s="84"/>
+      <c r="FP258" s="84"/>
+      <c r="FQ258" s="84"/>
+      <c r="FR258" s="84"/>
+      <c r="FS258" s="84"/>
+      <c r="FT258" s="84"/>
+      <c r="FU258" s="84"/>
+      <c r="FV258" s="84"/>
+      <c r="FW258" s="84"/>
+      <c r="FX258" s="84"/>
+      <c r="FY258" s="84"/>
+      <c r="FZ258" s="84"/>
+      <c r="GA258" s="84"/>
+      <c r="GB258" s="84"/>
+      <c r="GC258" s="84"/>
+      <c r="GD258" s="84"/>
+      <c r="GE258" s="84"/>
+      <c r="GF258" s="84"/>
+      <c r="GG258" s="84"/>
+      <c r="GH258" s="84"/>
+      <c r="GI258" s="84"/>
+      <c r="GJ258" s="84"/>
+      <c r="GK258" s="84"/>
+      <c r="GL258" s="84"/>
+      <c r="GM258" s="84"/>
+      <c r="GN258" s="84"/>
+      <c r="GO258" s="84"/>
+      <c r="GP258" s="84"/>
+      <c r="GQ258" s="84"/>
+      <c r="GR258" s="84"/>
+      <c r="GS258" s="84"/>
+      <c r="GT258" s="84"/>
+      <c r="GU258" s="84"/>
+      <c r="GV258" s="84"/>
+      <c r="GW258" s="84"/>
+      <c r="GX258" s="84"/>
+      <c r="GY258" s="84"/>
+      <c r="GZ258" s="84"/>
+      <c r="HA258" s="84"/>
+      <c r="HB258" s="84"/>
+      <c r="HC258" s="84"/>
+      <c r="HD258" s="84"/>
+      <c r="HE258" s="84"/>
+      <c r="HF258" s="84"/>
+      <c r="HG258" s="84"/>
+      <c r="HH258" s="84"/>
+      <c r="HI258" s="84"/>
+      <c r="HJ258" s="84"/>
+      <c r="HK258" s="84"/>
+      <c r="HL258" s="84"/>
+      <c r="HM258" s="84"/>
+      <c r="HN258" s="84"/>
+      <c r="HO258" s="84"/>
+      <c r="HP258" s="84"/>
+      <c r="HQ258" s="84"/>
+      <c r="HR258" s="84"/>
+      <c r="HS258" s="84"/>
+      <c r="HT258" s="84"/>
+      <c r="HU258" s="84"/>
+      <c r="HV258" s="84"/>
+      <c r="HW258" s="84"/>
+      <c r="HX258" s="84"/>
+      <c r="HY258" s="84"/>
+      <c r="HZ258" s="84"/>
+      <c r="IA258" s="84"/>
+      <c r="IB258" s="84"/>
+      <c r="IC258" s="84"/>
+      <c r="ID258" s="84"/>
+      <c r="IE258" s="84"/>
+      <c r="IF258" s="84"/>
+      <c r="IG258" s="84"/>
+      <c r="IH258" s="84"/>
+      <c r="II258" s="84"/>
+      <c r="IJ258" s="84"/>
+      <c r="IK258" s="84"/>
+      <c r="IL258" s="84"/>
+      <c r="IM258" s="84"/>
+      <c r="IN258" s="84"/>
+      <c r="IO258" s="84"/>
+      <c r="IP258" s="84"/>
+      <c r="IQ258" s="84"/>
+      <c r="IR258" s="84"/>
+      <c r="IS258" s="84"/>
+      <c r="IT258" s="84"/>
+      <c r="IU258" s="84"/>
+      <c r="IV258" s="84"/>
+      <c r="IW258" s="84"/>
+      <c r="IX258" s="84"/>
+      <c r="IY258" s="84"/>
+      <c r="IZ258" s="84"/>
+      <c r="JA258" s="84"/>
+      <c r="JB258" s="84"/>
+      <c r="JC258" s="84"/>
+      <c r="JD258" s="84"/>
+      <c r="JE258" s="84"/>
+      <c r="JF258" s="84"/>
+      <c r="JG258" s="84"/>
+      <c r="JH258" s="84"/>
+      <c r="JI258" s="84"/>
+      <c r="JJ258" s="84"/>
+      <c r="JK258" s="84"/>
+      <c r="JL258" s="84"/>
+      <c r="JM258" s="84"/>
+      <c r="JN258" s="84"/>
+      <c r="JO258" s="84"/>
+      <c r="JP258" s="84"/>
+      <c r="JQ258" s="84"/>
+      <c r="JR258" s="84"/>
+      <c r="JS258" s="84"/>
+      <c r="JT258" s="84"/>
+      <c r="JU258" s="84"/>
+      <c r="JV258" s="84"/>
+      <c r="JW258" s="84"/>
+      <c r="JX258" s="84"/>
+      <c r="JY258" s="84"/>
+      <c r="JZ258" s="84"/>
+      <c r="KA258" s="84"/>
+      <c r="KB258" s="84"/>
+      <c r="KC258" s="84"/>
+      <c r="KD258" s="84"/>
+      <c r="KE258" s="84"/>
+      <c r="KF258" s="84"/>
+      <c r="KG258" s="84"/>
+      <c r="KH258" s="84"/>
+      <c r="KI258" s="84"/>
+      <c r="KJ258" s="84"/>
+      <c r="KK258" s="84"/>
+      <c r="KL258" s="84"/>
+      <c r="KM258" s="84"/>
+      <c r="KN258" s="84"/>
+      <c r="KO258" s="84"/>
+      <c r="KP258" s="84"/>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added CaptOpposite1CCW for CaptType.CAPT_OPP_1CCW.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377A4C32-D003-44C7-9222-D8FF6DEEE178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B88E306-062C-4E31-944E-A7830CE9427D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="189">
   <si>
     <t>setup</t>
   </si>
@@ -585,6 +585,21 @@
   </si>
   <si>
     <t>OWN_CONT capture</t>
+  </si>
+  <si>
+    <t>OPP1CCW</t>
+  </si>
+  <si>
+    <t>2 4 6</t>
+  </si>
+  <si>
+    <t>capt initiated by most CCW hole</t>
+  </si>
+  <si>
+    <t>capt initiated by opp hole</t>
+  </si>
+  <si>
+    <t>no capture</t>
   </si>
 </sst>
 </file>
@@ -1588,12 +1603,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AMK258"/>
+  <dimension ref="A1:AMK268"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AK256" sqref="AK256"/>
+      <selection pane="bottomLeft" activeCell="AQ264" sqref="AQ264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -47367,6 +47382,3216 @@
       <c r="KO258" s="84"/>
       <c r="KP258" s="84"/>
     </row>
+    <row r="259" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A259" s="46">
+        <v>118</v>
+      </c>
+      <c r="B259" s="29">
+        <v>2</v>
+      </c>
+      <c r="C259" s="29">
+        <v>4</v>
+      </c>
+      <c r="D259" s="29">
+        <v>0</v>
+      </c>
+      <c r="E259" s="29">
+        <v>3</v>
+      </c>
+      <c r="F259" s="28"/>
+      <c r="I259" s="30"/>
+      <c r="J259" s="28"/>
+      <c r="M259" s="30"/>
+      <c r="N259" s="29">
+        <v>2</v>
+      </c>
+      <c r="O259" s="29">
+        <v>1</v>
+      </c>
+      <c r="P259" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q259" s="28">
+        <v>3</v>
+      </c>
+      <c r="R259" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S259" s="65"/>
+      <c r="T259" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="U259" s="65"/>
+      <c r="V259" s="65"/>
+      <c r="W259" s="65"/>
+      <c r="X259" s="65"/>
+      <c r="Y259" s="65"/>
+      <c r="Z259" s="65"/>
+      <c r="AA259" s="65"/>
+      <c r="AB259" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC259" s="65"/>
+      <c r="AD259" s="65"/>
+      <c r="AE259" s="65"/>
+      <c r="AF259" s="65"/>
+      <c r="AG259" s="91"/>
+      <c r="AH259" s="29">
+        <v>0</v>
+      </c>
+      <c r="AI259" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ259" s="29">
+        <v>0</v>
+      </c>
+      <c r="AK259" s="29">
+        <v>3</v>
+      </c>
+      <c r="AP259" s="29">
+        <v>8</v>
+      </c>
+      <c r="AQ259" s="29">
+        <v>1</v>
+      </c>
+      <c r="AR259" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS259" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="AT259" s="93"/>
+      <c r="AU259" s="93"/>
+      <c r="AV259" s="93"/>
+      <c r="AW259" s="93"/>
+      <c r="AX259" s="93"/>
+      <c r="AY259" s="93"/>
+      <c r="AZ259" s="93"/>
+      <c r="BA259" s="93"/>
+      <c r="BB259" s="93"/>
+      <c r="BC259" s="93"/>
+      <c r="BD259" s="93"/>
+      <c r="BE259" s="93"/>
+      <c r="BF259" s="93"/>
+      <c r="BG259" s="93"/>
+      <c r="BH259" s="93"/>
+      <c r="BI259" s="93"/>
+      <c r="BJ259" s="93"/>
+      <c r="BK259" s="93"/>
+      <c r="BL259" s="93"/>
+      <c r="BM259" s="93"/>
+      <c r="BN259" s="93"/>
+      <c r="BO259" s="93"/>
+      <c r="BP259" s="93"/>
+      <c r="BQ259" s="93"/>
+      <c r="BR259" s="93"/>
+      <c r="BS259" s="93"/>
+      <c r="BT259" s="93"/>
+      <c r="BU259" s="93"/>
+      <c r="BV259" s="93"/>
+      <c r="BW259" s="93"/>
+      <c r="BX259" s="93"/>
+      <c r="BY259" s="93"/>
+      <c r="BZ259" s="93"/>
+      <c r="CA259" s="93"/>
+      <c r="CB259" s="93"/>
+      <c r="CC259" s="93"/>
+      <c r="CD259" s="93"/>
+      <c r="CE259" s="93"/>
+      <c r="CF259" s="93"/>
+      <c r="CG259" s="93"/>
+      <c r="CH259" s="93"/>
+      <c r="CI259" s="93"/>
+      <c r="CJ259" s="93"/>
+      <c r="CK259" s="93"/>
+      <c r="CL259" s="93"/>
+      <c r="CM259" s="93"/>
+      <c r="CN259" s="93"/>
+      <c r="CO259" s="93"/>
+      <c r="CP259" s="93"/>
+      <c r="CQ259" s="93"/>
+      <c r="CR259" s="93"/>
+      <c r="CS259" s="93"/>
+      <c r="CT259" s="93"/>
+      <c r="CU259" s="93"/>
+      <c r="CV259" s="93"/>
+      <c r="CW259" s="93"/>
+      <c r="CX259" s="93"/>
+      <c r="CY259" s="93"/>
+      <c r="CZ259" s="93"/>
+      <c r="DA259" s="93"/>
+      <c r="DB259" s="93"/>
+      <c r="DC259" s="93"/>
+      <c r="DD259" s="93"/>
+      <c r="DE259" s="93"/>
+      <c r="DF259" s="93"/>
+      <c r="DG259" s="93"/>
+      <c r="DH259" s="93"/>
+      <c r="DI259" s="93"/>
+      <c r="DJ259" s="93"/>
+      <c r="DK259" s="93"/>
+      <c r="DL259" s="93"/>
+      <c r="DM259" s="93"/>
+      <c r="DN259" s="93"/>
+      <c r="DO259" s="93"/>
+      <c r="DP259" s="93"/>
+      <c r="DQ259" s="93"/>
+      <c r="DR259" s="93"/>
+      <c r="DS259" s="93"/>
+      <c r="DT259" s="93"/>
+      <c r="DU259" s="93"/>
+      <c r="DV259" s="93"/>
+      <c r="DW259" s="93"/>
+      <c r="DX259" s="93"/>
+      <c r="DY259" s="93"/>
+      <c r="DZ259" s="93"/>
+      <c r="EA259" s="93"/>
+      <c r="EB259" s="93"/>
+      <c r="EC259" s="93"/>
+      <c r="ED259" s="93"/>
+      <c r="EE259" s="93"/>
+      <c r="EF259" s="93"/>
+      <c r="EG259" s="93"/>
+      <c r="EH259" s="93"/>
+      <c r="EI259" s="93"/>
+      <c r="EJ259" s="93"/>
+      <c r="EK259" s="93"/>
+      <c r="EL259" s="93"/>
+      <c r="EM259" s="93"/>
+      <c r="EN259" s="93"/>
+      <c r="EO259" s="93"/>
+      <c r="EP259" s="93"/>
+      <c r="EQ259" s="93"/>
+      <c r="ER259" s="93"/>
+      <c r="ES259" s="93"/>
+      <c r="ET259" s="93"/>
+      <c r="EU259" s="93"/>
+      <c r="EV259" s="93"/>
+      <c r="EW259" s="93"/>
+      <c r="EX259" s="93"/>
+      <c r="EY259" s="93"/>
+      <c r="EZ259" s="93"/>
+      <c r="FA259" s="93"/>
+      <c r="FB259" s="93"/>
+      <c r="FC259" s="93"/>
+      <c r="FD259" s="93"/>
+      <c r="FE259" s="93"/>
+      <c r="FF259" s="93"/>
+      <c r="FG259" s="93"/>
+      <c r="FH259" s="93"/>
+      <c r="FI259" s="93"/>
+      <c r="FJ259" s="93"/>
+      <c r="FK259" s="93"/>
+      <c r="FL259" s="93"/>
+      <c r="FM259" s="93"/>
+      <c r="FN259" s="93"/>
+      <c r="FO259" s="93"/>
+      <c r="FP259" s="93"/>
+      <c r="FQ259" s="93"/>
+      <c r="FR259" s="93"/>
+      <c r="FS259" s="93"/>
+      <c r="FT259" s="93"/>
+      <c r="FU259" s="93"/>
+      <c r="FV259" s="93"/>
+      <c r="FW259" s="93"/>
+      <c r="FX259" s="93"/>
+      <c r="FY259" s="93"/>
+      <c r="FZ259" s="93"/>
+      <c r="GA259" s="93"/>
+      <c r="GB259" s="93"/>
+      <c r="GC259" s="93"/>
+      <c r="GD259" s="93"/>
+      <c r="GE259" s="93"/>
+      <c r="GF259" s="93"/>
+      <c r="GG259" s="93"/>
+      <c r="GH259" s="93"/>
+      <c r="GI259" s="93"/>
+      <c r="GJ259" s="93"/>
+      <c r="GK259" s="93"/>
+      <c r="GL259" s="93"/>
+      <c r="GM259" s="93"/>
+      <c r="GN259" s="93"/>
+      <c r="GO259" s="93"/>
+      <c r="GP259" s="93"/>
+      <c r="GQ259" s="93"/>
+      <c r="GR259" s="93"/>
+      <c r="GS259" s="93"/>
+      <c r="GT259" s="93"/>
+      <c r="GU259" s="93"/>
+      <c r="GV259" s="93"/>
+      <c r="GW259" s="93"/>
+      <c r="GX259" s="93"/>
+      <c r="GY259" s="93"/>
+      <c r="GZ259" s="93"/>
+      <c r="HA259" s="93"/>
+      <c r="HB259" s="93"/>
+      <c r="HC259" s="93"/>
+      <c r="HD259" s="93"/>
+      <c r="HE259" s="93"/>
+      <c r="HF259" s="93"/>
+      <c r="HG259" s="93"/>
+      <c r="HH259" s="93"/>
+      <c r="HI259" s="93"/>
+      <c r="HJ259" s="93"/>
+      <c r="HK259" s="93"/>
+      <c r="HL259" s="93"/>
+      <c r="HM259" s="93"/>
+      <c r="HN259" s="93"/>
+      <c r="HO259" s="93"/>
+      <c r="HP259" s="93"/>
+      <c r="HQ259" s="93"/>
+      <c r="HR259" s="93"/>
+      <c r="HS259" s="93"/>
+      <c r="HT259" s="93"/>
+      <c r="HU259" s="93"/>
+      <c r="HV259" s="93"/>
+      <c r="HW259" s="93"/>
+      <c r="HX259" s="93"/>
+      <c r="HY259" s="93"/>
+      <c r="HZ259" s="93"/>
+      <c r="IA259" s="93"/>
+      <c r="IB259" s="93"/>
+      <c r="IC259" s="93"/>
+      <c r="ID259" s="93"/>
+      <c r="IE259" s="93"/>
+      <c r="IF259" s="93"/>
+      <c r="IG259" s="93"/>
+      <c r="IH259" s="93"/>
+      <c r="II259" s="93"/>
+      <c r="IJ259" s="93"/>
+      <c r="IK259" s="93"/>
+      <c r="IL259" s="93"/>
+      <c r="IM259" s="93"/>
+      <c r="IN259" s="93"/>
+      <c r="IO259" s="93"/>
+      <c r="IP259" s="93"/>
+      <c r="IQ259" s="93"/>
+      <c r="IR259" s="93"/>
+      <c r="IS259" s="93"/>
+      <c r="IT259" s="93"/>
+      <c r="IU259" s="93"/>
+      <c r="IV259" s="93"/>
+      <c r="IW259" s="93"/>
+      <c r="IX259" s="93"/>
+      <c r="IY259" s="93"/>
+      <c r="IZ259" s="93"/>
+      <c r="JA259" s="93"/>
+      <c r="JB259" s="93"/>
+      <c r="JC259" s="93"/>
+      <c r="JD259" s="93"/>
+      <c r="JE259" s="93"/>
+      <c r="JF259" s="93"/>
+      <c r="JG259" s="93"/>
+      <c r="JH259" s="93"/>
+      <c r="JI259" s="93"/>
+      <c r="JJ259" s="93"/>
+      <c r="JK259" s="93"/>
+      <c r="JL259" s="93"/>
+      <c r="JM259" s="93"/>
+      <c r="JN259" s="93"/>
+      <c r="JO259" s="93"/>
+      <c r="JP259" s="93"/>
+      <c r="JQ259" s="93"/>
+      <c r="JR259" s="93"/>
+      <c r="JS259" s="93"/>
+      <c r="JT259" s="93"/>
+      <c r="JU259" s="93"/>
+      <c r="JV259" s="93"/>
+      <c r="JW259" s="93"/>
+      <c r="JX259" s="93"/>
+      <c r="JY259" s="93"/>
+      <c r="JZ259" s="93"/>
+      <c r="KA259" s="93"/>
+      <c r="KB259" s="93"/>
+      <c r="KC259" s="93"/>
+      <c r="KD259" s="93"/>
+      <c r="KE259" s="93"/>
+      <c r="KF259" s="93"/>
+      <c r="KG259" s="93"/>
+      <c r="KH259" s="93"/>
+      <c r="KI259" s="93"/>
+      <c r="KJ259" s="93"/>
+      <c r="KK259" s="93"/>
+      <c r="KL259" s="93"/>
+      <c r="KM259" s="93"/>
+      <c r="KN259" s="93"/>
+      <c r="KO259" s="93"/>
+      <c r="KP259" s="93"/>
+    </row>
+    <row r="260" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="41"/>
+      <c r="B260" s="33">
+        <v>3</v>
+      </c>
+      <c r="C260" s="33">
+        <v>3</v>
+      </c>
+      <c r="D260" s="33">
+        <v>3</v>
+      </c>
+      <c r="E260" s="85">
+        <v>3</v>
+      </c>
+      <c r="F260" s="32"/>
+      <c r="I260" s="34"/>
+      <c r="J260" s="32"/>
+      <c r="M260" s="34"/>
+      <c r="Q260" s="32"/>
+      <c r="R260" s="34"/>
+      <c r="S260" s="67"/>
+      <c r="T260" s="67"/>
+      <c r="U260" s="67"/>
+      <c r="V260" s="67"/>
+      <c r="W260" s="67"/>
+      <c r="X260" s="67"/>
+      <c r="Y260" s="67"/>
+      <c r="Z260" s="67"/>
+      <c r="AA260" s="67"/>
+      <c r="AB260" s="67"/>
+      <c r="AC260" s="67"/>
+      <c r="AD260" s="67"/>
+      <c r="AE260" s="67"/>
+      <c r="AF260" s="67"/>
+      <c r="AG260" s="68"/>
+      <c r="AH260" s="33">
+        <v>3</v>
+      </c>
+      <c r="AI260" s="33">
+        <v>3</v>
+      </c>
+      <c r="AJ260" s="33">
+        <v>3</v>
+      </c>
+      <c r="AK260" s="33">
+        <v>3</v>
+      </c>
+      <c r="AR260" s="83"/>
+      <c r="AT260" s="84"/>
+      <c r="AU260" s="84"/>
+      <c r="AV260" s="84"/>
+      <c r="AW260" s="84"/>
+      <c r="AX260" s="84"/>
+      <c r="AY260" s="84"/>
+      <c r="AZ260" s="84"/>
+      <c r="BA260" s="84"/>
+      <c r="BB260" s="84"/>
+      <c r="BC260" s="84"/>
+      <c r="BD260" s="84"/>
+      <c r="BE260" s="84"/>
+      <c r="BF260" s="84"/>
+      <c r="BG260" s="84"/>
+      <c r="BH260" s="84"/>
+      <c r="BI260" s="84"/>
+      <c r="BJ260" s="84"/>
+      <c r="BK260" s="84"/>
+      <c r="BL260" s="84"/>
+      <c r="BM260" s="84"/>
+      <c r="BN260" s="84"/>
+      <c r="BO260" s="84"/>
+      <c r="BP260" s="84"/>
+      <c r="BQ260" s="84"/>
+      <c r="BR260" s="84"/>
+      <c r="BS260" s="84"/>
+      <c r="BT260" s="84"/>
+      <c r="BU260" s="84"/>
+      <c r="BV260" s="84"/>
+      <c r="BW260" s="84"/>
+      <c r="BX260" s="84"/>
+      <c r="BY260" s="84"/>
+      <c r="BZ260" s="84"/>
+      <c r="CA260" s="84"/>
+      <c r="CB260" s="84"/>
+      <c r="CC260" s="84"/>
+      <c r="CD260" s="84"/>
+      <c r="CE260" s="84"/>
+      <c r="CF260" s="84"/>
+      <c r="CG260" s="84"/>
+      <c r="CH260" s="84"/>
+      <c r="CI260" s="84"/>
+      <c r="CJ260" s="84"/>
+      <c r="CK260" s="84"/>
+      <c r="CL260" s="84"/>
+      <c r="CM260" s="84"/>
+      <c r="CN260" s="84"/>
+      <c r="CO260" s="84"/>
+      <c r="CP260" s="84"/>
+      <c r="CQ260" s="84"/>
+      <c r="CR260" s="84"/>
+      <c r="CS260" s="84"/>
+      <c r="CT260" s="84"/>
+      <c r="CU260" s="84"/>
+      <c r="CV260" s="84"/>
+      <c r="CW260" s="84"/>
+      <c r="CX260" s="84"/>
+      <c r="CY260" s="84"/>
+      <c r="CZ260" s="84"/>
+      <c r="DA260" s="84"/>
+      <c r="DB260" s="84"/>
+      <c r="DC260" s="84"/>
+      <c r="DD260" s="84"/>
+      <c r="DE260" s="84"/>
+      <c r="DF260" s="84"/>
+      <c r="DG260" s="84"/>
+      <c r="DH260" s="84"/>
+      <c r="DI260" s="84"/>
+      <c r="DJ260" s="84"/>
+      <c r="DK260" s="84"/>
+      <c r="DL260" s="84"/>
+      <c r="DM260" s="84"/>
+      <c r="DN260" s="84"/>
+      <c r="DO260" s="84"/>
+      <c r="DP260" s="84"/>
+      <c r="DQ260" s="84"/>
+      <c r="DR260" s="84"/>
+      <c r="DS260" s="84"/>
+      <c r="DT260" s="84"/>
+      <c r="DU260" s="84"/>
+      <c r="DV260" s="84"/>
+      <c r="DW260" s="84"/>
+      <c r="DX260" s="84"/>
+      <c r="DY260" s="84"/>
+      <c r="DZ260" s="84"/>
+      <c r="EA260" s="84"/>
+      <c r="EB260" s="84"/>
+      <c r="EC260" s="84"/>
+      <c r="ED260" s="84"/>
+      <c r="EE260" s="84"/>
+      <c r="EF260" s="84"/>
+      <c r="EG260" s="84"/>
+      <c r="EH260" s="84"/>
+      <c r="EI260" s="84"/>
+      <c r="EJ260" s="84"/>
+      <c r="EK260" s="84"/>
+      <c r="EL260" s="84"/>
+      <c r="EM260" s="84"/>
+      <c r="EN260" s="84"/>
+      <c r="EO260" s="84"/>
+      <c r="EP260" s="84"/>
+      <c r="EQ260" s="84"/>
+      <c r="ER260" s="84"/>
+      <c r="ES260" s="84"/>
+      <c r="ET260" s="84"/>
+      <c r="EU260" s="84"/>
+      <c r="EV260" s="84"/>
+      <c r="EW260" s="84"/>
+      <c r="EX260" s="84"/>
+      <c r="EY260" s="84"/>
+      <c r="EZ260" s="84"/>
+      <c r="FA260" s="84"/>
+      <c r="FB260" s="84"/>
+      <c r="FC260" s="84"/>
+      <c r="FD260" s="84"/>
+      <c r="FE260" s="84"/>
+      <c r="FF260" s="84"/>
+      <c r="FG260" s="84"/>
+      <c r="FH260" s="84"/>
+      <c r="FI260" s="84"/>
+      <c r="FJ260" s="84"/>
+      <c r="FK260" s="84"/>
+      <c r="FL260" s="84"/>
+      <c r="FM260" s="84"/>
+      <c r="FN260" s="84"/>
+      <c r="FO260" s="84"/>
+      <c r="FP260" s="84"/>
+      <c r="FQ260" s="84"/>
+      <c r="FR260" s="84"/>
+      <c r="FS260" s="84"/>
+      <c r="FT260" s="84"/>
+      <c r="FU260" s="84"/>
+      <c r="FV260" s="84"/>
+      <c r="FW260" s="84"/>
+      <c r="FX260" s="84"/>
+      <c r="FY260" s="84"/>
+      <c r="FZ260" s="84"/>
+      <c r="GA260" s="84"/>
+      <c r="GB260" s="84"/>
+      <c r="GC260" s="84"/>
+      <c r="GD260" s="84"/>
+      <c r="GE260" s="84"/>
+      <c r="GF260" s="84"/>
+      <c r="GG260" s="84"/>
+      <c r="GH260" s="84"/>
+      <c r="GI260" s="84"/>
+      <c r="GJ260" s="84"/>
+      <c r="GK260" s="84"/>
+      <c r="GL260" s="84"/>
+      <c r="GM260" s="84"/>
+      <c r="GN260" s="84"/>
+      <c r="GO260" s="84"/>
+      <c r="GP260" s="84"/>
+      <c r="GQ260" s="84"/>
+      <c r="GR260" s="84"/>
+      <c r="GS260" s="84"/>
+      <c r="GT260" s="84"/>
+      <c r="GU260" s="84"/>
+      <c r="GV260" s="84"/>
+      <c r="GW260" s="84"/>
+      <c r="GX260" s="84"/>
+      <c r="GY260" s="84"/>
+      <c r="GZ260" s="84"/>
+      <c r="HA260" s="84"/>
+      <c r="HB260" s="84"/>
+      <c r="HC260" s="84"/>
+      <c r="HD260" s="84"/>
+      <c r="HE260" s="84"/>
+      <c r="HF260" s="84"/>
+      <c r="HG260" s="84"/>
+      <c r="HH260" s="84"/>
+      <c r="HI260" s="84"/>
+      <c r="HJ260" s="84"/>
+      <c r="HK260" s="84"/>
+      <c r="HL260" s="84"/>
+      <c r="HM260" s="84"/>
+      <c r="HN260" s="84"/>
+      <c r="HO260" s="84"/>
+      <c r="HP260" s="84"/>
+      <c r="HQ260" s="84"/>
+      <c r="HR260" s="84"/>
+      <c r="HS260" s="84"/>
+      <c r="HT260" s="84"/>
+      <c r="HU260" s="84"/>
+      <c r="HV260" s="84"/>
+      <c r="HW260" s="84"/>
+      <c r="HX260" s="84"/>
+      <c r="HY260" s="84"/>
+      <c r="HZ260" s="84"/>
+      <c r="IA260" s="84"/>
+      <c r="IB260" s="84"/>
+      <c r="IC260" s="84"/>
+      <c r="ID260" s="84"/>
+      <c r="IE260" s="84"/>
+      <c r="IF260" s="84"/>
+      <c r="IG260" s="84"/>
+      <c r="IH260" s="84"/>
+      <c r="II260" s="84"/>
+      <c r="IJ260" s="84"/>
+      <c r="IK260" s="84"/>
+      <c r="IL260" s="84"/>
+      <c r="IM260" s="84"/>
+      <c r="IN260" s="84"/>
+      <c r="IO260" s="84"/>
+      <c r="IP260" s="84"/>
+      <c r="IQ260" s="84"/>
+      <c r="IR260" s="84"/>
+      <c r="IS260" s="84"/>
+      <c r="IT260" s="84"/>
+      <c r="IU260" s="84"/>
+      <c r="IV260" s="84"/>
+      <c r="IW260" s="84"/>
+      <c r="IX260" s="84"/>
+      <c r="IY260" s="84"/>
+      <c r="IZ260" s="84"/>
+      <c r="JA260" s="84"/>
+      <c r="JB260" s="84"/>
+      <c r="JC260" s="84"/>
+      <c r="JD260" s="84"/>
+      <c r="JE260" s="84"/>
+      <c r="JF260" s="84"/>
+      <c r="JG260" s="84"/>
+      <c r="JH260" s="84"/>
+      <c r="JI260" s="84"/>
+      <c r="JJ260" s="84"/>
+      <c r="JK260" s="84"/>
+      <c r="JL260" s="84"/>
+      <c r="JM260" s="84"/>
+      <c r="JN260" s="84"/>
+      <c r="JO260" s="84"/>
+      <c r="JP260" s="84"/>
+      <c r="JQ260" s="84"/>
+      <c r="JR260" s="84"/>
+      <c r="JS260" s="84"/>
+      <c r="JT260" s="84"/>
+      <c r="JU260" s="84"/>
+      <c r="JV260" s="84"/>
+      <c r="JW260" s="84"/>
+      <c r="JX260" s="84"/>
+      <c r="JY260" s="84"/>
+      <c r="JZ260" s="84"/>
+      <c r="KA260" s="84"/>
+      <c r="KB260" s="84"/>
+      <c r="KC260" s="84"/>
+      <c r="KD260" s="84"/>
+      <c r="KE260" s="84"/>
+      <c r="KF260" s="84"/>
+      <c r="KG260" s="84"/>
+      <c r="KH260" s="84"/>
+      <c r="KI260" s="84"/>
+      <c r="KJ260" s="84"/>
+      <c r="KK260" s="84"/>
+      <c r="KL260" s="84"/>
+      <c r="KM260" s="84"/>
+      <c r="KN260" s="84"/>
+      <c r="KO260" s="84"/>
+      <c r="KP260" s="84"/>
+    </row>
+    <row r="261" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A261" s="46">
+        <v>119</v>
+      </c>
+      <c r="B261" s="29">
+        <v>2</v>
+      </c>
+      <c r="C261" s="29">
+        <v>4</v>
+      </c>
+      <c r="D261" s="29">
+        <v>0</v>
+      </c>
+      <c r="E261" s="87">
+        <v>3</v>
+      </c>
+      <c r="F261" s="28"/>
+      <c r="I261" s="30"/>
+      <c r="J261" s="28"/>
+      <c r="M261" s="30"/>
+      <c r="N261" s="29">
+        <v>2</v>
+      </c>
+      <c r="O261" s="29">
+        <v>1</v>
+      </c>
+      <c r="P261" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q261" s="28">
+        <v>4</v>
+      </c>
+      <c r="R261" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S261" s="65"/>
+      <c r="T261" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="U261" s="65"/>
+      <c r="V261" s="65"/>
+      <c r="W261" s="65"/>
+      <c r="X261" s="65"/>
+      <c r="Y261" s="65"/>
+      <c r="Z261" s="65"/>
+      <c r="AA261" s="65"/>
+      <c r="AB261" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC261" s="65"/>
+      <c r="AD261" s="65"/>
+      <c r="AE261" s="65"/>
+      <c r="AF261" s="65"/>
+      <c r="AG261" s="91"/>
+      <c r="AH261" s="29">
+        <v>0</v>
+      </c>
+      <c r="AI261" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ261" s="29">
+        <v>0</v>
+      </c>
+      <c r="AK261" s="29">
+        <v>3</v>
+      </c>
+      <c r="AP261" s="29">
+        <v>8</v>
+      </c>
+      <c r="AQ261" s="29">
+        <v>1</v>
+      </c>
+      <c r="AR261" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS261" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="AT261" s="93"/>
+      <c r="AU261" s="93"/>
+      <c r="AV261" s="93"/>
+      <c r="AW261" s="93"/>
+      <c r="AX261" s="93"/>
+      <c r="AY261" s="93"/>
+      <c r="AZ261" s="93"/>
+      <c r="BA261" s="93"/>
+      <c r="BB261" s="93"/>
+      <c r="BC261" s="93"/>
+      <c r="BD261" s="93"/>
+      <c r="BE261" s="93"/>
+      <c r="BF261" s="93"/>
+      <c r="BG261" s="93"/>
+      <c r="BH261" s="93"/>
+      <c r="BI261" s="93"/>
+      <c r="BJ261" s="93"/>
+      <c r="BK261" s="93"/>
+      <c r="BL261" s="93"/>
+      <c r="BM261" s="93"/>
+      <c r="BN261" s="93"/>
+      <c r="BO261" s="93"/>
+      <c r="BP261" s="93"/>
+      <c r="BQ261" s="93"/>
+      <c r="BR261" s="93"/>
+      <c r="BS261" s="93"/>
+      <c r="BT261" s="93"/>
+      <c r="BU261" s="93"/>
+      <c r="BV261" s="93"/>
+      <c r="BW261" s="93"/>
+      <c r="BX261" s="93"/>
+      <c r="BY261" s="93"/>
+      <c r="BZ261" s="93"/>
+      <c r="CA261" s="93"/>
+      <c r="CB261" s="93"/>
+      <c r="CC261" s="93"/>
+      <c r="CD261" s="93"/>
+      <c r="CE261" s="93"/>
+      <c r="CF261" s="93"/>
+      <c r="CG261" s="93"/>
+      <c r="CH261" s="93"/>
+      <c r="CI261" s="93"/>
+      <c r="CJ261" s="93"/>
+      <c r="CK261" s="93"/>
+      <c r="CL261" s="93"/>
+      <c r="CM261" s="93"/>
+      <c r="CN261" s="93"/>
+      <c r="CO261" s="93"/>
+      <c r="CP261" s="93"/>
+      <c r="CQ261" s="93"/>
+      <c r="CR261" s="93"/>
+      <c r="CS261" s="93"/>
+      <c r="CT261" s="93"/>
+      <c r="CU261" s="93"/>
+      <c r="CV261" s="93"/>
+      <c r="CW261" s="93"/>
+      <c r="CX261" s="93"/>
+      <c r="CY261" s="93"/>
+      <c r="CZ261" s="93"/>
+      <c r="DA261" s="93"/>
+      <c r="DB261" s="93"/>
+      <c r="DC261" s="93"/>
+      <c r="DD261" s="93"/>
+      <c r="DE261" s="93"/>
+      <c r="DF261" s="93"/>
+      <c r="DG261" s="93"/>
+      <c r="DH261" s="93"/>
+      <c r="DI261" s="93"/>
+      <c r="DJ261" s="93"/>
+      <c r="DK261" s="93"/>
+      <c r="DL261" s="93"/>
+      <c r="DM261" s="93"/>
+      <c r="DN261" s="93"/>
+      <c r="DO261" s="93"/>
+      <c r="DP261" s="93"/>
+      <c r="DQ261" s="93"/>
+      <c r="DR261" s="93"/>
+      <c r="DS261" s="93"/>
+      <c r="DT261" s="93"/>
+      <c r="DU261" s="93"/>
+      <c r="DV261" s="93"/>
+      <c r="DW261" s="93"/>
+      <c r="DX261" s="93"/>
+      <c r="DY261" s="93"/>
+      <c r="DZ261" s="93"/>
+      <c r="EA261" s="93"/>
+      <c r="EB261" s="93"/>
+      <c r="EC261" s="93"/>
+      <c r="ED261" s="93"/>
+      <c r="EE261" s="93"/>
+      <c r="EF261" s="93"/>
+      <c r="EG261" s="93"/>
+      <c r="EH261" s="93"/>
+      <c r="EI261" s="93"/>
+      <c r="EJ261" s="93"/>
+      <c r="EK261" s="93"/>
+      <c r="EL261" s="93"/>
+      <c r="EM261" s="93"/>
+      <c r="EN261" s="93"/>
+      <c r="EO261" s="93"/>
+      <c r="EP261" s="93"/>
+      <c r="EQ261" s="93"/>
+      <c r="ER261" s="93"/>
+      <c r="ES261" s="93"/>
+      <c r="ET261" s="93"/>
+      <c r="EU261" s="93"/>
+      <c r="EV261" s="93"/>
+      <c r="EW261" s="93"/>
+      <c r="EX261" s="93"/>
+      <c r="EY261" s="93"/>
+      <c r="EZ261" s="93"/>
+      <c r="FA261" s="93"/>
+      <c r="FB261" s="93"/>
+      <c r="FC261" s="93"/>
+      <c r="FD261" s="93"/>
+      <c r="FE261" s="93"/>
+      <c r="FF261" s="93"/>
+      <c r="FG261" s="93"/>
+      <c r="FH261" s="93"/>
+      <c r="FI261" s="93"/>
+      <c r="FJ261" s="93"/>
+      <c r="FK261" s="93"/>
+      <c r="FL261" s="93"/>
+      <c r="FM261" s="93"/>
+      <c r="FN261" s="93"/>
+      <c r="FO261" s="93"/>
+      <c r="FP261" s="93"/>
+      <c r="FQ261" s="93"/>
+      <c r="FR261" s="93"/>
+      <c r="FS261" s="93"/>
+      <c r="FT261" s="93"/>
+      <c r="FU261" s="93"/>
+      <c r="FV261" s="93"/>
+      <c r="FW261" s="93"/>
+      <c r="FX261" s="93"/>
+      <c r="FY261" s="93"/>
+      <c r="FZ261" s="93"/>
+      <c r="GA261" s="93"/>
+      <c r="GB261" s="93"/>
+      <c r="GC261" s="93"/>
+      <c r="GD261" s="93"/>
+      <c r="GE261" s="93"/>
+      <c r="GF261" s="93"/>
+      <c r="GG261" s="93"/>
+      <c r="GH261" s="93"/>
+      <c r="GI261" s="93"/>
+      <c r="GJ261" s="93"/>
+      <c r="GK261" s="93"/>
+      <c r="GL261" s="93"/>
+      <c r="GM261" s="93"/>
+      <c r="GN261" s="93"/>
+      <c r="GO261" s="93"/>
+      <c r="GP261" s="93"/>
+      <c r="GQ261" s="93"/>
+      <c r="GR261" s="93"/>
+      <c r="GS261" s="93"/>
+      <c r="GT261" s="93"/>
+      <c r="GU261" s="93"/>
+      <c r="GV261" s="93"/>
+      <c r="GW261" s="93"/>
+      <c r="GX261" s="93"/>
+      <c r="GY261" s="93"/>
+      <c r="GZ261" s="93"/>
+      <c r="HA261" s="93"/>
+      <c r="HB261" s="93"/>
+      <c r="HC261" s="93"/>
+      <c r="HD261" s="93"/>
+      <c r="HE261" s="93"/>
+      <c r="HF261" s="93"/>
+      <c r="HG261" s="93"/>
+      <c r="HH261" s="93"/>
+      <c r="HI261" s="93"/>
+      <c r="HJ261" s="93"/>
+      <c r="HK261" s="93"/>
+      <c r="HL261" s="93"/>
+      <c r="HM261" s="93"/>
+      <c r="HN261" s="93"/>
+      <c r="HO261" s="93"/>
+      <c r="HP261" s="93"/>
+      <c r="HQ261" s="93"/>
+      <c r="HR261" s="93"/>
+      <c r="HS261" s="93"/>
+      <c r="HT261" s="93"/>
+      <c r="HU261" s="93"/>
+      <c r="HV261" s="93"/>
+      <c r="HW261" s="93"/>
+      <c r="HX261" s="93"/>
+      <c r="HY261" s="93"/>
+      <c r="HZ261" s="93"/>
+      <c r="IA261" s="93"/>
+      <c r="IB261" s="93"/>
+      <c r="IC261" s="93"/>
+      <c r="ID261" s="93"/>
+      <c r="IE261" s="93"/>
+      <c r="IF261" s="93"/>
+      <c r="IG261" s="93"/>
+      <c r="IH261" s="93"/>
+      <c r="II261" s="93"/>
+      <c r="IJ261" s="93"/>
+      <c r="IK261" s="93"/>
+      <c r="IL261" s="93"/>
+      <c r="IM261" s="93"/>
+      <c r="IN261" s="93"/>
+      <c r="IO261" s="93"/>
+      <c r="IP261" s="93"/>
+      <c r="IQ261" s="93"/>
+      <c r="IR261" s="93"/>
+      <c r="IS261" s="93"/>
+      <c r="IT261" s="93"/>
+      <c r="IU261" s="93"/>
+      <c r="IV261" s="93"/>
+      <c r="IW261" s="93"/>
+      <c r="IX261" s="93"/>
+      <c r="IY261" s="93"/>
+      <c r="IZ261" s="93"/>
+      <c r="JA261" s="93"/>
+      <c r="JB261" s="93"/>
+      <c r="JC261" s="93"/>
+      <c r="JD261" s="93"/>
+      <c r="JE261" s="93"/>
+      <c r="JF261" s="93"/>
+      <c r="JG261" s="93"/>
+      <c r="JH261" s="93"/>
+      <c r="JI261" s="93"/>
+      <c r="JJ261" s="93"/>
+      <c r="JK261" s="93"/>
+      <c r="JL261" s="93"/>
+      <c r="JM261" s="93"/>
+      <c r="JN261" s="93"/>
+      <c r="JO261" s="93"/>
+      <c r="JP261" s="93"/>
+      <c r="JQ261" s="93"/>
+      <c r="JR261" s="93"/>
+      <c r="JS261" s="93"/>
+      <c r="JT261" s="93"/>
+      <c r="JU261" s="93"/>
+      <c r="JV261" s="93"/>
+      <c r="JW261" s="93"/>
+      <c r="JX261" s="93"/>
+      <c r="JY261" s="93"/>
+      <c r="JZ261" s="93"/>
+      <c r="KA261" s="93"/>
+      <c r="KB261" s="93"/>
+      <c r="KC261" s="93"/>
+      <c r="KD261" s="93"/>
+      <c r="KE261" s="93"/>
+      <c r="KF261" s="93"/>
+      <c r="KG261" s="93"/>
+      <c r="KH261" s="93"/>
+      <c r="KI261" s="93"/>
+      <c r="KJ261" s="93"/>
+      <c r="KK261" s="93"/>
+      <c r="KL261" s="93"/>
+      <c r="KM261" s="93"/>
+      <c r="KN261" s="93"/>
+      <c r="KO261" s="93"/>
+      <c r="KP261" s="93"/>
+    </row>
+    <row r="262" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="41"/>
+      <c r="B262" s="33">
+        <v>3</v>
+      </c>
+      <c r="C262" s="33">
+        <v>3</v>
+      </c>
+      <c r="D262" s="33">
+        <v>3</v>
+      </c>
+      <c r="E262" s="33">
+        <v>3</v>
+      </c>
+      <c r="F262" s="32"/>
+      <c r="I262" s="34"/>
+      <c r="J262" s="32"/>
+      <c r="M262" s="34"/>
+      <c r="Q262" s="32"/>
+      <c r="R262" s="34"/>
+      <c r="S262" s="67"/>
+      <c r="T262" s="67"/>
+      <c r="U262" s="67"/>
+      <c r="V262" s="67"/>
+      <c r="W262" s="67"/>
+      <c r="X262" s="67"/>
+      <c r="Y262" s="67"/>
+      <c r="Z262" s="67"/>
+      <c r="AA262" s="67"/>
+      <c r="AB262" s="67"/>
+      <c r="AC262" s="67"/>
+      <c r="AD262" s="67"/>
+      <c r="AE262" s="67"/>
+      <c r="AF262" s="67"/>
+      <c r="AG262" s="68"/>
+      <c r="AH262" s="33">
+        <v>3</v>
+      </c>
+      <c r="AI262" s="33">
+        <v>3</v>
+      </c>
+      <c r="AJ262" s="33">
+        <v>3</v>
+      </c>
+      <c r="AK262" s="33">
+        <v>3</v>
+      </c>
+      <c r="AR262" s="83"/>
+      <c r="AT262" s="84"/>
+      <c r="AU262" s="84"/>
+      <c r="AV262" s="84"/>
+      <c r="AW262" s="84"/>
+      <c r="AX262" s="84"/>
+      <c r="AY262" s="84"/>
+      <c r="AZ262" s="84"/>
+      <c r="BA262" s="84"/>
+      <c r="BB262" s="84"/>
+      <c r="BC262" s="84"/>
+      <c r="BD262" s="84"/>
+      <c r="BE262" s="84"/>
+      <c r="BF262" s="84"/>
+      <c r="BG262" s="84"/>
+      <c r="BH262" s="84"/>
+      <c r="BI262" s="84"/>
+      <c r="BJ262" s="84"/>
+      <c r="BK262" s="84"/>
+      <c r="BL262" s="84"/>
+      <c r="BM262" s="84"/>
+      <c r="BN262" s="84"/>
+      <c r="BO262" s="84"/>
+      <c r="BP262" s="84"/>
+      <c r="BQ262" s="84"/>
+      <c r="BR262" s="84"/>
+      <c r="BS262" s="84"/>
+      <c r="BT262" s="84"/>
+      <c r="BU262" s="84"/>
+      <c r="BV262" s="84"/>
+      <c r="BW262" s="84"/>
+      <c r="BX262" s="84"/>
+      <c r="BY262" s="84"/>
+      <c r="BZ262" s="84"/>
+      <c r="CA262" s="84"/>
+      <c r="CB262" s="84"/>
+      <c r="CC262" s="84"/>
+      <c r="CD262" s="84"/>
+      <c r="CE262" s="84"/>
+      <c r="CF262" s="84"/>
+      <c r="CG262" s="84"/>
+      <c r="CH262" s="84"/>
+      <c r="CI262" s="84"/>
+      <c r="CJ262" s="84"/>
+      <c r="CK262" s="84"/>
+      <c r="CL262" s="84"/>
+      <c r="CM262" s="84"/>
+      <c r="CN262" s="84"/>
+      <c r="CO262" s="84"/>
+      <c r="CP262" s="84"/>
+      <c r="CQ262" s="84"/>
+      <c r="CR262" s="84"/>
+      <c r="CS262" s="84"/>
+      <c r="CT262" s="84"/>
+      <c r="CU262" s="84"/>
+      <c r="CV262" s="84"/>
+      <c r="CW262" s="84"/>
+      <c r="CX262" s="84"/>
+      <c r="CY262" s="84"/>
+      <c r="CZ262" s="84"/>
+      <c r="DA262" s="84"/>
+      <c r="DB262" s="84"/>
+      <c r="DC262" s="84"/>
+      <c r="DD262" s="84"/>
+      <c r="DE262" s="84"/>
+      <c r="DF262" s="84"/>
+      <c r="DG262" s="84"/>
+      <c r="DH262" s="84"/>
+      <c r="DI262" s="84"/>
+      <c r="DJ262" s="84"/>
+      <c r="DK262" s="84"/>
+      <c r="DL262" s="84"/>
+      <c r="DM262" s="84"/>
+      <c r="DN262" s="84"/>
+      <c r="DO262" s="84"/>
+      <c r="DP262" s="84"/>
+      <c r="DQ262" s="84"/>
+      <c r="DR262" s="84"/>
+      <c r="DS262" s="84"/>
+      <c r="DT262" s="84"/>
+      <c r="DU262" s="84"/>
+      <c r="DV262" s="84"/>
+      <c r="DW262" s="84"/>
+      <c r="DX262" s="84"/>
+      <c r="DY262" s="84"/>
+      <c r="DZ262" s="84"/>
+      <c r="EA262" s="84"/>
+      <c r="EB262" s="84"/>
+      <c r="EC262" s="84"/>
+      <c r="ED262" s="84"/>
+      <c r="EE262" s="84"/>
+      <c r="EF262" s="84"/>
+      <c r="EG262" s="84"/>
+      <c r="EH262" s="84"/>
+      <c r="EI262" s="84"/>
+      <c r="EJ262" s="84"/>
+      <c r="EK262" s="84"/>
+      <c r="EL262" s="84"/>
+      <c r="EM262" s="84"/>
+      <c r="EN262" s="84"/>
+      <c r="EO262" s="84"/>
+      <c r="EP262" s="84"/>
+      <c r="EQ262" s="84"/>
+      <c r="ER262" s="84"/>
+      <c r="ES262" s="84"/>
+      <c r="ET262" s="84"/>
+      <c r="EU262" s="84"/>
+      <c r="EV262" s="84"/>
+      <c r="EW262" s="84"/>
+      <c r="EX262" s="84"/>
+      <c r="EY262" s="84"/>
+      <c r="EZ262" s="84"/>
+      <c r="FA262" s="84"/>
+      <c r="FB262" s="84"/>
+      <c r="FC262" s="84"/>
+      <c r="FD262" s="84"/>
+      <c r="FE262" s="84"/>
+      <c r="FF262" s="84"/>
+      <c r="FG262" s="84"/>
+      <c r="FH262" s="84"/>
+      <c r="FI262" s="84"/>
+      <c r="FJ262" s="84"/>
+      <c r="FK262" s="84"/>
+      <c r="FL262" s="84"/>
+      <c r="FM262" s="84"/>
+      <c r="FN262" s="84"/>
+      <c r="FO262" s="84"/>
+      <c r="FP262" s="84"/>
+      <c r="FQ262" s="84"/>
+      <c r="FR262" s="84"/>
+      <c r="FS262" s="84"/>
+      <c r="FT262" s="84"/>
+      <c r="FU262" s="84"/>
+      <c r="FV262" s="84"/>
+      <c r="FW262" s="84"/>
+      <c r="FX262" s="84"/>
+      <c r="FY262" s="84"/>
+      <c r="FZ262" s="84"/>
+      <c r="GA262" s="84"/>
+      <c r="GB262" s="84"/>
+      <c r="GC262" s="84"/>
+      <c r="GD262" s="84"/>
+      <c r="GE262" s="84"/>
+      <c r="GF262" s="84"/>
+      <c r="GG262" s="84"/>
+      <c r="GH262" s="84"/>
+      <c r="GI262" s="84"/>
+      <c r="GJ262" s="84"/>
+      <c r="GK262" s="84"/>
+      <c r="GL262" s="84"/>
+      <c r="GM262" s="84"/>
+      <c r="GN262" s="84"/>
+      <c r="GO262" s="84"/>
+      <c r="GP262" s="84"/>
+      <c r="GQ262" s="84"/>
+      <c r="GR262" s="84"/>
+      <c r="GS262" s="84"/>
+      <c r="GT262" s="84"/>
+      <c r="GU262" s="84"/>
+      <c r="GV262" s="84"/>
+      <c r="GW262" s="84"/>
+      <c r="GX262" s="84"/>
+      <c r="GY262" s="84"/>
+      <c r="GZ262" s="84"/>
+      <c r="HA262" s="84"/>
+      <c r="HB262" s="84"/>
+      <c r="HC262" s="84"/>
+      <c r="HD262" s="84"/>
+      <c r="HE262" s="84"/>
+      <c r="HF262" s="84"/>
+      <c r="HG262" s="84"/>
+      <c r="HH262" s="84"/>
+      <c r="HI262" s="84"/>
+      <c r="HJ262" s="84"/>
+      <c r="HK262" s="84"/>
+      <c r="HL262" s="84"/>
+      <c r="HM262" s="84"/>
+      <c r="HN262" s="84"/>
+      <c r="HO262" s="84"/>
+      <c r="HP262" s="84"/>
+      <c r="HQ262" s="84"/>
+      <c r="HR262" s="84"/>
+      <c r="HS262" s="84"/>
+      <c r="HT262" s="84"/>
+      <c r="HU262" s="84"/>
+      <c r="HV262" s="84"/>
+      <c r="HW262" s="84"/>
+      <c r="HX262" s="84"/>
+      <c r="HY262" s="84"/>
+      <c r="HZ262" s="84"/>
+      <c r="IA262" s="84"/>
+      <c r="IB262" s="84"/>
+      <c r="IC262" s="84"/>
+      <c r="ID262" s="84"/>
+      <c r="IE262" s="84"/>
+      <c r="IF262" s="84"/>
+      <c r="IG262" s="84"/>
+      <c r="IH262" s="84"/>
+      <c r="II262" s="84"/>
+      <c r="IJ262" s="84"/>
+      <c r="IK262" s="84"/>
+      <c r="IL262" s="84"/>
+      <c r="IM262" s="84"/>
+      <c r="IN262" s="84"/>
+      <c r="IO262" s="84"/>
+      <c r="IP262" s="84"/>
+      <c r="IQ262" s="84"/>
+      <c r="IR262" s="84"/>
+      <c r="IS262" s="84"/>
+      <c r="IT262" s="84"/>
+      <c r="IU262" s="84"/>
+      <c r="IV262" s="84"/>
+      <c r="IW262" s="84"/>
+      <c r="IX262" s="84"/>
+      <c r="IY262" s="84"/>
+      <c r="IZ262" s="84"/>
+      <c r="JA262" s="84"/>
+      <c r="JB262" s="84"/>
+      <c r="JC262" s="84"/>
+      <c r="JD262" s="84"/>
+      <c r="JE262" s="84"/>
+      <c r="JF262" s="84"/>
+      <c r="JG262" s="84"/>
+      <c r="JH262" s="84"/>
+      <c r="JI262" s="84"/>
+      <c r="JJ262" s="84"/>
+      <c r="JK262" s="84"/>
+      <c r="JL262" s="84"/>
+      <c r="JM262" s="84"/>
+      <c r="JN262" s="84"/>
+      <c r="JO262" s="84"/>
+      <c r="JP262" s="84"/>
+      <c r="JQ262" s="84"/>
+      <c r="JR262" s="84"/>
+      <c r="JS262" s="84"/>
+      <c r="JT262" s="84"/>
+      <c r="JU262" s="84"/>
+      <c r="JV262" s="84"/>
+      <c r="JW262" s="84"/>
+      <c r="JX262" s="84"/>
+      <c r="JY262" s="84"/>
+      <c r="JZ262" s="84"/>
+      <c r="KA262" s="84"/>
+      <c r="KB262" s="84"/>
+      <c r="KC262" s="84"/>
+      <c r="KD262" s="84"/>
+      <c r="KE262" s="84"/>
+      <c r="KF262" s="84"/>
+      <c r="KG262" s="84"/>
+      <c r="KH262" s="84"/>
+      <c r="KI262" s="84"/>
+      <c r="KJ262" s="84"/>
+      <c r="KK262" s="84"/>
+      <c r="KL262" s="84"/>
+      <c r="KM262" s="84"/>
+      <c r="KN262" s="84"/>
+      <c r="KO262" s="84"/>
+      <c r="KP262" s="84"/>
+    </row>
+    <row r="263" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A263" s="46">
+        <v>120</v>
+      </c>
+      <c r="B263" s="87">
+        <v>3</v>
+      </c>
+      <c r="C263" s="29">
+        <v>0</v>
+      </c>
+      <c r="D263" s="29">
+        <v>2</v>
+      </c>
+      <c r="E263" s="29">
+        <v>3</v>
+      </c>
+      <c r="F263" s="28"/>
+      <c r="I263" s="30"/>
+      <c r="J263" s="28"/>
+      <c r="M263" s="30"/>
+      <c r="N263" s="29">
+        <v>2</v>
+      </c>
+      <c r="O263" s="29">
+        <v>1</v>
+      </c>
+      <c r="P263" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q263" s="28">
+        <v>7</v>
+      </c>
+      <c r="R263" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S263" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="T263" s="65"/>
+      <c r="U263" s="65"/>
+      <c r="V263" s="65"/>
+      <c r="W263" s="65"/>
+      <c r="X263" s="65"/>
+      <c r="Y263" s="65"/>
+      <c r="Z263" s="65"/>
+      <c r="AA263" s="65"/>
+      <c r="AB263" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC263" s="65"/>
+      <c r="AD263" s="65"/>
+      <c r="AE263" s="65"/>
+      <c r="AF263" s="65"/>
+      <c r="AG263" s="91"/>
+      <c r="AH263" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI263" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ263" s="29">
+        <v>2</v>
+      </c>
+      <c r="AK263" s="29">
+        <v>3</v>
+      </c>
+      <c r="AP263" s="29">
+        <v>2</v>
+      </c>
+      <c r="AQ263" s="29">
+        <v>11</v>
+      </c>
+      <c r="AR263" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS263" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="AT263" s="93"/>
+      <c r="AU263" s="93"/>
+      <c r="AV263" s="93"/>
+      <c r="AW263" s="93"/>
+      <c r="AX263" s="93"/>
+      <c r="AY263" s="93"/>
+      <c r="AZ263" s="93"/>
+      <c r="BA263" s="93"/>
+      <c r="BB263" s="93"/>
+      <c r="BC263" s="93"/>
+      <c r="BD263" s="93"/>
+      <c r="BE263" s="93"/>
+      <c r="BF263" s="93"/>
+      <c r="BG263" s="93"/>
+      <c r="BH263" s="93"/>
+      <c r="BI263" s="93"/>
+      <c r="BJ263" s="93"/>
+      <c r="BK263" s="93"/>
+      <c r="BL263" s="93"/>
+      <c r="BM263" s="93"/>
+      <c r="BN263" s="93"/>
+      <c r="BO263" s="93"/>
+      <c r="BP263" s="93"/>
+      <c r="BQ263" s="93"/>
+      <c r="BR263" s="93"/>
+      <c r="BS263" s="93"/>
+      <c r="BT263" s="93"/>
+      <c r="BU263" s="93"/>
+      <c r="BV263" s="93"/>
+      <c r="BW263" s="93"/>
+      <c r="BX263" s="93"/>
+      <c r="BY263" s="93"/>
+      <c r="BZ263" s="93"/>
+      <c r="CA263" s="93"/>
+      <c r="CB263" s="93"/>
+      <c r="CC263" s="93"/>
+      <c r="CD263" s="93"/>
+      <c r="CE263" s="93"/>
+      <c r="CF263" s="93"/>
+      <c r="CG263" s="93"/>
+      <c r="CH263" s="93"/>
+      <c r="CI263" s="93"/>
+      <c r="CJ263" s="93"/>
+      <c r="CK263" s="93"/>
+      <c r="CL263" s="93"/>
+      <c r="CM263" s="93"/>
+      <c r="CN263" s="93"/>
+      <c r="CO263" s="93"/>
+      <c r="CP263" s="93"/>
+      <c r="CQ263" s="93"/>
+      <c r="CR263" s="93"/>
+      <c r="CS263" s="93"/>
+      <c r="CT263" s="93"/>
+      <c r="CU263" s="93"/>
+      <c r="CV263" s="93"/>
+      <c r="CW263" s="93"/>
+      <c r="CX263" s="93"/>
+      <c r="CY263" s="93"/>
+      <c r="CZ263" s="93"/>
+      <c r="DA263" s="93"/>
+      <c r="DB263" s="93"/>
+      <c r="DC263" s="93"/>
+      <c r="DD263" s="93"/>
+      <c r="DE263" s="93"/>
+      <c r="DF263" s="93"/>
+      <c r="DG263" s="93"/>
+      <c r="DH263" s="93"/>
+      <c r="DI263" s="93"/>
+      <c r="DJ263" s="93"/>
+      <c r="DK263" s="93"/>
+      <c r="DL263" s="93"/>
+      <c r="DM263" s="93"/>
+      <c r="DN263" s="93"/>
+      <c r="DO263" s="93"/>
+      <c r="DP263" s="93"/>
+      <c r="DQ263" s="93"/>
+      <c r="DR263" s="93"/>
+      <c r="DS263" s="93"/>
+      <c r="DT263" s="93"/>
+      <c r="DU263" s="93"/>
+      <c r="DV263" s="93"/>
+      <c r="DW263" s="93"/>
+      <c r="DX263" s="93"/>
+      <c r="DY263" s="93"/>
+      <c r="DZ263" s="93"/>
+      <c r="EA263" s="93"/>
+      <c r="EB263" s="93"/>
+      <c r="EC263" s="93"/>
+      <c r="ED263" s="93"/>
+      <c r="EE263" s="93"/>
+      <c r="EF263" s="93"/>
+      <c r="EG263" s="93"/>
+      <c r="EH263" s="93"/>
+      <c r="EI263" s="93"/>
+      <c r="EJ263" s="93"/>
+      <c r="EK263" s="93"/>
+      <c r="EL263" s="93"/>
+      <c r="EM263" s="93"/>
+      <c r="EN263" s="93"/>
+      <c r="EO263" s="93"/>
+      <c r="EP263" s="93"/>
+      <c r="EQ263" s="93"/>
+      <c r="ER263" s="93"/>
+      <c r="ES263" s="93"/>
+      <c r="ET263" s="93"/>
+      <c r="EU263" s="93"/>
+      <c r="EV263" s="93"/>
+      <c r="EW263" s="93"/>
+      <c r="EX263" s="93"/>
+      <c r="EY263" s="93"/>
+      <c r="EZ263" s="93"/>
+      <c r="FA263" s="93"/>
+      <c r="FB263" s="93"/>
+      <c r="FC263" s="93"/>
+      <c r="FD263" s="93"/>
+      <c r="FE263" s="93"/>
+      <c r="FF263" s="93"/>
+      <c r="FG263" s="93"/>
+      <c r="FH263" s="93"/>
+      <c r="FI263" s="93"/>
+      <c r="FJ263" s="93"/>
+      <c r="FK263" s="93"/>
+      <c r="FL263" s="93"/>
+      <c r="FM263" s="93"/>
+      <c r="FN263" s="93"/>
+      <c r="FO263" s="93"/>
+      <c r="FP263" s="93"/>
+      <c r="FQ263" s="93"/>
+      <c r="FR263" s="93"/>
+      <c r="FS263" s="93"/>
+      <c r="FT263" s="93"/>
+      <c r="FU263" s="93"/>
+      <c r="FV263" s="93"/>
+      <c r="FW263" s="93"/>
+      <c r="FX263" s="93"/>
+      <c r="FY263" s="93"/>
+      <c r="FZ263" s="93"/>
+      <c r="GA263" s="93"/>
+      <c r="GB263" s="93"/>
+      <c r="GC263" s="93"/>
+      <c r="GD263" s="93"/>
+      <c r="GE263" s="93"/>
+      <c r="GF263" s="93"/>
+      <c r="GG263" s="93"/>
+      <c r="GH263" s="93"/>
+      <c r="GI263" s="93"/>
+      <c r="GJ263" s="93"/>
+      <c r="GK263" s="93"/>
+      <c r="GL263" s="93"/>
+      <c r="GM263" s="93"/>
+      <c r="GN263" s="93"/>
+      <c r="GO263" s="93"/>
+      <c r="GP263" s="93"/>
+      <c r="GQ263" s="93"/>
+      <c r="GR263" s="93"/>
+      <c r="GS263" s="93"/>
+      <c r="GT263" s="93"/>
+      <c r="GU263" s="93"/>
+      <c r="GV263" s="93"/>
+      <c r="GW263" s="93"/>
+      <c r="GX263" s="93"/>
+      <c r="GY263" s="93"/>
+      <c r="GZ263" s="93"/>
+      <c r="HA263" s="93"/>
+      <c r="HB263" s="93"/>
+      <c r="HC263" s="93"/>
+      <c r="HD263" s="93"/>
+      <c r="HE263" s="93"/>
+      <c r="HF263" s="93"/>
+      <c r="HG263" s="93"/>
+      <c r="HH263" s="93"/>
+      <c r="HI263" s="93"/>
+      <c r="HJ263" s="93"/>
+      <c r="HK263" s="93"/>
+      <c r="HL263" s="93"/>
+      <c r="HM263" s="93"/>
+      <c r="HN263" s="93"/>
+      <c r="HO263" s="93"/>
+      <c r="HP263" s="93"/>
+      <c r="HQ263" s="93"/>
+      <c r="HR263" s="93"/>
+      <c r="HS263" s="93"/>
+      <c r="HT263" s="93"/>
+      <c r="HU263" s="93"/>
+      <c r="HV263" s="93"/>
+      <c r="HW263" s="93"/>
+      <c r="HX263" s="93"/>
+      <c r="HY263" s="93"/>
+      <c r="HZ263" s="93"/>
+      <c r="IA263" s="93"/>
+      <c r="IB263" s="93"/>
+      <c r="IC263" s="93"/>
+      <c r="ID263" s="93"/>
+      <c r="IE263" s="93"/>
+      <c r="IF263" s="93"/>
+      <c r="IG263" s="93"/>
+      <c r="IH263" s="93"/>
+      <c r="II263" s="93"/>
+      <c r="IJ263" s="93"/>
+      <c r="IK263" s="93"/>
+      <c r="IL263" s="93"/>
+      <c r="IM263" s="93"/>
+      <c r="IN263" s="93"/>
+      <c r="IO263" s="93"/>
+      <c r="IP263" s="93"/>
+      <c r="IQ263" s="93"/>
+      <c r="IR263" s="93"/>
+      <c r="IS263" s="93"/>
+      <c r="IT263" s="93"/>
+      <c r="IU263" s="93"/>
+      <c r="IV263" s="93"/>
+      <c r="IW263" s="93"/>
+      <c r="IX263" s="93"/>
+      <c r="IY263" s="93"/>
+      <c r="IZ263" s="93"/>
+      <c r="JA263" s="93"/>
+      <c r="JB263" s="93"/>
+      <c r="JC263" s="93"/>
+      <c r="JD263" s="93"/>
+      <c r="JE263" s="93"/>
+      <c r="JF263" s="93"/>
+      <c r="JG263" s="93"/>
+      <c r="JH263" s="93"/>
+      <c r="JI263" s="93"/>
+      <c r="JJ263" s="93"/>
+      <c r="JK263" s="93"/>
+      <c r="JL263" s="93"/>
+      <c r="JM263" s="93"/>
+      <c r="JN263" s="93"/>
+      <c r="JO263" s="93"/>
+      <c r="JP263" s="93"/>
+      <c r="JQ263" s="93"/>
+      <c r="JR263" s="93"/>
+      <c r="JS263" s="93"/>
+      <c r="JT263" s="93"/>
+      <c r="JU263" s="93"/>
+      <c r="JV263" s="93"/>
+      <c r="JW263" s="93"/>
+      <c r="JX263" s="93"/>
+      <c r="JY263" s="93"/>
+      <c r="JZ263" s="93"/>
+      <c r="KA263" s="93"/>
+      <c r="KB263" s="93"/>
+      <c r="KC263" s="93"/>
+      <c r="KD263" s="93"/>
+      <c r="KE263" s="93"/>
+      <c r="KF263" s="93"/>
+      <c r="KG263" s="93"/>
+      <c r="KH263" s="93"/>
+      <c r="KI263" s="93"/>
+      <c r="KJ263" s="93"/>
+      <c r="KK263" s="93"/>
+      <c r="KL263" s="93"/>
+      <c r="KM263" s="93"/>
+      <c r="KN263" s="93"/>
+      <c r="KO263" s="93"/>
+      <c r="KP263" s="93"/>
+    </row>
+    <row r="264" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A264" s="41"/>
+      <c r="B264" s="33">
+        <v>2</v>
+      </c>
+      <c r="C264" s="33">
+        <v>8</v>
+      </c>
+      <c r="D264" s="33">
+        <v>0</v>
+      </c>
+      <c r="E264" s="33">
+        <v>3</v>
+      </c>
+      <c r="F264" s="32"/>
+      <c r="I264" s="34"/>
+      <c r="J264" s="32"/>
+      <c r="M264" s="34"/>
+      <c r="Q264" s="32"/>
+      <c r="R264" s="34"/>
+      <c r="S264" s="67"/>
+      <c r="T264" s="67"/>
+      <c r="U264" s="67"/>
+      <c r="V264" s="67"/>
+      <c r="W264" s="67"/>
+      <c r="X264" s="67"/>
+      <c r="Y264" s="67"/>
+      <c r="Z264" s="67"/>
+      <c r="AA264" s="67"/>
+      <c r="AB264" s="67"/>
+      <c r="AC264" s="67"/>
+      <c r="AD264" s="67"/>
+      <c r="AE264" s="67"/>
+      <c r="AF264" s="67"/>
+      <c r="AG264" s="68"/>
+      <c r="AH264" s="33">
+        <v>0</v>
+      </c>
+      <c r="AI264" s="33">
+        <v>0</v>
+      </c>
+      <c r="AJ264" s="33">
+        <v>0</v>
+      </c>
+      <c r="AK264" s="33">
+        <v>3</v>
+      </c>
+      <c r="AR264" s="83"/>
+      <c r="AT264" s="84"/>
+      <c r="AU264" s="84"/>
+      <c r="AV264" s="84"/>
+      <c r="AW264" s="84"/>
+      <c r="AX264" s="84"/>
+      <c r="AY264" s="84"/>
+      <c r="AZ264" s="84"/>
+      <c r="BA264" s="84"/>
+      <c r="BB264" s="84"/>
+      <c r="BC264" s="84"/>
+      <c r="BD264" s="84"/>
+      <c r="BE264" s="84"/>
+      <c r="BF264" s="84"/>
+      <c r="BG264" s="84"/>
+      <c r="BH264" s="84"/>
+      <c r="BI264" s="84"/>
+      <c r="BJ264" s="84"/>
+      <c r="BK264" s="84"/>
+      <c r="BL264" s="84"/>
+      <c r="BM264" s="84"/>
+      <c r="BN264" s="84"/>
+      <c r="BO264" s="84"/>
+      <c r="BP264" s="84"/>
+      <c r="BQ264" s="84"/>
+      <c r="BR264" s="84"/>
+      <c r="BS264" s="84"/>
+      <c r="BT264" s="84"/>
+      <c r="BU264" s="84"/>
+      <c r="BV264" s="84"/>
+      <c r="BW264" s="84"/>
+      <c r="BX264" s="84"/>
+      <c r="BY264" s="84"/>
+      <c r="BZ264" s="84"/>
+      <c r="CA264" s="84"/>
+      <c r="CB264" s="84"/>
+      <c r="CC264" s="84"/>
+      <c r="CD264" s="84"/>
+      <c r="CE264" s="84"/>
+      <c r="CF264" s="84"/>
+      <c r="CG264" s="84"/>
+      <c r="CH264" s="84"/>
+      <c r="CI264" s="84"/>
+      <c r="CJ264" s="84"/>
+      <c r="CK264" s="84"/>
+      <c r="CL264" s="84"/>
+      <c r="CM264" s="84"/>
+      <c r="CN264" s="84"/>
+      <c r="CO264" s="84"/>
+      <c r="CP264" s="84"/>
+      <c r="CQ264" s="84"/>
+      <c r="CR264" s="84"/>
+      <c r="CS264" s="84"/>
+      <c r="CT264" s="84"/>
+      <c r="CU264" s="84"/>
+      <c r="CV264" s="84"/>
+      <c r="CW264" s="84"/>
+      <c r="CX264" s="84"/>
+      <c r="CY264" s="84"/>
+      <c r="CZ264" s="84"/>
+      <c r="DA264" s="84"/>
+      <c r="DB264" s="84"/>
+      <c r="DC264" s="84"/>
+      <c r="DD264" s="84"/>
+      <c r="DE264" s="84"/>
+      <c r="DF264" s="84"/>
+      <c r="DG264" s="84"/>
+      <c r="DH264" s="84"/>
+      <c r="DI264" s="84"/>
+      <c r="DJ264" s="84"/>
+      <c r="DK264" s="84"/>
+      <c r="DL264" s="84"/>
+      <c r="DM264" s="84"/>
+      <c r="DN264" s="84"/>
+      <c r="DO264" s="84"/>
+      <c r="DP264" s="84"/>
+      <c r="DQ264" s="84"/>
+      <c r="DR264" s="84"/>
+      <c r="DS264" s="84"/>
+      <c r="DT264" s="84"/>
+      <c r="DU264" s="84"/>
+      <c r="DV264" s="84"/>
+      <c r="DW264" s="84"/>
+      <c r="DX264" s="84"/>
+      <c r="DY264" s="84"/>
+      <c r="DZ264" s="84"/>
+      <c r="EA264" s="84"/>
+      <c r="EB264" s="84"/>
+      <c r="EC264" s="84"/>
+      <c r="ED264" s="84"/>
+      <c r="EE264" s="84"/>
+      <c r="EF264" s="84"/>
+      <c r="EG264" s="84"/>
+      <c r="EH264" s="84"/>
+      <c r="EI264" s="84"/>
+      <c r="EJ264" s="84"/>
+      <c r="EK264" s="84"/>
+      <c r="EL264" s="84"/>
+      <c r="EM264" s="84"/>
+      <c r="EN264" s="84"/>
+      <c r="EO264" s="84"/>
+      <c r="EP264" s="84"/>
+      <c r="EQ264" s="84"/>
+      <c r="ER264" s="84"/>
+      <c r="ES264" s="84"/>
+      <c r="ET264" s="84"/>
+      <c r="EU264" s="84"/>
+      <c r="EV264" s="84"/>
+      <c r="EW264" s="84"/>
+      <c r="EX264" s="84"/>
+      <c r="EY264" s="84"/>
+      <c r="EZ264" s="84"/>
+      <c r="FA264" s="84"/>
+      <c r="FB264" s="84"/>
+      <c r="FC264" s="84"/>
+      <c r="FD264" s="84"/>
+      <c r="FE264" s="84"/>
+      <c r="FF264" s="84"/>
+      <c r="FG264" s="84"/>
+      <c r="FH264" s="84"/>
+      <c r="FI264" s="84"/>
+      <c r="FJ264" s="84"/>
+      <c r="FK264" s="84"/>
+      <c r="FL264" s="84"/>
+      <c r="FM264" s="84"/>
+      <c r="FN264" s="84"/>
+      <c r="FO264" s="84"/>
+      <c r="FP264" s="84"/>
+      <c r="FQ264" s="84"/>
+      <c r="FR264" s="84"/>
+      <c r="FS264" s="84"/>
+      <c r="FT264" s="84"/>
+      <c r="FU264" s="84"/>
+      <c r="FV264" s="84"/>
+      <c r="FW264" s="84"/>
+      <c r="FX264" s="84"/>
+      <c r="FY264" s="84"/>
+      <c r="FZ264" s="84"/>
+      <c r="GA264" s="84"/>
+      <c r="GB264" s="84"/>
+      <c r="GC264" s="84"/>
+      <c r="GD264" s="84"/>
+      <c r="GE264" s="84"/>
+      <c r="GF264" s="84"/>
+      <c r="GG264" s="84"/>
+      <c r="GH264" s="84"/>
+      <c r="GI264" s="84"/>
+      <c r="GJ264" s="84"/>
+      <c r="GK264" s="84"/>
+      <c r="GL264" s="84"/>
+      <c r="GM264" s="84"/>
+      <c r="GN264" s="84"/>
+      <c r="GO264" s="84"/>
+      <c r="GP264" s="84"/>
+      <c r="GQ264" s="84"/>
+      <c r="GR264" s="84"/>
+      <c r="GS264" s="84"/>
+      <c r="GT264" s="84"/>
+      <c r="GU264" s="84"/>
+      <c r="GV264" s="84"/>
+      <c r="GW264" s="84"/>
+      <c r="GX264" s="84"/>
+      <c r="GY264" s="84"/>
+      <c r="GZ264" s="84"/>
+      <c r="HA264" s="84"/>
+      <c r="HB264" s="84"/>
+      <c r="HC264" s="84"/>
+      <c r="HD264" s="84"/>
+      <c r="HE264" s="84"/>
+      <c r="HF264" s="84"/>
+      <c r="HG264" s="84"/>
+      <c r="HH264" s="84"/>
+      <c r="HI264" s="84"/>
+      <c r="HJ264" s="84"/>
+      <c r="HK264" s="84"/>
+      <c r="HL264" s="84"/>
+      <c r="HM264" s="84"/>
+      <c r="HN264" s="84"/>
+      <c r="HO264" s="84"/>
+      <c r="HP264" s="84"/>
+      <c r="HQ264" s="84"/>
+      <c r="HR264" s="84"/>
+      <c r="HS264" s="84"/>
+      <c r="HT264" s="84"/>
+      <c r="HU264" s="84"/>
+      <c r="HV264" s="84"/>
+      <c r="HW264" s="84"/>
+      <c r="HX264" s="84"/>
+      <c r="HY264" s="84"/>
+      <c r="HZ264" s="84"/>
+      <c r="IA264" s="84"/>
+      <c r="IB264" s="84"/>
+      <c r="IC264" s="84"/>
+      <c r="ID264" s="84"/>
+      <c r="IE264" s="84"/>
+      <c r="IF264" s="84"/>
+      <c r="IG264" s="84"/>
+      <c r="IH264" s="84"/>
+      <c r="II264" s="84"/>
+      <c r="IJ264" s="84"/>
+      <c r="IK264" s="84"/>
+      <c r="IL264" s="84"/>
+      <c r="IM264" s="84"/>
+      <c r="IN264" s="84"/>
+      <c r="IO264" s="84"/>
+      <c r="IP264" s="84"/>
+      <c r="IQ264" s="84"/>
+      <c r="IR264" s="84"/>
+      <c r="IS264" s="84"/>
+      <c r="IT264" s="84"/>
+      <c r="IU264" s="84"/>
+      <c r="IV264" s="84"/>
+      <c r="IW264" s="84"/>
+      <c r="IX264" s="84"/>
+      <c r="IY264" s="84"/>
+      <c r="IZ264" s="84"/>
+      <c r="JA264" s="84"/>
+      <c r="JB264" s="84"/>
+      <c r="JC264" s="84"/>
+      <c r="JD264" s="84"/>
+      <c r="JE264" s="84"/>
+      <c r="JF264" s="84"/>
+      <c r="JG264" s="84"/>
+      <c r="JH264" s="84"/>
+      <c r="JI264" s="84"/>
+      <c r="JJ264" s="84"/>
+      <c r="JK264" s="84"/>
+      <c r="JL264" s="84"/>
+      <c r="JM264" s="84"/>
+      <c r="JN264" s="84"/>
+      <c r="JO264" s="84"/>
+      <c r="JP264" s="84"/>
+      <c r="JQ264" s="84"/>
+      <c r="JR264" s="84"/>
+      <c r="JS264" s="84"/>
+      <c r="JT264" s="84"/>
+      <c r="JU264" s="84"/>
+      <c r="JV264" s="84"/>
+      <c r="JW264" s="84"/>
+      <c r="JX264" s="84"/>
+      <c r="JY264" s="84"/>
+      <c r="JZ264" s="84"/>
+      <c r="KA264" s="84"/>
+      <c r="KB264" s="84"/>
+      <c r="KC264" s="84"/>
+      <c r="KD264" s="84"/>
+      <c r="KE264" s="84"/>
+      <c r="KF264" s="84"/>
+      <c r="KG264" s="84"/>
+      <c r="KH264" s="84"/>
+      <c r="KI264" s="84"/>
+      <c r="KJ264" s="84"/>
+      <c r="KK264" s="84"/>
+      <c r="KL264" s="84"/>
+      <c r="KM264" s="84"/>
+      <c r="KN264" s="84"/>
+      <c r="KO264" s="84"/>
+      <c r="KP264" s="84"/>
+    </row>
+    <row r="265" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A265" s="46">
+        <v>121</v>
+      </c>
+      <c r="B265" s="29">
+        <v>3</v>
+      </c>
+      <c r="C265" s="29">
+        <v>0</v>
+      </c>
+      <c r="D265" s="29">
+        <v>2</v>
+      </c>
+      <c r="E265" s="29">
+        <v>3</v>
+      </c>
+      <c r="F265" s="28"/>
+      <c r="I265" s="30"/>
+      <c r="J265" s="28"/>
+      <c r="M265" s="30"/>
+      <c r="N265" s="29">
+        <v>2</v>
+      </c>
+      <c r="O265" s="29">
+        <v>1</v>
+      </c>
+      <c r="P265" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q265" s="28">
+        <v>0</v>
+      </c>
+      <c r="R265" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S265" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="T265" s="65"/>
+      <c r="U265" s="65"/>
+      <c r="V265" s="65"/>
+      <c r="W265" s="65"/>
+      <c r="X265" s="65"/>
+      <c r="Y265" s="65"/>
+      <c r="Z265" s="65"/>
+      <c r="AA265" s="65"/>
+      <c r="AB265" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC265" s="65"/>
+      <c r="AD265" s="65"/>
+      <c r="AE265" s="65"/>
+      <c r="AF265" s="65"/>
+      <c r="AG265" s="91"/>
+      <c r="AH265" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI265" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ265" s="29">
+        <v>2</v>
+      </c>
+      <c r="AK265" s="29">
+        <v>3</v>
+      </c>
+      <c r="AP265" s="29">
+        <v>2</v>
+      </c>
+      <c r="AQ265" s="29">
+        <v>11</v>
+      </c>
+      <c r="AR265" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS265" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="AT265" s="93"/>
+      <c r="AU265" s="93"/>
+      <c r="AV265" s="93"/>
+      <c r="AW265" s="93"/>
+      <c r="AX265" s="93"/>
+      <c r="AY265" s="93"/>
+      <c r="AZ265" s="93"/>
+      <c r="BA265" s="93"/>
+      <c r="BB265" s="93"/>
+      <c r="BC265" s="93"/>
+      <c r="BD265" s="93"/>
+      <c r="BE265" s="93"/>
+      <c r="BF265" s="93"/>
+      <c r="BG265" s="93"/>
+      <c r="BH265" s="93"/>
+      <c r="BI265" s="93"/>
+      <c r="BJ265" s="93"/>
+      <c r="BK265" s="93"/>
+      <c r="BL265" s="93"/>
+      <c r="BM265" s="93"/>
+      <c r="BN265" s="93"/>
+      <c r="BO265" s="93"/>
+      <c r="BP265" s="93"/>
+      <c r="BQ265" s="93"/>
+      <c r="BR265" s="93"/>
+      <c r="BS265" s="93"/>
+      <c r="BT265" s="93"/>
+      <c r="BU265" s="93"/>
+      <c r="BV265" s="93"/>
+      <c r="BW265" s="93"/>
+      <c r="BX265" s="93"/>
+      <c r="BY265" s="93"/>
+      <c r="BZ265" s="93"/>
+      <c r="CA265" s="93"/>
+      <c r="CB265" s="93"/>
+      <c r="CC265" s="93"/>
+      <c r="CD265" s="93"/>
+      <c r="CE265" s="93"/>
+      <c r="CF265" s="93"/>
+      <c r="CG265" s="93"/>
+      <c r="CH265" s="93"/>
+      <c r="CI265" s="93"/>
+      <c r="CJ265" s="93"/>
+      <c r="CK265" s="93"/>
+      <c r="CL265" s="93"/>
+      <c r="CM265" s="93"/>
+      <c r="CN265" s="93"/>
+      <c r="CO265" s="93"/>
+      <c r="CP265" s="93"/>
+      <c r="CQ265" s="93"/>
+      <c r="CR265" s="93"/>
+      <c r="CS265" s="93"/>
+      <c r="CT265" s="93"/>
+      <c r="CU265" s="93"/>
+      <c r="CV265" s="93"/>
+      <c r="CW265" s="93"/>
+      <c r="CX265" s="93"/>
+      <c r="CY265" s="93"/>
+      <c r="CZ265" s="93"/>
+      <c r="DA265" s="93"/>
+      <c r="DB265" s="93"/>
+      <c r="DC265" s="93"/>
+      <c r="DD265" s="93"/>
+      <c r="DE265" s="93"/>
+      <c r="DF265" s="93"/>
+      <c r="DG265" s="93"/>
+      <c r="DH265" s="93"/>
+      <c r="DI265" s="93"/>
+      <c r="DJ265" s="93"/>
+      <c r="DK265" s="93"/>
+      <c r="DL265" s="93"/>
+      <c r="DM265" s="93"/>
+      <c r="DN265" s="93"/>
+      <c r="DO265" s="93"/>
+      <c r="DP265" s="93"/>
+      <c r="DQ265" s="93"/>
+      <c r="DR265" s="93"/>
+      <c r="DS265" s="93"/>
+      <c r="DT265" s="93"/>
+      <c r="DU265" s="93"/>
+      <c r="DV265" s="93"/>
+      <c r="DW265" s="93"/>
+      <c r="DX265" s="93"/>
+      <c r="DY265" s="93"/>
+      <c r="DZ265" s="93"/>
+      <c r="EA265" s="93"/>
+      <c r="EB265" s="93"/>
+      <c r="EC265" s="93"/>
+      <c r="ED265" s="93"/>
+      <c r="EE265" s="93"/>
+      <c r="EF265" s="93"/>
+      <c r="EG265" s="93"/>
+      <c r="EH265" s="93"/>
+      <c r="EI265" s="93"/>
+      <c r="EJ265" s="93"/>
+      <c r="EK265" s="93"/>
+      <c r="EL265" s="93"/>
+      <c r="EM265" s="93"/>
+      <c r="EN265" s="93"/>
+      <c r="EO265" s="93"/>
+      <c r="EP265" s="93"/>
+      <c r="EQ265" s="93"/>
+      <c r="ER265" s="93"/>
+      <c r="ES265" s="93"/>
+      <c r="ET265" s="93"/>
+      <c r="EU265" s="93"/>
+      <c r="EV265" s="93"/>
+      <c r="EW265" s="93"/>
+      <c r="EX265" s="93"/>
+      <c r="EY265" s="93"/>
+      <c r="EZ265" s="93"/>
+      <c r="FA265" s="93"/>
+      <c r="FB265" s="93"/>
+      <c r="FC265" s="93"/>
+      <c r="FD265" s="93"/>
+      <c r="FE265" s="93"/>
+      <c r="FF265" s="93"/>
+      <c r="FG265" s="93"/>
+      <c r="FH265" s="93"/>
+      <c r="FI265" s="93"/>
+      <c r="FJ265" s="93"/>
+      <c r="FK265" s="93"/>
+      <c r="FL265" s="93"/>
+      <c r="FM265" s="93"/>
+      <c r="FN265" s="93"/>
+      <c r="FO265" s="93"/>
+      <c r="FP265" s="93"/>
+      <c r="FQ265" s="93"/>
+      <c r="FR265" s="93"/>
+      <c r="FS265" s="93"/>
+      <c r="FT265" s="93"/>
+      <c r="FU265" s="93"/>
+      <c r="FV265" s="93"/>
+      <c r="FW265" s="93"/>
+      <c r="FX265" s="93"/>
+      <c r="FY265" s="93"/>
+      <c r="FZ265" s="93"/>
+      <c r="GA265" s="93"/>
+      <c r="GB265" s="93"/>
+      <c r="GC265" s="93"/>
+      <c r="GD265" s="93"/>
+      <c r="GE265" s="93"/>
+      <c r="GF265" s="93"/>
+      <c r="GG265" s="93"/>
+      <c r="GH265" s="93"/>
+      <c r="GI265" s="93"/>
+      <c r="GJ265" s="93"/>
+      <c r="GK265" s="93"/>
+      <c r="GL265" s="93"/>
+      <c r="GM265" s="93"/>
+      <c r="GN265" s="93"/>
+      <c r="GO265" s="93"/>
+      <c r="GP265" s="93"/>
+      <c r="GQ265" s="93"/>
+      <c r="GR265" s="93"/>
+      <c r="GS265" s="93"/>
+      <c r="GT265" s="93"/>
+      <c r="GU265" s="93"/>
+      <c r="GV265" s="93"/>
+      <c r="GW265" s="93"/>
+      <c r="GX265" s="93"/>
+      <c r="GY265" s="93"/>
+      <c r="GZ265" s="93"/>
+      <c r="HA265" s="93"/>
+      <c r="HB265" s="93"/>
+      <c r="HC265" s="93"/>
+      <c r="HD265" s="93"/>
+      <c r="HE265" s="93"/>
+      <c r="HF265" s="93"/>
+      <c r="HG265" s="93"/>
+      <c r="HH265" s="93"/>
+      <c r="HI265" s="93"/>
+      <c r="HJ265" s="93"/>
+      <c r="HK265" s="93"/>
+      <c r="HL265" s="93"/>
+      <c r="HM265" s="93"/>
+      <c r="HN265" s="93"/>
+      <c r="HO265" s="93"/>
+      <c r="HP265" s="93"/>
+      <c r="HQ265" s="93"/>
+      <c r="HR265" s="93"/>
+      <c r="HS265" s="93"/>
+      <c r="HT265" s="93"/>
+      <c r="HU265" s="93"/>
+      <c r="HV265" s="93"/>
+      <c r="HW265" s="93"/>
+      <c r="HX265" s="93"/>
+      <c r="HY265" s="93"/>
+      <c r="HZ265" s="93"/>
+      <c r="IA265" s="93"/>
+      <c r="IB265" s="93"/>
+      <c r="IC265" s="93"/>
+      <c r="ID265" s="93"/>
+      <c r="IE265" s="93"/>
+      <c r="IF265" s="93"/>
+      <c r="IG265" s="93"/>
+      <c r="IH265" s="93"/>
+      <c r="II265" s="93"/>
+      <c r="IJ265" s="93"/>
+      <c r="IK265" s="93"/>
+      <c r="IL265" s="93"/>
+      <c r="IM265" s="93"/>
+      <c r="IN265" s="93"/>
+      <c r="IO265" s="93"/>
+      <c r="IP265" s="93"/>
+      <c r="IQ265" s="93"/>
+      <c r="IR265" s="93"/>
+      <c r="IS265" s="93"/>
+      <c r="IT265" s="93"/>
+      <c r="IU265" s="93"/>
+      <c r="IV265" s="93"/>
+      <c r="IW265" s="93"/>
+      <c r="IX265" s="93"/>
+      <c r="IY265" s="93"/>
+      <c r="IZ265" s="93"/>
+      <c r="JA265" s="93"/>
+      <c r="JB265" s="93"/>
+      <c r="JC265" s="93"/>
+      <c r="JD265" s="93"/>
+      <c r="JE265" s="93"/>
+      <c r="JF265" s="93"/>
+      <c r="JG265" s="93"/>
+      <c r="JH265" s="93"/>
+      <c r="JI265" s="93"/>
+      <c r="JJ265" s="93"/>
+      <c r="JK265" s="93"/>
+      <c r="JL265" s="93"/>
+      <c r="JM265" s="93"/>
+      <c r="JN265" s="93"/>
+      <c r="JO265" s="93"/>
+      <c r="JP265" s="93"/>
+      <c r="JQ265" s="93"/>
+      <c r="JR265" s="93"/>
+      <c r="JS265" s="93"/>
+      <c r="JT265" s="93"/>
+      <c r="JU265" s="93"/>
+      <c r="JV265" s="93"/>
+      <c r="JW265" s="93"/>
+      <c r="JX265" s="93"/>
+      <c r="JY265" s="93"/>
+      <c r="JZ265" s="93"/>
+      <c r="KA265" s="93"/>
+      <c r="KB265" s="93"/>
+      <c r="KC265" s="93"/>
+      <c r="KD265" s="93"/>
+      <c r="KE265" s="93"/>
+      <c r="KF265" s="93"/>
+      <c r="KG265" s="93"/>
+      <c r="KH265" s="93"/>
+      <c r="KI265" s="93"/>
+      <c r="KJ265" s="93"/>
+      <c r="KK265" s="93"/>
+      <c r="KL265" s="93"/>
+      <c r="KM265" s="93"/>
+      <c r="KN265" s="93"/>
+      <c r="KO265" s="93"/>
+      <c r="KP265" s="93"/>
+    </row>
+    <row r="266" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="41"/>
+      <c r="B266" s="85">
+        <v>2</v>
+      </c>
+      <c r="C266" s="33">
+        <v>8</v>
+      </c>
+      <c r="D266" s="33">
+        <v>0</v>
+      </c>
+      <c r="E266" s="33">
+        <v>3</v>
+      </c>
+      <c r="F266" s="32"/>
+      <c r="I266" s="34"/>
+      <c r="J266" s="32"/>
+      <c r="M266" s="34"/>
+      <c r="Q266" s="32"/>
+      <c r="R266" s="34"/>
+      <c r="S266" s="67"/>
+      <c r="T266" s="67"/>
+      <c r="U266" s="67"/>
+      <c r="V266" s="67"/>
+      <c r="W266" s="67"/>
+      <c r="X266" s="67"/>
+      <c r="Y266" s="67"/>
+      <c r="Z266" s="67"/>
+      <c r="AA266" s="67"/>
+      <c r="AB266" s="67"/>
+      <c r="AC266" s="67"/>
+      <c r="AD266" s="67"/>
+      <c r="AE266" s="67"/>
+      <c r="AF266" s="67"/>
+      <c r="AG266" s="68"/>
+      <c r="AH266" s="33">
+        <v>0</v>
+      </c>
+      <c r="AI266" s="33">
+        <v>0</v>
+      </c>
+      <c r="AJ266" s="33">
+        <v>0</v>
+      </c>
+      <c r="AK266" s="33">
+        <v>3</v>
+      </c>
+      <c r="AR266" s="83"/>
+      <c r="AT266" s="84"/>
+      <c r="AU266" s="84"/>
+      <c r="AV266" s="84"/>
+      <c r="AW266" s="84"/>
+      <c r="AX266" s="84"/>
+      <c r="AY266" s="84"/>
+      <c r="AZ266" s="84"/>
+      <c r="BA266" s="84"/>
+      <c r="BB266" s="84"/>
+      <c r="BC266" s="84"/>
+      <c r="BD266" s="84"/>
+      <c r="BE266" s="84"/>
+      <c r="BF266" s="84"/>
+      <c r="BG266" s="84"/>
+      <c r="BH266" s="84"/>
+      <c r="BI266" s="84"/>
+      <c r="BJ266" s="84"/>
+      <c r="BK266" s="84"/>
+      <c r="BL266" s="84"/>
+      <c r="BM266" s="84"/>
+      <c r="BN266" s="84"/>
+      <c r="BO266" s="84"/>
+      <c r="BP266" s="84"/>
+      <c r="BQ266" s="84"/>
+      <c r="BR266" s="84"/>
+      <c r="BS266" s="84"/>
+      <c r="BT266" s="84"/>
+      <c r="BU266" s="84"/>
+      <c r="BV266" s="84"/>
+      <c r="BW266" s="84"/>
+      <c r="BX266" s="84"/>
+      <c r="BY266" s="84"/>
+      <c r="BZ266" s="84"/>
+      <c r="CA266" s="84"/>
+      <c r="CB266" s="84"/>
+      <c r="CC266" s="84"/>
+      <c r="CD266" s="84"/>
+      <c r="CE266" s="84"/>
+      <c r="CF266" s="84"/>
+      <c r="CG266" s="84"/>
+      <c r="CH266" s="84"/>
+      <c r="CI266" s="84"/>
+      <c r="CJ266" s="84"/>
+      <c r="CK266" s="84"/>
+      <c r="CL266" s="84"/>
+      <c r="CM266" s="84"/>
+      <c r="CN266" s="84"/>
+      <c r="CO266" s="84"/>
+      <c r="CP266" s="84"/>
+      <c r="CQ266" s="84"/>
+      <c r="CR266" s="84"/>
+      <c r="CS266" s="84"/>
+      <c r="CT266" s="84"/>
+      <c r="CU266" s="84"/>
+      <c r="CV266" s="84"/>
+      <c r="CW266" s="84"/>
+      <c r="CX266" s="84"/>
+      <c r="CY266" s="84"/>
+      <c r="CZ266" s="84"/>
+      <c r="DA266" s="84"/>
+      <c r="DB266" s="84"/>
+      <c r="DC266" s="84"/>
+      <c r="DD266" s="84"/>
+      <c r="DE266" s="84"/>
+      <c r="DF266" s="84"/>
+      <c r="DG266" s="84"/>
+      <c r="DH266" s="84"/>
+      <c r="DI266" s="84"/>
+      <c r="DJ266" s="84"/>
+      <c r="DK266" s="84"/>
+      <c r="DL266" s="84"/>
+      <c r="DM266" s="84"/>
+      <c r="DN266" s="84"/>
+      <c r="DO266" s="84"/>
+      <c r="DP266" s="84"/>
+      <c r="DQ266" s="84"/>
+      <c r="DR266" s="84"/>
+      <c r="DS266" s="84"/>
+      <c r="DT266" s="84"/>
+      <c r="DU266" s="84"/>
+      <c r="DV266" s="84"/>
+      <c r="DW266" s="84"/>
+      <c r="DX266" s="84"/>
+      <c r="DY266" s="84"/>
+      <c r="DZ266" s="84"/>
+      <c r="EA266" s="84"/>
+      <c r="EB266" s="84"/>
+      <c r="EC266" s="84"/>
+      <c r="ED266" s="84"/>
+      <c r="EE266" s="84"/>
+      <c r="EF266" s="84"/>
+      <c r="EG266" s="84"/>
+      <c r="EH266" s="84"/>
+      <c r="EI266" s="84"/>
+      <c r="EJ266" s="84"/>
+      <c r="EK266" s="84"/>
+      <c r="EL266" s="84"/>
+      <c r="EM266" s="84"/>
+      <c r="EN266" s="84"/>
+      <c r="EO266" s="84"/>
+      <c r="EP266" s="84"/>
+      <c r="EQ266" s="84"/>
+      <c r="ER266" s="84"/>
+      <c r="ES266" s="84"/>
+      <c r="ET266" s="84"/>
+      <c r="EU266" s="84"/>
+      <c r="EV266" s="84"/>
+      <c r="EW266" s="84"/>
+      <c r="EX266" s="84"/>
+      <c r="EY266" s="84"/>
+      <c r="EZ266" s="84"/>
+      <c r="FA266" s="84"/>
+      <c r="FB266" s="84"/>
+      <c r="FC266" s="84"/>
+      <c r="FD266" s="84"/>
+      <c r="FE266" s="84"/>
+      <c r="FF266" s="84"/>
+      <c r="FG266" s="84"/>
+      <c r="FH266" s="84"/>
+      <c r="FI266" s="84"/>
+      <c r="FJ266" s="84"/>
+      <c r="FK266" s="84"/>
+      <c r="FL266" s="84"/>
+      <c r="FM266" s="84"/>
+      <c r="FN266" s="84"/>
+      <c r="FO266" s="84"/>
+      <c r="FP266" s="84"/>
+      <c r="FQ266" s="84"/>
+      <c r="FR266" s="84"/>
+      <c r="FS266" s="84"/>
+      <c r="FT266" s="84"/>
+      <c r="FU266" s="84"/>
+      <c r="FV266" s="84"/>
+      <c r="FW266" s="84"/>
+      <c r="FX266" s="84"/>
+      <c r="FY266" s="84"/>
+      <c r="FZ266" s="84"/>
+      <c r="GA266" s="84"/>
+      <c r="GB266" s="84"/>
+      <c r="GC266" s="84"/>
+      <c r="GD266" s="84"/>
+      <c r="GE266" s="84"/>
+      <c r="GF266" s="84"/>
+      <c r="GG266" s="84"/>
+      <c r="GH266" s="84"/>
+      <c r="GI266" s="84"/>
+      <c r="GJ266" s="84"/>
+      <c r="GK266" s="84"/>
+      <c r="GL266" s="84"/>
+      <c r="GM266" s="84"/>
+      <c r="GN266" s="84"/>
+      <c r="GO266" s="84"/>
+      <c r="GP266" s="84"/>
+      <c r="GQ266" s="84"/>
+      <c r="GR266" s="84"/>
+      <c r="GS266" s="84"/>
+      <c r="GT266" s="84"/>
+      <c r="GU266" s="84"/>
+      <c r="GV266" s="84"/>
+      <c r="GW266" s="84"/>
+      <c r="GX266" s="84"/>
+      <c r="GY266" s="84"/>
+      <c r="GZ266" s="84"/>
+      <c r="HA266" s="84"/>
+      <c r="HB266" s="84"/>
+      <c r="HC266" s="84"/>
+      <c r="HD266" s="84"/>
+      <c r="HE266" s="84"/>
+      <c r="HF266" s="84"/>
+      <c r="HG266" s="84"/>
+      <c r="HH266" s="84"/>
+      <c r="HI266" s="84"/>
+      <c r="HJ266" s="84"/>
+      <c r="HK266" s="84"/>
+      <c r="HL266" s="84"/>
+      <c r="HM266" s="84"/>
+      <c r="HN266" s="84"/>
+      <c r="HO266" s="84"/>
+      <c r="HP266" s="84"/>
+      <c r="HQ266" s="84"/>
+      <c r="HR266" s="84"/>
+      <c r="HS266" s="84"/>
+      <c r="HT266" s="84"/>
+      <c r="HU266" s="84"/>
+      <c r="HV266" s="84"/>
+      <c r="HW266" s="84"/>
+      <c r="HX266" s="84"/>
+      <c r="HY266" s="84"/>
+      <c r="HZ266" s="84"/>
+      <c r="IA266" s="84"/>
+      <c r="IB266" s="84"/>
+      <c r="IC266" s="84"/>
+      <c r="ID266" s="84"/>
+      <c r="IE266" s="84"/>
+      <c r="IF266" s="84"/>
+      <c r="IG266" s="84"/>
+      <c r="IH266" s="84"/>
+      <c r="II266" s="84"/>
+      <c r="IJ266" s="84"/>
+      <c r="IK266" s="84"/>
+      <c r="IL266" s="84"/>
+      <c r="IM266" s="84"/>
+      <c r="IN266" s="84"/>
+      <c r="IO266" s="84"/>
+      <c r="IP266" s="84"/>
+      <c r="IQ266" s="84"/>
+      <c r="IR266" s="84"/>
+      <c r="IS266" s="84"/>
+      <c r="IT266" s="84"/>
+      <c r="IU266" s="84"/>
+      <c r="IV266" s="84"/>
+      <c r="IW266" s="84"/>
+      <c r="IX266" s="84"/>
+      <c r="IY266" s="84"/>
+      <c r="IZ266" s="84"/>
+      <c r="JA266" s="84"/>
+      <c r="JB266" s="84"/>
+      <c r="JC266" s="84"/>
+      <c r="JD266" s="84"/>
+      <c r="JE266" s="84"/>
+      <c r="JF266" s="84"/>
+      <c r="JG266" s="84"/>
+      <c r="JH266" s="84"/>
+      <c r="JI266" s="84"/>
+      <c r="JJ266" s="84"/>
+      <c r="JK266" s="84"/>
+      <c r="JL266" s="84"/>
+      <c r="JM266" s="84"/>
+      <c r="JN266" s="84"/>
+      <c r="JO266" s="84"/>
+      <c r="JP266" s="84"/>
+      <c r="JQ266" s="84"/>
+      <c r="JR266" s="84"/>
+      <c r="JS266" s="84"/>
+      <c r="JT266" s="84"/>
+      <c r="JU266" s="84"/>
+      <c r="JV266" s="84"/>
+      <c r="JW266" s="84"/>
+      <c r="JX266" s="84"/>
+      <c r="JY266" s="84"/>
+      <c r="JZ266" s="84"/>
+      <c r="KA266" s="84"/>
+      <c r="KB266" s="84"/>
+      <c r="KC266" s="84"/>
+      <c r="KD266" s="84"/>
+      <c r="KE266" s="84"/>
+      <c r="KF266" s="84"/>
+      <c r="KG266" s="84"/>
+      <c r="KH266" s="84"/>
+      <c r="KI266" s="84"/>
+      <c r="KJ266" s="84"/>
+      <c r="KK266" s="84"/>
+      <c r="KL266" s="84"/>
+      <c r="KM266" s="84"/>
+      <c r="KN266" s="84"/>
+      <c r="KO266" s="84"/>
+      <c r="KP266" s="84"/>
+    </row>
+    <row r="267" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A267" s="46">
+        <v>122</v>
+      </c>
+      <c r="B267" s="29">
+        <v>3</v>
+      </c>
+      <c r="C267" s="29">
+        <v>0</v>
+      </c>
+      <c r="D267" s="87">
+        <v>2</v>
+      </c>
+      <c r="E267" s="29">
+        <v>3</v>
+      </c>
+      <c r="F267" s="28"/>
+      <c r="I267" s="30"/>
+      <c r="J267" s="28"/>
+      <c r="M267" s="30"/>
+      <c r="N267" s="29">
+        <v>2</v>
+      </c>
+      <c r="O267" s="29">
+        <v>1</v>
+      </c>
+      <c r="P267" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q267" s="28">
+        <v>5</v>
+      </c>
+      <c r="R267" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S267" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="T267" s="65"/>
+      <c r="U267" s="65"/>
+      <c r="V267" s="65"/>
+      <c r="W267" s="65"/>
+      <c r="X267" s="65"/>
+      <c r="Y267" s="65"/>
+      <c r="Z267" s="65"/>
+      <c r="AA267" s="65"/>
+      <c r="AB267" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC267" s="65"/>
+      <c r="AD267" s="65"/>
+      <c r="AE267" s="65"/>
+      <c r="AF267" s="65"/>
+      <c r="AG267" s="91"/>
+      <c r="AH267" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI267" s="29">
+        <v>0</v>
+      </c>
+      <c r="AJ267" s="29">
+        <v>2</v>
+      </c>
+      <c r="AK267" s="29">
+        <v>3</v>
+      </c>
+      <c r="AP267" s="29">
+        <v>2</v>
+      </c>
+      <c r="AQ267" s="29">
+        <v>1</v>
+      </c>
+      <c r="AR267" s="92" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS267" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="AT267" s="93"/>
+      <c r="AU267" s="93"/>
+      <c r="AV267" s="93"/>
+      <c r="AW267" s="93"/>
+      <c r="AX267" s="93"/>
+      <c r="AY267" s="93"/>
+      <c r="AZ267" s="93"/>
+      <c r="BA267" s="93"/>
+      <c r="BB267" s="93"/>
+      <c r="BC267" s="93"/>
+      <c r="BD267" s="93"/>
+      <c r="BE267" s="93"/>
+      <c r="BF267" s="93"/>
+      <c r="BG267" s="93"/>
+      <c r="BH267" s="93"/>
+      <c r="BI267" s="93"/>
+      <c r="BJ267" s="93"/>
+      <c r="BK267" s="93"/>
+      <c r="BL267" s="93"/>
+      <c r="BM267" s="93"/>
+      <c r="BN267" s="93"/>
+      <c r="BO267" s="93"/>
+      <c r="BP267" s="93"/>
+      <c r="BQ267" s="93"/>
+      <c r="BR267" s="93"/>
+      <c r="BS267" s="93"/>
+      <c r="BT267" s="93"/>
+      <c r="BU267" s="93"/>
+      <c r="BV267" s="93"/>
+      <c r="BW267" s="93"/>
+      <c r="BX267" s="93"/>
+      <c r="BY267" s="93"/>
+      <c r="BZ267" s="93"/>
+      <c r="CA267" s="93"/>
+      <c r="CB267" s="93"/>
+      <c r="CC267" s="93"/>
+      <c r="CD267" s="93"/>
+      <c r="CE267" s="93"/>
+      <c r="CF267" s="93"/>
+      <c r="CG267" s="93"/>
+      <c r="CH267" s="93"/>
+      <c r="CI267" s="93"/>
+      <c r="CJ267" s="93"/>
+      <c r="CK267" s="93"/>
+      <c r="CL267" s="93"/>
+      <c r="CM267" s="93"/>
+      <c r="CN267" s="93"/>
+      <c r="CO267" s="93"/>
+      <c r="CP267" s="93"/>
+      <c r="CQ267" s="93"/>
+      <c r="CR267" s="93"/>
+      <c r="CS267" s="93"/>
+      <c r="CT267" s="93"/>
+      <c r="CU267" s="93"/>
+      <c r="CV267" s="93"/>
+      <c r="CW267" s="93"/>
+      <c r="CX267" s="93"/>
+      <c r="CY267" s="93"/>
+      <c r="CZ267" s="93"/>
+      <c r="DA267" s="93"/>
+      <c r="DB267" s="93"/>
+      <c r="DC267" s="93"/>
+      <c r="DD267" s="93"/>
+      <c r="DE267" s="93"/>
+      <c r="DF267" s="93"/>
+      <c r="DG267" s="93"/>
+      <c r="DH267" s="93"/>
+      <c r="DI267" s="93"/>
+      <c r="DJ267" s="93"/>
+      <c r="DK267" s="93"/>
+      <c r="DL267" s="93"/>
+      <c r="DM267" s="93"/>
+      <c r="DN267" s="93"/>
+      <c r="DO267" s="93"/>
+      <c r="DP267" s="93"/>
+      <c r="DQ267" s="93"/>
+      <c r="DR267" s="93"/>
+      <c r="DS267" s="93"/>
+      <c r="DT267" s="93"/>
+      <c r="DU267" s="93"/>
+      <c r="DV267" s="93"/>
+      <c r="DW267" s="93"/>
+      <c r="DX267" s="93"/>
+      <c r="DY267" s="93"/>
+      <c r="DZ267" s="93"/>
+      <c r="EA267" s="93"/>
+      <c r="EB267" s="93"/>
+      <c r="EC267" s="93"/>
+      <c r="ED267" s="93"/>
+      <c r="EE267" s="93"/>
+      <c r="EF267" s="93"/>
+      <c r="EG267" s="93"/>
+      <c r="EH267" s="93"/>
+      <c r="EI267" s="93"/>
+      <c r="EJ267" s="93"/>
+      <c r="EK267" s="93"/>
+      <c r="EL267" s="93"/>
+      <c r="EM267" s="93"/>
+      <c r="EN267" s="93"/>
+      <c r="EO267" s="93"/>
+      <c r="EP267" s="93"/>
+      <c r="EQ267" s="93"/>
+      <c r="ER267" s="93"/>
+      <c r="ES267" s="93"/>
+      <c r="ET267" s="93"/>
+      <c r="EU267" s="93"/>
+      <c r="EV267" s="93"/>
+      <c r="EW267" s="93"/>
+      <c r="EX267" s="93"/>
+      <c r="EY267" s="93"/>
+      <c r="EZ267" s="93"/>
+      <c r="FA267" s="93"/>
+      <c r="FB267" s="93"/>
+      <c r="FC267" s="93"/>
+      <c r="FD267" s="93"/>
+      <c r="FE267" s="93"/>
+      <c r="FF267" s="93"/>
+      <c r="FG267" s="93"/>
+      <c r="FH267" s="93"/>
+      <c r="FI267" s="93"/>
+      <c r="FJ267" s="93"/>
+      <c r="FK267" s="93"/>
+      <c r="FL267" s="93"/>
+      <c r="FM267" s="93"/>
+      <c r="FN267" s="93"/>
+      <c r="FO267" s="93"/>
+      <c r="FP267" s="93"/>
+      <c r="FQ267" s="93"/>
+      <c r="FR267" s="93"/>
+      <c r="FS267" s="93"/>
+      <c r="FT267" s="93"/>
+      <c r="FU267" s="93"/>
+      <c r="FV267" s="93"/>
+      <c r="FW267" s="93"/>
+      <c r="FX267" s="93"/>
+      <c r="FY267" s="93"/>
+      <c r="FZ267" s="93"/>
+      <c r="GA267" s="93"/>
+      <c r="GB267" s="93"/>
+      <c r="GC267" s="93"/>
+      <c r="GD267" s="93"/>
+      <c r="GE267" s="93"/>
+      <c r="GF267" s="93"/>
+      <c r="GG267" s="93"/>
+      <c r="GH267" s="93"/>
+      <c r="GI267" s="93"/>
+      <c r="GJ267" s="93"/>
+      <c r="GK267" s="93"/>
+      <c r="GL267" s="93"/>
+      <c r="GM267" s="93"/>
+      <c r="GN267" s="93"/>
+      <c r="GO267" s="93"/>
+      <c r="GP267" s="93"/>
+      <c r="GQ267" s="93"/>
+      <c r="GR267" s="93"/>
+      <c r="GS267" s="93"/>
+      <c r="GT267" s="93"/>
+      <c r="GU267" s="93"/>
+      <c r="GV267" s="93"/>
+      <c r="GW267" s="93"/>
+      <c r="GX267" s="93"/>
+      <c r="GY267" s="93"/>
+      <c r="GZ267" s="93"/>
+      <c r="HA267" s="93"/>
+      <c r="HB267" s="93"/>
+      <c r="HC267" s="93"/>
+      <c r="HD267" s="93"/>
+      <c r="HE267" s="93"/>
+      <c r="HF267" s="93"/>
+      <c r="HG267" s="93"/>
+      <c r="HH267" s="93"/>
+      <c r="HI267" s="93"/>
+      <c r="HJ267" s="93"/>
+      <c r="HK267" s="93"/>
+      <c r="HL267" s="93"/>
+      <c r="HM267" s="93"/>
+      <c r="HN267" s="93"/>
+      <c r="HO267" s="93"/>
+      <c r="HP267" s="93"/>
+      <c r="HQ267" s="93"/>
+      <c r="HR267" s="93"/>
+      <c r="HS267" s="93"/>
+      <c r="HT267" s="93"/>
+      <c r="HU267" s="93"/>
+      <c r="HV267" s="93"/>
+      <c r="HW267" s="93"/>
+      <c r="HX267" s="93"/>
+      <c r="HY267" s="93"/>
+      <c r="HZ267" s="93"/>
+      <c r="IA267" s="93"/>
+      <c r="IB267" s="93"/>
+      <c r="IC267" s="93"/>
+      <c r="ID267" s="93"/>
+      <c r="IE267" s="93"/>
+      <c r="IF267" s="93"/>
+      <c r="IG267" s="93"/>
+      <c r="IH267" s="93"/>
+      <c r="II267" s="93"/>
+      <c r="IJ267" s="93"/>
+      <c r="IK267" s="93"/>
+      <c r="IL267" s="93"/>
+      <c r="IM267" s="93"/>
+      <c r="IN267" s="93"/>
+      <c r="IO267" s="93"/>
+      <c r="IP267" s="93"/>
+      <c r="IQ267" s="93"/>
+      <c r="IR267" s="93"/>
+      <c r="IS267" s="93"/>
+      <c r="IT267" s="93"/>
+      <c r="IU267" s="93"/>
+      <c r="IV267" s="93"/>
+      <c r="IW267" s="93"/>
+      <c r="IX267" s="93"/>
+      <c r="IY267" s="93"/>
+      <c r="IZ267" s="93"/>
+      <c r="JA267" s="93"/>
+      <c r="JB267" s="93"/>
+      <c r="JC267" s="93"/>
+      <c r="JD267" s="93"/>
+      <c r="JE267" s="93"/>
+      <c r="JF267" s="93"/>
+      <c r="JG267" s="93"/>
+      <c r="JH267" s="93"/>
+      <c r="JI267" s="93"/>
+      <c r="JJ267" s="93"/>
+      <c r="JK267" s="93"/>
+      <c r="JL267" s="93"/>
+      <c r="JM267" s="93"/>
+      <c r="JN267" s="93"/>
+      <c r="JO267" s="93"/>
+      <c r="JP267" s="93"/>
+      <c r="JQ267" s="93"/>
+      <c r="JR267" s="93"/>
+      <c r="JS267" s="93"/>
+      <c r="JT267" s="93"/>
+      <c r="JU267" s="93"/>
+      <c r="JV267" s="93"/>
+      <c r="JW267" s="93"/>
+      <c r="JX267" s="93"/>
+      <c r="JY267" s="93"/>
+      <c r="JZ267" s="93"/>
+      <c r="KA267" s="93"/>
+      <c r="KB267" s="93"/>
+      <c r="KC267" s="93"/>
+      <c r="KD267" s="93"/>
+      <c r="KE267" s="93"/>
+      <c r="KF267" s="93"/>
+      <c r="KG267" s="93"/>
+      <c r="KH267" s="93"/>
+      <c r="KI267" s="93"/>
+      <c r="KJ267" s="93"/>
+      <c r="KK267" s="93"/>
+      <c r="KL267" s="93"/>
+      <c r="KM267" s="93"/>
+      <c r="KN267" s="93"/>
+      <c r="KO267" s="93"/>
+      <c r="KP267" s="93"/>
+    </row>
+    <row r="268" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A268" s="41"/>
+      <c r="B268" s="33">
+        <v>2</v>
+      </c>
+      <c r="C268" s="33">
+        <v>8</v>
+      </c>
+      <c r="D268" s="33">
+        <v>0</v>
+      </c>
+      <c r="E268" s="33">
+        <v>3</v>
+      </c>
+      <c r="F268" s="32"/>
+      <c r="I268" s="34"/>
+      <c r="J268" s="32"/>
+      <c r="M268" s="34"/>
+      <c r="Q268" s="32"/>
+      <c r="R268" s="34"/>
+      <c r="S268" s="67"/>
+      <c r="T268" s="67"/>
+      <c r="U268" s="67"/>
+      <c r="V268" s="67"/>
+      <c r="W268" s="67"/>
+      <c r="X268" s="67"/>
+      <c r="Y268" s="67"/>
+      <c r="Z268" s="67"/>
+      <c r="AA268" s="67"/>
+      <c r="AB268" s="67"/>
+      <c r="AC268" s="67"/>
+      <c r="AD268" s="67"/>
+      <c r="AE268" s="67"/>
+      <c r="AF268" s="67"/>
+      <c r="AG268" s="68"/>
+      <c r="AH268" s="33">
+        <v>2</v>
+      </c>
+      <c r="AI268" s="33">
+        <v>8</v>
+      </c>
+      <c r="AJ268" s="33">
+        <v>0</v>
+      </c>
+      <c r="AK268" s="33">
+        <v>3</v>
+      </c>
+      <c r="AR268" s="83"/>
+      <c r="AT268" s="84"/>
+      <c r="AU268" s="84"/>
+      <c r="AV268" s="84"/>
+      <c r="AW268" s="84"/>
+      <c r="AX268" s="84"/>
+      <c r="AY268" s="84"/>
+      <c r="AZ268" s="84"/>
+      <c r="BA268" s="84"/>
+      <c r="BB268" s="84"/>
+      <c r="BC268" s="84"/>
+      <c r="BD268" s="84"/>
+      <c r="BE268" s="84"/>
+      <c r="BF268" s="84"/>
+      <c r="BG268" s="84"/>
+      <c r="BH268" s="84"/>
+      <c r="BI268" s="84"/>
+      <c r="BJ268" s="84"/>
+      <c r="BK268" s="84"/>
+      <c r="BL268" s="84"/>
+      <c r="BM268" s="84"/>
+      <c r="BN268" s="84"/>
+      <c r="BO268" s="84"/>
+      <c r="BP268" s="84"/>
+      <c r="BQ268" s="84"/>
+      <c r="BR268" s="84"/>
+      <c r="BS268" s="84"/>
+      <c r="BT268" s="84"/>
+      <c r="BU268" s="84"/>
+      <c r="BV268" s="84"/>
+      <c r="BW268" s="84"/>
+      <c r="BX268" s="84"/>
+      <c r="BY268" s="84"/>
+      <c r="BZ268" s="84"/>
+      <c r="CA268" s="84"/>
+      <c r="CB268" s="84"/>
+      <c r="CC268" s="84"/>
+      <c r="CD268" s="84"/>
+      <c r="CE268" s="84"/>
+      <c r="CF268" s="84"/>
+      <c r="CG268" s="84"/>
+      <c r="CH268" s="84"/>
+      <c r="CI268" s="84"/>
+      <c r="CJ268" s="84"/>
+      <c r="CK268" s="84"/>
+      <c r="CL268" s="84"/>
+      <c r="CM268" s="84"/>
+      <c r="CN268" s="84"/>
+      <c r="CO268" s="84"/>
+      <c r="CP268" s="84"/>
+      <c r="CQ268" s="84"/>
+      <c r="CR268" s="84"/>
+      <c r="CS268" s="84"/>
+      <c r="CT268" s="84"/>
+      <c r="CU268" s="84"/>
+      <c r="CV268" s="84"/>
+      <c r="CW268" s="84"/>
+      <c r="CX268" s="84"/>
+      <c r="CY268" s="84"/>
+      <c r="CZ268" s="84"/>
+      <c r="DA268" s="84"/>
+      <c r="DB268" s="84"/>
+      <c r="DC268" s="84"/>
+      <c r="DD268" s="84"/>
+      <c r="DE268" s="84"/>
+      <c r="DF268" s="84"/>
+      <c r="DG268" s="84"/>
+      <c r="DH268" s="84"/>
+      <c r="DI268" s="84"/>
+      <c r="DJ268" s="84"/>
+      <c r="DK268" s="84"/>
+      <c r="DL268" s="84"/>
+      <c r="DM268" s="84"/>
+      <c r="DN268" s="84"/>
+      <c r="DO268" s="84"/>
+      <c r="DP268" s="84"/>
+      <c r="DQ268" s="84"/>
+      <c r="DR268" s="84"/>
+      <c r="DS268" s="84"/>
+      <c r="DT268" s="84"/>
+      <c r="DU268" s="84"/>
+      <c r="DV268" s="84"/>
+      <c r="DW268" s="84"/>
+      <c r="DX268" s="84"/>
+      <c r="DY268" s="84"/>
+      <c r="DZ268" s="84"/>
+      <c r="EA268" s="84"/>
+      <c r="EB268" s="84"/>
+      <c r="EC268" s="84"/>
+      <c r="ED268" s="84"/>
+      <c r="EE268" s="84"/>
+      <c r="EF268" s="84"/>
+      <c r="EG268" s="84"/>
+      <c r="EH268" s="84"/>
+      <c r="EI268" s="84"/>
+      <c r="EJ268" s="84"/>
+      <c r="EK268" s="84"/>
+      <c r="EL268" s="84"/>
+      <c r="EM268" s="84"/>
+      <c r="EN268" s="84"/>
+      <c r="EO268" s="84"/>
+      <c r="EP268" s="84"/>
+      <c r="EQ268" s="84"/>
+      <c r="ER268" s="84"/>
+      <c r="ES268" s="84"/>
+      <c r="ET268" s="84"/>
+      <c r="EU268" s="84"/>
+      <c r="EV268" s="84"/>
+      <c r="EW268" s="84"/>
+      <c r="EX268" s="84"/>
+      <c r="EY268" s="84"/>
+      <c r="EZ268" s="84"/>
+      <c r="FA268" s="84"/>
+      <c r="FB268" s="84"/>
+      <c r="FC268" s="84"/>
+      <c r="FD268" s="84"/>
+      <c r="FE268" s="84"/>
+      <c r="FF268" s="84"/>
+      <c r="FG268" s="84"/>
+      <c r="FH268" s="84"/>
+      <c r="FI268" s="84"/>
+      <c r="FJ268" s="84"/>
+      <c r="FK268" s="84"/>
+      <c r="FL268" s="84"/>
+      <c r="FM268" s="84"/>
+      <c r="FN268" s="84"/>
+      <c r="FO268" s="84"/>
+      <c r="FP268" s="84"/>
+      <c r="FQ268" s="84"/>
+      <c r="FR268" s="84"/>
+      <c r="FS268" s="84"/>
+      <c r="FT268" s="84"/>
+      <c r="FU268" s="84"/>
+      <c r="FV268" s="84"/>
+      <c r="FW268" s="84"/>
+      <c r="FX268" s="84"/>
+      <c r="FY268" s="84"/>
+      <c r="FZ268" s="84"/>
+      <c r="GA268" s="84"/>
+      <c r="GB268" s="84"/>
+      <c r="GC268" s="84"/>
+      <c r="GD268" s="84"/>
+      <c r="GE268" s="84"/>
+      <c r="GF268" s="84"/>
+      <c r="GG268" s="84"/>
+      <c r="GH268" s="84"/>
+      <c r="GI268" s="84"/>
+      <c r="GJ268" s="84"/>
+      <c r="GK268" s="84"/>
+      <c r="GL268" s="84"/>
+      <c r="GM268" s="84"/>
+      <c r="GN268" s="84"/>
+      <c r="GO268" s="84"/>
+      <c r="GP268" s="84"/>
+      <c r="GQ268" s="84"/>
+      <c r="GR268" s="84"/>
+      <c r="GS268" s="84"/>
+      <c r="GT268" s="84"/>
+      <c r="GU268" s="84"/>
+      <c r="GV268" s="84"/>
+      <c r="GW268" s="84"/>
+      <c r="GX268" s="84"/>
+      <c r="GY268" s="84"/>
+      <c r="GZ268" s="84"/>
+      <c r="HA268" s="84"/>
+      <c r="HB268" s="84"/>
+      <c r="HC268" s="84"/>
+      <c r="HD268" s="84"/>
+      <c r="HE268" s="84"/>
+      <c r="HF268" s="84"/>
+      <c r="HG268" s="84"/>
+      <c r="HH268" s="84"/>
+      <c r="HI268" s="84"/>
+      <c r="HJ268" s="84"/>
+      <c r="HK268" s="84"/>
+      <c r="HL268" s="84"/>
+      <c r="HM268" s="84"/>
+      <c r="HN268" s="84"/>
+      <c r="HO268" s="84"/>
+      <c r="HP268" s="84"/>
+      <c r="HQ268" s="84"/>
+      <c r="HR268" s="84"/>
+      <c r="HS268" s="84"/>
+      <c r="HT268" s="84"/>
+      <c r="HU268" s="84"/>
+      <c r="HV268" s="84"/>
+      <c r="HW268" s="84"/>
+      <c r="HX268" s="84"/>
+      <c r="HY268" s="84"/>
+      <c r="HZ268" s="84"/>
+      <c r="IA268" s="84"/>
+      <c r="IB268" s="84"/>
+      <c r="IC268" s="84"/>
+      <c r="ID268" s="84"/>
+      <c r="IE268" s="84"/>
+      <c r="IF268" s="84"/>
+      <c r="IG268" s="84"/>
+      <c r="IH268" s="84"/>
+      <c r="II268" s="84"/>
+      <c r="IJ268" s="84"/>
+      <c r="IK268" s="84"/>
+      <c r="IL268" s="84"/>
+      <c r="IM268" s="84"/>
+      <c r="IN268" s="84"/>
+      <c r="IO268" s="84"/>
+      <c r="IP268" s="84"/>
+      <c r="IQ268" s="84"/>
+      <c r="IR268" s="84"/>
+      <c r="IS268" s="84"/>
+      <c r="IT268" s="84"/>
+      <c r="IU268" s="84"/>
+      <c r="IV268" s="84"/>
+      <c r="IW268" s="84"/>
+      <c r="IX268" s="84"/>
+      <c r="IY268" s="84"/>
+      <c r="IZ268" s="84"/>
+      <c r="JA268" s="84"/>
+      <c r="JB268" s="84"/>
+      <c r="JC268" s="84"/>
+      <c r="JD268" s="84"/>
+      <c r="JE268" s="84"/>
+      <c r="JF268" s="84"/>
+      <c r="JG268" s="84"/>
+      <c r="JH268" s="84"/>
+      <c r="JI268" s="84"/>
+      <c r="JJ268" s="84"/>
+      <c r="JK268" s="84"/>
+      <c r="JL268" s="84"/>
+      <c r="JM268" s="84"/>
+      <c r="JN268" s="84"/>
+      <c r="JO268" s="84"/>
+      <c r="JP268" s="84"/>
+      <c r="JQ268" s="84"/>
+      <c r="JR268" s="84"/>
+      <c r="JS268" s="84"/>
+      <c r="JT268" s="84"/>
+      <c r="JU268" s="84"/>
+      <c r="JV268" s="84"/>
+      <c r="JW268" s="84"/>
+      <c r="JX268" s="84"/>
+      <c r="JY268" s="84"/>
+      <c r="JZ268" s="84"/>
+      <c r="KA268" s="84"/>
+      <c r="KB268" s="84"/>
+      <c r="KC268" s="84"/>
+      <c r="KD268" s="84"/>
+      <c r="KE268" s="84"/>
+      <c r="KF268" s="84"/>
+      <c r="KG268" s="84"/>
+      <c r="KH268" s="84"/>
+      <c r="KI268" s="84"/>
+      <c r="KJ268" s="84"/>
+      <c r="KK268" s="84"/>
+      <c r="KL268" s="84"/>
+      <c r="KM268" s="84"/>
+      <c r="KN268" s="84"/>
+      <c r="KO268" s="84"/>
+      <c r="KP268" s="84"/>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added capture types PASS_STORE_CAPT and PULL_ACROSS captures.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B88E306-062C-4E31-944E-A7830CE9427D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B7F8D-5A99-44A7-A19B-0772F1D99544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capture_test_data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="201">
   <si>
     <t>setup</t>
   </si>
@@ -601,6 +601,42 @@
   <si>
     <t>no capture</t>
   </si>
+  <si>
+    <t>STORE</t>
+  </si>
+  <si>
+    <t>no capture -- not 1 seed</t>
+  </si>
+  <si>
+    <t>False passively capts Ts store, opp side</t>
+  </si>
+  <si>
+    <t>True passively capts Fs store, opp side</t>
+  </si>
+  <si>
+    <t>False passively capts Ts store, own side</t>
+  </si>
+  <si>
+    <t>True passively capts Fs store, own side</t>
+  </si>
+  <si>
+    <t>True passively capts Fs store, both</t>
+  </si>
+  <si>
+    <t>PULL</t>
+  </si>
+  <si>
+    <t>True Pulls</t>
+  </si>
+  <si>
+    <t>False Pulls</t>
+  </si>
+  <si>
+    <t>T pulls from T</t>
+  </si>
+  <si>
+    <t>T pulls from F</t>
+  </si>
 </sst>
 </file>
 
@@ -1088,7 +1124,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1270,6 +1306,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1603,12 +1641,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AMK268"/>
+  <dimension ref="A1:AMK292"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AQ264" sqref="AQ264"/>
+      <selection pane="bottomLeft" activeCell="P281" sqref="P281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -50592,6 +50630,4076 @@
       <c r="KO268" s="84"/>
       <c r="KP268" s="84"/>
     </row>
+    <row r="269" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="A269" s="40">
+        <v>123</v>
+      </c>
+      <c r="B269" s="97">
+        <v>3</v>
+      </c>
+      <c r="C269" s="97">
+        <v>3</v>
+      </c>
+      <c r="D269" s="97">
+        <v>1</v>
+      </c>
+      <c r="E269" s="97">
+        <v>3</v>
+      </c>
+      <c r="N269">
+        <v>3</v>
+      </c>
+      <c r="O269">
+        <v>4</v>
+      </c>
+      <c r="P269" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q269" s="23">
+        <v>5</v>
+      </c>
+      <c r="R269" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="V269" s="60">
+        <v>1</v>
+      </c>
+      <c r="AB269" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="AH269" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI269" s="97">
+        <v>3</v>
+      </c>
+      <c r="AJ269" s="97">
+        <v>1</v>
+      </c>
+      <c r="AK269" s="97">
+        <v>3</v>
+      </c>
+      <c r="AP269">
+        <v>0</v>
+      </c>
+      <c r="AQ269">
+        <v>7</v>
+      </c>
+      <c r="AR269" s="80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS269" s="29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="270" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B270" s="97">
+        <v>3</v>
+      </c>
+      <c r="C270" s="97">
+        <v>1</v>
+      </c>
+      <c r="D270" s="97">
+        <v>0</v>
+      </c>
+      <c r="E270" s="97">
+        <v>3</v>
+      </c>
+      <c r="AH270" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI270" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ270" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK270" s="97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="271" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A271" s="46">
+        <v>124</v>
+      </c>
+      <c r="B271" s="98">
+        <v>3</v>
+      </c>
+      <c r="C271" s="98">
+        <v>3</v>
+      </c>
+      <c r="D271" s="98">
+        <v>1</v>
+      </c>
+      <c r="E271" s="98">
+        <v>3</v>
+      </c>
+      <c r="F271" s="28"/>
+      <c r="I271" s="30"/>
+      <c r="J271" s="28"/>
+      <c r="M271" s="30"/>
+      <c r="N271" s="29">
+        <v>3</v>
+      </c>
+      <c r="O271" s="29">
+        <v>4</v>
+      </c>
+      <c r="P271" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q271" s="28">
+        <v>1</v>
+      </c>
+      <c r="R271" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S271" s="65"/>
+      <c r="T271" s="65"/>
+      <c r="U271" s="65"/>
+      <c r="V271" s="65">
+        <v>1</v>
+      </c>
+      <c r="W271" s="65"/>
+      <c r="X271" s="65"/>
+      <c r="Y271" s="65"/>
+      <c r="Z271" s="65"/>
+      <c r="AA271" s="65"/>
+      <c r="AB271" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC271" s="65"/>
+      <c r="AD271" s="65"/>
+      <c r="AE271" s="65"/>
+      <c r="AF271" s="65"/>
+      <c r="AG271" s="91"/>
+      <c r="AH271" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI271" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ271" s="98">
+        <v>1</v>
+      </c>
+      <c r="AK271" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP271" s="29">
+        <v>7</v>
+      </c>
+      <c r="AQ271" s="29">
+        <v>0</v>
+      </c>
+      <c r="AR271" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS271" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="AT271" s="93"/>
+      <c r="AU271" s="93"/>
+      <c r="AV271" s="93"/>
+      <c r="AW271" s="93"/>
+      <c r="AX271" s="93"/>
+      <c r="AY271" s="93"/>
+      <c r="AZ271" s="93"/>
+      <c r="BA271" s="93"/>
+      <c r="BB271" s="93"/>
+      <c r="BC271" s="93"/>
+      <c r="BD271" s="93"/>
+      <c r="BE271" s="93"/>
+      <c r="BF271" s="93"/>
+      <c r="BG271" s="93"/>
+      <c r="BH271" s="93"/>
+      <c r="BI271" s="93"/>
+      <c r="BJ271" s="93"/>
+      <c r="BK271" s="93"/>
+      <c r="BL271" s="93"/>
+      <c r="BM271" s="93"/>
+      <c r="BN271" s="93"/>
+      <c r="BO271" s="93"/>
+      <c r="BP271" s="93"/>
+      <c r="BQ271" s="93"/>
+      <c r="BR271" s="93"/>
+      <c r="BS271" s="93"/>
+      <c r="BT271" s="93"/>
+      <c r="BU271" s="93"/>
+      <c r="BV271" s="93"/>
+      <c r="BW271" s="93"/>
+      <c r="BX271" s="93"/>
+      <c r="BY271" s="93"/>
+      <c r="BZ271" s="93"/>
+      <c r="CA271" s="93"/>
+      <c r="CB271" s="93"/>
+      <c r="CC271" s="93"/>
+      <c r="CD271" s="93"/>
+      <c r="CE271" s="93"/>
+      <c r="CF271" s="93"/>
+      <c r="CG271" s="93"/>
+      <c r="CH271" s="93"/>
+      <c r="CI271" s="93"/>
+      <c r="CJ271" s="93"/>
+      <c r="CK271" s="93"/>
+      <c r="CL271" s="93"/>
+      <c r="CM271" s="93"/>
+      <c r="CN271" s="93"/>
+      <c r="CO271" s="93"/>
+      <c r="CP271" s="93"/>
+      <c r="CQ271" s="93"/>
+      <c r="CR271" s="93"/>
+      <c r="CS271" s="93"/>
+      <c r="CT271" s="93"/>
+      <c r="CU271" s="93"/>
+      <c r="CV271" s="93"/>
+      <c r="CW271" s="93"/>
+      <c r="CX271" s="93"/>
+      <c r="CY271" s="93"/>
+      <c r="CZ271" s="93"/>
+      <c r="DA271" s="93"/>
+      <c r="DB271" s="93"/>
+      <c r="DC271" s="93"/>
+      <c r="DD271" s="93"/>
+      <c r="DE271" s="93"/>
+      <c r="DF271" s="93"/>
+      <c r="DG271" s="93"/>
+      <c r="DH271" s="93"/>
+      <c r="DI271" s="93"/>
+      <c r="DJ271" s="93"/>
+      <c r="DK271" s="93"/>
+      <c r="DL271" s="93"/>
+      <c r="DM271" s="93"/>
+      <c r="DN271" s="93"/>
+      <c r="DO271" s="93"/>
+      <c r="DP271" s="93"/>
+      <c r="DQ271" s="93"/>
+      <c r="DR271" s="93"/>
+      <c r="DS271" s="93"/>
+      <c r="DT271" s="93"/>
+      <c r="DU271" s="93"/>
+      <c r="DV271" s="93"/>
+      <c r="DW271" s="93"/>
+      <c r="DX271" s="93"/>
+      <c r="DY271" s="93"/>
+      <c r="DZ271" s="93"/>
+      <c r="EA271" s="93"/>
+      <c r="EB271" s="93"/>
+      <c r="EC271" s="93"/>
+      <c r="ED271" s="93"/>
+      <c r="EE271" s="93"/>
+      <c r="EF271" s="93"/>
+      <c r="EG271" s="93"/>
+      <c r="EH271" s="93"/>
+      <c r="EI271" s="93"/>
+      <c r="EJ271" s="93"/>
+      <c r="EK271" s="93"/>
+      <c r="EL271" s="93"/>
+      <c r="EM271" s="93"/>
+      <c r="EN271" s="93"/>
+      <c r="EO271" s="93"/>
+      <c r="EP271" s="93"/>
+      <c r="EQ271" s="93"/>
+      <c r="ER271" s="93"/>
+      <c r="ES271" s="93"/>
+      <c r="ET271" s="93"/>
+      <c r="EU271" s="93"/>
+      <c r="EV271" s="93"/>
+      <c r="EW271" s="93"/>
+      <c r="EX271" s="93"/>
+      <c r="EY271" s="93"/>
+      <c r="EZ271" s="93"/>
+      <c r="FA271" s="93"/>
+      <c r="FB271" s="93"/>
+      <c r="FC271" s="93"/>
+      <c r="FD271" s="93"/>
+      <c r="FE271" s="93"/>
+      <c r="FF271" s="93"/>
+      <c r="FG271" s="93"/>
+      <c r="FH271" s="93"/>
+      <c r="FI271" s="93"/>
+      <c r="FJ271" s="93"/>
+      <c r="FK271" s="93"/>
+      <c r="FL271" s="93"/>
+      <c r="FM271" s="93"/>
+      <c r="FN271" s="93"/>
+      <c r="FO271" s="93"/>
+      <c r="FP271" s="93"/>
+      <c r="FQ271" s="93"/>
+      <c r="FR271" s="93"/>
+      <c r="FS271" s="93"/>
+      <c r="FT271" s="93"/>
+      <c r="FU271" s="93"/>
+      <c r="FV271" s="93"/>
+      <c r="FW271" s="93"/>
+      <c r="FX271" s="93"/>
+      <c r="FY271" s="93"/>
+      <c r="FZ271" s="93"/>
+      <c r="GA271" s="93"/>
+      <c r="GB271" s="93"/>
+      <c r="GC271" s="93"/>
+      <c r="GD271" s="93"/>
+      <c r="GE271" s="93"/>
+      <c r="GF271" s="93"/>
+      <c r="GG271" s="93"/>
+      <c r="GH271" s="93"/>
+      <c r="GI271" s="93"/>
+      <c r="GJ271" s="93"/>
+      <c r="GK271" s="93"/>
+      <c r="GL271" s="93"/>
+      <c r="GM271" s="93"/>
+      <c r="GN271" s="93"/>
+      <c r="GO271" s="93"/>
+      <c r="GP271" s="93"/>
+      <c r="GQ271" s="93"/>
+      <c r="GR271" s="93"/>
+      <c r="GS271" s="93"/>
+      <c r="GT271" s="93"/>
+      <c r="GU271" s="93"/>
+      <c r="GV271" s="93"/>
+      <c r="GW271" s="93"/>
+      <c r="GX271" s="93"/>
+      <c r="GY271" s="93"/>
+      <c r="GZ271" s="93"/>
+      <c r="HA271" s="93"/>
+      <c r="HB271" s="93"/>
+      <c r="HC271" s="93"/>
+      <c r="HD271" s="93"/>
+      <c r="HE271" s="93"/>
+      <c r="HF271" s="93"/>
+      <c r="HG271" s="93"/>
+      <c r="HH271" s="93"/>
+      <c r="HI271" s="93"/>
+      <c r="HJ271" s="93"/>
+      <c r="HK271" s="93"/>
+      <c r="HL271" s="93"/>
+      <c r="HM271" s="93"/>
+      <c r="HN271" s="93"/>
+      <c r="HO271" s="93"/>
+      <c r="HP271" s="93"/>
+      <c r="HQ271" s="93"/>
+      <c r="HR271" s="93"/>
+      <c r="HS271" s="93"/>
+      <c r="HT271" s="93"/>
+      <c r="HU271" s="93"/>
+      <c r="HV271" s="93"/>
+      <c r="HW271" s="93"/>
+      <c r="HX271" s="93"/>
+      <c r="HY271" s="93"/>
+      <c r="HZ271" s="93"/>
+      <c r="IA271" s="93"/>
+      <c r="IB271" s="93"/>
+      <c r="IC271" s="93"/>
+      <c r="ID271" s="93"/>
+      <c r="IE271" s="93"/>
+      <c r="IF271" s="93"/>
+      <c r="IG271" s="93"/>
+      <c r="IH271" s="93"/>
+      <c r="II271" s="93"/>
+      <c r="IJ271" s="93"/>
+      <c r="IK271" s="93"/>
+      <c r="IL271" s="93"/>
+      <c r="IM271" s="93"/>
+      <c r="IN271" s="93"/>
+      <c r="IO271" s="93"/>
+      <c r="IP271" s="93"/>
+      <c r="IQ271" s="93"/>
+      <c r="IR271" s="93"/>
+      <c r="IS271" s="93"/>
+      <c r="IT271" s="93"/>
+      <c r="IU271" s="93"/>
+      <c r="IV271" s="93"/>
+      <c r="IW271" s="93"/>
+      <c r="IX271" s="93"/>
+      <c r="IY271" s="93"/>
+      <c r="IZ271" s="93"/>
+      <c r="JA271" s="93"/>
+      <c r="JB271" s="93"/>
+      <c r="JC271" s="93"/>
+      <c r="JD271" s="93"/>
+      <c r="JE271" s="93"/>
+      <c r="JF271" s="93"/>
+      <c r="JG271" s="93"/>
+      <c r="JH271" s="93"/>
+      <c r="JI271" s="93"/>
+      <c r="JJ271" s="93"/>
+      <c r="JK271" s="93"/>
+      <c r="JL271" s="93"/>
+      <c r="JM271" s="93"/>
+      <c r="JN271" s="93"/>
+      <c r="JO271" s="93"/>
+      <c r="JP271" s="93"/>
+      <c r="JQ271" s="93"/>
+      <c r="JR271" s="93"/>
+      <c r="JS271" s="93"/>
+      <c r="JT271" s="93"/>
+      <c r="JU271" s="93"/>
+      <c r="JV271" s="93"/>
+      <c r="JW271" s="93"/>
+      <c r="JX271" s="93"/>
+      <c r="JY271" s="93"/>
+      <c r="JZ271" s="93"/>
+      <c r="KA271" s="93"/>
+      <c r="KB271" s="93"/>
+      <c r="KC271" s="93"/>
+      <c r="KD271" s="93"/>
+      <c r="KE271" s="93"/>
+      <c r="KF271" s="93"/>
+      <c r="KG271" s="93"/>
+      <c r="KH271" s="93"/>
+      <c r="KI271" s="93"/>
+      <c r="KJ271" s="93"/>
+      <c r="KK271" s="93"/>
+      <c r="KL271" s="93"/>
+      <c r="KM271" s="93"/>
+      <c r="KN271" s="93"/>
+      <c r="KO271" s="93"/>
+      <c r="KP271" s="93"/>
+    </row>
+    <row r="272" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B272" s="97">
+        <v>3</v>
+      </c>
+      <c r="C272" s="97">
+        <v>1</v>
+      </c>
+      <c r="D272" s="97">
+        <v>0</v>
+      </c>
+      <c r="E272" s="97">
+        <v>3</v>
+      </c>
+      <c r="AH272" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI272" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ272" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK272" s="97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="273" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A273" s="46">
+        <v>125</v>
+      </c>
+      <c r="B273" s="98">
+        <v>3</v>
+      </c>
+      <c r="C273" s="98">
+        <v>3</v>
+      </c>
+      <c r="D273" s="98">
+        <v>1</v>
+      </c>
+      <c r="E273" s="98">
+        <v>3</v>
+      </c>
+      <c r="F273" s="28"/>
+      <c r="I273" s="30"/>
+      <c r="J273" s="28"/>
+      <c r="M273" s="30"/>
+      <c r="N273" s="29">
+        <v>3</v>
+      </c>
+      <c r="O273" s="29">
+        <v>4</v>
+      </c>
+      <c r="P273" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q273" s="28">
+        <v>0</v>
+      </c>
+      <c r="R273" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S273" s="65"/>
+      <c r="T273" s="65"/>
+      <c r="U273" s="65"/>
+      <c r="V273" s="65"/>
+      <c r="W273" s="65"/>
+      <c r="X273" s="65"/>
+      <c r="Y273" s="65"/>
+      <c r="Z273" s="65"/>
+      <c r="AA273" s="65"/>
+      <c r="AB273" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC273" s="65"/>
+      <c r="AD273" s="65"/>
+      <c r="AE273" s="65"/>
+      <c r="AF273" s="65"/>
+      <c r="AG273" s="91"/>
+      <c r="AH273" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI273" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ273" s="98">
+        <v>1</v>
+      </c>
+      <c r="AK273" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP273" s="29">
+        <v>3</v>
+      </c>
+      <c r="AQ273" s="29">
+        <v>4</v>
+      </c>
+      <c r="AR273" s="92" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS273" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="AT273" s="93"/>
+      <c r="AU273" s="93"/>
+      <c r="AV273" s="93"/>
+      <c r="AW273" s="93"/>
+      <c r="AX273" s="93"/>
+      <c r="AY273" s="93"/>
+      <c r="AZ273" s="93"/>
+      <c r="BA273" s="93"/>
+      <c r="BB273" s="93"/>
+      <c r="BC273" s="93"/>
+      <c r="BD273" s="93"/>
+      <c r="BE273" s="93"/>
+      <c r="BF273" s="93"/>
+      <c r="BG273" s="93"/>
+      <c r="BH273" s="93"/>
+      <c r="BI273" s="93"/>
+      <c r="BJ273" s="93"/>
+      <c r="BK273" s="93"/>
+      <c r="BL273" s="93"/>
+      <c r="BM273" s="93"/>
+      <c r="BN273" s="93"/>
+      <c r="BO273" s="93"/>
+      <c r="BP273" s="93"/>
+      <c r="BQ273" s="93"/>
+      <c r="BR273" s="93"/>
+      <c r="BS273" s="93"/>
+      <c r="BT273" s="93"/>
+      <c r="BU273" s="93"/>
+      <c r="BV273" s="93"/>
+      <c r="BW273" s="93"/>
+      <c r="BX273" s="93"/>
+      <c r="BY273" s="93"/>
+      <c r="BZ273" s="93"/>
+      <c r="CA273" s="93"/>
+      <c r="CB273" s="93"/>
+      <c r="CC273" s="93"/>
+      <c r="CD273" s="93"/>
+      <c r="CE273" s="93"/>
+      <c r="CF273" s="93"/>
+      <c r="CG273" s="93"/>
+      <c r="CH273" s="93"/>
+      <c r="CI273" s="93"/>
+      <c r="CJ273" s="93"/>
+      <c r="CK273" s="93"/>
+      <c r="CL273" s="93"/>
+      <c r="CM273" s="93"/>
+      <c r="CN273" s="93"/>
+      <c r="CO273" s="93"/>
+      <c r="CP273" s="93"/>
+      <c r="CQ273" s="93"/>
+      <c r="CR273" s="93"/>
+      <c r="CS273" s="93"/>
+      <c r="CT273" s="93"/>
+      <c r="CU273" s="93"/>
+      <c r="CV273" s="93"/>
+      <c r="CW273" s="93"/>
+      <c r="CX273" s="93"/>
+      <c r="CY273" s="93"/>
+      <c r="CZ273" s="93"/>
+      <c r="DA273" s="93"/>
+      <c r="DB273" s="93"/>
+      <c r="DC273" s="93"/>
+      <c r="DD273" s="93"/>
+      <c r="DE273" s="93"/>
+      <c r="DF273" s="93"/>
+      <c r="DG273" s="93"/>
+      <c r="DH273" s="93"/>
+      <c r="DI273" s="93"/>
+      <c r="DJ273" s="93"/>
+      <c r="DK273" s="93"/>
+      <c r="DL273" s="93"/>
+      <c r="DM273" s="93"/>
+      <c r="DN273" s="93"/>
+      <c r="DO273" s="93"/>
+      <c r="DP273" s="93"/>
+      <c r="DQ273" s="93"/>
+      <c r="DR273" s="93"/>
+      <c r="DS273" s="93"/>
+      <c r="DT273" s="93"/>
+      <c r="DU273" s="93"/>
+      <c r="DV273" s="93"/>
+      <c r="DW273" s="93"/>
+      <c r="DX273" s="93"/>
+      <c r="DY273" s="93"/>
+      <c r="DZ273" s="93"/>
+      <c r="EA273" s="93"/>
+      <c r="EB273" s="93"/>
+      <c r="EC273" s="93"/>
+      <c r="ED273" s="93"/>
+      <c r="EE273" s="93"/>
+      <c r="EF273" s="93"/>
+      <c r="EG273" s="93"/>
+      <c r="EH273" s="93"/>
+      <c r="EI273" s="93"/>
+      <c r="EJ273" s="93"/>
+      <c r="EK273" s="93"/>
+      <c r="EL273" s="93"/>
+      <c r="EM273" s="93"/>
+      <c r="EN273" s="93"/>
+      <c r="EO273" s="93"/>
+      <c r="EP273" s="93"/>
+      <c r="EQ273" s="93"/>
+      <c r="ER273" s="93"/>
+      <c r="ES273" s="93"/>
+      <c r="ET273" s="93"/>
+      <c r="EU273" s="93"/>
+      <c r="EV273" s="93"/>
+      <c r="EW273" s="93"/>
+      <c r="EX273" s="93"/>
+      <c r="EY273" s="93"/>
+      <c r="EZ273" s="93"/>
+      <c r="FA273" s="93"/>
+      <c r="FB273" s="93"/>
+      <c r="FC273" s="93"/>
+      <c r="FD273" s="93"/>
+      <c r="FE273" s="93"/>
+      <c r="FF273" s="93"/>
+      <c r="FG273" s="93"/>
+      <c r="FH273" s="93"/>
+      <c r="FI273" s="93"/>
+      <c r="FJ273" s="93"/>
+      <c r="FK273" s="93"/>
+      <c r="FL273" s="93"/>
+      <c r="FM273" s="93"/>
+      <c r="FN273" s="93"/>
+      <c r="FO273" s="93"/>
+      <c r="FP273" s="93"/>
+      <c r="FQ273" s="93"/>
+      <c r="FR273" s="93"/>
+      <c r="FS273" s="93"/>
+      <c r="FT273" s="93"/>
+      <c r="FU273" s="93"/>
+      <c r="FV273" s="93"/>
+      <c r="FW273" s="93"/>
+      <c r="FX273" s="93"/>
+      <c r="FY273" s="93"/>
+      <c r="FZ273" s="93"/>
+      <c r="GA273" s="93"/>
+      <c r="GB273" s="93"/>
+      <c r="GC273" s="93"/>
+      <c r="GD273" s="93"/>
+      <c r="GE273" s="93"/>
+      <c r="GF273" s="93"/>
+      <c r="GG273" s="93"/>
+      <c r="GH273" s="93"/>
+      <c r="GI273" s="93"/>
+      <c r="GJ273" s="93"/>
+      <c r="GK273" s="93"/>
+      <c r="GL273" s="93"/>
+      <c r="GM273" s="93"/>
+      <c r="GN273" s="93"/>
+      <c r="GO273" s="93"/>
+      <c r="GP273" s="93"/>
+      <c r="GQ273" s="93"/>
+      <c r="GR273" s="93"/>
+      <c r="GS273" s="93"/>
+      <c r="GT273" s="93"/>
+      <c r="GU273" s="93"/>
+      <c r="GV273" s="93"/>
+      <c r="GW273" s="93"/>
+      <c r="GX273" s="93"/>
+      <c r="GY273" s="93"/>
+      <c r="GZ273" s="93"/>
+      <c r="HA273" s="93"/>
+      <c r="HB273" s="93"/>
+      <c r="HC273" s="93"/>
+      <c r="HD273" s="93"/>
+      <c r="HE273" s="93"/>
+      <c r="HF273" s="93"/>
+      <c r="HG273" s="93"/>
+      <c r="HH273" s="93"/>
+      <c r="HI273" s="93"/>
+      <c r="HJ273" s="93"/>
+      <c r="HK273" s="93"/>
+      <c r="HL273" s="93"/>
+      <c r="HM273" s="93"/>
+      <c r="HN273" s="93"/>
+      <c r="HO273" s="93"/>
+      <c r="HP273" s="93"/>
+      <c r="HQ273" s="93"/>
+      <c r="HR273" s="93"/>
+      <c r="HS273" s="93"/>
+      <c r="HT273" s="93"/>
+      <c r="HU273" s="93"/>
+      <c r="HV273" s="93"/>
+      <c r="HW273" s="93"/>
+      <c r="HX273" s="93"/>
+      <c r="HY273" s="93"/>
+      <c r="HZ273" s="93"/>
+      <c r="IA273" s="93"/>
+      <c r="IB273" s="93"/>
+      <c r="IC273" s="93"/>
+      <c r="ID273" s="93"/>
+      <c r="IE273" s="93"/>
+      <c r="IF273" s="93"/>
+      <c r="IG273" s="93"/>
+      <c r="IH273" s="93"/>
+      <c r="II273" s="93"/>
+      <c r="IJ273" s="93"/>
+      <c r="IK273" s="93"/>
+      <c r="IL273" s="93"/>
+      <c r="IM273" s="93"/>
+      <c r="IN273" s="93"/>
+      <c r="IO273" s="93"/>
+      <c r="IP273" s="93"/>
+      <c r="IQ273" s="93"/>
+      <c r="IR273" s="93"/>
+      <c r="IS273" s="93"/>
+      <c r="IT273" s="93"/>
+      <c r="IU273" s="93"/>
+      <c r="IV273" s="93"/>
+      <c r="IW273" s="93"/>
+      <c r="IX273" s="93"/>
+      <c r="IY273" s="93"/>
+      <c r="IZ273" s="93"/>
+      <c r="JA273" s="93"/>
+      <c r="JB273" s="93"/>
+      <c r="JC273" s="93"/>
+      <c r="JD273" s="93"/>
+      <c r="JE273" s="93"/>
+      <c r="JF273" s="93"/>
+      <c r="JG273" s="93"/>
+      <c r="JH273" s="93"/>
+      <c r="JI273" s="93"/>
+      <c r="JJ273" s="93"/>
+      <c r="JK273" s="93"/>
+      <c r="JL273" s="93"/>
+      <c r="JM273" s="93"/>
+      <c r="JN273" s="93"/>
+      <c r="JO273" s="93"/>
+      <c r="JP273" s="93"/>
+      <c r="JQ273" s="93"/>
+      <c r="JR273" s="93"/>
+      <c r="JS273" s="93"/>
+      <c r="JT273" s="93"/>
+      <c r="JU273" s="93"/>
+      <c r="JV273" s="93"/>
+      <c r="JW273" s="93"/>
+      <c r="JX273" s="93"/>
+      <c r="JY273" s="93"/>
+      <c r="JZ273" s="93"/>
+      <c r="KA273" s="93"/>
+      <c r="KB273" s="93"/>
+      <c r="KC273" s="93"/>
+      <c r="KD273" s="93"/>
+      <c r="KE273" s="93"/>
+      <c r="KF273" s="93"/>
+      <c r="KG273" s="93"/>
+      <c r="KH273" s="93"/>
+      <c r="KI273" s="93"/>
+      <c r="KJ273" s="93"/>
+      <c r="KK273" s="93"/>
+      <c r="KL273" s="93"/>
+      <c r="KM273" s="93"/>
+      <c r="KN273" s="93"/>
+      <c r="KO273" s="93"/>
+      <c r="KP273" s="93"/>
+    </row>
+    <row r="274" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B274" s="97">
+        <v>3</v>
+      </c>
+      <c r="C274" s="97">
+        <v>1</v>
+      </c>
+      <c r="D274" s="97">
+        <v>0</v>
+      </c>
+      <c r="E274" s="97">
+        <v>3</v>
+      </c>
+      <c r="AH274" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI274" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ274" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK274" s="97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A275" s="46">
+        <v>126</v>
+      </c>
+      <c r="B275" s="98">
+        <v>3</v>
+      </c>
+      <c r="C275" s="98">
+        <v>3</v>
+      </c>
+      <c r="D275" s="98">
+        <v>1</v>
+      </c>
+      <c r="E275" s="98">
+        <v>3</v>
+      </c>
+      <c r="F275" s="28"/>
+      <c r="I275" s="30"/>
+      <c r="J275" s="28"/>
+      <c r="M275" s="30"/>
+      <c r="N275" s="29">
+        <v>3</v>
+      </c>
+      <c r="O275" s="29">
+        <v>4</v>
+      </c>
+      <c r="P275" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q275" s="28">
+        <v>5</v>
+      </c>
+      <c r="R275" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S275" s="65"/>
+      <c r="T275" s="65"/>
+      <c r="U275" s="65"/>
+      <c r="V275" s="65"/>
+      <c r="W275" s="65"/>
+      <c r="X275" s="65"/>
+      <c r="Y275" s="65"/>
+      <c r="Z275" s="65"/>
+      <c r="AA275" s="65"/>
+      <c r="AB275" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC275" s="65"/>
+      <c r="AD275" s="65"/>
+      <c r="AE275" s="65"/>
+      <c r="AF275" s="65"/>
+      <c r="AG275" s="91"/>
+      <c r="AH275" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI275" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ275" s="98">
+        <v>1</v>
+      </c>
+      <c r="AK275" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP275" s="29">
+        <v>0</v>
+      </c>
+      <c r="AQ275" s="29">
+        <v>7</v>
+      </c>
+      <c r="AR275" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS275" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="AT275" s="93"/>
+      <c r="AU275" s="93"/>
+      <c r="AV275" s="93"/>
+      <c r="AW275" s="93"/>
+      <c r="AX275" s="93"/>
+      <c r="AY275" s="93"/>
+      <c r="AZ275" s="93"/>
+      <c r="BA275" s="93"/>
+      <c r="BB275" s="93"/>
+      <c r="BC275" s="93"/>
+      <c r="BD275" s="93"/>
+      <c r="BE275" s="93"/>
+      <c r="BF275" s="93"/>
+      <c r="BG275" s="93"/>
+      <c r="BH275" s="93"/>
+      <c r="BI275" s="93"/>
+      <c r="BJ275" s="93"/>
+      <c r="BK275" s="93"/>
+      <c r="BL275" s="93"/>
+      <c r="BM275" s="93"/>
+      <c r="BN275" s="93"/>
+      <c r="BO275" s="93"/>
+      <c r="BP275" s="93"/>
+      <c r="BQ275" s="93"/>
+      <c r="BR275" s="93"/>
+      <c r="BS275" s="93"/>
+      <c r="BT275" s="93"/>
+      <c r="BU275" s="93"/>
+      <c r="BV275" s="93"/>
+      <c r="BW275" s="93"/>
+      <c r="BX275" s="93"/>
+      <c r="BY275" s="93"/>
+      <c r="BZ275" s="93"/>
+      <c r="CA275" s="93"/>
+      <c r="CB275" s="93"/>
+      <c r="CC275" s="93"/>
+      <c r="CD275" s="93"/>
+      <c r="CE275" s="93"/>
+      <c r="CF275" s="93"/>
+      <c r="CG275" s="93"/>
+      <c r="CH275" s="93"/>
+      <c r="CI275" s="93"/>
+      <c r="CJ275" s="93"/>
+      <c r="CK275" s="93"/>
+      <c r="CL275" s="93"/>
+      <c r="CM275" s="93"/>
+      <c r="CN275" s="93"/>
+      <c r="CO275" s="93"/>
+      <c r="CP275" s="93"/>
+      <c r="CQ275" s="93"/>
+      <c r="CR275" s="93"/>
+      <c r="CS275" s="93"/>
+      <c r="CT275" s="93"/>
+      <c r="CU275" s="93"/>
+      <c r="CV275" s="93"/>
+      <c r="CW275" s="93"/>
+      <c r="CX275" s="93"/>
+      <c r="CY275" s="93"/>
+      <c r="CZ275" s="93"/>
+      <c r="DA275" s="93"/>
+      <c r="DB275" s="93"/>
+      <c r="DC275" s="93"/>
+      <c r="DD275" s="93"/>
+      <c r="DE275" s="93"/>
+      <c r="DF275" s="93"/>
+      <c r="DG275" s="93"/>
+      <c r="DH275" s="93"/>
+      <c r="DI275" s="93"/>
+      <c r="DJ275" s="93"/>
+      <c r="DK275" s="93"/>
+      <c r="DL275" s="93"/>
+      <c r="DM275" s="93"/>
+      <c r="DN275" s="93"/>
+      <c r="DO275" s="93"/>
+      <c r="DP275" s="93"/>
+      <c r="DQ275" s="93"/>
+      <c r="DR275" s="93"/>
+      <c r="DS275" s="93"/>
+      <c r="DT275" s="93"/>
+      <c r="DU275" s="93"/>
+      <c r="DV275" s="93"/>
+      <c r="DW275" s="93"/>
+      <c r="DX275" s="93"/>
+      <c r="DY275" s="93"/>
+      <c r="DZ275" s="93"/>
+      <c r="EA275" s="93"/>
+      <c r="EB275" s="93"/>
+      <c r="EC275" s="93"/>
+      <c r="ED275" s="93"/>
+      <c r="EE275" s="93"/>
+      <c r="EF275" s="93"/>
+      <c r="EG275" s="93"/>
+      <c r="EH275" s="93"/>
+      <c r="EI275" s="93"/>
+      <c r="EJ275" s="93"/>
+      <c r="EK275" s="93"/>
+      <c r="EL275" s="93"/>
+      <c r="EM275" s="93"/>
+      <c r="EN275" s="93"/>
+      <c r="EO275" s="93"/>
+      <c r="EP275" s="93"/>
+      <c r="EQ275" s="93"/>
+      <c r="ER275" s="93"/>
+      <c r="ES275" s="93"/>
+      <c r="ET275" s="93"/>
+      <c r="EU275" s="93"/>
+      <c r="EV275" s="93"/>
+      <c r="EW275" s="93"/>
+      <c r="EX275" s="93"/>
+      <c r="EY275" s="93"/>
+      <c r="EZ275" s="93"/>
+      <c r="FA275" s="93"/>
+      <c r="FB275" s="93"/>
+      <c r="FC275" s="93"/>
+      <c r="FD275" s="93"/>
+      <c r="FE275" s="93"/>
+      <c r="FF275" s="93"/>
+      <c r="FG275" s="93"/>
+      <c r="FH275" s="93"/>
+      <c r="FI275" s="93"/>
+      <c r="FJ275" s="93"/>
+      <c r="FK275" s="93"/>
+      <c r="FL275" s="93"/>
+      <c r="FM275" s="93"/>
+      <c r="FN275" s="93"/>
+      <c r="FO275" s="93"/>
+      <c r="FP275" s="93"/>
+      <c r="FQ275" s="93"/>
+      <c r="FR275" s="93"/>
+      <c r="FS275" s="93"/>
+      <c r="FT275" s="93"/>
+      <c r="FU275" s="93"/>
+      <c r="FV275" s="93"/>
+      <c r="FW275" s="93"/>
+      <c r="FX275" s="93"/>
+      <c r="FY275" s="93"/>
+      <c r="FZ275" s="93"/>
+      <c r="GA275" s="93"/>
+      <c r="GB275" s="93"/>
+      <c r="GC275" s="93"/>
+      <c r="GD275" s="93"/>
+      <c r="GE275" s="93"/>
+      <c r="GF275" s="93"/>
+      <c r="GG275" s="93"/>
+      <c r="GH275" s="93"/>
+      <c r="GI275" s="93"/>
+      <c r="GJ275" s="93"/>
+      <c r="GK275" s="93"/>
+      <c r="GL275" s="93"/>
+      <c r="GM275" s="93"/>
+      <c r="GN275" s="93"/>
+      <c r="GO275" s="93"/>
+      <c r="GP275" s="93"/>
+      <c r="GQ275" s="93"/>
+      <c r="GR275" s="93"/>
+      <c r="GS275" s="93"/>
+      <c r="GT275" s="93"/>
+      <c r="GU275" s="93"/>
+      <c r="GV275" s="93"/>
+      <c r="GW275" s="93"/>
+      <c r="GX275" s="93"/>
+      <c r="GY275" s="93"/>
+      <c r="GZ275" s="93"/>
+      <c r="HA275" s="93"/>
+      <c r="HB275" s="93"/>
+      <c r="HC275" s="93"/>
+      <c r="HD275" s="93"/>
+      <c r="HE275" s="93"/>
+      <c r="HF275" s="93"/>
+      <c r="HG275" s="93"/>
+      <c r="HH275" s="93"/>
+      <c r="HI275" s="93"/>
+      <c r="HJ275" s="93"/>
+      <c r="HK275" s="93"/>
+      <c r="HL275" s="93"/>
+      <c r="HM275" s="93"/>
+      <c r="HN275" s="93"/>
+      <c r="HO275" s="93"/>
+      <c r="HP275" s="93"/>
+      <c r="HQ275" s="93"/>
+      <c r="HR275" s="93"/>
+      <c r="HS275" s="93"/>
+      <c r="HT275" s="93"/>
+      <c r="HU275" s="93"/>
+      <c r="HV275" s="93"/>
+      <c r="HW275" s="93"/>
+      <c r="HX275" s="93"/>
+      <c r="HY275" s="93"/>
+      <c r="HZ275" s="93"/>
+      <c r="IA275" s="93"/>
+      <c r="IB275" s="93"/>
+      <c r="IC275" s="93"/>
+      <c r="ID275" s="93"/>
+      <c r="IE275" s="93"/>
+      <c r="IF275" s="93"/>
+      <c r="IG275" s="93"/>
+      <c r="IH275" s="93"/>
+      <c r="II275" s="93"/>
+      <c r="IJ275" s="93"/>
+      <c r="IK275" s="93"/>
+      <c r="IL275" s="93"/>
+      <c r="IM275" s="93"/>
+      <c r="IN275" s="93"/>
+      <c r="IO275" s="93"/>
+      <c r="IP275" s="93"/>
+      <c r="IQ275" s="93"/>
+      <c r="IR275" s="93"/>
+      <c r="IS275" s="93"/>
+      <c r="IT275" s="93"/>
+      <c r="IU275" s="93"/>
+      <c r="IV275" s="93"/>
+      <c r="IW275" s="93"/>
+      <c r="IX275" s="93"/>
+      <c r="IY275" s="93"/>
+      <c r="IZ275" s="93"/>
+      <c r="JA275" s="93"/>
+      <c r="JB275" s="93"/>
+      <c r="JC275" s="93"/>
+      <c r="JD275" s="93"/>
+      <c r="JE275" s="93"/>
+      <c r="JF275" s="93"/>
+      <c r="JG275" s="93"/>
+      <c r="JH275" s="93"/>
+      <c r="JI275" s="93"/>
+      <c r="JJ275" s="93"/>
+      <c r="JK275" s="93"/>
+      <c r="JL275" s="93"/>
+      <c r="JM275" s="93"/>
+      <c r="JN275" s="93"/>
+      <c r="JO275" s="93"/>
+      <c r="JP275" s="93"/>
+      <c r="JQ275" s="93"/>
+      <c r="JR275" s="93"/>
+      <c r="JS275" s="93"/>
+      <c r="JT275" s="93"/>
+      <c r="JU275" s="93"/>
+      <c r="JV275" s="93"/>
+      <c r="JW275" s="93"/>
+      <c r="JX275" s="93"/>
+      <c r="JY275" s="93"/>
+      <c r="JZ275" s="93"/>
+      <c r="KA275" s="93"/>
+      <c r="KB275" s="93"/>
+      <c r="KC275" s="93"/>
+      <c r="KD275" s="93"/>
+      <c r="KE275" s="93"/>
+      <c r="KF275" s="93"/>
+      <c r="KG275" s="93"/>
+      <c r="KH275" s="93"/>
+      <c r="KI275" s="93"/>
+      <c r="KJ275" s="93"/>
+      <c r="KK275" s="93"/>
+      <c r="KL275" s="93"/>
+      <c r="KM275" s="93"/>
+      <c r="KN275" s="93"/>
+      <c r="KO275" s="93"/>
+      <c r="KP275" s="93"/>
+    </row>
+    <row r="276" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B276" s="97">
+        <v>3</v>
+      </c>
+      <c r="C276" s="97">
+        <v>1</v>
+      </c>
+      <c r="D276" s="97">
+        <v>0</v>
+      </c>
+      <c r="E276" s="97">
+        <v>3</v>
+      </c>
+      <c r="AH276" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI276" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ276" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK276" s="97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="46">
+        <v>127</v>
+      </c>
+      <c r="B277" s="98">
+        <v>3</v>
+      </c>
+      <c r="C277" s="98">
+        <v>3</v>
+      </c>
+      <c r="D277" s="98">
+        <v>1</v>
+      </c>
+      <c r="E277" s="98">
+        <v>3</v>
+      </c>
+      <c r="F277" s="28"/>
+      <c r="I277" s="30"/>
+      <c r="J277" s="28"/>
+      <c r="M277" s="30"/>
+      <c r="N277" s="29">
+        <v>3</v>
+      </c>
+      <c r="O277" s="29">
+        <v>4</v>
+      </c>
+      <c r="P277" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q277" s="28">
+        <v>1</v>
+      </c>
+      <c r="R277" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S277" s="65"/>
+      <c r="T277" s="65"/>
+      <c r="U277" s="65"/>
+      <c r="V277" s="65">
+        <v>2</v>
+      </c>
+      <c r="W277" s="65"/>
+      <c r="X277" s="65"/>
+      <c r="Y277" s="65"/>
+      <c r="Z277" s="65"/>
+      <c r="AA277" s="65"/>
+      <c r="AB277" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC277" s="65"/>
+      <c r="AD277" s="65"/>
+      <c r="AE277" s="65"/>
+      <c r="AF277" s="65"/>
+      <c r="AG277" s="91"/>
+      <c r="AH277" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI277" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ277" s="98">
+        <v>1</v>
+      </c>
+      <c r="AK277" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP277" s="29">
+        <v>0</v>
+      </c>
+      <c r="AQ277" s="29">
+        <v>7</v>
+      </c>
+      <c r="AR277" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS277" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="AT277" s="93"/>
+      <c r="AU277" s="93"/>
+      <c r="AV277" s="93"/>
+      <c r="AW277" s="93"/>
+      <c r="AX277" s="93"/>
+      <c r="AY277" s="93"/>
+      <c r="AZ277" s="93"/>
+      <c r="BA277" s="93"/>
+      <c r="BB277" s="93"/>
+      <c r="BC277" s="93"/>
+      <c r="BD277" s="93"/>
+      <c r="BE277" s="93"/>
+      <c r="BF277" s="93"/>
+      <c r="BG277" s="93"/>
+      <c r="BH277" s="93"/>
+      <c r="BI277" s="93"/>
+      <c r="BJ277" s="93"/>
+      <c r="BK277" s="93"/>
+      <c r="BL277" s="93"/>
+      <c r="BM277" s="93"/>
+      <c r="BN277" s="93"/>
+      <c r="BO277" s="93"/>
+      <c r="BP277" s="93"/>
+      <c r="BQ277" s="93"/>
+      <c r="BR277" s="93"/>
+      <c r="BS277" s="93"/>
+      <c r="BT277" s="93"/>
+      <c r="BU277" s="93"/>
+      <c r="BV277" s="93"/>
+      <c r="BW277" s="93"/>
+      <c r="BX277" s="93"/>
+      <c r="BY277" s="93"/>
+      <c r="BZ277" s="93"/>
+      <c r="CA277" s="93"/>
+      <c r="CB277" s="93"/>
+      <c r="CC277" s="93"/>
+      <c r="CD277" s="93"/>
+      <c r="CE277" s="93"/>
+      <c r="CF277" s="93"/>
+      <c r="CG277" s="93"/>
+      <c r="CH277" s="93"/>
+      <c r="CI277" s="93"/>
+      <c r="CJ277" s="93"/>
+      <c r="CK277" s="93"/>
+      <c r="CL277" s="93"/>
+      <c r="CM277" s="93"/>
+      <c r="CN277" s="93"/>
+      <c r="CO277" s="93"/>
+      <c r="CP277" s="93"/>
+      <c r="CQ277" s="93"/>
+      <c r="CR277" s="93"/>
+      <c r="CS277" s="93"/>
+      <c r="CT277" s="93"/>
+      <c r="CU277" s="93"/>
+      <c r="CV277" s="93"/>
+      <c r="CW277" s="93"/>
+      <c r="CX277" s="93"/>
+      <c r="CY277" s="93"/>
+      <c r="CZ277" s="93"/>
+      <c r="DA277" s="93"/>
+      <c r="DB277" s="93"/>
+      <c r="DC277" s="93"/>
+      <c r="DD277" s="93"/>
+      <c r="DE277" s="93"/>
+      <c r="DF277" s="93"/>
+      <c r="DG277" s="93"/>
+      <c r="DH277" s="93"/>
+      <c r="DI277" s="93"/>
+      <c r="DJ277" s="93"/>
+      <c r="DK277" s="93"/>
+      <c r="DL277" s="93"/>
+      <c r="DM277" s="93"/>
+      <c r="DN277" s="93"/>
+      <c r="DO277" s="93"/>
+      <c r="DP277" s="93"/>
+      <c r="DQ277" s="93"/>
+      <c r="DR277" s="93"/>
+      <c r="DS277" s="93"/>
+      <c r="DT277" s="93"/>
+      <c r="DU277" s="93"/>
+      <c r="DV277" s="93"/>
+      <c r="DW277" s="93"/>
+      <c r="DX277" s="93"/>
+      <c r="DY277" s="93"/>
+      <c r="DZ277" s="93"/>
+      <c r="EA277" s="93"/>
+      <c r="EB277" s="93"/>
+      <c r="EC277" s="93"/>
+      <c r="ED277" s="93"/>
+      <c r="EE277" s="93"/>
+      <c r="EF277" s="93"/>
+      <c r="EG277" s="93"/>
+      <c r="EH277" s="93"/>
+      <c r="EI277" s="93"/>
+      <c r="EJ277" s="93"/>
+      <c r="EK277" s="93"/>
+      <c r="EL277" s="93"/>
+      <c r="EM277" s="93"/>
+      <c r="EN277" s="93"/>
+      <c r="EO277" s="93"/>
+      <c r="EP277" s="93"/>
+      <c r="EQ277" s="93"/>
+      <c r="ER277" s="93"/>
+      <c r="ES277" s="93"/>
+      <c r="ET277" s="93"/>
+      <c r="EU277" s="93"/>
+      <c r="EV277" s="93"/>
+      <c r="EW277" s="93"/>
+      <c r="EX277" s="93"/>
+      <c r="EY277" s="93"/>
+      <c r="EZ277" s="93"/>
+      <c r="FA277" s="93"/>
+      <c r="FB277" s="93"/>
+      <c r="FC277" s="93"/>
+      <c r="FD277" s="93"/>
+      <c r="FE277" s="93"/>
+      <c r="FF277" s="93"/>
+      <c r="FG277" s="93"/>
+      <c r="FH277" s="93"/>
+      <c r="FI277" s="93"/>
+      <c r="FJ277" s="93"/>
+      <c r="FK277" s="93"/>
+      <c r="FL277" s="93"/>
+      <c r="FM277" s="93"/>
+      <c r="FN277" s="93"/>
+      <c r="FO277" s="93"/>
+      <c r="FP277" s="93"/>
+      <c r="FQ277" s="93"/>
+      <c r="FR277" s="93"/>
+      <c r="FS277" s="93"/>
+      <c r="FT277" s="93"/>
+      <c r="FU277" s="93"/>
+      <c r="FV277" s="93"/>
+      <c r="FW277" s="93"/>
+      <c r="FX277" s="93"/>
+      <c r="FY277" s="93"/>
+      <c r="FZ277" s="93"/>
+      <c r="GA277" s="93"/>
+      <c r="GB277" s="93"/>
+      <c r="GC277" s="93"/>
+      <c r="GD277" s="93"/>
+      <c r="GE277" s="93"/>
+      <c r="GF277" s="93"/>
+      <c r="GG277" s="93"/>
+      <c r="GH277" s="93"/>
+      <c r="GI277" s="93"/>
+      <c r="GJ277" s="93"/>
+      <c r="GK277" s="93"/>
+      <c r="GL277" s="93"/>
+      <c r="GM277" s="93"/>
+      <c r="GN277" s="93"/>
+      <c r="GO277" s="93"/>
+      <c r="GP277" s="93"/>
+      <c r="GQ277" s="93"/>
+      <c r="GR277" s="93"/>
+      <c r="GS277" s="93"/>
+      <c r="GT277" s="93"/>
+      <c r="GU277" s="93"/>
+      <c r="GV277" s="93"/>
+      <c r="GW277" s="93"/>
+      <c r="GX277" s="93"/>
+      <c r="GY277" s="93"/>
+      <c r="GZ277" s="93"/>
+      <c r="HA277" s="93"/>
+      <c r="HB277" s="93"/>
+      <c r="HC277" s="93"/>
+      <c r="HD277" s="93"/>
+      <c r="HE277" s="93"/>
+      <c r="HF277" s="93"/>
+      <c r="HG277" s="93"/>
+      <c r="HH277" s="93"/>
+      <c r="HI277" s="93"/>
+      <c r="HJ277" s="93"/>
+      <c r="HK277" s="93"/>
+      <c r="HL277" s="93"/>
+      <c r="HM277" s="93"/>
+      <c r="HN277" s="93"/>
+      <c r="HO277" s="93"/>
+      <c r="HP277" s="93"/>
+      <c r="HQ277" s="93"/>
+      <c r="HR277" s="93"/>
+      <c r="HS277" s="93"/>
+      <c r="HT277" s="93"/>
+      <c r="HU277" s="93"/>
+      <c r="HV277" s="93"/>
+      <c r="HW277" s="93"/>
+      <c r="HX277" s="93"/>
+      <c r="HY277" s="93"/>
+      <c r="HZ277" s="93"/>
+      <c r="IA277" s="93"/>
+      <c r="IB277" s="93"/>
+      <c r="IC277" s="93"/>
+      <c r="ID277" s="93"/>
+      <c r="IE277" s="93"/>
+      <c r="IF277" s="93"/>
+      <c r="IG277" s="93"/>
+      <c r="IH277" s="93"/>
+      <c r="II277" s="93"/>
+      <c r="IJ277" s="93"/>
+      <c r="IK277" s="93"/>
+      <c r="IL277" s="93"/>
+      <c r="IM277" s="93"/>
+      <c r="IN277" s="93"/>
+      <c r="IO277" s="93"/>
+      <c r="IP277" s="93"/>
+      <c r="IQ277" s="93"/>
+      <c r="IR277" s="93"/>
+      <c r="IS277" s="93"/>
+      <c r="IT277" s="93"/>
+      <c r="IU277" s="93"/>
+      <c r="IV277" s="93"/>
+      <c r="IW277" s="93"/>
+      <c r="IX277" s="93"/>
+      <c r="IY277" s="93"/>
+      <c r="IZ277" s="93"/>
+      <c r="JA277" s="93"/>
+      <c r="JB277" s="93"/>
+      <c r="JC277" s="93"/>
+      <c r="JD277" s="93"/>
+      <c r="JE277" s="93"/>
+      <c r="JF277" s="93"/>
+      <c r="JG277" s="93"/>
+      <c r="JH277" s="93"/>
+      <c r="JI277" s="93"/>
+      <c r="JJ277" s="93"/>
+      <c r="JK277" s="93"/>
+      <c r="JL277" s="93"/>
+      <c r="JM277" s="93"/>
+      <c r="JN277" s="93"/>
+      <c r="JO277" s="93"/>
+      <c r="JP277" s="93"/>
+      <c r="JQ277" s="93"/>
+      <c r="JR277" s="93"/>
+      <c r="JS277" s="93"/>
+      <c r="JT277" s="93"/>
+      <c r="JU277" s="93"/>
+      <c r="JV277" s="93"/>
+      <c r="JW277" s="93"/>
+      <c r="JX277" s="93"/>
+      <c r="JY277" s="93"/>
+      <c r="JZ277" s="93"/>
+      <c r="KA277" s="93"/>
+      <c r="KB277" s="93"/>
+      <c r="KC277" s="93"/>
+      <c r="KD277" s="93"/>
+      <c r="KE277" s="93"/>
+      <c r="KF277" s="93"/>
+      <c r="KG277" s="93"/>
+      <c r="KH277" s="93"/>
+      <c r="KI277" s="93"/>
+      <c r="KJ277" s="93"/>
+      <c r="KK277" s="93"/>
+      <c r="KL277" s="93"/>
+      <c r="KM277" s="93"/>
+      <c r="KN277" s="93"/>
+      <c r="KO277" s="93"/>
+      <c r="KP277" s="93"/>
+    </row>
+    <row r="278" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B278" s="97">
+        <v>3</v>
+      </c>
+      <c r="C278" s="97">
+        <v>1</v>
+      </c>
+      <c r="D278" s="97">
+        <v>0</v>
+      </c>
+      <c r="E278" s="97">
+        <v>3</v>
+      </c>
+      <c r="AH278" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI278" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ278" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK278" s="97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A279" s="46">
+        <v>128</v>
+      </c>
+      <c r="B279" s="98">
+        <v>3</v>
+      </c>
+      <c r="C279" s="98">
+        <v>3</v>
+      </c>
+      <c r="D279" s="98">
+        <v>1</v>
+      </c>
+      <c r="E279" s="98">
+        <v>3</v>
+      </c>
+      <c r="F279" s="28"/>
+      <c r="I279" s="30"/>
+      <c r="J279" s="28"/>
+      <c r="M279" s="30"/>
+      <c r="N279" s="29">
+        <v>3</v>
+      </c>
+      <c r="O279" s="29">
+        <v>4</v>
+      </c>
+      <c r="P279" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q279" s="28">
+        <v>5</v>
+      </c>
+      <c r="R279" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S279" s="65"/>
+      <c r="T279" s="65"/>
+      <c r="U279" s="65"/>
+      <c r="V279" s="65">
+        <v>2</v>
+      </c>
+      <c r="W279" s="65"/>
+      <c r="X279" s="65"/>
+      <c r="Y279" s="65"/>
+      <c r="Z279" s="65"/>
+      <c r="AA279" s="65"/>
+      <c r="AB279" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC279" s="65"/>
+      <c r="AD279" s="65"/>
+      <c r="AE279" s="65"/>
+      <c r="AF279" s="65"/>
+      <c r="AG279" s="91"/>
+      <c r="AH279" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI279" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ279" s="98">
+        <v>1</v>
+      </c>
+      <c r="AK279" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP279" s="29">
+        <v>7</v>
+      </c>
+      <c r="AQ279" s="29">
+        <v>0</v>
+      </c>
+      <c r="AR279" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS279" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="AT279" s="93"/>
+      <c r="AU279" s="93"/>
+      <c r="AV279" s="93"/>
+      <c r="AW279" s="93"/>
+      <c r="AX279" s="93"/>
+      <c r="AY279" s="93"/>
+      <c r="AZ279" s="93"/>
+      <c r="BA279" s="93"/>
+      <c r="BB279" s="93"/>
+      <c r="BC279" s="93"/>
+      <c r="BD279" s="93"/>
+      <c r="BE279" s="93"/>
+      <c r="BF279" s="93"/>
+      <c r="BG279" s="93"/>
+      <c r="BH279" s="93"/>
+      <c r="BI279" s="93"/>
+      <c r="BJ279" s="93"/>
+      <c r="BK279" s="93"/>
+      <c r="BL279" s="93"/>
+      <c r="BM279" s="93"/>
+      <c r="BN279" s="93"/>
+      <c r="BO279" s="93"/>
+      <c r="BP279" s="93"/>
+      <c r="BQ279" s="93"/>
+      <c r="BR279" s="93"/>
+      <c r="BS279" s="93"/>
+      <c r="BT279" s="93"/>
+      <c r="BU279" s="93"/>
+      <c r="BV279" s="93"/>
+      <c r="BW279" s="93"/>
+      <c r="BX279" s="93"/>
+      <c r="BY279" s="93"/>
+      <c r="BZ279" s="93"/>
+      <c r="CA279" s="93"/>
+      <c r="CB279" s="93"/>
+      <c r="CC279" s="93"/>
+      <c r="CD279" s="93"/>
+      <c r="CE279" s="93"/>
+      <c r="CF279" s="93"/>
+      <c r="CG279" s="93"/>
+      <c r="CH279" s="93"/>
+      <c r="CI279" s="93"/>
+      <c r="CJ279" s="93"/>
+      <c r="CK279" s="93"/>
+      <c r="CL279" s="93"/>
+      <c r="CM279" s="93"/>
+      <c r="CN279" s="93"/>
+      <c r="CO279" s="93"/>
+      <c r="CP279" s="93"/>
+      <c r="CQ279" s="93"/>
+      <c r="CR279" s="93"/>
+      <c r="CS279" s="93"/>
+      <c r="CT279" s="93"/>
+      <c r="CU279" s="93"/>
+      <c r="CV279" s="93"/>
+      <c r="CW279" s="93"/>
+      <c r="CX279" s="93"/>
+      <c r="CY279" s="93"/>
+      <c r="CZ279" s="93"/>
+      <c r="DA279" s="93"/>
+      <c r="DB279" s="93"/>
+      <c r="DC279" s="93"/>
+      <c r="DD279" s="93"/>
+      <c r="DE279" s="93"/>
+      <c r="DF279" s="93"/>
+      <c r="DG279" s="93"/>
+      <c r="DH279" s="93"/>
+      <c r="DI279" s="93"/>
+      <c r="DJ279" s="93"/>
+      <c r="DK279" s="93"/>
+      <c r="DL279" s="93"/>
+      <c r="DM279" s="93"/>
+      <c r="DN279" s="93"/>
+      <c r="DO279" s="93"/>
+      <c r="DP279" s="93"/>
+      <c r="DQ279" s="93"/>
+      <c r="DR279" s="93"/>
+      <c r="DS279" s="93"/>
+      <c r="DT279" s="93"/>
+      <c r="DU279" s="93"/>
+      <c r="DV279" s="93"/>
+      <c r="DW279" s="93"/>
+      <c r="DX279" s="93"/>
+      <c r="DY279" s="93"/>
+      <c r="DZ279" s="93"/>
+      <c r="EA279" s="93"/>
+      <c r="EB279" s="93"/>
+      <c r="EC279" s="93"/>
+      <c r="ED279" s="93"/>
+      <c r="EE279" s="93"/>
+      <c r="EF279" s="93"/>
+      <c r="EG279" s="93"/>
+      <c r="EH279" s="93"/>
+      <c r="EI279" s="93"/>
+      <c r="EJ279" s="93"/>
+      <c r="EK279" s="93"/>
+      <c r="EL279" s="93"/>
+      <c r="EM279" s="93"/>
+      <c r="EN279" s="93"/>
+      <c r="EO279" s="93"/>
+      <c r="EP279" s="93"/>
+      <c r="EQ279" s="93"/>
+      <c r="ER279" s="93"/>
+      <c r="ES279" s="93"/>
+      <c r="ET279" s="93"/>
+      <c r="EU279" s="93"/>
+      <c r="EV279" s="93"/>
+      <c r="EW279" s="93"/>
+      <c r="EX279" s="93"/>
+      <c r="EY279" s="93"/>
+      <c r="EZ279" s="93"/>
+      <c r="FA279" s="93"/>
+      <c r="FB279" s="93"/>
+      <c r="FC279" s="93"/>
+      <c r="FD279" s="93"/>
+      <c r="FE279" s="93"/>
+      <c r="FF279" s="93"/>
+      <c r="FG279" s="93"/>
+      <c r="FH279" s="93"/>
+      <c r="FI279" s="93"/>
+      <c r="FJ279" s="93"/>
+      <c r="FK279" s="93"/>
+      <c r="FL279" s="93"/>
+      <c r="FM279" s="93"/>
+      <c r="FN279" s="93"/>
+      <c r="FO279" s="93"/>
+      <c r="FP279" s="93"/>
+      <c r="FQ279" s="93"/>
+      <c r="FR279" s="93"/>
+      <c r="FS279" s="93"/>
+      <c r="FT279" s="93"/>
+      <c r="FU279" s="93"/>
+      <c r="FV279" s="93"/>
+      <c r="FW279" s="93"/>
+      <c r="FX279" s="93"/>
+      <c r="FY279" s="93"/>
+      <c r="FZ279" s="93"/>
+      <c r="GA279" s="93"/>
+      <c r="GB279" s="93"/>
+      <c r="GC279" s="93"/>
+      <c r="GD279" s="93"/>
+      <c r="GE279" s="93"/>
+      <c r="GF279" s="93"/>
+      <c r="GG279" s="93"/>
+      <c r="GH279" s="93"/>
+      <c r="GI279" s="93"/>
+      <c r="GJ279" s="93"/>
+      <c r="GK279" s="93"/>
+      <c r="GL279" s="93"/>
+      <c r="GM279" s="93"/>
+      <c r="GN279" s="93"/>
+      <c r="GO279" s="93"/>
+      <c r="GP279" s="93"/>
+      <c r="GQ279" s="93"/>
+      <c r="GR279" s="93"/>
+      <c r="GS279" s="93"/>
+      <c r="GT279" s="93"/>
+      <c r="GU279" s="93"/>
+      <c r="GV279" s="93"/>
+      <c r="GW279" s="93"/>
+      <c r="GX279" s="93"/>
+      <c r="GY279" s="93"/>
+      <c r="GZ279" s="93"/>
+      <c r="HA279" s="93"/>
+      <c r="HB279" s="93"/>
+      <c r="HC279" s="93"/>
+      <c r="HD279" s="93"/>
+      <c r="HE279" s="93"/>
+      <c r="HF279" s="93"/>
+      <c r="HG279" s="93"/>
+      <c r="HH279" s="93"/>
+      <c r="HI279" s="93"/>
+      <c r="HJ279" s="93"/>
+      <c r="HK279" s="93"/>
+      <c r="HL279" s="93"/>
+      <c r="HM279" s="93"/>
+      <c r="HN279" s="93"/>
+      <c r="HO279" s="93"/>
+      <c r="HP279" s="93"/>
+      <c r="HQ279" s="93"/>
+      <c r="HR279" s="93"/>
+      <c r="HS279" s="93"/>
+      <c r="HT279" s="93"/>
+      <c r="HU279" s="93"/>
+      <c r="HV279" s="93"/>
+      <c r="HW279" s="93"/>
+      <c r="HX279" s="93"/>
+      <c r="HY279" s="93"/>
+      <c r="HZ279" s="93"/>
+      <c r="IA279" s="93"/>
+      <c r="IB279" s="93"/>
+      <c r="IC279" s="93"/>
+      <c r="ID279" s="93"/>
+      <c r="IE279" s="93"/>
+      <c r="IF279" s="93"/>
+      <c r="IG279" s="93"/>
+      <c r="IH279" s="93"/>
+      <c r="II279" s="93"/>
+      <c r="IJ279" s="93"/>
+      <c r="IK279" s="93"/>
+      <c r="IL279" s="93"/>
+      <c r="IM279" s="93"/>
+      <c r="IN279" s="93"/>
+      <c r="IO279" s="93"/>
+      <c r="IP279" s="93"/>
+      <c r="IQ279" s="93"/>
+      <c r="IR279" s="93"/>
+      <c r="IS279" s="93"/>
+      <c r="IT279" s="93"/>
+      <c r="IU279" s="93"/>
+      <c r="IV279" s="93"/>
+      <c r="IW279" s="93"/>
+      <c r="IX279" s="93"/>
+      <c r="IY279" s="93"/>
+      <c r="IZ279" s="93"/>
+      <c r="JA279" s="93"/>
+      <c r="JB279" s="93"/>
+      <c r="JC279" s="93"/>
+      <c r="JD279" s="93"/>
+      <c r="JE279" s="93"/>
+      <c r="JF279" s="93"/>
+      <c r="JG279" s="93"/>
+      <c r="JH279" s="93"/>
+      <c r="JI279" s="93"/>
+      <c r="JJ279" s="93"/>
+      <c r="JK279" s="93"/>
+      <c r="JL279" s="93"/>
+      <c r="JM279" s="93"/>
+      <c r="JN279" s="93"/>
+      <c r="JO279" s="93"/>
+      <c r="JP279" s="93"/>
+      <c r="JQ279" s="93"/>
+      <c r="JR279" s="93"/>
+      <c r="JS279" s="93"/>
+      <c r="JT279" s="93"/>
+      <c r="JU279" s="93"/>
+      <c r="JV279" s="93"/>
+      <c r="JW279" s="93"/>
+      <c r="JX279" s="93"/>
+      <c r="JY279" s="93"/>
+      <c r="JZ279" s="93"/>
+      <c r="KA279" s="93"/>
+      <c r="KB279" s="93"/>
+      <c r="KC279" s="93"/>
+      <c r="KD279" s="93"/>
+      <c r="KE279" s="93"/>
+      <c r="KF279" s="93"/>
+      <c r="KG279" s="93"/>
+      <c r="KH279" s="93"/>
+      <c r="KI279" s="93"/>
+      <c r="KJ279" s="93"/>
+      <c r="KK279" s="93"/>
+      <c r="KL279" s="93"/>
+      <c r="KM279" s="93"/>
+      <c r="KN279" s="93"/>
+      <c r="KO279" s="93"/>
+      <c r="KP279" s="93"/>
+    </row>
+    <row r="280" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B280" s="97">
+        <v>3</v>
+      </c>
+      <c r="C280" s="97">
+        <v>1</v>
+      </c>
+      <c r="D280" s="97">
+        <v>0</v>
+      </c>
+      <c r="E280" s="97">
+        <v>3</v>
+      </c>
+      <c r="AH280" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI280" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ280" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK280" s="97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="281" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A281" s="46">
+        <v>129</v>
+      </c>
+      <c r="B281" s="98">
+        <v>3</v>
+      </c>
+      <c r="C281" s="98">
+        <v>3</v>
+      </c>
+      <c r="D281" s="98">
+        <v>1</v>
+      </c>
+      <c r="E281" s="98">
+        <v>3</v>
+      </c>
+      <c r="F281" s="28"/>
+      <c r="I281" s="30"/>
+      <c r="J281" s="28"/>
+      <c r="M281" s="30"/>
+      <c r="N281" s="29">
+        <v>3</v>
+      </c>
+      <c r="O281" s="29">
+        <v>4</v>
+      </c>
+      <c r="P281" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q281" s="28">
+        <v>5</v>
+      </c>
+      <c r="R281" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S281" s="65"/>
+      <c r="T281" s="65"/>
+      <c r="U281" s="65"/>
+      <c r="V281" s="65">
+        <v>1</v>
+      </c>
+      <c r="W281" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="X281" s="65"/>
+      <c r="Y281" s="65"/>
+      <c r="Z281" s="65"/>
+      <c r="AA281" s="65"/>
+      <c r="AB281" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC281" s="65"/>
+      <c r="AD281" s="65"/>
+      <c r="AE281" s="65"/>
+      <c r="AF281" s="65"/>
+      <c r="AG281" s="91"/>
+      <c r="AH281" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI281" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ281" s="98">
+        <v>4</v>
+      </c>
+      <c r="AK281" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP281" s="29">
+        <v>3</v>
+      </c>
+      <c r="AQ281" s="29">
+        <v>4</v>
+      </c>
+      <c r="AR281" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS281" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="AT281" s="93"/>
+      <c r="AU281" s="93"/>
+      <c r="AV281" s="93"/>
+      <c r="AW281" s="93"/>
+      <c r="AX281" s="93"/>
+      <c r="AY281" s="93"/>
+      <c r="AZ281" s="93"/>
+      <c r="BA281" s="93"/>
+      <c r="BB281" s="93"/>
+      <c r="BC281" s="93"/>
+      <c r="BD281" s="93"/>
+      <c r="BE281" s="93"/>
+      <c r="BF281" s="93"/>
+      <c r="BG281" s="93"/>
+      <c r="BH281" s="93"/>
+      <c r="BI281" s="93"/>
+      <c r="BJ281" s="93"/>
+      <c r="BK281" s="93"/>
+      <c r="BL281" s="93"/>
+      <c r="BM281" s="93"/>
+      <c r="BN281" s="93"/>
+      <c r="BO281" s="93"/>
+      <c r="BP281" s="93"/>
+      <c r="BQ281" s="93"/>
+      <c r="BR281" s="93"/>
+      <c r="BS281" s="93"/>
+      <c r="BT281" s="93"/>
+      <c r="BU281" s="93"/>
+      <c r="BV281" s="93"/>
+      <c r="BW281" s="93"/>
+      <c r="BX281" s="93"/>
+      <c r="BY281" s="93"/>
+      <c r="BZ281" s="93"/>
+      <c r="CA281" s="93"/>
+      <c r="CB281" s="93"/>
+      <c r="CC281" s="93"/>
+      <c r="CD281" s="93"/>
+      <c r="CE281" s="93"/>
+      <c r="CF281" s="93"/>
+      <c r="CG281" s="93"/>
+      <c r="CH281" s="93"/>
+      <c r="CI281" s="93"/>
+      <c r="CJ281" s="93"/>
+      <c r="CK281" s="93"/>
+      <c r="CL281" s="93"/>
+      <c r="CM281" s="93"/>
+      <c r="CN281" s="93"/>
+      <c r="CO281" s="93"/>
+      <c r="CP281" s="93"/>
+      <c r="CQ281" s="93"/>
+      <c r="CR281" s="93"/>
+      <c r="CS281" s="93"/>
+      <c r="CT281" s="93"/>
+      <c r="CU281" s="93"/>
+      <c r="CV281" s="93"/>
+      <c r="CW281" s="93"/>
+      <c r="CX281" s="93"/>
+      <c r="CY281" s="93"/>
+      <c r="CZ281" s="93"/>
+      <c r="DA281" s="93"/>
+      <c r="DB281" s="93"/>
+      <c r="DC281" s="93"/>
+      <c r="DD281" s="93"/>
+      <c r="DE281" s="93"/>
+      <c r="DF281" s="93"/>
+      <c r="DG281" s="93"/>
+      <c r="DH281" s="93"/>
+      <c r="DI281" s="93"/>
+      <c r="DJ281" s="93"/>
+      <c r="DK281" s="93"/>
+      <c r="DL281" s="93"/>
+      <c r="DM281" s="93"/>
+      <c r="DN281" s="93"/>
+      <c r="DO281" s="93"/>
+      <c r="DP281" s="93"/>
+      <c r="DQ281" s="93"/>
+      <c r="DR281" s="93"/>
+      <c r="DS281" s="93"/>
+      <c r="DT281" s="93"/>
+      <c r="DU281" s="93"/>
+      <c r="DV281" s="93"/>
+      <c r="DW281" s="93"/>
+      <c r="DX281" s="93"/>
+      <c r="DY281" s="93"/>
+      <c r="DZ281" s="93"/>
+      <c r="EA281" s="93"/>
+      <c r="EB281" s="93"/>
+      <c r="EC281" s="93"/>
+      <c r="ED281" s="93"/>
+      <c r="EE281" s="93"/>
+      <c r="EF281" s="93"/>
+      <c r="EG281" s="93"/>
+      <c r="EH281" s="93"/>
+      <c r="EI281" s="93"/>
+      <c r="EJ281" s="93"/>
+      <c r="EK281" s="93"/>
+      <c r="EL281" s="93"/>
+      <c r="EM281" s="93"/>
+      <c r="EN281" s="93"/>
+      <c r="EO281" s="93"/>
+      <c r="EP281" s="93"/>
+      <c r="EQ281" s="93"/>
+      <c r="ER281" s="93"/>
+      <c r="ES281" s="93"/>
+      <c r="ET281" s="93"/>
+      <c r="EU281" s="93"/>
+      <c r="EV281" s="93"/>
+      <c r="EW281" s="93"/>
+      <c r="EX281" s="93"/>
+      <c r="EY281" s="93"/>
+      <c r="EZ281" s="93"/>
+      <c r="FA281" s="93"/>
+      <c r="FB281" s="93"/>
+      <c r="FC281" s="93"/>
+      <c r="FD281" s="93"/>
+      <c r="FE281" s="93"/>
+      <c r="FF281" s="93"/>
+      <c r="FG281" s="93"/>
+      <c r="FH281" s="93"/>
+      <c r="FI281" s="93"/>
+      <c r="FJ281" s="93"/>
+      <c r="FK281" s="93"/>
+      <c r="FL281" s="93"/>
+      <c r="FM281" s="93"/>
+      <c r="FN281" s="93"/>
+      <c r="FO281" s="93"/>
+      <c r="FP281" s="93"/>
+      <c r="FQ281" s="93"/>
+      <c r="FR281" s="93"/>
+      <c r="FS281" s="93"/>
+      <c r="FT281" s="93"/>
+      <c r="FU281" s="93"/>
+      <c r="FV281" s="93"/>
+      <c r="FW281" s="93"/>
+      <c r="FX281" s="93"/>
+      <c r="FY281" s="93"/>
+      <c r="FZ281" s="93"/>
+      <c r="GA281" s="93"/>
+      <c r="GB281" s="93"/>
+      <c r="GC281" s="93"/>
+      <c r="GD281" s="93"/>
+      <c r="GE281" s="93"/>
+      <c r="GF281" s="93"/>
+      <c r="GG281" s="93"/>
+      <c r="GH281" s="93"/>
+      <c r="GI281" s="93"/>
+      <c r="GJ281" s="93"/>
+      <c r="GK281" s="93"/>
+      <c r="GL281" s="93"/>
+      <c r="GM281" s="93"/>
+      <c r="GN281" s="93"/>
+      <c r="GO281" s="93"/>
+      <c r="GP281" s="93"/>
+      <c r="GQ281" s="93"/>
+      <c r="GR281" s="93"/>
+      <c r="GS281" s="93"/>
+      <c r="GT281" s="93"/>
+      <c r="GU281" s="93"/>
+      <c r="GV281" s="93"/>
+      <c r="GW281" s="93"/>
+      <c r="GX281" s="93"/>
+      <c r="GY281" s="93"/>
+      <c r="GZ281" s="93"/>
+      <c r="HA281" s="93"/>
+      <c r="HB281" s="93"/>
+      <c r="HC281" s="93"/>
+      <c r="HD281" s="93"/>
+      <c r="HE281" s="93"/>
+      <c r="HF281" s="93"/>
+      <c r="HG281" s="93"/>
+      <c r="HH281" s="93"/>
+      <c r="HI281" s="93"/>
+      <c r="HJ281" s="93"/>
+      <c r="HK281" s="93"/>
+      <c r="HL281" s="93"/>
+      <c r="HM281" s="93"/>
+      <c r="HN281" s="93"/>
+      <c r="HO281" s="93"/>
+      <c r="HP281" s="93"/>
+      <c r="HQ281" s="93"/>
+      <c r="HR281" s="93"/>
+      <c r="HS281" s="93"/>
+      <c r="HT281" s="93"/>
+      <c r="HU281" s="93"/>
+      <c r="HV281" s="93"/>
+      <c r="HW281" s="93"/>
+      <c r="HX281" s="93"/>
+      <c r="HY281" s="93"/>
+      <c r="HZ281" s="93"/>
+      <c r="IA281" s="93"/>
+      <c r="IB281" s="93"/>
+      <c r="IC281" s="93"/>
+      <c r="ID281" s="93"/>
+      <c r="IE281" s="93"/>
+      <c r="IF281" s="93"/>
+      <c r="IG281" s="93"/>
+      <c r="IH281" s="93"/>
+      <c r="II281" s="93"/>
+      <c r="IJ281" s="93"/>
+      <c r="IK281" s="93"/>
+      <c r="IL281" s="93"/>
+      <c r="IM281" s="93"/>
+      <c r="IN281" s="93"/>
+      <c r="IO281" s="93"/>
+      <c r="IP281" s="93"/>
+      <c r="IQ281" s="93"/>
+      <c r="IR281" s="93"/>
+      <c r="IS281" s="93"/>
+      <c r="IT281" s="93"/>
+      <c r="IU281" s="93"/>
+      <c r="IV281" s="93"/>
+      <c r="IW281" s="93"/>
+      <c r="IX281" s="93"/>
+      <c r="IY281" s="93"/>
+      <c r="IZ281" s="93"/>
+      <c r="JA281" s="93"/>
+      <c r="JB281" s="93"/>
+      <c r="JC281" s="93"/>
+      <c r="JD281" s="93"/>
+      <c r="JE281" s="93"/>
+      <c r="JF281" s="93"/>
+      <c r="JG281" s="93"/>
+      <c r="JH281" s="93"/>
+      <c r="JI281" s="93"/>
+      <c r="JJ281" s="93"/>
+      <c r="JK281" s="93"/>
+      <c r="JL281" s="93"/>
+      <c r="JM281" s="93"/>
+      <c r="JN281" s="93"/>
+      <c r="JO281" s="93"/>
+      <c r="JP281" s="93"/>
+      <c r="JQ281" s="93"/>
+      <c r="JR281" s="93"/>
+      <c r="JS281" s="93"/>
+      <c r="JT281" s="93"/>
+      <c r="JU281" s="93"/>
+      <c r="JV281" s="93"/>
+      <c r="JW281" s="93"/>
+      <c r="JX281" s="93"/>
+      <c r="JY281" s="93"/>
+      <c r="JZ281" s="93"/>
+      <c r="KA281" s="93"/>
+      <c r="KB281" s="93"/>
+      <c r="KC281" s="93"/>
+      <c r="KD281" s="93"/>
+      <c r="KE281" s="93"/>
+      <c r="KF281" s="93"/>
+      <c r="KG281" s="93"/>
+      <c r="KH281" s="93"/>
+      <c r="KI281" s="93"/>
+      <c r="KJ281" s="93"/>
+      <c r="KK281" s="93"/>
+      <c r="KL281" s="93"/>
+      <c r="KM281" s="93"/>
+      <c r="KN281" s="93"/>
+      <c r="KO281" s="93"/>
+      <c r="KP281" s="93"/>
+    </row>
+    <row r="282" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B282" s="97">
+        <v>3</v>
+      </c>
+      <c r="C282" s="97">
+        <v>1</v>
+      </c>
+      <c r="D282" s="97">
+        <v>3</v>
+      </c>
+      <c r="E282" s="97">
+        <v>0</v>
+      </c>
+      <c r="AH282" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI282" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ282" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK282" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="46">
+        <v>130</v>
+      </c>
+      <c r="B283" s="98">
+        <v>3</v>
+      </c>
+      <c r="C283" s="98">
+        <v>3</v>
+      </c>
+      <c r="D283" s="98">
+        <v>1</v>
+      </c>
+      <c r="E283" s="98">
+        <v>3</v>
+      </c>
+      <c r="F283" s="28"/>
+      <c r="I283" s="30"/>
+      <c r="J283" s="28"/>
+      <c r="M283" s="30"/>
+      <c r="N283" s="29">
+        <v>3</v>
+      </c>
+      <c r="O283" s="29">
+        <v>4</v>
+      </c>
+      <c r="P283" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q283" s="28">
+        <v>1</v>
+      </c>
+      <c r="R283" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S283" s="65"/>
+      <c r="T283" s="65"/>
+      <c r="U283" s="65"/>
+      <c r="V283" s="65">
+        <v>1</v>
+      </c>
+      <c r="W283" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="X283" s="65"/>
+      <c r="Y283" s="65"/>
+      <c r="Z283" s="65"/>
+      <c r="AA283" s="65"/>
+      <c r="AB283" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC283" s="65"/>
+      <c r="AD283" s="65"/>
+      <c r="AE283" s="65"/>
+      <c r="AF283" s="65"/>
+      <c r="AG283" s="91"/>
+      <c r="AH283" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI283" s="98">
+        <v>0</v>
+      </c>
+      <c r="AJ283" s="98">
+        <v>1</v>
+      </c>
+      <c r="AK283" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP283" s="29">
+        <v>3</v>
+      </c>
+      <c r="AQ283" s="29">
+        <v>4</v>
+      </c>
+      <c r="AR283" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS283" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="AT283" s="93"/>
+      <c r="AU283" s="93"/>
+      <c r="AV283" s="93"/>
+      <c r="AW283" s="93"/>
+      <c r="AX283" s="93"/>
+      <c r="AY283" s="93"/>
+      <c r="AZ283" s="93"/>
+      <c r="BA283" s="93"/>
+      <c r="BB283" s="93"/>
+      <c r="BC283" s="93"/>
+      <c r="BD283" s="93"/>
+      <c r="BE283" s="93"/>
+      <c r="BF283" s="93"/>
+      <c r="BG283" s="93"/>
+      <c r="BH283" s="93"/>
+      <c r="BI283" s="93"/>
+      <c r="BJ283" s="93"/>
+      <c r="BK283" s="93"/>
+      <c r="BL283" s="93"/>
+      <c r="BM283" s="93"/>
+      <c r="BN283" s="93"/>
+      <c r="BO283" s="93"/>
+      <c r="BP283" s="93"/>
+      <c r="BQ283" s="93"/>
+      <c r="BR283" s="93"/>
+      <c r="BS283" s="93"/>
+      <c r="BT283" s="93"/>
+      <c r="BU283" s="93"/>
+      <c r="BV283" s="93"/>
+      <c r="BW283" s="93"/>
+      <c r="BX283" s="93"/>
+      <c r="BY283" s="93"/>
+      <c r="BZ283" s="93"/>
+      <c r="CA283" s="93"/>
+      <c r="CB283" s="93"/>
+      <c r="CC283" s="93"/>
+      <c r="CD283" s="93"/>
+      <c r="CE283" s="93"/>
+      <c r="CF283" s="93"/>
+      <c r="CG283" s="93"/>
+      <c r="CH283" s="93"/>
+      <c r="CI283" s="93"/>
+      <c r="CJ283" s="93"/>
+      <c r="CK283" s="93"/>
+      <c r="CL283" s="93"/>
+      <c r="CM283" s="93"/>
+      <c r="CN283" s="93"/>
+      <c r="CO283" s="93"/>
+      <c r="CP283" s="93"/>
+      <c r="CQ283" s="93"/>
+      <c r="CR283" s="93"/>
+      <c r="CS283" s="93"/>
+      <c r="CT283" s="93"/>
+      <c r="CU283" s="93"/>
+      <c r="CV283" s="93"/>
+      <c r="CW283" s="93"/>
+      <c r="CX283" s="93"/>
+      <c r="CY283" s="93"/>
+      <c r="CZ283" s="93"/>
+      <c r="DA283" s="93"/>
+      <c r="DB283" s="93"/>
+      <c r="DC283" s="93"/>
+      <c r="DD283" s="93"/>
+      <c r="DE283" s="93"/>
+      <c r="DF283" s="93"/>
+      <c r="DG283" s="93"/>
+      <c r="DH283" s="93"/>
+      <c r="DI283" s="93"/>
+      <c r="DJ283" s="93"/>
+      <c r="DK283" s="93"/>
+      <c r="DL283" s="93"/>
+      <c r="DM283" s="93"/>
+      <c r="DN283" s="93"/>
+      <c r="DO283" s="93"/>
+      <c r="DP283" s="93"/>
+      <c r="DQ283" s="93"/>
+      <c r="DR283" s="93"/>
+      <c r="DS283" s="93"/>
+      <c r="DT283" s="93"/>
+      <c r="DU283" s="93"/>
+      <c r="DV283" s="93"/>
+      <c r="DW283" s="93"/>
+      <c r="DX283" s="93"/>
+      <c r="DY283" s="93"/>
+      <c r="DZ283" s="93"/>
+      <c r="EA283" s="93"/>
+      <c r="EB283" s="93"/>
+      <c r="EC283" s="93"/>
+      <c r="ED283" s="93"/>
+      <c r="EE283" s="93"/>
+      <c r="EF283" s="93"/>
+      <c r="EG283" s="93"/>
+      <c r="EH283" s="93"/>
+      <c r="EI283" s="93"/>
+      <c r="EJ283" s="93"/>
+      <c r="EK283" s="93"/>
+      <c r="EL283" s="93"/>
+      <c r="EM283" s="93"/>
+      <c r="EN283" s="93"/>
+      <c r="EO283" s="93"/>
+      <c r="EP283" s="93"/>
+      <c r="EQ283" s="93"/>
+      <c r="ER283" s="93"/>
+      <c r="ES283" s="93"/>
+      <c r="ET283" s="93"/>
+      <c r="EU283" s="93"/>
+      <c r="EV283" s="93"/>
+      <c r="EW283" s="93"/>
+      <c r="EX283" s="93"/>
+      <c r="EY283" s="93"/>
+      <c r="EZ283" s="93"/>
+      <c r="FA283" s="93"/>
+      <c r="FB283" s="93"/>
+      <c r="FC283" s="93"/>
+      <c r="FD283" s="93"/>
+      <c r="FE283" s="93"/>
+      <c r="FF283" s="93"/>
+      <c r="FG283" s="93"/>
+      <c r="FH283" s="93"/>
+      <c r="FI283" s="93"/>
+      <c r="FJ283" s="93"/>
+      <c r="FK283" s="93"/>
+      <c r="FL283" s="93"/>
+      <c r="FM283" s="93"/>
+      <c r="FN283" s="93"/>
+      <c r="FO283" s="93"/>
+      <c r="FP283" s="93"/>
+      <c r="FQ283" s="93"/>
+      <c r="FR283" s="93"/>
+      <c r="FS283" s="93"/>
+      <c r="FT283" s="93"/>
+      <c r="FU283" s="93"/>
+      <c r="FV283" s="93"/>
+      <c r="FW283" s="93"/>
+      <c r="FX283" s="93"/>
+      <c r="FY283" s="93"/>
+      <c r="FZ283" s="93"/>
+      <c r="GA283" s="93"/>
+      <c r="GB283" s="93"/>
+      <c r="GC283" s="93"/>
+      <c r="GD283" s="93"/>
+      <c r="GE283" s="93"/>
+      <c r="GF283" s="93"/>
+      <c r="GG283" s="93"/>
+      <c r="GH283" s="93"/>
+      <c r="GI283" s="93"/>
+      <c r="GJ283" s="93"/>
+      <c r="GK283" s="93"/>
+      <c r="GL283" s="93"/>
+      <c r="GM283" s="93"/>
+      <c r="GN283" s="93"/>
+      <c r="GO283" s="93"/>
+      <c r="GP283" s="93"/>
+      <c r="GQ283" s="93"/>
+      <c r="GR283" s="93"/>
+      <c r="GS283" s="93"/>
+      <c r="GT283" s="93"/>
+      <c r="GU283" s="93"/>
+      <c r="GV283" s="93"/>
+      <c r="GW283" s="93"/>
+      <c r="GX283" s="93"/>
+      <c r="GY283" s="93"/>
+      <c r="GZ283" s="93"/>
+      <c r="HA283" s="93"/>
+      <c r="HB283" s="93"/>
+      <c r="HC283" s="93"/>
+      <c r="HD283" s="93"/>
+      <c r="HE283" s="93"/>
+      <c r="HF283" s="93"/>
+      <c r="HG283" s="93"/>
+      <c r="HH283" s="93"/>
+      <c r="HI283" s="93"/>
+      <c r="HJ283" s="93"/>
+      <c r="HK283" s="93"/>
+      <c r="HL283" s="93"/>
+      <c r="HM283" s="93"/>
+      <c r="HN283" s="93"/>
+      <c r="HO283" s="93"/>
+      <c r="HP283" s="93"/>
+      <c r="HQ283" s="93"/>
+      <c r="HR283" s="93"/>
+      <c r="HS283" s="93"/>
+      <c r="HT283" s="93"/>
+      <c r="HU283" s="93"/>
+      <c r="HV283" s="93"/>
+      <c r="HW283" s="93"/>
+      <c r="HX283" s="93"/>
+      <c r="HY283" s="93"/>
+      <c r="HZ283" s="93"/>
+      <c r="IA283" s="93"/>
+      <c r="IB283" s="93"/>
+      <c r="IC283" s="93"/>
+      <c r="ID283" s="93"/>
+      <c r="IE283" s="93"/>
+      <c r="IF283" s="93"/>
+      <c r="IG283" s="93"/>
+      <c r="IH283" s="93"/>
+      <c r="II283" s="93"/>
+      <c r="IJ283" s="93"/>
+      <c r="IK283" s="93"/>
+      <c r="IL283" s="93"/>
+      <c r="IM283" s="93"/>
+      <c r="IN283" s="93"/>
+      <c r="IO283" s="93"/>
+      <c r="IP283" s="93"/>
+      <c r="IQ283" s="93"/>
+      <c r="IR283" s="93"/>
+      <c r="IS283" s="93"/>
+      <c r="IT283" s="93"/>
+      <c r="IU283" s="93"/>
+      <c r="IV283" s="93"/>
+      <c r="IW283" s="93"/>
+      <c r="IX283" s="93"/>
+      <c r="IY283" s="93"/>
+      <c r="IZ283" s="93"/>
+      <c r="JA283" s="93"/>
+      <c r="JB283" s="93"/>
+      <c r="JC283" s="93"/>
+      <c r="JD283" s="93"/>
+      <c r="JE283" s="93"/>
+      <c r="JF283" s="93"/>
+      <c r="JG283" s="93"/>
+      <c r="JH283" s="93"/>
+      <c r="JI283" s="93"/>
+      <c r="JJ283" s="93"/>
+      <c r="JK283" s="93"/>
+      <c r="JL283" s="93"/>
+      <c r="JM283" s="93"/>
+      <c r="JN283" s="93"/>
+      <c r="JO283" s="93"/>
+      <c r="JP283" s="93"/>
+      <c r="JQ283" s="93"/>
+      <c r="JR283" s="93"/>
+      <c r="JS283" s="93"/>
+      <c r="JT283" s="93"/>
+      <c r="JU283" s="93"/>
+      <c r="JV283" s="93"/>
+      <c r="JW283" s="93"/>
+      <c r="JX283" s="93"/>
+      <c r="JY283" s="93"/>
+      <c r="JZ283" s="93"/>
+      <c r="KA283" s="93"/>
+      <c r="KB283" s="93"/>
+      <c r="KC283" s="93"/>
+      <c r="KD283" s="93"/>
+      <c r="KE283" s="93"/>
+      <c r="KF283" s="93"/>
+      <c r="KG283" s="93"/>
+      <c r="KH283" s="93"/>
+      <c r="KI283" s="93"/>
+      <c r="KJ283" s="93"/>
+      <c r="KK283" s="93"/>
+      <c r="KL283" s="93"/>
+      <c r="KM283" s="93"/>
+      <c r="KN283" s="93"/>
+      <c r="KO283" s="93"/>
+      <c r="KP283" s="93"/>
+    </row>
+    <row r="284" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B284" s="97">
+        <v>3</v>
+      </c>
+      <c r="C284" s="97">
+        <v>1</v>
+      </c>
+      <c r="D284" s="97">
+        <v>3</v>
+      </c>
+      <c r="E284" s="97">
+        <v>0</v>
+      </c>
+      <c r="AH284" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI284" s="97">
+        <v>4</v>
+      </c>
+      <c r="AJ284" s="97">
+        <v>3</v>
+      </c>
+      <c r="AK284" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A285" s="46">
+        <v>131</v>
+      </c>
+      <c r="B285" s="98">
+        <v>3</v>
+      </c>
+      <c r="C285" s="98">
+        <v>3</v>
+      </c>
+      <c r="D285" s="98">
+        <v>1</v>
+      </c>
+      <c r="E285" s="98">
+        <v>3</v>
+      </c>
+      <c r="F285" s="28"/>
+      <c r="I285" s="30"/>
+      <c r="J285" s="28"/>
+      <c r="M285" s="30"/>
+      <c r="N285" s="29">
+        <v>3</v>
+      </c>
+      <c r="O285" s="29">
+        <v>4</v>
+      </c>
+      <c r="P285" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q285" s="28">
+        <v>0</v>
+      </c>
+      <c r="R285" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S285" s="65"/>
+      <c r="T285" s="65"/>
+      <c r="U285" s="65"/>
+      <c r="V285" s="65"/>
+      <c r="W285" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="X285" s="65"/>
+      <c r="Y285" s="65"/>
+      <c r="Z285" s="65"/>
+      <c r="AA285" s="65"/>
+      <c r="AB285" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC285" s="65"/>
+      <c r="AD285" s="65"/>
+      <c r="AE285" s="65"/>
+      <c r="AF285" s="65"/>
+      <c r="AG285" s="91"/>
+      <c r="AH285" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI285" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ285" s="98">
+        <v>1</v>
+      </c>
+      <c r="AK285" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP285" s="29">
+        <v>3</v>
+      </c>
+      <c r="AQ285" s="29">
+        <v>4</v>
+      </c>
+      <c r="AR285" s="92" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS285" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="AT285" s="93"/>
+      <c r="AU285" s="93"/>
+      <c r="AV285" s="93"/>
+      <c r="AW285" s="93"/>
+      <c r="AX285" s="93"/>
+      <c r="AY285" s="93"/>
+      <c r="AZ285" s="93"/>
+      <c r="BA285" s="93"/>
+      <c r="BB285" s="93"/>
+      <c r="BC285" s="93"/>
+      <c r="BD285" s="93"/>
+      <c r="BE285" s="93"/>
+      <c r="BF285" s="93"/>
+      <c r="BG285" s="93"/>
+      <c r="BH285" s="93"/>
+      <c r="BI285" s="93"/>
+      <c r="BJ285" s="93"/>
+      <c r="BK285" s="93"/>
+      <c r="BL285" s="93"/>
+      <c r="BM285" s="93"/>
+      <c r="BN285" s="93"/>
+      <c r="BO285" s="93"/>
+      <c r="BP285" s="93"/>
+      <c r="BQ285" s="93"/>
+      <c r="BR285" s="93"/>
+      <c r="BS285" s="93"/>
+      <c r="BT285" s="93"/>
+      <c r="BU285" s="93"/>
+      <c r="BV285" s="93"/>
+      <c r="BW285" s="93"/>
+      <c r="BX285" s="93"/>
+      <c r="BY285" s="93"/>
+      <c r="BZ285" s="93"/>
+      <c r="CA285" s="93"/>
+      <c r="CB285" s="93"/>
+      <c r="CC285" s="93"/>
+      <c r="CD285" s="93"/>
+      <c r="CE285" s="93"/>
+      <c r="CF285" s="93"/>
+      <c r="CG285" s="93"/>
+      <c r="CH285" s="93"/>
+      <c r="CI285" s="93"/>
+      <c r="CJ285" s="93"/>
+      <c r="CK285" s="93"/>
+      <c r="CL285" s="93"/>
+      <c r="CM285" s="93"/>
+      <c r="CN285" s="93"/>
+      <c r="CO285" s="93"/>
+      <c r="CP285" s="93"/>
+      <c r="CQ285" s="93"/>
+      <c r="CR285" s="93"/>
+      <c r="CS285" s="93"/>
+      <c r="CT285" s="93"/>
+      <c r="CU285" s="93"/>
+      <c r="CV285" s="93"/>
+      <c r="CW285" s="93"/>
+      <c r="CX285" s="93"/>
+      <c r="CY285" s="93"/>
+      <c r="CZ285" s="93"/>
+      <c r="DA285" s="93"/>
+      <c r="DB285" s="93"/>
+      <c r="DC285" s="93"/>
+      <c r="DD285" s="93"/>
+      <c r="DE285" s="93"/>
+      <c r="DF285" s="93"/>
+      <c r="DG285" s="93"/>
+      <c r="DH285" s="93"/>
+      <c r="DI285" s="93"/>
+      <c r="DJ285" s="93"/>
+      <c r="DK285" s="93"/>
+      <c r="DL285" s="93"/>
+      <c r="DM285" s="93"/>
+      <c r="DN285" s="93"/>
+      <c r="DO285" s="93"/>
+      <c r="DP285" s="93"/>
+      <c r="DQ285" s="93"/>
+      <c r="DR285" s="93"/>
+      <c r="DS285" s="93"/>
+      <c r="DT285" s="93"/>
+      <c r="DU285" s="93"/>
+      <c r="DV285" s="93"/>
+      <c r="DW285" s="93"/>
+      <c r="DX285" s="93"/>
+      <c r="DY285" s="93"/>
+      <c r="DZ285" s="93"/>
+      <c r="EA285" s="93"/>
+      <c r="EB285" s="93"/>
+      <c r="EC285" s="93"/>
+      <c r="ED285" s="93"/>
+      <c r="EE285" s="93"/>
+      <c r="EF285" s="93"/>
+      <c r="EG285" s="93"/>
+      <c r="EH285" s="93"/>
+      <c r="EI285" s="93"/>
+      <c r="EJ285" s="93"/>
+      <c r="EK285" s="93"/>
+      <c r="EL285" s="93"/>
+      <c r="EM285" s="93"/>
+      <c r="EN285" s="93"/>
+      <c r="EO285" s="93"/>
+      <c r="EP285" s="93"/>
+      <c r="EQ285" s="93"/>
+      <c r="ER285" s="93"/>
+      <c r="ES285" s="93"/>
+      <c r="ET285" s="93"/>
+      <c r="EU285" s="93"/>
+      <c r="EV285" s="93"/>
+      <c r="EW285" s="93"/>
+      <c r="EX285" s="93"/>
+      <c r="EY285" s="93"/>
+      <c r="EZ285" s="93"/>
+      <c r="FA285" s="93"/>
+      <c r="FB285" s="93"/>
+      <c r="FC285" s="93"/>
+      <c r="FD285" s="93"/>
+      <c r="FE285" s="93"/>
+      <c r="FF285" s="93"/>
+      <c r="FG285" s="93"/>
+      <c r="FH285" s="93"/>
+      <c r="FI285" s="93"/>
+      <c r="FJ285" s="93"/>
+      <c r="FK285" s="93"/>
+      <c r="FL285" s="93"/>
+      <c r="FM285" s="93"/>
+      <c r="FN285" s="93"/>
+      <c r="FO285" s="93"/>
+      <c r="FP285" s="93"/>
+      <c r="FQ285" s="93"/>
+      <c r="FR285" s="93"/>
+      <c r="FS285" s="93"/>
+      <c r="FT285" s="93"/>
+      <c r="FU285" s="93"/>
+      <c r="FV285" s="93"/>
+      <c r="FW285" s="93"/>
+      <c r="FX285" s="93"/>
+      <c r="FY285" s="93"/>
+      <c r="FZ285" s="93"/>
+      <c r="GA285" s="93"/>
+      <c r="GB285" s="93"/>
+      <c r="GC285" s="93"/>
+      <c r="GD285" s="93"/>
+      <c r="GE285" s="93"/>
+      <c r="GF285" s="93"/>
+      <c r="GG285" s="93"/>
+      <c r="GH285" s="93"/>
+      <c r="GI285" s="93"/>
+      <c r="GJ285" s="93"/>
+      <c r="GK285" s="93"/>
+      <c r="GL285" s="93"/>
+      <c r="GM285" s="93"/>
+      <c r="GN285" s="93"/>
+      <c r="GO285" s="93"/>
+      <c r="GP285" s="93"/>
+      <c r="GQ285" s="93"/>
+      <c r="GR285" s="93"/>
+      <c r="GS285" s="93"/>
+      <c r="GT285" s="93"/>
+      <c r="GU285" s="93"/>
+      <c r="GV285" s="93"/>
+      <c r="GW285" s="93"/>
+      <c r="GX285" s="93"/>
+      <c r="GY285" s="93"/>
+      <c r="GZ285" s="93"/>
+      <c r="HA285" s="93"/>
+      <c r="HB285" s="93"/>
+      <c r="HC285" s="93"/>
+      <c r="HD285" s="93"/>
+      <c r="HE285" s="93"/>
+      <c r="HF285" s="93"/>
+      <c r="HG285" s="93"/>
+      <c r="HH285" s="93"/>
+      <c r="HI285" s="93"/>
+      <c r="HJ285" s="93"/>
+      <c r="HK285" s="93"/>
+      <c r="HL285" s="93"/>
+      <c r="HM285" s="93"/>
+      <c r="HN285" s="93"/>
+      <c r="HO285" s="93"/>
+      <c r="HP285" s="93"/>
+      <c r="HQ285" s="93"/>
+      <c r="HR285" s="93"/>
+      <c r="HS285" s="93"/>
+      <c r="HT285" s="93"/>
+      <c r="HU285" s="93"/>
+      <c r="HV285" s="93"/>
+      <c r="HW285" s="93"/>
+      <c r="HX285" s="93"/>
+      <c r="HY285" s="93"/>
+      <c r="HZ285" s="93"/>
+      <c r="IA285" s="93"/>
+      <c r="IB285" s="93"/>
+      <c r="IC285" s="93"/>
+      <c r="ID285" s="93"/>
+      <c r="IE285" s="93"/>
+      <c r="IF285" s="93"/>
+      <c r="IG285" s="93"/>
+      <c r="IH285" s="93"/>
+      <c r="II285" s="93"/>
+      <c r="IJ285" s="93"/>
+      <c r="IK285" s="93"/>
+      <c r="IL285" s="93"/>
+      <c r="IM285" s="93"/>
+      <c r="IN285" s="93"/>
+      <c r="IO285" s="93"/>
+      <c r="IP285" s="93"/>
+      <c r="IQ285" s="93"/>
+      <c r="IR285" s="93"/>
+      <c r="IS285" s="93"/>
+      <c r="IT285" s="93"/>
+      <c r="IU285" s="93"/>
+      <c r="IV285" s="93"/>
+      <c r="IW285" s="93"/>
+      <c r="IX285" s="93"/>
+      <c r="IY285" s="93"/>
+      <c r="IZ285" s="93"/>
+      <c r="JA285" s="93"/>
+      <c r="JB285" s="93"/>
+      <c r="JC285" s="93"/>
+      <c r="JD285" s="93"/>
+      <c r="JE285" s="93"/>
+      <c r="JF285" s="93"/>
+      <c r="JG285" s="93"/>
+      <c r="JH285" s="93"/>
+      <c r="JI285" s="93"/>
+      <c r="JJ285" s="93"/>
+      <c r="JK285" s="93"/>
+      <c r="JL285" s="93"/>
+      <c r="JM285" s="93"/>
+      <c r="JN285" s="93"/>
+      <c r="JO285" s="93"/>
+      <c r="JP285" s="93"/>
+      <c r="JQ285" s="93"/>
+      <c r="JR285" s="93"/>
+      <c r="JS285" s="93"/>
+      <c r="JT285" s="93"/>
+      <c r="JU285" s="93"/>
+      <c r="JV285" s="93"/>
+      <c r="JW285" s="93"/>
+      <c r="JX285" s="93"/>
+      <c r="JY285" s="93"/>
+      <c r="JZ285" s="93"/>
+      <c r="KA285" s="93"/>
+      <c r="KB285" s="93"/>
+      <c r="KC285" s="93"/>
+      <c r="KD285" s="93"/>
+      <c r="KE285" s="93"/>
+      <c r="KF285" s="93"/>
+      <c r="KG285" s="93"/>
+      <c r="KH285" s="93"/>
+      <c r="KI285" s="93"/>
+      <c r="KJ285" s="93"/>
+      <c r="KK285" s="93"/>
+      <c r="KL285" s="93"/>
+      <c r="KM285" s="93"/>
+      <c r="KN285" s="93"/>
+      <c r="KO285" s="93"/>
+      <c r="KP285" s="93"/>
+    </row>
+    <row r="286" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B286" s="97">
+        <v>3</v>
+      </c>
+      <c r="C286" s="97">
+        <v>1</v>
+      </c>
+      <c r="D286" s="97">
+        <v>3</v>
+      </c>
+      <c r="E286" s="97">
+        <v>0</v>
+      </c>
+      <c r="AH286" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI286" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ286" s="97">
+        <v>3</v>
+      </c>
+      <c r="AK286" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A287" s="46">
+        <v>132</v>
+      </c>
+      <c r="B287" s="98">
+        <v>3</v>
+      </c>
+      <c r="C287" s="98">
+        <v>3</v>
+      </c>
+      <c r="D287" s="87">
+        <v>1</v>
+      </c>
+      <c r="E287" s="98">
+        <v>3</v>
+      </c>
+      <c r="F287" s="28"/>
+      <c r="I287" s="30"/>
+      <c r="J287" s="28"/>
+      <c r="M287" s="30"/>
+      <c r="N287" s="29">
+        <v>3</v>
+      </c>
+      <c r="O287" s="29">
+        <v>4</v>
+      </c>
+      <c r="P287" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q287" s="28">
+        <v>5</v>
+      </c>
+      <c r="R287" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S287" s="65"/>
+      <c r="T287" s="65"/>
+      <c r="U287" s="65"/>
+      <c r="V287" s="65">
+        <v>2</v>
+      </c>
+      <c r="W287" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="X287" s="65"/>
+      <c r="Y287" s="65"/>
+      <c r="Z287" s="65"/>
+      <c r="AA287" s="65"/>
+      <c r="AB287" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC287" s="65"/>
+      <c r="AD287" s="65"/>
+      <c r="AE287" s="65"/>
+      <c r="AF287" s="65"/>
+      <c r="AG287" s="91"/>
+      <c r="AH287" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI287" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ287" s="98">
+        <v>4</v>
+      </c>
+      <c r="AK287" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP287" s="29">
+        <v>3</v>
+      </c>
+      <c r="AQ287" s="29">
+        <v>4</v>
+      </c>
+      <c r="AR287" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS287" s="28"/>
+      <c r="AT287" s="93"/>
+      <c r="AU287" s="93"/>
+      <c r="AV287" s="93"/>
+      <c r="AW287" s="93"/>
+      <c r="AX287" s="93"/>
+      <c r="AY287" s="93"/>
+      <c r="AZ287" s="93"/>
+      <c r="BA287" s="93"/>
+      <c r="BB287" s="93"/>
+      <c r="BC287" s="93"/>
+      <c r="BD287" s="93"/>
+      <c r="BE287" s="93"/>
+      <c r="BF287" s="93"/>
+      <c r="BG287" s="93"/>
+      <c r="BH287" s="93"/>
+      <c r="BI287" s="93"/>
+      <c r="BJ287" s="93"/>
+      <c r="BK287" s="93"/>
+      <c r="BL287" s="93"/>
+      <c r="BM287" s="93"/>
+      <c r="BN287" s="93"/>
+      <c r="BO287" s="93"/>
+      <c r="BP287" s="93"/>
+      <c r="BQ287" s="93"/>
+      <c r="BR287" s="93"/>
+      <c r="BS287" s="93"/>
+      <c r="BT287" s="93"/>
+      <c r="BU287" s="93"/>
+      <c r="BV287" s="93"/>
+      <c r="BW287" s="93"/>
+      <c r="BX287" s="93"/>
+      <c r="BY287" s="93"/>
+      <c r="BZ287" s="93"/>
+      <c r="CA287" s="93"/>
+      <c r="CB287" s="93"/>
+      <c r="CC287" s="93"/>
+      <c r="CD287" s="93"/>
+      <c r="CE287" s="93"/>
+      <c r="CF287" s="93"/>
+      <c r="CG287" s="93"/>
+      <c r="CH287" s="93"/>
+      <c r="CI287" s="93"/>
+      <c r="CJ287" s="93"/>
+      <c r="CK287" s="93"/>
+      <c r="CL287" s="93"/>
+      <c r="CM287" s="93"/>
+      <c r="CN287" s="93"/>
+      <c r="CO287" s="93"/>
+      <c r="CP287" s="93"/>
+      <c r="CQ287" s="93"/>
+      <c r="CR287" s="93"/>
+      <c r="CS287" s="93"/>
+      <c r="CT287" s="93"/>
+      <c r="CU287" s="93"/>
+      <c r="CV287" s="93"/>
+      <c r="CW287" s="93"/>
+      <c r="CX287" s="93"/>
+      <c r="CY287" s="93"/>
+      <c r="CZ287" s="93"/>
+      <c r="DA287" s="93"/>
+      <c r="DB287" s="93"/>
+      <c r="DC287" s="93"/>
+      <c r="DD287" s="93"/>
+      <c r="DE287" s="93"/>
+      <c r="DF287" s="93"/>
+      <c r="DG287" s="93"/>
+      <c r="DH287" s="93"/>
+      <c r="DI287" s="93"/>
+      <c r="DJ287" s="93"/>
+      <c r="DK287" s="93"/>
+      <c r="DL287" s="93"/>
+      <c r="DM287" s="93"/>
+      <c r="DN287" s="93"/>
+      <c r="DO287" s="93"/>
+      <c r="DP287" s="93"/>
+      <c r="DQ287" s="93"/>
+      <c r="DR287" s="93"/>
+      <c r="DS287" s="93"/>
+      <c r="DT287" s="93"/>
+      <c r="DU287" s="93"/>
+      <c r="DV287" s="93"/>
+      <c r="DW287" s="93"/>
+      <c r="DX287" s="93"/>
+      <c r="DY287" s="93"/>
+      <c r="DZ287" s="93"/>
+      <c r="EA287" s="93"/>
+      <c r="EB287" s="93"/>
+      <c r="EC287" s="93"/>
+      <c r="ED287" s="93"/>
+      <c r="EE287" s="93"/>
+      <c r="EF287" s="93"/>
+      <c r="EG287" s="93"/>
+      <c r="EH287" s="93"/>
+      <c r="EI287" s="93"/>
+      <c r="EJ287" s="93"/>
+      <c r="EK287" s="93"/>
+      <c r="EL287" s="93"/>
+      <c r="EM287" s="93"/>
+      <c r="EN287" s="93"/>
+      <c r="EO287" s="93"/>
+      <c r="EP287" s="93"/>
+      <c r="EQ287" s="93"/>
+      <c r="ER287" s="93"/>
+      <c r="ES287" s="93"/>
+      <c r="ET287" s="93"/>
+      <c r="EU287" s="93"/>
+      <c r="EV287" s="93"/>
+      <c r="EW287" s="93"/>
+      <c r="EX287" s="93"/>
+      <c r="EY287" s="93"/>
+      <c r="EZ287" s="93"/>
+      <c r="FA287" s="93"/>
+      <c r="FB287" s="93"/>
+      <c r="FC287" s="93"/>
+      <c r="FD287" s="93"/>
+      <c r="FE287" s="93"/>
+      <c r="FF287" s="93"/>
+      <c r="FG287" s="93"/>
+      <c r="FH287" s="93"/>
+      <c r="FI287" s="93"/>
+      <c r="FJ287" s="93"/>
+      <c r="FK287" s="93"/>
+      <c r="FL287" s="93"/>
+      <c r="FM287" s="93"/>
+      <c r="FN287" s="93"/>
+      <c r="FO287" s="93"/>
+      <c r="FP287" s="93"/>
+      <c r="FQ287" s="93"/>
+      <c r="FR287" s="93"/>
+      <c r="FS287" s="93"/>
+      <c r="FT287" s="93"/>
+      <c r="FU287" s="93"/>
+      <c r="FV287" s="93"/>
+      <c r="FW287" s="93"/>
+      <c r="FX287" s="93"/>
+      <c r="FY287" s="93"/>
+      <c r="FZ287" s="93"/>
+      <c r="GA287" s="93"/>
+      <c r="GB287" s="93"/>
+      <c r="GC287" s="93"/>
+      <c r="GD287" s="93"/>
+      <c r="GE287" s="93"/>
+      <c r="GF287" s="93"/>
+      <c r="GG287" s="93"/>
+      <c r="GH287" s="93"/>
+      <c r="GI287" s="93"/>
+      <c r="GJ287" s="93"/>
+      <c r="GK287" s="93"/>
+      <c r="GL287" s="93"/>
+      <c r="GM287" s="93"/>
+      <c r="GN287" s="93"/>
+      <c r="GO287" s="93"/>
+      <c r="GP287" s="93"/>
+      <c r="GQ287" s="93"/>
+      <c r="GR287" s="93"/>
+      <c r="GS287" s="93"/>
+      <c r="GT287" s="93"/>
+      <c r="GU287" s="93"/>
+      <c r="GV287" s="93"/>
+      <c r="GW287" s="93"/>
+      <c r="GX287" s="93"/>
+      <c r="GY287" s="93"/>
+      <c r="GZ287" s="93"/>
+      <c r="HA287" s="93"/>
+      <c r="HB287" s="93"/>
+      <c r="HC287" s="93"/>
+      <c r="HD287" s="93"/>
+      <c r="HE287" s="93"/>
+      <c r="HF287" s="93"/>
+      <c r="HG287" s="93"/>
+      <c r="HH287" s="93"/>
+      <c r="HI287" s="93"/>
+      <c r="HJ287" s="93"/>
+      <c r="HK287" s="93"/>
+      <c r="HL287" s="93"/>
+      <c r="HM287" s="93"/>
+      <c r="HN287" s="93"/>
+      <c r="HO287" s="93"/>
+      <c r="HP287" s="93"/>
+      <c r="HQ287" s="93"/>
+      <c r="HR287" s="93"/>
+      <c r="HS287" s="93"/>
+      <c r="HT287" s="93"/>
+      <c r="HU287" s="93"/>
+      <c r="HV287" s="93"/>
+      <c r="HW287" s="93"/>
+      <c r="HX287" s="93"/>
+      <c r="HY287" s="93"/>
+      <c r="HZ287" s="93"/>
+      <c r="IA287" s="93"/>
+      <c r="IB287" s="93"/>
+      <c r="IC287" s="93"/>
+      <c r="ID287" s="93"/>
+      <c r="IE287" s="93"/>
+      <c r="IF287" s="93"/>
+      <c r="IG287" s="93"/>
+      <c r="IH287" s="93"/>
+      <c r="II287" s="93"/>
+      <c r="IJ287" s="93"/>
+      <c r="IK287" s="93"/>
+      <c r="IL287" s="93"/>
+      <c r="IM287" s="93"/>
+      <c r="IN287" s="93"/>
+      <c r="IO287" s="93"/>
+      <c r="IP287" s="93"/>
+      <c r="IQ287" s="93"/>
+      <c r="IR287" s="93"/>
+      <c r="IS287" s="93"/>
+      <c r="IT287" s="93"/>
+      <c r="IU287" s="93"/>
+      <c r="IV287" s="93"/>
+      <c r="IW287" s="93"/>
+      <c r="IX287" s="93"/>
+      <c r="IY287" s="93"/>
+      <c r="IZ287" s="93"/>
+      <c r="JA287" s="93"/>
+      <c r="JB287" s="93"/>
+      <c r="JC287" s="93"/>
+      <c r="JD287" s="93"/>
+      <c r="JE287" s="93"/>
+      <c r="JF287" s="93"/>
+      <c r="JG287" s="93"/>
+      <c r="JH287" s="93"/>
+      <c r="JI287" s="93"/>
+      <c r="JJ287" s="93"/>
+      <c r="JK287" s="93"/>
+      <c r="JL287" s="93"/>
+      <c r="JM287" s="93"/>
+      <c r="JN287" s="93"/>
+      <c r="JO287" s="93"/>
+      <c r="JP287" s="93"/>
+      <c r="JQ287" s="93"/>
+      <c r="JR287" s="93"/>
+      <c r="JS287" s="93"/>
+      <c r="JT287" s="93"/>
+      <c r="JU287" s="93"/>
+      <c r="JV287" s="93"/>
+      <c r="JW287" s="93"/>
+      <c r="JX287" s="93"/>
+      <c r="JY287" s="93"/>
+      <c r="JZ287" s="93"/>
+      <c r="KA287" s="93"/>
+      <c r="KB287" s="93"/>
+      <c r="KC287" s="93"/>
+      <c r="KD287" s="93"/>
+      <c r="KE287" s="93"/>
+      <c r="KF287" s="93"/>
+      <c r="KG287" s="93"/>
+      <c r="KH287" s="93"/>
+      <c r="KI287" s="93"/>
+      <c r="KJ287" s="93"/>
+      <c r="KK287" s="93"/>
+      <c r="KL287" s="93"/>
+      <c r="KM287" s="93"/>
+      <c r="KN287" s="93"/>
+      <c r="KO287" s="93"/>
+      <c r="KP287" s="93"/>
+    </row>
+    <row r="288" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B288" s="97">
+        <v>3</v>
+      </c>
+      <c r="C288" s="97">
+        <v>1</v>
+      </c>
+      <c r="D288" s="97">
+        <v>3</v>
+      </c>
+      <c r="E288" s="97">
+        <v>0</v>
+      </c>
+      <c r="AH288" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI288" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ288" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK288" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A289" s="46">
+        <v>133</v>
+      </c>
+      <c r="B289" s="98">
+        <v>3</v>
+      </c>
+      <c r="C289" s="98">
+        <v>3</v>
+      </c>
+      <c r="D289" s="98">
+        <v>1</v>
+      </c>
+      <c r="E289" s="98">
+        <v>3</v>
+      </c>
+      <c r="F289" s="28"/>
+      <c r="I289" s="30"/>
+      <c r="J289" s="28"/>
+      <c r="M289" s="30"/>
+      <c r="N289" s="29">
+        <v>3</v>
+      </c>
+      <c r="O289" s="29">
+        <v>4</v>
+      </c>
+      <c r="P289" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q289" s="28">
+        <v>1</v>
+      </c>
+      <c r="R289" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S289" s="65"/>
+      <c r="T289" s="65"/>
+      <c r="U289" s="65"/>
+      <c r="V289" s="65"/>
+      <c r="W289" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="X289" s="65"/>
+      <c r="Y289" s="65"/>
+      <c r="Z289" s="65"/>
+      <c r="AA289" s="65"/>
+      <c r="AB289" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC289" s="65"/>
+      <c r="AD289" s="65"/>
+      <c r="AE289" s="65"/>
+      <c r="AF289" s="65"/>
+      <c r="AG289" s="91"/>
+      <c r="AH289" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI289" s="98">
+        <v>0</v>
+      </c>
+      <c r="AJ289" s="98">
+        <v>1</v>
+      </c>
+      <c r="AK289" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP289" s="29">
+        <v>3</v>
+      </c>
+      <c r="AQ289" s="29">
+        <v>4</v>
+      </c>
+      <c r="AR289" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS289" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="AT289" s="93"/>
+      <c r="AU289" s="93"/>
+      <c r="AV289" s="93"/>
+      <c r="AW289" s="93"/>
+      <c r="AX289" s="93"/>
+      <c r="AY289" s="93"/>
+      <c r="AZ289" s="93"/>
+      <c r="BA289" s="93"/>
+      <c r="BB289" s="93"/>
+      <c r="BC289" s="93"/>
+      <c r="BD289" s="93"/>
+      <c r="BE289" s="93"/>
+      <c r="BF289" s="93"/>
+      <c r="BG289" s="93"/>
+      <c r="BH289" s="93"/>
+      <c r="BI289" s="93"/>
+      <c r="BJ289" s="93"/>
+      <c r="BK289" s="93"/>
+      <c r="BL289" s="93"/>
+      <c r="BM289" s="93"/>
+      <c r="BN289" s="93"/>
+      <c r="BO289" s="93"/>
+      <c r="BP289" s="93"/>
+      <c r="BQ289" s="93"/>
+      <c r="BR289" s="93"/>
+      <c r="BS289" s="93"/>
+      <c r="BT289" s="93"/>
+      <c r="BU289" s="93"/>
+      <c r="BV289" s="93"/>
+      <c r="BW289" s="93"/>
+      <c r="BX289" s="93"/>
+      <c r="BY289" s="93"/>
+      <c r="BZ289" s="93"/>
+      <c r="CA289" s="93"/>
+      <c r="CB289" s="93"/>
+      <c r="CC289" s="93"/>
+      <c r="CD289" s="93"/>
+      <c r="CE289" s="93"/>
+      <c r="CF289" s="93"/>
+      <c r="CG289" s="93"/>
+      <c r="CH289" s="93"/>
+      <c r="CI289" s="93"/>
+      <c r="CJ289" s="93"/>
+      <c r="CK289" s="93"/>
+      <c r="CL289" s="93"/>
+      <c r="CM289" s="93"/>
+      <c r="CN289" s="93"/>
+      <c r="CO289" s="93"/>
+      <c r="CP289" s="93"/>
+      <c r="CQ289" s="93"/>
+      <c r="CR289" s="93"/>
+      <c r="CS289" s="93"/>
+      <c r="CT289" s="93"/>
+      <c r="CU289" s="93"/>
+      <c r="CV289" s="93"/>
+      <c r="CW289" s="93"/>
+      <c r="CX289" s="93"/>
+      <c r="CY289" s="93"/>
+      <c r="CZ289" s="93"/>
+      <c r="DA289" s="93"/>
+      <c r="DB289" s="93"/>
+      <c r="DC289" s="93"/>
+      <c r="DD289" s="93"/>
+      <c r="DE289" s="93"/>
+      <c r="DF289" s="93"/>
+      <c r="DG289" s="93"/>
+      <c r="DH289" s="93"/>
+      <c r="DI289" s="93"/>
+      <c r="DJ289" s="93"/>
+      <c r="DK289" s="93"/>
+      <c r="DL289" s="93"/>
+      <c r="DM289" s="93"/>
+      <c r="DN289" s="93"/>
+      <c r="DO289" s="93"/>
+      <c r="DP289" s="93"/>
+      <c r="DQ289" s="93"/>
+      <c r="DR289" s="93"/>
+      <c r="DS289" s="93"/>
+      <c r="DT289" s="93"/>
+      <c r="DU289" s="93"/>
+      <c r="DV289" s="93"/>
+      <c r="DW289" s="93"/>
+      <c r="DX289" s="93"/>
+      <c r="DY289" s="93"/>
+      <c r="DZ289" s="93"/>
+      <c r="EA289" s="93"/>
+      <c r="EB289" s="93"/>
+      <c r="EC289" s="93"/>
+      <c r="ED289" s="93"/>
+      <c r="EE289" s="93"/>
+      <c r="EF289" s="93"/>
+      <c r="EG289" s="93"/>
+      <c r="EH289" s="93"/>
+      <c r="EI289" s="93"/>
+      <c r="EJ289" s="93"/>
+      <c r="EK289" s="93"/>
+      <c r="EL289" s="93"/>
+      <c r="EM289" s="93"/>
+      <c r="EN289" s="93"/>
+      <c r="EO289" s="93"/>
+      <c r="EP289" s="93"/>
+      <c r="EQ289" s="93"/>
+      <c r="ER289" s="93"/>
+      <c r="ES289" s="93"/>
+      <c r="ET289" s="93"/>
+      <c r="EU289" s="93"/>
+      <c r="EV289" s="93"/>
+      <c r="EW289" s="93"/>
+      <c r="EX289" s="93"/>
+      <c r="EY289" s="93"/>
+      <c r="EZ289" s="93"/>
+      <c r="FA289" s="93"/>
+      <c r="FB289" s="93"/>
+      <c r="FC289" s="93"/>
+      <c r="FD289" s="93"/>
+      <c r="FE289" s="93"/>
+      <c r="FF289" s="93"/>
+      <c r="FG289" s="93"/>
+      <c r="FH289" s="93"/>
+      <c r="FI289" s="93"/>
+      <c r="FJ289" s="93"/>
+      <c r="FK289" s="93"/>
+      <c r="FL289" s="93"/>
+      <c r="FM289" s="93"/>
+      <c r="FN289" s="93"/>
+      <c r="FO289" s="93"/>
+      <c r="FP289" s="93"/>
+      <c r="FQ289" s="93"/>
+      <c r="FR289" s="93"/>
+      <c r="FS289" s="93"/>
+      <c r="FT289" s="93"/>
+      <c r="FU289" s="93"/>
+      <c r="FV289" s="93"/>
+      <c r="FW289" s="93"/>
+      <c r="FX289" s="93"/>
+      <c r="FY289" s="93"/>
+      <c r="FZ289" s="93"/>
+      <c r="GA289" s="93"/>
+      <c r="GB289" s="93"/>
+      <c r="GC289" s="93"/>
+      <c r="GD289" s="93"/>
+      <c r="GE289" s="93"/>
+      <c r="GF289" s="93"/>
+      <c r="GG289" s="93"/>
+      <c r="GH289" s="93"/>
+      <c r="GI289" s="93"/>
+      <c r="GJ289" s="93"/>
+      <c r="GK289" s="93"/>
+      <c r="GL289" s="93"/>
+      <c r="GM289" s="93"/>
+      <c r="GN289" s="93"/>
+      <c r="GO289" s="93"/>
+      <c r="GP289" s="93"/>
+      <c r="GQ289" s="93"/>
+      <c r="GR289" s="93"/>
+      <c r="GS289" s="93"/>
+      <c r="GT289" s="93"/>
+      <c r="GU289" s="93"/>
+      <c r="GV289" s="93"/>
+      <c r="GW289" s="93"/>
+      <c r="GX289" s="93"/>
+      <c r="GY289" s="93"/>
+      <c r="GZ289" s="93"/>
+      <c r="HA289" s="93"/>
+      <c r="HB289" s="93"/>
+      <c r="HC289" s="93"/>
+      <c r="HD289" s="93"/>
+      <c r="HE289" s="93"/>
+      <c r="HF289" s="93"/>
+      <c r="HG289" s="93"/>
+      <c r="HH289" s="93"/>
+      <c r="HI289" s="93"/>
+      <c r="HJ289" s="93"/>
+      <c r="HK289" s="93"/>
+      <c r="HL289" s="93"/>
+      <c r="HM289" s="93"/>
+      <c r="HN289" s="93"/>
+      <c r="HO289" s="93"/>
+      <c r="HP289" s="93"/>
+      <c r="HQ289" s="93"/>
+      <c r="HR289" s="93"/>
+      <c r="HS289" s="93"/>
+      <c r="HT289" s="93"/>
+      <c r="HU289" s="93"/>
+      <c r="HV289" s="93"/>
+      <c r="HW289" s="93"/>
+      <c r="HX289" s="93"/>
+      <c r="HY289" s="93"/>
+      <c r="HZ289" s="93"/>
+      <c r="IA289" s="93"/>
+      <c r="IB289" s="93"/>
+      <c r="IC289" s="93"/>
+      <c r="ID289" s="93"/>
+      <c r="IE289" s="93"/>
+      <c r="IF289" s="93"/>
+      <c r="IG289" s="93"/>
+      <c r="IH289" s="93"/>
+      <c r="II289" s="93"/>
+      <c r="IJ289" s="93"/>
+      <c r="IK289" s="93"/>
+      <c r="IL289" s="93"/>
+      <c r="IM289" s="93"/>
+      <c r="IN289" s="93"/>
+      <c r="IO289" s="93"/>
+      <c r="IP289" s="93"/>
+      <c r="IQ289" s="93"/>
+      <c r="IR289" s="93"/>
+      <c r="IS289" s="93"/>
+      <c r="IT289" s="93"/>
+      <c r="IU289" s="93"/>
+      <c r="IV289" s="93"/>
+      <c r="IW289" s="93"/>
+      <c r="IX289" s="93"/>
+      <c r="IY289" s="93"/>
+      <c r="IZ289" s="93"/>
+      <c r="JA289" s="93"/>
+      <c r="JB289" s="93"/>
+      <c r="JC289" s="93"/>
+      <c r="JD289" s="93"/>
+      <c r="JE289" s="93"/>
+      <c r="JF289" s="93"/>
+      <c r="JG289" s="93"/>
+      <c r="JH289" s="93"/>
+      <c r="JI289" s="93"/>
+      <c r="JJ289" s="93"/>
+      <c r="JK289" s="93"/>
+      <c r="JL289" s="93"/>
+      <c r="JM289" s="93"/>
+      <c r="JN289" s="93"/>
+      <c r="JO289" s="93"/>
+      <c r="JP289" s="93"/>
+      <c r="JQ289" s="93"/>
+      <c r="JR289" s="93"/>
+      <c r="JS289" s="93"/>
+      <c r="JT289" s="93"/>
+      <c r="JU289" s="93"/>
+      <c r="JV289" s="93"/>
+      <c r="JW289" s="93"/>
+      <c r="JX289" s="93"/>
+      <c r="JY289" s="93"/>
+      <c r="JZ289" s="93"/>
+      <c r="KA289" s="93"/>
+      <c r="KB289" s="93"/>
+      <c r="KC289" s="93"/>
+      <c r="KD289" s="93"/>
+      <c r="KE289" s="93"/>
+      <c r="KF289" s="93"/>
+      <c r="KG289" s="93"/>
+      <c r="KH289" s="93"/>
+      <c r="KI289" s="93"/>
+      <c r="KJ289" s="93"/>
+      <c r="KK289" s="93"/>
+      <c r="KL289" s="93"/>
+      <c r="KM289" s="93"/>
+      <c r="KN289" s="93"/>
+      <c r="KO289" s="93"/>
+      <c r="KP289" s="93"/>
+    </row>
+    <row r="290" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B290" s="97">
+        <v>3</v>
+      </c>
+      <c r="C290" s="97">
+        <v>1</v>
+      </c>
+      <c r="D290" s="97">
+        <v>3</v>
+      </c>
+      <c r="E290" s="97">
+        <v>0</v>
+      </c>
+      <c r="AH290" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI290" s="97">
+        <v>4</v>
+      </c>
+      <c r="AJ290" s="97">
+        <v>3</v>
+      </c>
+      <c r="AK290" s="97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A291" s="46">
+        <v>134</v>
+      </c>
+      <c r="B291" s="98">
+        <v>3</v>
+      </c>
+      <c r="C291" s="98">
+        <v>3</v>
+      </c>
+      <c r="D291" s="98">
+        <v>1</v>
+      </c>
+      <c r="E291" s="98">
+        <v>3</v>
+      </c>
+      <c r="F291" s="28"/>
+      <c r="I291" s="30"/>
+      <c r="J291" s="28"/>
+      <c r="M291" s="30"/>
+      <c r="N291" s="29">
+        <v>3</v>
+      </c>
+      <c r="O291" s="29">
+        <v>4</v>
+      </c>
+      <c r="P291" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q291" s="28">
+        <v>5</v>
+      </c>
+      <c r="R291" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S291" s="65"/>
+      <c r="T291" s="65"/>
+      <c r="U291" s="65"/>
+      <c r="V291" s="65"/>
+      <c r="W291" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="X291" s="65"/>
+      <c r="Y291" s="65"/>
+      <c r="Z291" s="65"/>
+      <c r="AA291" s="65"/>
+      <c r="AB291" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC291" s="65"/>
+      <c r="AD291" s="65"/>
+      <c r="AE291" s="65"/>
+      <c r="AF291" s="65"/>
+      <c r="AG291" s="91"/>
+      <c r="AH291" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI291" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ291" s="98">
+        <v>4</v>
+      </c>
+      <c r="AK291" s="98">
+        <v>3</v>
+      </c>
+      <c r="AP291" s="29">
+        <v>3</v>
+      </c>
+      <c r="AQ291" s="29">
+        <v>4</v>
+      </c>
+      <c r="AR291" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS291" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="AT291" s="93"/>
+      <c r="AU291" s="93"/>
+      <c r="AV291" s="93"/>
+      <c r="AW291" s="93"/>
+      <c r="AX291" s="93"/>
+      <c r="AY291" s="93"/>
+      <c r="AZ291" s="93"/>
+      <c r="BA291" s="93"/>
+      <c r="BB291" s="93"/>
+      <c r="BC291" s="93"/>
+      <c r="BD291" s="93"/>
+      <c r="BE291" s="93"/>
+      <c r="BF291" s="93"/>
+      <c r="BG291" s="93"/>
+      <c r="BH291" s="93"/>
+      <c r="BI291" s="93"/>
+      <c r="BJ291" s="93"/>
+      <c r="BK291" s="93"/>
+      <c r="BL291" s="93"/>
+      <c r="BM291" s="93"/>
+      <c r="BN291" s="93"/>
+      <c r="BO291" s="93"/>
+      <c r="BP291" s="93"/>
+      <c r="BQ291" s="93"/>
+      <c r="BR291" s="93"/>
+      <c r="BS291" s="93"/>
+      <c r="BT291" s="93"/>
+      <c r="BU291" s="93"/>
+      <c r="BV291" s="93"/>
+      <c r="BW291" s="93"/>
+      <c r="BX291" s="93"/>
+      <c r="BY291" s="93"/>
+      <c r="BZ291" s="93"/>
+      <c r="CA291" s="93"/>
+      <c r="CB291" s="93"/>
+      <c r="CC291" s="93"/>
+      <c r="CD291" s="93"/>
+      <c r="CE291" s="93"/>
+      <c r="CF291" s="93"/>
+      <c r="CG291" s="93"/>
+      <c r="CH291" s="93"/>
+      <c r="CI291" s="93"/>
+      <c r="CJ291" s="93"/>
+      <c r="CK291" s="93"/>
+      <c r="CL291" s="93"/>
+      <c r="CM291" s="93"/>
+      <c r="CN291" s="93"/>
+      <c r="CO291" s="93"/>
+      <c r="CP291" s="93"/>
+      <c r="CQ291" s="93"/>
+      <c r="CR291" s="93"/>
+      <c r="CS291" s="93"/>
+      <c r="CT291" s="93"/>
+      <c r="CU291" s="93"/>
+      <c r="CV291" s="93"/>
+      <c r="CW291" s="93"/>
+      <c r="CX291" s="93"/>
+      <c r="CY291" s="93"/>
+      <c r="CZ291" s="93"/>
+      <c r="DA291" s="93"/>
+      <c r="DB291" s="93"/>
+      <c r="DC291" s="93"/>
+      <c r="DD291" s="93"/>
+      <c r="DE291" s="93"/>
+      <c r="DF291" s="93"/>
+      <c r="DG291" s="93"/>
+      <c r="DH291" s="93"/>
+      <c r="DI291" s="93"/>
+      <c r="DJ291" s="93"/>
+      <c r="DK291" s="93"/>
+      <c r="DL291" s="93"/>
+      <c r="DM291" s="93"/>
+      <c r="DN291" s="93"/>
+      <c r="DO291" s="93"/>
+      <c r="DP291" s="93"/>
+      <c r="DQ291" s="93"/>
+      <c r="DR291" s="93"/>
+      <c r="DS291" s="93"/>
+      <c r="DT291" s="93"/>
+      <c r="DU291" s="93"/>
+      <c r="DV291" s="93"/>
+      <c r="DW291" s="93"/>
+      <c r="DX291" s="93"/>
+      <c r="DY291" s="93"/>
+      <c r="DZ291" s="93"/>
+      <c r="EA291" s="93"/>
+      <c r="EB291" s="93"/>
+      <c r="EC291" s="93"/>
+      <c r="ED291" s="93"/>
+      <c r="EE291" s="93"/>
+      <c r="EF291" s="93"/>
+      <c r="EG291" s="93"/>
+      <c r="EH291" s="93"/>
+      <c r="EI291" s="93"/>
+      <c r="EJ291" s="93"/>
+      <c r="EK291" s="93"/>
+      <c r="EL291" s="93"/>
+      <c r="EM291" s="93"/>
+      <c r="EN291" s="93"/>
+      <c r="EO291" s="93"/>
+      <c r="EP291" s="93"/>
+      <c r="EQ291" s="93"/>
+      <c r="ER291" s="93"/>
+      <c r="ES291" s="93"/>
+      <c r="ET291" s="93"/>
+      <c r="EU291" s="93"/>
+      <c r="EV291" s="93"/>
+      <c r="EW291" s="93"/>
+      <c r="EX291" s="93"/>
+      <c r="EY291" s="93"/>
+      <c r="EZ291" s="93"/>
+      <c r="FA291" s="93"/>
+      <c r="FB291" s="93"/>
+      <c r="FC291" s="93"/>
+      <c r="FD291" s="93"/>
+      <c r="FE291" s="93"/>
+      <c r="FF291" s="93"/>
+      <c r="FG291" s="93"/>
+      <c r="FH291" s="93"/>
+      <c r="FI291" s="93"/>
+      <c r="FJ291" s="93"/>
+      <c r="FK291" s="93"/>
+      <c r="FL291" s="93"/>
+      <c r="FM291" s="93"/>
+      <c r="FN291" s="93"/>
+      <c r="FO291" s="93"/>
+      <c r="FP291" s="93"/>
+      <c r="FQ291" s="93"/>
+      <c r="FR291" s="93"/>
+      <c r="FS291" s="93"/>
+      <c r="FT291" s="93"/>
+      <c r="FU291" s="93"/>
+      <c r="FV291" s="93"/>
+      <c r="FW291" s="93"/>
+      <c r="FX291" s="93"/>
+      <c r="FY291" s="93"/>
+      <c r="FZ291" s="93"/>
+      <c r="GA291" s="93"/>
+      <c r="GB291" s="93"/>
+      <c r="GC291" s="93"/>
+      <c r="GD291" s="93"/>
+      <c r="GE291" s="93"/>
+      <c r="GF291" s="93"/>
+      <c r="GG291" s="93"/>
+      <c r="GH291" s="93"/>
+      <c r="GI291" s="93"/>
+      <c r="GJ291" s="93"/>
+      <c r="GK291" s="93"/>
+      <c r="GL291" s="93"/>
+      <c r="GM291" s="93"/>
+      <c r="GN291" s="93"/>
+      <c r="GO291" s="93"/>
+      <c r="GP291" s="93"/>
+      <c r="GQ291" s="93"/>
+      <c r="GR291" s="93"/>
+      <c r="GS291" s="93"/>
+      <c r="GT291" s="93"/>
+      <c r="GU291" s="93"/>
+      <c r="GV291" s="93"/>
+      <c r="GW291" s="93"/>
+      <c r="GX291" s="93"/>
+      <c r="GY291" s="93"/>
+      <c r="GZ291" s="93"/>
+      <c r="HA291" s="93"/>
+      <c r="HB291" s="93"/>
+      <c r="HC291" s="93"/>
+      <c r="HD291" s="93"/>
+      <c r="HE291" s="93"/>
+      <c r="HF291" s="93"/>
+      <c r="HG291" s="93"/>
+      <c r="HH291" s="93"/>
+      <c r="HI291" s="93"/>
+      <c r="HJ291" s="93"/>
+      <c r="HK291" s="93"/>
+      <c r="HL291" s="93"/>
+      <c r="HM291" s="93"/>
+      <c r="HN291" s="93"/>
+      <c r="HO291" s="93"/>
+      <c r="HP291" s="93"/>
+      <c r="HQ291" s="93"/>
+      <c r="HR291" s="93"/>
+      <c r="HS291" s="93"/>
+      <c r="HT291" s="93"/>
+      <c r="HU291" s="93"/>
+      <c r="HV291" s="93"/>
+      <c r="HW291" s="93"/>
+      <c r="HX291" s="93"/>
+      <c r="HY291" s="93"/>
+      <c r="HZ291" s="93"/>
+      <c r="IA291" s="93"/>
+      <c r="IB291" s="93"/>
+      <c r="IC291" s="93"/>
+      <c r="ID291" s="93"/>
+      <c r="IE291" s="93"/>
+      <c r="IF291" s="93"/>
+      <c r="IG291" s="93"/>
+      <c r="IH291" s="93"/>
+      <c r="II291" s="93"/>
+      <c r="IJ291" s="93"/>
+      <c r="IK291" s="93"/>
+      <c r="IL291" s="93"/>
+      <c r="IM291" s="93"/>
+      <c r="IN291" s="93"/>
+      <c r="IO291" s="93"/>
+      <c r="IP291" s="93"/>
+      <c r="IQ291" s="93"/>
+      <c r="IR291" s="93"/>
+      <c r="IS291" s="93"/>
+      <c r="IT291" s="93"/>
+      <c r="IU291" s="93"/>
+      <c r="IV291" s="93"/>
+      <c r="IW291" s="93"/>
+      <c r="IX291" s="93"/>
+      <c r="IY291" s="93"/>
+      <c r="IZ291" s="93"/>
+      <c r="JA291" s="93"/>
+      <c r="JB291" s="93"/>
+      <c r="JC291" s="93"/>
+      <c r="JD291" s="93"/>
+      <c r="JE291" s="93"/>
+      <c r="JF291" s="93"/>
+      <c r="JG291" s="93"/>
+      <c r="JH291" s="93"/>
+      <c r="JI291" s="93"/>
+      <c r="JJ291" s="93"/>
+      <c r="JK291" s="93"/>
+      <c r="JL291" s="93"/>
+      <c r="JM291" s="93"/>
+      <c r="JN291" s="93"/>
+      <c r="JO291" s="93"/>
+      <c r="JP291" s="93"/>
+      <c r="JQ291" s="93"/>
+      <c r="JR291" s="93"/>
+      <c r="JS291" s="93"/>
+      <c r="JT291" s="93"/>
+      <c r="JU291" s="93"/>
+      <c r="JV291" s="93"/>
+      <c r="JW291" s="93"/>
+      <c r="JX291" s="93"/>
+      <c r="JY291" s="93"/>
+      <c r="JZ291" s="93"/>
+      <c r="KA291" s="93"/>
+      <c r="KB291" s="93"/>
+      <c r="KC291" s="93"/>
+      <c r="KD291" s="93"/>
+      <c r="KE291" s="93"/>
+      <c r="KF291" s="93"/>
+      <c r="KG291" s="93"/>
+      <c r="KH291" s="93"/>
+      <c r="KI291" s="93"/>
+      <c r="KJ291" s="93"/>
+      <c r="KK291" s="93"/>
+      <c r="KL291" s="93"/>
+      <c r="KM291" s="93"/>
+      <c r="KN291" s="93"/>
+      <c r="KO291" s="93"/>
+      <c r="KP291" s="93"/>
+    </row>
+    <row r="292" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="B292" s="97">
+        <v>3</v>
+      </c>
+      <c r="C292" s="97">
+        <v>1</v>
+      </c>
+      <c r="D292" s="97">
+        <v>3</v>
+      </c>
+      <c r="E292" s="97">
+        <v>0</v>
+      </c>
+      <c r="AH292" s="97">
+        <v>3</v>
+      </c>
+      <c r="AI292" s="97">
+        <v>1</v>
+      </c>
+      <c r="AJ292" s="97">
+        <v>0</v>
+      </c>
+      <c r="AK292" s="97">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
Changed the Grand Slam keep_left & _right to behave as described by the Hanson's on p 62--the only clear description I've found. Only used in one game and it might not be right there, game notes updated for Olowuka.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6B9989-B582-499C-B50E-8ED92BED04CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573056C8-CDD1-45E6-A248-30BF405281C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t>GS capt all but left (from true perspective)</t>
-  </si>
-  <si>
-    <t>technically GS, but keeping all, not a capt</t>
   </si>
   <si>
     <t>OPP_GETS</t>
@@ -646,6 +643,9 @@
   <si>
     <t>1 3 5</t>
   </si>
+  <si>
+    <t>capture the only cup, gs rules doesn't apply</t>
+  </si>
 </sst>
 </file>
 
@@ -875,7 +875,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1117,6 +1117,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1139,7 +1150,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1322,6 +1333,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1658,9 +1672,9 @@
   <dimension ref="A1:AMK312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A296" sqref="A296"/>
+      <selection pane="bottomLeft" activeCell="AS67" sqref="AS67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2764,7 +2778,7 @@
         <v>8</v>
       </c>
       <c r="T2" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="U2" s="49">
         <v>0</v>
@@ -3851,7 +3865,7 @@
         <v>19</v>
       </c>
       <c r="W3" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X3" s="51" t="s">
         <v>20</v>
@@ -3863,16 +3877,16 @@
         <v>22</v>
       </c>
       <c r="AA3" s="51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB3" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC3" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="AC3" s="51" t="s">
-        <v>143</v>
-      </c>
       <c r="AD3" s="51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE3" s="51" t="s">
         <v>23</v>
@@ -4631,7 +4645,7 @@
         <v>33</v>
       </c>
       <c r="AS5" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AT5" s="73"/>
       <c r="AU5" s="73"/>
@@ -6001,7 +6015,7 @@
       <c r="T11" s="55"/>
       <c r="U11" s="54"/>
       <c r="V11" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W11" s="54"/>
       <c r="X11" s="55"/>
@@ -9254,7 +9268,7 @@
         <v>31</v>
       </c>
       <c r="U21" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V21" s="59"/>
       <c r="W21" s="59"/>
@@ -9368,10 +9382,10 @@
       </c>
       <c r="T23" s="55"/>
       <c r="U23" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V23" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W23" s="54"/>
       <c r="X23" s="55"/>
@@ -10016,10 +10030,10 @@
         <v>31</v>
       </c>
       <c r="U25" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V25" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W25" s="59"/>
       <c r="AG25" s="61"/>
@@ -10134,10 +10148,10 @@
       </c>
       <c r="T27" s="55"/>
       <c r="U27" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V27" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W27" s="54"/>
       <c r="X27" s="55"/>
@@ -10789,7 +10803,7 @@
         <v>31</v>
       </c>
       <c r="U29" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V29" s="59"/>
       <c r="W29" s="59"/>
@@ -10907,7 +10921,7 @@
       </c>
       <c r="T31" s="55"/>
       <c r="U31" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V31" s="54"/>
       <c r="W31" s="54"/>
@@ -11667,7 +11681,7 @@
         <v>34</v>
       </c>
       <c r="U35" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V35" s="54"/>
       <c r="W35" s="54"/>
@@ -12313,11 +12327,11 @@
         <v>34</v>
       </c>
       <c r="U37" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V37" s="59"/>
       <c r="W37" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AG37" s="61"/>
       <c r="AH37">
@@ -12429,13 +12443,13 @@
       </c>
       <c r="T39" s="55"/>
       <c r="U39" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V39" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W39" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X39" s="55"/>
       <c r="Y39" s="55"/>
@@ -13079,11 +13093,11 @@
         <v>34</v>
       </c>
       <c r="U41" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V41" s="59"/>
       <c r="W41" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AG41" s="61"/>
       <c r="AH41">
@@ -13195,11 +13209,11 @@
       </c>
       <c r="T43" s="55"/>
       <c r="U43" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V43" s="54"/>
       <c r="W43" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X43" s="55"/>
       <c r="Y43" s="55"/>
@@ -14153,7 +14167,7 @@
       </c>
       <c r="U49" s="54"/>
       <c r="V49" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W49" s="54"/>
       <c r="X49" s="55"/>
@@ -14309,7 +14323,7 @@
       </c>
       <c r="U51" s="54"/>
       <c r="V51" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W51" s="54"/>
       <c r="X51" s="55"/>
@@ -14457,7 +14471,7 @@
       </c>
       <c r="T53" s="55"/>
       <c r="U53" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V53" s="55">
         <v>1</v>
@@ -15108,7 +15122,7 @@
       </c>
       <c r="T55" s="55"/>
       <c r="U55" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V55" s="55">
         <v>1</v>
@@ -15776,7 +15790,7 @@
       </c>
       <c r="T57" s="55"/>
       <c r="U57" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V57" s="55">
         <v>1</v>
@@ -16444,7 +16458,7 @@
       </c>
       <c r="T59" s="55"/>
       <c r="U59" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V59" s="55">
         <v>1</v>
@@ -17112,7 +17126,7 @@
       </c>
       <c r="T61" s="55"/>
       <c r="U61" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V61" s="55">
         <v>1</v>
@@ -17780,7 +17794,7 @@
       </c>
       <c r="T63" s="55"/>
       <c r="U63" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V63" s="55">
         <v>1</v>
@@ -18448,7 +18462,7 @@
       </c>
       <c r="T65" s="55"/>
       <c r="U65" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V65" s="55">
         <v>1</v>
@@ -18466,33 +18480,33 @@
       <c r="AE65" s="55"/>
       <c r="AF65" s="55"/>
       <c r="AG65" s="63"/>
-      <c r="AH65" s="13">
-        <v>0</v>
-      </c>
-      <c r="AI65" s="13">
-        <v>0</v>
-      </c>
-      <c r="AJ65" s="13">
-        <v>0</v>
-      </c>
-      <c r="AK65" s="13">
-        <v>2</v>
+      <c r="AH65" s="98">
+        <v>0</v>
+      </c>
+      <c r="AI65" s="98">
+        <v>0</v>
+      </c>
+      <c r="AJ65" s="98">
+        <v>0</v>
+      </c>
+      <c r="AK65" s="98">
+        <v>0</v>
       </c>
       <c r="AL65" s="13"/>
       <c r="AM65" s="13"/>
       <c r="AN65" s="13"/>
       <c r="AO65" s="13"/>
       <c r="AP65" s="13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AQ65" s="13">
         <v>5</v>
       </c>
       <c r="AR65" s="81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS65" s="17" t="s">
-        <v>67</v>
+        <v>203</v>
       </c>
       <c r="AT65" s="88"/>
       <c r="AU65" s="88"/>
@@ -18794,16 +18808,16 @@
       <c r="AE66" s="57"/>
       <c r="AF66" s="57"/>
       <c r="AG66" s="58"/>
-      <c r="AH66" s="18">
-        <v>3</v>
-      </c>
-      <c r="AI66" s="18">
-        <v>3</v>
-      </c>
-      <c r="AJ66" s="18">
-        <v>3</v>
-      </c>
-      <c r="AK66" s="18">
+      <c r="AH66" s="99">
+        <v>3</v>
+      </c>
+      <c r="AI66" s="100">
+        <v>3</v>
+      </c>
+      <c r="AJ66" s="100">
+        <v>3</v>
+      </c>
+      <c r="AK66" s="100">
         <v>3</v>
       </c>
       <c r="AL66" s="18"/>
@@ -19116,7 +19130,7 @@
       </c>
       <c r="T67" s="55"/>
       <c r="U67" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V67" s="55">
         <v>1</v>
@@ -19134,16 +19148,16 @@
       <c r="AE67" s="55"/>
       <c r="AF67" s="55"/>
       <c r="AG67" s="63"/>
-      <c r="AH67" s="13">
-        <v>3</v>
-      </c>
-      <c r="AI67" s="13">
-        <v>3</v>
-      </c>
-      <c r="AJ67" s="13">
-        <v>3</v>
-      </c>
-      <c r="AK67" s="13">
+      <c r="AH67" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI67" s="98">
+        <v>3</v>
+      </c>
+      <c r="AJ67" s="98">
+        <v>3</v>
+      </c>
+      <c r="AK67" s="98">
         <v>3</v>
       </c>
       <c r="AL67" s="13"/>
@@ -19154,13 +19168,13 @@
         <v>5</v>
       </c>
       <c r="AQ67" s="13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AR67" s="81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS67" s="17" t="s">
-        <v>67</v>
+        <v>203</v>
       </c>
       <c r="AT67" s="88"/>
       <c r="AU67" s="88"/>
@@ -19462,17 +19476,17 @@
       <c r="AE68" s="57"/>
       <c r="AF68" s="57"/>
       <c r="AG68" s="58"/>
-      <c r="AH68" s="18">
-        <v>0</v>
-      </c>
-      <c r="AI68" s="18">
-        <v>0</v>
-      </c>
-      <c r="AJ68" s="18">
-        <v>0</v>
-      </c>
-      <c r="AK68" s="18">
-        <v>2</v>
+      <c r="AH68" s="98">
+        <v>0</v>
+      </c>
+      <c r="AI68" s="98">
+        <v>0</v>
+      </c>
+      <c r="AJ68" s="98">
+        <v>0</v>
+      </c>
+      <c r="AK68" s="98">
+        <v>0</v>
       </c>
       <c r="AL68" s="18"/>
       <c r="AM68" s="18"/>
@@ -19784,7 +19798,7 @@
       </c>
       <c r="T69" s="55"/>
       <c r="U69" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V69" s="55">
         <v>1</v>
@@ -19828,7 +19842,7 @@
         <v>1</v>
       </c>
       <c r="AS69" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AT69" s="88"/>
       <c r="AU69" s="88"/>
@@ -20452,7 +20466,7 @@
       </c>
       <c r="T71" s="55"/>
       <c r="U71" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V71" s="55">
         <v>1</v>
@@ -20496,7 +20510,7 @@
         <v>1</v>
       </c>
       <c r="AS71" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AT71" s="88"/>
       <c r="AU71" s="88"/>
@@ -21120,7 +21134,7 @@
       </c>
       <c r="T73" s="55"/>
       <c r="U73" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V73" s="55">
         <v>1</v>
@@ -21129,7 +21143,7 @@
       <c r="X73" s="55"/>
       <c r="Y73" s="55"/>
       <c r="Z73" s="55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA73" s="55"/>
       <c r="AB73" s="55"/>
@@ -21164,7 +21178,7 @@
         <v>1</v>
       </c>
       <c r="AS73" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AT73" s="88"/>
       <c r="AU73" s="88"/>
@@ -21746,7 +21760,7 @@
     </row>
     <row r="75" spans="1:302" x14ac:dyDescent="0.2">
       <c r="A75" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B75" s="13">
         <v>2</v>
@@ -21788,7 +21802,7 @@
       </c>
       <c r="T75" s="55"/>
       <c r="U75" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V75" s="55">
         <v>1</v>
@@ -21797,7 +21811,7 @@
       <c r="X75" s="55"/>
       <c r="Y75" s="55"/>
       <c r="Z75" s="55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA75" s="55"/>
       <c r="AB75" s="55"/>
@@ -21832,7 +21846,7 @@
         <v>1</v>
       </c>
       <c r="AS75" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AT75" s="88"/>
       <c r="AU75" s="88"/>
@@ -22456,7 +22470,7 @@
       </c>
       <c r="T77" s="55"/>
       <c r="U77" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V77" s="55">
         <v>1</v>
@@ -22500,7 +22514,7 @@
         <v>1</v>
       </c>
       <c r="AS77" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:302" x14ac:dyDescent="0.2">
@@ -22610,7 +22624,7 @@
       </c>
       <c r="T79" s="55"/>
       <c r="U79" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V79" s="55">
         <v>1</v>
@@ -22654,7 +22668,7 @@
         <v>1</v>
       </c>
       <c r="AS79" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:302" x14ac:dyDescent="0.2">
@@ -22764,7 +22778,7 @@
       </c>
       <c r="T81" s="55"/>
       <c r="U81" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V81" s="55">
         <v>1</v>
@@ -22773,7 +22787,7 @@
       <c r="X81" s="55"/>
       <c r="Y81" s="55"/>
       <c r="Z81" s="55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA81" s="55"/>
       <c r="AB81" s="55"/>
@@ -22808,7 +22822,7 @@
         <v>1</v>
       </c>
       <c r="AS81" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:45" x14ac:dyDescent="0.2">
@@ -22915,10 +22929,10 @@
       </c>
       <c r="S83" s="55"/>
       <c r="T83" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U83" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V83" s="55">
         <v>1</v>
@@ -22962,7 +22976,7 @@
         <v>0</v>
       </c>
       <c r="AS83" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:45" x14ac:dyDescent="0.2">
@@ -23069,10 +23083,10 @@
       </c>
       <c r="S85" s="55"/>
       <c r="T85" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U85" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V85" s="55">
         <v>1</v>
@@ -23116,7 +23130,7 @@
         <v>0</v>
       </c>
       <c r="AS85" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:45" x14ac:dyDescent="0.2">
@@ -23223,10 +23237,10 @@
       </c>
       <c r="S87" s="55"/>
       <c r="T87" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U87" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V87" s="55">
         <v>1</v>
@@ -23235,7 +23249,7 @@
       <c r="X87" s="55"/>
       <c r="Y87" s="55"/>
       <c r="Z87" s="55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA87" s="55"/>
       <c r="AB87" s="55"/>
@@ -23270,7 +23284,7 @@
         <v>0</v>
       </c>
       <c r="AS87" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:45" x14ac:dyDescent="0.2">
@@ -23377,10 +23391,10 @@
       </c>
       <c r="S89" s="55"/>
       <c r="T89" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U89" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V89" s="55">
         <v>1</v>
@@ -23389,7 +23403,7 @@
       <c r="X89" s="55"/>
       <c r="Y89" s="55"/>
       <c r="Z89" s="55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA89" s="55"/>
       <c r="AB89" s="55"/>
@@ -23424,7 +23438,7 @@
         <v>0</v>
       </c>
       <c r="AS89" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:45" x14ac:dyDescent="0.2">
@@ -23531,10 +23545,10 @@
       </c>
       <c r="S91" s="55"/>
       <c r="T91" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U91" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V91" s="55"/>
       <c r="W91" s="55"/>
@@ -23574,7 +23588,7 @@
         <v>1</v>
       </c>
       <c r="AS91" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="1:45" x14ac:dyDescent="0.2">
@@ -23681,10 +23695,10 @@
       </c>
       <c r="S93" s="55"/>
       <c r="T93" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U93" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V93" s="55"/>
       <c r="W93" s="55"/>
@@ -23724,7 +23738,7 @@
         <v>1</v>
       </c>
       <c r="AS93" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:45" x14ac:dyDescent="0.2">
@@ -23831,10 +23845,10 @@
       </c>
       <c r="S95" s="55"/>
       <c r="T95" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U95" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V95" s="55"/>
       <c r="W95" s="55"/>
@@ -23876,7 +23890,7 @@
         <v>1</v>
       </c>
       <c r="AS95" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="1:45" x14ac:dyDescent="0.2">
@@ -23983,10 +23997,10 @@
       </c>
       <c r="S97" s="55"/>
       <c r="T97" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U97" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V97" s="55"/>
       <c r="W97" s="55"/>
@@ -24028,7 +24042,7 @@
         <v>1</v>
       </c>
       <c r="AS97" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="98" spans="1:45" x14ac:dyDescent="0.2">
@@ -24139,7 +24153,7 @@
       <c r="V99" s="55"/>
       <c r="W99" s="55"/>
       <c r="X99" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y99" s="55"/>
       <c r="Z99" s="55"/>
@@ -24287,7 +24301,7 @@
       <c r="V101" s="55"/>
       <c r="W101" s="55"/>
       <c r="X101" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y101" s="55"/>
       <c r="Z101" s="55"/>
@@ -24324,7 +24338,7 @@
         <v>0</v>
       </c>
       <c r="AS101" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="102" spans="1:45" x14ac:dyDescent="0.2">
@@ -24435,7 +24449,7 @@
       <c r="V103" s="55"/>
       <c r="W103" s="55"/>
       <c r="X103" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y103" s="55"/>
       <c r="Z103" s="55"/>
@@ -24472,7 +24486,7 @@
         <v>1</v>
       </c>
       <c r="AS103" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="104" spans="1:45" x14ac:dyDescent="0.2">
@@ -24583,7 +24597,7 @@
       <c r="V105" s="55"/>
       <c r="W105" s="55"/>
       <c r="X105" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y105" s="55"/>
       <c r="Z105" s="55"/>
@@ -24620,7 +24634,7 @@
         <v>0</v>
       </c>
       <c r="AS105" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="106" spans="1:45" x14ac:dyDescent="0.2">
@@ -24733,7 +24747,7 @@
       </c>
       <c r="W107" s="55"/>
       <c r="X107" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y107" s="55"/>
       <c r="Z107" s="55"/>
@@ -24770,7 +24784,7 @@
         <v>0</v>
       </c>
       <c r="AS107" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:45" x14ac:dyDescent="0.2">
@@ -24883,7 +24897,7 @@
       </c>
       <c r="W109" s="55"/>
       <c r="X109" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y109" s="55"/>
       <c r="Z109" s="55"/>
@@ -24920,7 +24934,7 @@
         <v>0</v>
       </c>
       <c r="AS109" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" spans="1:45" x14ac:dyDescent="0.2">
@@ -25033,7 +25047,7 @@
       </c>
       <c r="W111" s="55"/>
       <c r="X111" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y111" s="55"/>
       <c r="Z111" s="55"/>
@@ -25070,7 +25084,7 @@
         <v>1</v>
       </c>
       <c r="AS111" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="1:45" x14ac:dyDescent="0.2">
@@ -25183,7 +25197,7 @@
       </c>
       <c r="W113" s="55"/>
       <c r="X113" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y113" s="55"/>
       <c r="Z113" s="55"/>
@@ -25220,7 +25234,7 @@
         <v>0</v>
       </c>
       <c r="AS113" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="114" spans="1:45" x14ac:dyDescent="0.2">
@@ -25333,10 +25347,10 @@
       </c>
       <c r="W115" s="55"/>
       <c r="X115" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y115" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z115" s="55"/>
       <c r="AA115" s="55"/>
@@ -25372,7 +25386,7 @@
         <v>1</v>
       </c>
       <c r="AS115" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:45" x14ac:dyDescent="0.2">
@@ -25485,10 +25499,10 @@
       </c>
       <c r="W117" s="55"/>
       <c r="X117" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y117" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z117" s="55"/>
       <c r="AA117" s="55"/>
@@ -25524,7 +25538,7 @@
         <v>0</v>
       </c>
       <c r="AS117" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="118" spans="1:45" x14ac:dyDescent="0.2">
@@ -25592,7 +25606,7 @@
     </row>
     <row r="119" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A119" s="40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B119" s="13">
         <v>3</v>
@@ -25637,10 +25651,10 @@
       </c>
       <c r="W119" s="55"/>
       <c r="X119" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y119" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z119" s="55"/>
       <c r="AA119" s="55"/>
@@ -25676,7 +25690,7 @@
         <v>1</v>
       </c>
       <c r="AS119" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:45" x14ac:dyDescent="0.2">
@@ -25744,7 +25758,7 @@
     </row>
     <row r="121" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A121" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B121" s="13">
         <v>3</v>
@@ -25789,10 +25803,10 @@
       </c>
       <c r="W121" s="55"/>
       <c r="X121" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y121" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z121" s="55"/>
       <c r="AA121" s="55"/>
@@ -25828,7 +25842,7 @@
         <v>1</v>
       </c>
       <c r="AS121" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="1:45" x14ac:dyDescent="0.2">
@@ -25896,7 +25910,7 @@
     </row>
     <row r="123" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A123" s="40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B123" s="13">
         <v>3</v>
@@ -25941,10 +25955,10 @@
       </c>
       <c r="W123" s="55"/>
       <c r="X123" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y123" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z123" s="55"/>
       <c r="AA123" s="55"/>
@@ -25980,7 +25994,7 @@
         <v>1</v>
       </c>
       <c r="AS123" s="26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="124" spans="1:45" x14ac:dyDescent="0.2">
@@ -26048,7 +26062,7 @@
     </row>
     <row r="125" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A125" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B125" s="13">
         <v>3</v>
@@ -26093,10 +26107,10 @@
       </c>
       <c r="W125" s="55"/>
       <c r="X125" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y125" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z125" s="55"/>
       <c r="AA125" s="55"/>
@@ -26132,7 +26146,7 @@
         <v>1</v>
       </c>
       <c r="AS125" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="126" spans="1:45" x14ac:dyDescent="0.2">
@@ -26243,10 +26257,10 @@
       <c r="V127" s="55"/>
       <c r="W127" s="55"/>
       <c r="X127" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y127" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z127" s="55"/>
       <c r="AA127" s="55"/>
@@ -26282,7 +26296,7 @@
         <v>1</v>
       </c>
       <c r="AS127" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="128" spans="1:45" x14ac:dyDescent="0.2">
@@ -26393,10 +26407,10 @@
       <c r="V129" s="55"/>
       <c r="W129" s="55"/>
       <c r="X129" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y129" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z129" s="55"/>
       <c r="AA129" s="55"/>
@@ -26432,7 +26446,7 @@
         <v>0</v>
       </c>
       <c r="AS129" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="130" spans="1:45" x14ac:dyDescent="0.2">
@@ -26543,10 +26557,10 @@
       <c r="V131" s="55"/>
       <c r="W131" s="55"/>
       <c r="X131" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y131" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z131" s="55"/>
       <c r="AA131" s="55"/>
@@ -26582,7 +26596,7 @@
         <v>1</v>
       </c>
       <c r="AS131" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="132" spans="1:45" x14ac:dyDescent="0.2">
@@ -26693,10 +26707,10 @@
       <c r="V133" s="55"/>
       <c r="W133" s="55"/>
       <c r="X133" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y133" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z133" s="55"/>
       <c r="AA133" s="55"/>
@@ -26732,7 +26746,7 @@
         <v>1</v>
       </c>
       <c r="AS133" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="134" spans="1:45" x14ac:dyDescent="0.2">
@@ -26843,10 +26857,10 @@
       <c r="V135" s="55"/>
       <c r="W135" s="55"/>
       <c r="X135" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y135" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z135" s="55"/>
       <c r="AA135" s="55"/>
@@ -26882,7 +26896,7 @@
         <v>0</v>
       </c>
       <c r="AS135" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="136" spans="1:45" x14ac:dyDescent="0.2">
@@ -26993,10 +27007,10 @@
       <c r="V137" s="55"/>
       <c r="W137" s="55"/>
       <c r="X137" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y137" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z137" s="55"/>
       <c r="AA137" s="55"/>
@@ -27038,7 +27052,7 @@
         <v>1</v>
       </c>
       <c r="AS137" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="138" spans="1:45" x14ac:dyDescent="0.2">
@@ -27151,10 +27165,10 @@
       <c r="V139" s="55"/>
       <c r="W139" s="55"/>
       <c r="X139" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y139" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z139" s="55"/>
       <c r="AA139" s="55"/>
@@ -27196,7 +27210,7 @@
         <v>1</v>
       </c>
       <c r="AS139" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="140" spans="1:45" x14ac:dyDescent="0.2">
@@ -27311,10 +27325,10 @@
       <c r="V141" s="55"/>
       <c r="W141" s="55"/>
       <c r="X141" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y141" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z141" s="55"/>
       <c r="AA141" s="55"/>
@@ -27356,7 +27370,7 @@
         <v>0</v>
       </c>
       <c r="AS141" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="142" spans="1:45" x14ac:dyDescent="0.2">
@@ -27469,10 +27483,10 @@
       <c r="V143" s="55"/>
       <c r="W143" s="55"/>
       <c r="X143" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y143" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z143" s="55"/>
       <c r="AA143" s="55"/>
@@ -27514,7 +27528,7 @@
         <v>0</v>
       </c>
       <c r="AS143" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="144" spans="1:45" x14ac:dyDescent="0.2">
@@ -27626,14 +27640,14 @@
       <c r="S145" s="54"/>
       <c r="T145" s="55"/>
       <c r="U145" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V145" s="54"/>
       <c r="W145" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X145" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y145" s="55"/>
       <c r="Z145" s="55"/>
@@ -27670,7 +27684,7 @@
         <v>31</v>
       </c>
       <c r="AS145" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="146" spans="1:302" x14ac:dyDescent="0.2">
@@ -27778,14 +27792,14 @@
       <c r="S147" s="54"/>
       <c r="T147" s="55"/>
       <c r="U147" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V147" s="54"/>
       <c r="W147" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X147" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y147" s="55"/>
       <c r="Z147" s="55"/>
@@ -27822,7 +27836,7 @@
         <v>31</v>
       </c>
       <c r="AS147" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="148" spans="1:302" x14ac:dyDescent="0.2">
@@ -27930,14 +27944,14 @@
       <c r="S149" s="54"/>
       <c r="T149" s="55"/>
       <c r="U149" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V149" s="54"/>
       <c r="W149" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X149" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y149" s="55"/>
       <c r="Z149" s="55"/>
@@ -27974,7 +27988,7 @@
         <v>31</v>
       </c>
       <c r="AS149" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="150" spans="1:302" x14ac:dyDescent="0.2">
@@ -28083,16 +28097,16 @@
       </c>
       <c r="S151" s="59"/>
       <c r="U151" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V151" s="59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W151" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X151" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AF151" s="60" t="b">
         <v>1</v>
@@ -28124,7 +28138,7 @@
         <v>31</v>
       </c>
       <c r="AS151" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="152" spans="1:302" x14ac:dyDescent="0.2">
@@ -28219,16 +28233,16 @@
       <c r="S153" s="54"/>
       <c r="T153" s="55"/>
       <c r="U153" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V153" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W153" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X153" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y153" s="55"/>
       <c r="Z153" s="55"/>
@@ -28377,14 +28391,14 @@
       </c>
       <c r="S155" s="59"/>
       <c r="U155" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V155" s="59"/>
       <c r="W155" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X155" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AG155" s="61" t="s">
         <v>31</v>
@@ -28415,7 +28429,7 @@
         <v>31</v>
       </c>
       <c r="AS155" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="156" spans="1:302" x14ac:dyDescent="0.2">
@@ -28498,14 +28512,14 @@
       <c r="S157" s="54"/>
       <c r="T157" s="55"/>
       <c r="U157" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V157" s="54"/>
       <c r="W157" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X157" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y157" s="55"/>
       <c r="Z157" s="55"/>
@@ -28538,7 +28552,7 @@
         <v>31</v>
       </c>
       <c r="AS157" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AT157" s="73"/>
       <c r="AU157" s="73"/>
@@ -29148,17 +29162,17 @@
       </c>
       <c r="S159" s="59"/>
       <c r="U159" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V159" s="59"/>
       <c r="W159" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X159" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y159" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AG159" s="61" t="s">
         <v>31</v>
@@ -29189,7 +29203,7 @@
         <v>31</v>
       </c>
       <c r="AS159" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="160" spans="1:302" x14ac:dyDescent="0.2">
@@ -29276,17 +29290,17 @@
       <c r="S161" s="54"/>
       <c r="T161" s="55"/>
       <c r="U161" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V161" s="54"/>
       <c r="W161" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X161" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y161" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Z161" s="55"/>
       <c r="AA161" s="55"/>
@@ -29322,7 +29336,7 @@
         <v>31</v>
       </c>
       <c r="AS161" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="162" spans="1:45" x14ac:dyDescent="0.2">
@@ -29432,14 +29446,14 @@
       <c r="S163" s="54"/>
       <c r="T163" s="55"/>
       <c r="U163" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V163" s="54"/>
       <c r="W163" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X163" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y163" s="55"/>
       <c r="Z163" s="55"/>
@@ -29476,7 +29490,7 @@
         <v>33</v>
       </c>
       <c r="AS163" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="164" spans="1:45" x14ac:dyDescent="0.2">
@@ -29584,17 +29598,17 @@
       <c r="S165" s="54"/>
       <c r="T165" s="55"/>
       <c r="U165" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V165" s="54"/>
       <c r="W165" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X165" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y165" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z165" s="55"/>
       <c r="AA165" s="55"/>
@@ -29630,7 +29644,7 @@
         <v>33</v>
       </c>
       <c r="AS165" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="166" spans="1:45" x14ac:dyDescent="0.2">
@@ -29738,17 +29752,17 @@
       <c r="S167" s="54"/>
       <c r="T167" s="55"/>
       <c r="U167" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V167" s="54"/>
       <c r="W167" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X167" s="55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y167" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z167" s="55"/>
       <c r="AA167" s="55"/>
@@ -29784,7 +29798,7 @@
         <v>31</v>
       </c>
       <c r="AS167" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="168" spans="1:45" x14ac:dyDescent="0.2">
@@ -29849,7 +29863,7 @@
       <c r="AQ168" s="18"/>
       <c r="AR168" s="78"/>
       <c r="AS168" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="169" spans="1:45" x14ac:dyDescent="0.2">
@@ -29934,7 +29948,7 @@
         <v>31</v>
       </c>
       <c r="AS169" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="170" spans="1:45" x14ac:dyDescent="0.2">
@@ -30082,7 +30096,7 @@
         <v>33</v>
       </c>
       <c r="AS171" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="172" spans="1:45" x14ac:dyDescent="0.2">
@@ -30192,14 +30206,14 @@
       <c r="U173" s="55"/>
       <c r="V173" s="55"/>
       <c r="W173" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X173" s="55"/>
       <c r="Y173" s="55"/>
       <c r="Z173" s="55"/>
       <c r="AA173" s="55"/>
       <c r="AB173" s="55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC173" s="55"/>
       <c r="AD173" s="55"/>
@@ -30232,7 +30246,7 @@
         <v>1</v>
       </c>
       <c r="AS173" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="174" spans="1:45" x14ac:dyDescent="0.2">
@@ -30264,7 +30278,7 @@
     </row>
     <row r="175" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A175" s="40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B175" s="13">
         <v>3</v>
@@ -30306,14 +30320,14 @@
       <c r="U175" s="55"/>
       <c r="V175" s="55"/>
       <c r="W175" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X175" s="55"/>
       <c r="Y175" s="55"/>
       <c r="Z175" s="55"/>
       <c r="AA175" s="55"/>
       <c r="AB175" s="55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC175" s="55"/>
       <c r="AD175" s="55">
@@ -30350,7 +30364,7 @@
         <v>0</v>
       </c>
       <c r="AS175" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="176" spans="1:45" x14ac:dyDescent="0.2">
@@ -30388,7 +30402,7 @@
     </row>
     <row r="177" spans="1:302" x14ac:dyDescent="0.2">
       <c r="A177" s="40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B177" s="13">
         <v>3</v>
@@ -30430,14 +30444,14 @@
       <c r="U177" s="55"/>
       <c r="V177" s="55"/>
       <c r="W177" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X177" s="55"/>
       <c r="Y177" s="55"/>
       <c r="Z177" s="55"/>
       <c r="AA177" s="55"/>
       <c r="AB177" s="55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC177" s="55"/>
       <c r="AD177" s="55">
@@ -30474,7 +30488,7 @@
         <v>1</v>
       </c>
       <c r="AS177" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="178" spans="1:302" x14ac:dyDescent="0.2">
@@ -30546,14 +30560,14 @@
       <c r="U179" s="64"/>
       <c r="V179" s="64"/>
       <c r="W179" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X179" s="65"/>
       <c r="Y179" s="65"/>
       <c r="Z179" s="65"/>
       <c r="AA179" s="65"/>
       <c r="AB179" s="55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC179" s="65"/>
       <c r="AD179" s="65"/>
@@ -30584,7 +30598,7 @@
         <v>31</v>
       </c>
       <c r="AS179" s="36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AT179" s="73"/>
       <c r="AU179" s="73"/>
@@ -31195,14 +31209,14 @@
       <c r="U181" s="64"/>
       <c r="V181" s="64"/>
       <c r="W181" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X181" s="65"/>
       <c r="Y181" s="65"/>
       <c r="Z181" s="65"/>
       <c r="AA181" s="65"/>
       <c r="AB181" s="55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC181" s="65"/>
       <c r="AD181" s="65"/>
@@ -31237,7 +31251,7 @@
         <v>33</v>
       </c>
       <c r="AS181" s="36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="182" spans="1:302" x14ac:dyDescent="0.2">
@@ -31347,14 +31361,14 @@
       <c r="U183" s="64"/>
       <c r="V183" s="64"/>
       <c r="W183" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X183" s="65"/>
       <c r="Y183" s="65"/>
       <c r="Z183" s="65"/>
       <c r="AA183" s="65"/>
       <c r="AB183" s="55" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AC183" s="65"/>
       <c r="AD183" s="65"/>
@@ -31389,7 +31403,7 @@
         <v>33</v>
       </c>
       <c r="AS183" s="36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="184" spans="1:302" x14ac:dyDescent="0.2">
@@ -31499,14 +31513,14 @@
       <c r="U185" s="55"/>
       <c r="V185" s="55"/>
       <c r="W185" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X185" s="55"/>
       <c r="Y185" s="55"/>
       <c r="Z185" s="55"/>
       <c r="AA185" s="55"/>
       <c r="AB185" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD185" s="55"/>
       <c r="AE185" s="55"/>
@@ -31538,7 +31552,7 @@
         <v>1</v>
       </c>
       <c r="AS185" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AU185" s="73">
         <f t="shared" ref="AU185" si="0">SUM(B185:E186)+SUM(N185:O185)</f>
@@ -31579,7 +31593,7 @@
     </row>
     <row r="187" spans="1:302" x14ac:dyDescent="0.2">
       <c r="A187" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B187" s="13">
         <v>3</v>
@@ -31626,7 +31640,7 @@
       <c r="Z187" s="55"/>
       <c r="AA187" s="55"/>
       <c r="AB187" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD187" s="55"/>
       <c r="AE187" s="55"/>
@@ -31658,7 +31672,7 @@
         <v>0</v>
       </c>
       <c r="AS187" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AU187" s="73">
         <f t="shared" ref="AU187" si="2">SUM(B187:E188)+SUM(N187:O187)</f>
@@ -31699,7 +31713,7 @@
     </row>
     <row r="189" spans="1:302" x14ac:dyDescent="0.2">
       <c r="A189" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B189" s="13">
         <v>3</v>
@@ -31746,7 +31760,7 @@
       <c r="Z189" s="55"/>
       <c r="AA189" s="55"/>
       <c r="AB189" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD189" s="55"/>
       <c r="AE189" s="55"/>
@@ -31778,7 +31792,7 @@
         <v>1</v>
       </c>
       <c r="AS189" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AT189" s="88"/>
       <c r="AU189" s="88">
@@ -32366,17 +32380,17 @@
       <c r="T191" s="65"/>
       <c r="U191" s="64"/>
       <c r="V191" s="64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W191" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X191" s="65"/>
       <c r="Y191" s="65"/>
       <c r="Z191" s="65"/>
       <c r="AA191" s="65"/>
       <c r="AB191" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC191" s="65"/>
       <c r="AD191" s="65"/>
@@ -32405,7 +32419,7 @@
         <v>31</v>
       </c>
       <c r="AS191" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AT191" s="73"/>
       <c r="AU191" s="73">
@@ -33021,17 +33035,17 @@
       <c r="T193" s="65"/>
       <c r="U193" s="64"/>
       <c r="V193" s="64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W193" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X193" s="65"/>
       <c r="Y193" s="65"/>
       <c r="Z193" s="65"/>
       <c r="AA193" s="65"/>
       <c r="AB193" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD193" s="65"/>
       <c r="AE193" s="65"/>
@@ -33063,7 +33077,7 @@
         <v>33</v>
       </c>
       <c r="AS193" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AU193" s="73">
         <f t="shared" ref="AU193:AU197" si="6">SUM(B193:E194)+SUM(N193:O193)</f>
@@ -33181,14 +33195,14 @@
       <c r="U195" s="55"/>
       <c r="V195" s="55"/>
       <c r="W195" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X195" s="55"/>
       <c r="Y195" s="55"/>
       <c r="Z195" s="55"/>
       <c r="AA195" s="55"/>
       <c r="AB195" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD195" s="55"/>
       <c r="AE195" s="55"/>
@@ -33220,7 +33234,7 @@
         <v>1</v>
       </c>
       <c r="AS195" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AU195" s="73">
         <f t="shared" si="6"/>
@@ -33305,14 +33319,14 @@
       <c r="U197" s="55"/>
       <c r="V197" s="55"/>
       <c r="W197" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X197" s="55"/>
       <c r="Y197" s="55"/>
       <c r="Z197" s="55"/>
       <c r="AA197" s="55"/>
       <c r="AB197" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AD197" s="55"/>
       <c r="AE197" s="55"/>
@@ -33344,7 +33358,7 @@
         <v>0</v>
       </c>
       <c r="AS197" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AU197" s="73">
         <f t="shared" si="6"/>
@@ -33460,18 +33474,18 @@
       <c r="S199" s="64"/>
       <c r="T199" s="65"/>
       <c r="U199" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V199" s="64"/>
       <c r="W199" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X199" s="65"/>
       <c r="Y199" s="65"/>
       <c r="Z199" s="65"/>
       <c r="AA199" s="65"/>
       <c r="AB199" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC199" s="65"/>
       <c r="AD199" s="65"/>
@@ -33504,7 +33518,7 @@
         <v>31</v>
       </c>
       <c r="AS199" s="36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="200" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -33856,20 +33870,20 @@
       <c r="S201" s="64"/>
       <c r="T201" s="65"/>
       <c r="U201" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V201" s="64" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W201" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X201" s="65"/>
       <c r="Y201" s="65"/>
       <c r="Z201" s="65"/>
       <c r="AA201" s="65"/>
       <c r="AB201" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC201" s="65"/>
       <c r="AD201" s="65"/>
@@ -33902,7 +33916,7 @@
         <v>31</v>
       </c>
       <c r="AS201" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="202" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -34258,18 +34272,18 @@
       <c r="S203" s="64"/>
       <c r="T203" s="65"/>
       <c r="U203" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V203" s="64"/>
       <c r="W203" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X203" s="65"/>
       <c r="Y203" s="65"/>
       <c r="Z203" s="65"/>
       <c r="AA203" s="65"/>
       <c r="AB203" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC203" s="65"/>
       <c r="AD203" s="65">
@@ -34310,7 +34324,7 @@
         <v>33</v>
       </c>
       <c r="AS203" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="204" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -34666,14 +34680,14 @@
       <c r="U205" s="64"/>
       <c r="V205" s="64"/>
       <c r="W205" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X205" s="65"/>
       <c r="Y205" s="65"/>
       <c r="Z205" s="65"/>
       <c r="AA205" s="65"/>
       <c r="AB205" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC205" s="65"/>
       <c r="AD205" s="65">
@@ -34710,7 +34724,7 @@
         <v>31</v>
       </c>
       <c r="AS205" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="206" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -35062,18 +35076,18 @@
       <c r="S207" s="64"/>
       <c r="T207" s="65"/>
       <c r="U207" s="64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="V207" s="64"/>
       <c r="W207" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X207" s="65"/>
       <c r="Y207" s="65"/>
       <c r="Z207" s="65"/>
       <c r="AA207" s="65"/>
       <c r="AB207" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC207" s="65"/>
       <c r="AD207" s="65"/>
@@ -35106,7 +35120,7 @@
         <v>31</v>
       </c>
       <c r="AS207" s="36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="208" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -35465,7 +35479,7 @@
       <c r="Z209" s="65"/>
       <c r="AA209" s="65"/>
       <c r="AB209" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC209" s="65"/>
       <c r="AD209" s="65"/>
@@ -35498,7 +35512,7 @@
         <v>31</v>
       </c>
       <c r="AS209" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AT209" s="88"/>
       <c r="AU209" s="88"/>
@@ -36114,7 +36128,7 @@
       <c r="Z211" s="65"/>
       <c r="AA211" s="65"/>
       <c r="AB211" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC211" s="65"/>
       <c r="AD211" s="65"/>
@@ -36147,7 +36161,7 @@
         <v>31</v>
       </c>
       <c r="AS211" s="36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AT211" s="88"/>
       <c r="AU211" s="88"/>
@@ -36763,7 +36777,7 @@
       <c r="Z213" s="65"/>
       <c r="AA213" s="65"/>
       <c r="AB213" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC213" s="65"/>
       <c r="AD213" s="65"/>
@@ -36796,7 +36810,7 @@
         <v>31</v>
       </c>
       <c r="AS213" s="36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AT213" s="88"/>
       <c r="AU213" s="88"/>
@@ -37412,7 +37426,7 @@
       <c r="Z215" s="65"/>
       <c r="AA215" s="65"/>
       <c r="AB215" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC215" s="65"/>
       <c r="AD215" s="65"/>
@@ -37445,7 +37459,7 @@
         <v>31</v>
       </c>
       <c r="AS215" s="36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AT215" s="88"/>
       <c r="AU215" s="88"/>
@@ -38061,7 +38075,7 @@
       <c r="Z217" s="65"/>
       <c r="AA217" s="65"/>
       <c r="AB217" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC217" s="65"/>
       <c r="AD217" s="65"/>
@@ -38094,7 +38108,7 @@
         <v>33</v>
       </c>
       <c r="AS217" s="36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AT217" s="88"/>
       <c r="AU217" s="88"/>
@@ -38710,7 +38724,7 @@
       <c r="Z219" s="65"/>
       <c r="AA219" s="65"/>
       <c r="AB219" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC219" s="65"/>
       <c r="AD219" s="65"/>
@@ -38743,7 +38757,7 @@
         <v>31</v>
       </c>
       <c r="AS219" s="36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AT219" s="88"/>
       <c r="AU219" s="88"/>
@@ -39312,7 +39326,7 @@
     </row>
     <row r="221" spans="1:302" x14ac:dyDescent="0.2">
       <c r="A221" s="40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B221" s="29">
         <v>2</v>
@@ -39352,18 +39366,18 @@
       <c r="S221" s="64"/>
       <c r="T221" s="65"/>
       <c r="U221" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V221" s="64"/>
       <c r="W221" s="64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X221" s="65"/>
       <c r="Y221" s="65"/>
       <c r="Z221" s="65"/>
       <c r="AA221" s="65"/>
       <c r="AB221" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC221" s="65"/>
       <c r="AD221" s="65"/>
@@ -39396,7 +39410,7 @@
         <v>31</v>
       </c>
       <c r="AS221" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AT221" s="88"/>
       <c r="AU221" s="88"/>
@@ -39965,7 +39979,7 @@
     </row>
     <row r="223" spans="1:302" x14ac:dyDescent="0.2">
       <c r="A223" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B223" s="29">
         <v>2</v>
@@ -40005,7 +40019,7 @@
       <c r="S223" s="64"/>
       <c r="T223" s="65"/>
       <c r="U223" s="64" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V223" s="64"/>
       <c r="W223" s="64"/>
@@ -40014,7 +40028,7 @@
       <c r="Z223" s="65"/>
       <c r="AA223" s="65"/>
       <c r="AB223" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC223" s="65"/>
       <c r="AD223" s="65"/>
@@ -40047,7 +40061,7 @@
         <v>31</v>
       </c>
       <c r="AS223" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AT223" s="88"/>
       <c r="AU223" s="88"/>
@@ -40665,7 +40679,7 @@
       <c r="Z225" s="65"/>
       <c r="AA225" s="65"/>
       <c r="AB225" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC225" s="65"/>
       <c r="AD225" s="65">
@@ -40704,7 +40718,7 @@
         <v>33</v>
       </c>
       <c r="AS225" s="36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AT225" s="88"/>
       <c r="AU225" s="88"/>
@@ -41322,7 +41336,7 @@
       <c r="Z227" s="65"/>
       <c r="AA227" s="65"/>
       <c r="AB227" s="55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC227" s="65"/>
       <c r="AD227" s="65">
@@ -41358,7 +41372,7 @@
         <v>33</v>
       </c>
       <c r="AS227" s="36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AT227" s="88"/>
       <c r="AU227" s="88"/>
@@ -41957,31 +41971,31 @@
         <v>44</v>
       </c>
       <c r="AB229" s="60" t="s">
+        <v>164</v>
+      </c>
+      <c r="AH229">
+        <v>3</v>
+      </c>
+      <c r="AI229">
+        <v>3</v>
+      </c>
+      <c r="AJ229">
+        <v>3</v>
+      </c>
+      <c r="AK229">
+        <v>3</v>
+      </c>
+      <c r="AP229">
+        <v>0</v>
+      </c>
+      <c r="AQ229">
+        <v>0</v>
+      </c>
+      <c r="AR229" s="80" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS229" t="s">
         <v>165</v>
-      </c>
-      <c r="AH229">
-        <v>3</v>
-      </c>
-      <c r="AI229">
-        <v>3</v>
-      </c>
-      <c r="AJ229">
-        <v>3</v>
-      </c>
-      <c r="AK229">
-        <v>3</v>
-      </c>
-      <c r="AP229">
-        <v>0</v>
-      </c>
-      <c r="AQ229">
-        <v>0</v>
-      </c>
-      <c r="AR229" s="80" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS229" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="230" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -42322,7 +42336,7 @@
         <v>44</v>
       </c>
       <c r="AB231" s="60" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AH231">
         <v>3</v>
@@ -42346,7 +42360,7 @@
         <v>1</v>
       </c>
       <c r="AS231" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="232" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -42693,7 +42707,7 @@
         <v>2</v>
       </c>
       <c r="W233" s="60" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AH233">
         <v>0</v>
@@ -42717,7 +42731,7 @@
         <v>1</v>
       </c>
       <c r="AS233" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="234" spans="1:302" x14ac:dyDescent="0.2">
@@ -42790,7 +42804,7 @@
       </c>
       <c r="V235" s="65"/>
       <c r="W235" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X235" s="65"/>
       <c r="Y235" s="65"/>
@@ -42824,7 +42838,7 @@
         <v>1</v>
       </c>
       <c r="AS235" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AT235" s="93"/>
       <c r="AU235" s="93"/>
@@ -43154,7 +43168,7 @@
       </c>
       <c r="V237" s="65"/>
       <c r="W237" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X237" s="65"/>
       <c r="Y237" s="65"/>
@@ -43188,7 +43202,7 @@
         <v>0</v>
       </c>
       <c r="AS237" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AT237" s="93"/>
       <c r="AU237" s="93"/>
@@ -43518,7 +43532,7 @@
       </c>
       <c r="V239" s="65"/>
       <c r="W239" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X239" s="65"/>
       <c r="Y239" s="65"/>
@@ -43552,7 +43566,7 @@
         <v>1</v>
       </c>
       <c r="AS239" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AT239" s="93"/>
       <c r="AU239" s="93"/>
@@ -43882,14 +43896,14 @@
       </c>
       <c r="V241" s="65"/>
       <c r="W241" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X241" s="65"/>
       <c r="Y241" s="65"/>
       <c r="Z241" s="65"/>
       <c r="AA241" s="65"/>
       <c r="AB241" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC241" s="65"/>
       <c r="AD241" s="65"/>
@@ -43918,10 +43932,10 @@
         <v>1</v>
       </c>
       <c r="AS241" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AT241" s="93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AU241" s="93"/>
       <c r="AV241" s="93"/>
@@ -44250,14 +44264,14 @@
       </c>
       <c r="V243" s="65"/>
       <c r="W243" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X243" s="65"/>
       <c r="Y243" s="65"/>
       <c r="Z243" s="65"/>
       <c r="AA243" s="65"/>
       <c r="AB243" s="65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC243" s="65"/>
       <c r="AD243" s="65"/>
@@ -44286,7 +44300,7 @@
         <v>1</v>
       </c>
       <c r="AS243" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AT243" s="93"/>
       <c r="AU243" s="93"/>
@@ -44616,7 +44630,7 @@
       </c>
       <c r="V245" s="65"/>
       <c r="W245" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X245" s="65"/>
       <c r="Y245" s="65"/>
@@ -44650,7 +44664,7 @@
         <v>0</v>
       </c>
       <c r="AS245" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AT245" s="93"/>
       <c r="AU245" s="93"/>
@@ -44980,14 +44994,14 @@
       </c>
       <c r="V247" s="65"/>
       <c r="W247" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X247" s="65"/>
       <c r="Y247" s="65"/>
       <c r="Z247" s="65"/>
       <c r="AA247" s="65"/>
       <c r="AB247" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC247" s="65"/>
       <c r="AD247" s="65"/>
@@ -45016,10 +45030,10 @@
         <v>1</v>
       </c>
       <c r="AS247" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AT247" s="93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AU247" s="93"/>
       <c r="AV247" s="93"/>
@@ -45304,12 +45318,12 @@
         <v>4</v>
       </c>
       <c r="AS248" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="249" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A249" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B249" s="29">
         <v>3</v>
@@ -45351,14 +45365,14 @@
       </c>
       <c r="V249" s="65"/>
       <c r="W249" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X249" s="65"/>
       <c r="Y249" s="65"/>
       <c r="Z249" s="65"/>
       <c r="AA249" s="65"/>
       <c r="AB249" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC249" s="65"/>
       <c r="AD249" s="65"/>
@@ -45387,10 +45401,10 @@
         <v>1</v>
       </c>
       <c r="AS249" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AT249" s="93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AU249" s="93"/>
       <c r="AV249" s="93"/>
@@ -45675,7 +45689,7 @@
         <v>4</v>
       </c>
       <c r="AS250" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="251" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
@@ -45722,14 +45736,14 @@
       </c>
       <c r="V251" s="65"/>
       <c r="W251" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X251" s="65"/>
       <c r="Y251" s="65"/>
       <c r="Z251" s="65"/>
       <c r="AA251" s="65"/>
       <c r="AB251" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC251" s="65"/>
       <c r="AD251" s="65"/>
@@ -45758,10 +45772,10 @@
         <v>1</v>
       </c>
       <c r="AS251" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AT251" s="93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AU251" s="93"/>
       <c r="AV251" s="93"/>
@@ -46090,14 +46104,14 @@
       </c>
       <c r="V253" s="65"/>
       <c r="W253" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="X253" s="65"/>
       <c r="Y253" s="65"/>
       <c r="Z253" s="65"/>
       <c r="AA253" s="65"/>
       <c r="AB253" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC253" s="65"/>
       <c r="AD253" s="65"/>
@@ -46126,10 +46140,10 @@
         <v>1</v>
       </c>
       <c r="AS253" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AT253" s="93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AU253" s="93"/>
       <c r="AV253" s="93"/>
@@ -46735,7 +46749,7 @@
         <v>3</v>
       </c>
       <c r="W255" s="60" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AH255">
         <v>0</v>
@@ -46759,7 +46773,7 @@
         <v>1</v>
       </c>
       <c r="AS255" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="256" spans="1:302" x14ac:dyDescent="0.2">
@@ -46834,7 +46848,7 @@
         <v>4</v>
       </c>
       <c r="W257" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X257" s="65"/>
       <c r="Y257" s="65"/>
@@ -46868,7 +46882,7 @@
         <v>1</v>
       </c>
       <c r="AS257" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AT257" s="93"/>
       <c r="AU257" s="93"/>
@@ -47471,7 +47485,7 @@
       </c>
       <c r="S259" s="65"/>
       <c r="T259" s="65" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U259" s="65"/>
       <c r="V259" s="65"/>
@@ -47481,7 +47495,7 @@
       <c r="Z259" s="65"/>
       <c r="AA259" s="65"/>
       <c r="AB259" s="65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC259" s="65"/>
       <c r="AD259" s="65"/>
@@ -47510,7 +47524,7 @@
         <v>1</v>
       </c>
       <c r="AS259" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AT259" s="93"/>
       <c r="AU259" s="93"/>
@@ -48113,7 +48127,7 @@
       </c>
       <c r="S261" s="65"/>
       <c r="T261" s="65" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="U261" s="65"/>
       <c r="V261" s="65"/>
@@ -48123,7 +48137,7 @@
       <c r="Z261" s="65"/>
       <c r="AA261" s="65"/>
       <c r="AB261" s="65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC261" s="65"/>
       <c r="AD261" s="65"/>
@@ -48152,7 +48166,7 @@
         <v>1</v>
       </c>
       <c r="AS261" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AT261" s="93"/>
       <c r="AU261" s="93"/>
@@ -48765,7 +48779,7 @@
       <c r="Z263" s="65"/>
       <c r="AA263" s="65"/>
       <c r="AB263" s="65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC263" s="65"/>
       <c r="AD263" s="65"/>
@@ -48794,7 +48808,7 @@
         <v>1</v>
       </c>
       <c r="AS263" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AT263" s="93"/>
       <c r="AU263" s="93"/>
@@ -49407,7 +49421,7 @@
       <c r="Z265" s="65"/>
       <c r="AA265" s="65"/>
       <c r="AB265" s="65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC265" s="65"/>
       <c r="AD265" s="65"/>
@@ -49436,7 +49450,7 @@
         <v>1</v>
       </c>
       <c r="AS265" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AT265" s="93"/>
       <c r="AU265" s="93"/>
@@ -50049,7 +50063,7 @@
       <c r="Z267" s="65"/>
       <c r="AA267" s="65"/>
       <c r="AB267" s="65" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC267" s="65"/>
       <c r="AD267" s="65"/>
@@ -50078,7 +50092,7 @@
         <v>0</v>
       </c>
       <c r="AS267" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AT267" s="93"/>
       <c r="AU267" s="93"/>
@@ -50679,7 +50693,7 @@
         <v>1</v>
       </c>
       <c r="AB269" s="60" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AH269">
         <v>3</v>
@@ -50703,7 +50717,7 @@
         <v>1</v>
       </c>
       <c r="AS269" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="270" spans="1:302" x14ac:dyDescent="0.2">
@@ -50779,7 +50793,7 @@
       <c r="Z271" s="65"/>
       <c r="AA271" s="65"/>
       <c r="AB271" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC271" s="65"/>
       <c r="AD271" s="65"/>
@@ -50808,7 +50822,7 @@
         <v>1</v>
       </c>
       <c r="AS271" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AT271" s="93"/>
       <c r="AU271" s="93"/>
@@ -51139,7 +51153,7 @@
       <c r="Z273" s="65"/>
       <c r="AA273" s="65"/>
       <c r="AB273" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC273" s="65"/>
       <c r="AD273" s="65"/>
@@ -51168,7 +51182,7 @@
         <v>0</v>
       </c>
       <c r="AS273" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AT273" s="93"/>
       <c r="AU273" s="93"/>
@@ -51499,7 +51513,7 @@
       <c r="Z275" s="65"/>
       <c r="AA275" s="65"/>
       <c r="AB275" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC275" s="65"/>
       <c r="AD275" s="65"/>
@@ -51528,7 +51542,7 @@
         <v>1</v>
       </c>
       <c r="AS275" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AT275" s="93"/>
       <c r="AU275" s="93"/>
@@ -51861,7 +51875,7 @@
       <c r="Z277" s="65"/>
       <c r="AA277" s="65"/>
       <c r="AB277" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC277" s="65"/>
       <c r="AD277" s="65"/>
@@ -51890,7 +51904,7 @@
         <v>1</v>
       </c>
       <c r="AS277" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AT277" s="93"/>
       <c r="AU277" s="93"/>
@@ -52223,7 +52237,7 @@
       <c r="Z279" s="65"/>
       <c r="AA279" s="65"/>
       <c r="AB279" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC279" s="65"/>
       <c r="AD279" s="65"/>
@@ -52252,7 +52266,7 @@
         <v>1</v>
       </c>
       <c r="AS279" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AT279" s="93"/>
       <c r="AU279" s="93"/>
@@ -52580,14 +52594,14 @@
         <v>1</v>
       </c>
       <c r="W281" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X281" s="65"/>
       <c r="Y281" s="65"/>
       <c r="Z281" s="65"/>
       <c r="AA281" s="65"/>
       <c r="AB281" s="65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AC281" s="65"/>
       <c r="AD281" s="65"/>
@@ -52616,7 +52630,7 @@
         <v>1</v>
       </c>
       <c r="AS281" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AT281" s="93"/>
       <c r="AU281" s="93"/>
@@ -52944,14 +52958,14 @@
         <v>1</v>
       </c>
       <c r="W283" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X283" s="65"/>
       <c r="Y283" s="65"/>
       <c r="Z283" s="65"/>
       <c r="AA283" s="65"/>
       <c r="AB283" s="65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AC283" s="65"/>
       <c r="AD283" s="65"/>
@@ -52980,7 +52994,7 @@
         <v>1</v>
       </c>
       <c r="AS283" s="28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AT283" s="93"/>
       <c r="AU283" s="93"/>
@@ -53306,14 +53320,14 @@
       <c r="U285" s="65"/>
       <c r="V285" s="65"/>
       <c r="W285" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X285" s="65"/>
       <c r="Y285" s="65"/>
       <c r="Z285" s="65"/>
       <c r="AA285" s="65"/>
       <c r="AB285" s="65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AC285" s="65"/>
       <c r="AD285" s="65"/>
@@ -53342,7 +53356,7 @@
         <v>0</v>
       </c>
       <c r="AS285" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AT285" s="93"/>
       <c r="AU285" s="93"/>
@@ -53670,14 +53684,14 @@
         <v>2</v>
       </c>
       <c r="W287" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X287" s="65"/>
       <c r="Y287" s="65"/>
       <c r="Z287" s="65"/>
       <c r="AA287" s="65"/>
       <c r="AB287" s="65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AC287" s="65"/>
       <c r="AD287" s="65"/>
@@ -54030,14 +54044,14 @@
       <c r="U289" s="65"/>
       <c r="V289" s="65"/>
       <c r="W289" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X289" s="65"/>
       <c r="Y289" s="65"/>
       <c r="Z289" s="65"/>
       <c r="AA289" s="65"/>
       <c r="AB289" s="65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AC289" s="65"/>
       <c r="AD289" s="65"/>
@@ -54066,7 +54080,7 @@
         <v>1</v>
       </c>
       <c r="AS289" s="28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AT289" s="93"/>
       <c r="AU289" s="93"/>
@@ -54392,14 +54406,14 @@
       <c r="U291" s="65"/>
       <c r="V291" s="65"/>
       <c r="W291" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="X291" s="65"/>
       <c r="Y291" s="65"/>
       <c r="Z291" s="65"/>
       <c r="AA291" s="65"/>
       <c r="AB291" s="65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AC291" s="65"/>
       <c r="AD291" s="65"/>
@@ -54428,7 +54442,7 @@
         <v>1</v>
       </c>
       <c r="AS291" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AT291" s="93"/>
       <c r="AU291" s="93"/>
@@ -54751,7 +54765,7 @@
       </c>
       <c r="S293" s="65"/>
       <c r="T293" s="65" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U293" s="65">
         <v>-1</v>
@@ -54759,7 +54773,7 @@
       <c r="V293" s="65"/>
       <c r="W293" s="65"/>
       <c r="X293" s="65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Y293" s="65"/>
       <c r="Z293" s="65"/>
@@ -55400,7 +55414,7 @@
       <c r="V295" s="65"/>
       <c r="W295" s="65"/>
       <c r="X295" s="65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Y295" s="65"/>
       <c r="Z295" s="65"/>

</xml_diff>

<commit_message>
Added a new cross capture type. Combined the separate classes into one. New game J_Odu_II uses it.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79E8F7F-CD48-4B8C-9E16-2DE595E361C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73979B4B-5B34-4033-8FDA-5A1413B46B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="205">
   <si>
     <t>setup</t>
   </si>
@@ -646,6 +646,9 @@
   <si>
     <t>capture the only cup, gs rules doesn't apply</t>
   </si>
+  <si>
+    <t>1_ANY</t>
+  </si>
 </sst>
 </file>
 
@@ -1150,7 +1153,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1334,39 +1337,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1703,9 +1673,9 @@
   <dimension ref="A1:AMK312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="J50" sqref="J50"/>
+      <selection pane="bottomLeft" activeCell="AQ298" sqref="AQ298"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16445,673 +16415,673 @@
       <c r="KO58" s="88"/>
       <c r="KP58" s="88"/>
     </row>
-    <row r="59" spans="1:302" s="109" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="99">
+    <row r="59" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="A59" s="40">
         <v>27</v>
       </c>
-      <c r="B59" s="100">
-        <v>0</v>
-      </c>
-      <c r="C59" s="100">
+      <c r="B59" s="13">
+        <v>0</v>
+      </c>
+      <c r="C59" s="13">
         <v>2</v>
       </c>
-      <c r="D59" s="100">
+      <c r="D59" s="13">
         <v>2</v>
       </c>
-      <c r="E59" s="100">
+      <c r="E59" s="13">
         <v>2</v>
       </c>
-      <c r="F59" s="101"/>
-      <c r="G59" s="100"/>
-      <c r="H59" s="100"/>
-      <c r="I59" s="102"/>
-      <c r="J59" s="101"/>
-      <c r="K59" s="100"/>
-      <c r="L59" s="100"/>
-      <c r="M59" s="102"/>
-      <c r="N59" s="100">
+      <c r="F59" s="14"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="13"/>
+      <c r="L59" s="13"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="13">
         <v>2</v>
       </c>
-      <c r="O59" s="100">
+      <c r="O59" s="13">
         <v>2</v>
       </c>
-      <c r="P59" s="100" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q59" s="101">
+      <c r="P59" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="14">
         <v>4</v>
       </c>
-      <c r="R59" s="102" t="s">
+      <c r="R59" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="S59" s="103" t="b">
+      <c r="S59" s="55" t="b">
         <v>1</v>
       </c>
-      <c r="T59" s="103"/>
-      <c r="U59" s="104" t="s">
+      <c r="T59" s="55"/>
+      <c r="U59" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="V59" s="103">
+      <c r="V59" s="55">
         <v>1</v>
       </c>
-      <c r="W59" s="103"/>
-      <c r="X59" s="103"/>
-      <c r="Y59" s="103"/>
-      <c r="Z59" s="103" t="s">
+      <c r="W59" s="55"/>
+      <c r="X59" s="55"/>
+      <c r="Y59" s="55"/>
+      <c r="Z59" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="AA59" s="103"/>
-      <c r="AB59" s="103"/>
-      <c r="AC59" s="103"/>
-      <c r="AD59" s="103"/>
-      <c r="AE59" s="103"/>
-      <c r="AF59" s="103"/>
-      <c r="AG59" s="105"/>
-      <c r="AH59" s="100">
-        <v>0</v>
-      </c>
-      <c r="AI59" s="100">
-        <v>0</v>
-      </c>
-      <c r="AJ59" s="100">
-        <v>0</v>
-      </c>
-      <c r="AK59" s="100">
+      <c r="AA59" s="55"/>
+      <c r="AB59" s="55"/>
+      <c r="AC59" s="55"/>
+      <c r="AD59" s="55"/>
+      <c r="AE59" s="55"/>
+      <c r="AF59" s="55"/>
+      <c r="AG59" s="63"/>
+      <c r="AH59" s="13">
+        <v>0</v>
+      </c>
+      <c r="AI59" s="13">
+        <v>0</v>
+      </c>
+      <c r="AJ59" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK59" s="13">
         <v>2</v>
       </c>
-      <c r="AL59" s="100"/>
-      <c r="AM59" s="100"/>
-      <c r="AN59" s="100"/>
-      <c r="AO59" s="100"/>
-      <c r="AP59" s="100">
+      <c r="AL59" s="13"/>
+      <c r="AM59" s="13"/>
+      <c r="AN59" s="13"/>
+      <c r="AO59" s="13"/>
+      <c r="AP59" s="13">
         <v>6</v>
       </c>
-      <c r="AQ59" s="100">
+      <c r="AQ59" s="13">
         <v>2</v>
       </c>
-      <c r="AR59" s="106" t="b">
+      <c r="AR59" s="81" t="b">
         <v>1</v>
       </c>
-      <c r="AS59" s="107" t="s">
+      <c r="AS59" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="AT59" s="108"/>
-      <c r="AU59" s="108"/>
-      <c r="AV59" s="108"/>
-      <c r="AW59" s="108"/>
-      <c r="AX59" s="108"/>
-      <c r="AY59" s="108"/>
-      <c r="AZ59" s="108"/>
-      <c r="BA59" s="108"/>
-      <c r="BB59" s="108"/>
-      <c r="BC59" s="108"/>
-      <c r="BD59" s="108"/>
-      <c r="BE59" s="108"/>
-      <c r="BF59" s="108"/>
-      <c r="BG59" s="108"/>
-      <c r="BH59" s="108"/>
-      <c r="BI59" s="108"/>
-      <c r="BJ59" s="108"/>
-      <c r="BK59" s="108"/>
-      <c r="BL59" s="108"/>
-      <c r="BM59" s="108"/>
-      <c r="BN59" s="108"/>
-      <c r="BO59" s="108"/>
-      <c r="BP59" s="108"/>
-      <c r="BQ59" s="108"/>
-      <c r="BR59" s="108"/>
-      <c r="BS59" s="108"/>
-      <c r="BT59" s="108"/>
-      <c r="BU59" s="108"/>
-      <c r="BV59" s="108"/>
-      <c r="BW59" s="108"/>
-      <c r="BX59" s="108"/>
-      <c r="BY59" s="108"/>
-      <c r="BZ59" s="108"/>
-      <c r="CA59" s="108"/>
-      <c r="CB59" s="108"/>
-      <c r="CC59" s="108"/>
-      <c r="CD59" s="108"/>
-      <c r="CE59" s="108"/>
-      <c r="CF59" s="108"/>
-      <c r="CG59" s="108"/>
-      <c r="CH59" s="108"/>
-      <c r="CI59" s="108"/>
-      <c r="CJ59" s="108"/>
-      <c r="CK59" s="108"/>
-      <c r="CL59" s="108"/>
-      <c r="CM59" s="108"/>
-      <c r="CN59" s="108"/>
-      <c r="CO59" s="108"/>
-      <c r="CP59" s="108"/>
-      <c r="CQ59" s="108"/>
-      <c r="CR59" s="108"/>
-      <c r="CS59" s="108"/>
-      <c r="CT59" s="108"/>
-      <c r="CU59" s="108"/>
-      <c r="CV59" s="108"/>
-      <c r="CW59" s="108"/>
-      <c r="CX59" s="108"/>
-      <c r="CY59" s="108"/>
-      <c r="CZ59" s="108"/>
-      <c r="DA59" s="108"/>
-      <c r="DB59" s="108"/>
-      <c r="DC59" s="108"/>
-      <c r="DD59" s="108"/>
-      <c r="DE59" s="108"/>
-      <c r="DF59" s="108"/>
-      <c r="DG59" s="108"/>
-      <c r="DH59" s="108"/>
-      <c r="DI59" s="108"/>
-      <c r="DJ59" s="108"/>
-      <c r="DK59" s="108"/>
-      <c r="DL59" s="108"/>
-      <c r="DM59" s="108"/>
-      <c r="DN59" s="108"/>
-      <c r="DO59" s="108"/>
-      <c r="DP59" s="108"/>
-      <c r="DQ59" s="108"/>
-      <c r="DR59" s="108"/>
-      <c r="DS59" s="108"/>
-      <c r="DT59" s="108"/>
-      <c r="DU59" s="108"/>
-      <c r="DV59" s="108"/>
-      <c r="DW59" s="108"/>
-      <c r="DX59" s="108"/>
-      <c r="DY59" s="108"/>
-      <c r="DZ59" s="108"/>
-      <c r="EA59" s="108"/>
-      <c r="EB59" s="108"/>
-      <c r="EC59" s="108"/>
-      <c r="ED59" s="108"/>
-      <c r="EE59" s="108"/>
-      <c r="EF59" s="108"/>
-      <c r="EG59" s="108"/>
-      <c r="EH59" s="108"/>
-      <c r="EI59" s="108"/>
-      <c r="EJ59" s="108"/>
-      <c r="EK59" s="108"/>
-      <c r="EL59" s="108"/>
-      <c r="EM59" s="108"/>
-      <c r="EN59" s="108"/>
-      <c r="EO59" s="108"/>
-      <c r="EP59" s="108"/>
-      <c r="EQ59" s="108"/>
-      <c r="ER59" s="108"/>
-      <c r="ES59" s="108"/>
-      <c r="ET59" s="108"/>
-      <c r="EU59" s="108"/>
-      <c r="EV59" s="108"/>
-      <c r="EW59" s="108"/>
-      <c r="EX59" s="108"/>
-      <c r="EY59" s="108"/>
-      <c r="EZ59" s="108"/>
-      <c r="FA59" s="108"/>
-      <c r="FB59" s="108"/>
-      <c r="FC59" s="108"/>
-      <c r="FD59" s="108"/>
-      <c r="FE59" s="108"/>
-      <c r="FF59" s="108"/>
-      <c r="FG59" s="108"/>
-      <c r="FH59" s="108"/>
-      <c r="FI59" s="108"/>
-      <c r="FJ59" s="108"/>
-      <c r="FK59" s="108"/>
-      <c r="FL59" s="108"/>
-      <c r="FM59" s="108"/>
-      <c r="FN59" s="108"/>
-      <c r="FO59" s="108"/>
-      <c r="FP59" s="108"/>
-      <c r="FQ59" s="108"/>
-      <c r="FR59" s="108"/>
-      <c r="FS59" s="108"/>
-      <c r="FT59" s="108"/>
-      <c r="FU59" s="108"/>
-      <c r="FV59" s="108"/>
-      <c r="FW59" s="108"/>
-      <c r="FX59" s="108"/>
-      <c r="FY59" s="108"/>
-      <c r="FZ59" s="108"/>
-      <c r="GA59" s="108"/>
-      <c r="GB59" s="108"/>
-      <c r="GC59" s="108"/>
-      <c r="GD59" s="108"/>
-      <c r="GE59" s="108"/>
-      <c r="GF59" s="108"/>
-      <c r="GG59" s="108"/>
-      <c r="GH59" s="108"/>
-      <c r="GI59" s="108"/>
-      <c r="GJ59" s="108"/>
-      <c r="GK59" s="108"/>
-      <c r="GL59" s="108"/>
-      <c r="GM59" s="108"/>
-      <c r="GN59" s="108"/>
-      <c r="GO59" s="108"/>
-      <c r="GP59" s="108"/>
-      <c r="GQ59" s="108"/>
-      <c r="GR59" s="108"/>
-      <c r="GS59" s="108"/>
-      <c r="GT59" s="108"/>
-      <c r="GU59" s="108"/>
-      <c r="GV59" s="108"/>
-      <c r="GW59" s="108"/>
-      <c r="GX59" s="108"/>
-      <c r="GY59" s="108"/>
-      <c r="GZ59" s="108"/>
-      <c r="HA59" s="108"/>
-      <c r="HB59" s="108"/>
-      <c r="HC59" s="108"/>
-      <c r="HD59" s="108"/>
-      <c r="HE59" s="108"/>
-      <c r="HF59" s="108"/>
-      <c r="HG59" s="108"/>
-      <c r="HH59" s="108"/>
-      <c r="HI59" s="108"/>
-      <c r="HJ59" s="108"/>
-      <c r="HK59" s="108"/>
-      <c r="HL59" s="108"/>
-      <c r="HM59" s="108"/>
-      <c r="HN59" s="108"/>
-      <c r="HO59" s="108"/>
-      <c r="HP59" s="108"/>
-      <c r="HQ59" s="108"/>
-      <c r="HR59" s="108"/>
-      <c r="HS59" s="108"/>
-      <c r="HT59" s="108"/>
-      <c r="HU59" s="108"/>
-      <c r="HV59" s="108"/>
-      <c r="HW59" s="108"/>
-      <c r="HX59" s="108"/>
-      <c r="HY59" s="108"/>
-      <c r="HZ59" s="108"/>
-      <c r="IA59" s="108"/>
-      <c r="IB59" s="108"/>
-      <c r="IC59" s="108"/>
-      <c r="ID59" s="108"/>
-      <c r="IE59" s="108"/>
-      <c r="IF59" s="108"/>
-      <c r="IG59" s="108"/>
-      <c r="IH59" s="108"/>
-      <c r="II59" s="108"/>
-      <c r="IJ59" s="108"/>
-      <c r="IK59" s="108"/>
-      <c r="IL59" s="108"/>
-      <c r="IM59" s="108"/>
-      <c r="IN59" s="108"/>
-      <c r="IO59" s="108"/>
-      <c r="IP59" s="108"/>
-      <c r="IQ59" s="108"/>
-      <c r="IR59" s="108"/>
-      <c r="IS59" s="108"/>
-      <c r="IT59" s="108"/>
-      <c r="IU59" s="108"/>
-      <c r="IV59" s="108"/>
-      <c r="IW59" s="108"/>
-      <c r="IX59" s="108"/>
-      <c r="IY59" s="108"/>
-      <c r="IZ59" s="108"/>
-      <c r="JA59" s="108"/>
-      <c r="JB59" s="108"/>
-      <c r="JC59" s="108"/>
-      <c r="JD59" s="108"/>
-      <c r="JE59" s="108"/>
-      <c r="JF59" s="108"/>
-      <c r="JG59" s="108"/>
-      <c r="JH59" s="108"/>
-      <c r="JI59" s="108"/>
-      <c r="JJ59" s="108"/>
-      <c r="JK59" s="108"/>
-      <c r="JL59" s="108"/>
-      <c r="JM59" s="108"/>
-      <c r="JN59" s="108"/>
-      <c r="JO59" s="108"/>
-      <c r="JP59" s="108"/>
-      <c r="JQ59" s="108"/>
-      <c r="JR59" s="108"/>
-      <c r="JS59" s="108"/>
-      <c r="JT59" s="108"/>
-      <c r="JU59" s="108"/>
-      <c r="JV59" s="108"/>
-      <c r="JW59" s="108"/>
-      <c r="JX59" s="108"/>
-      <c r="JY59" s="108"/>
-      <c r="JZ59" s="108"/>
-      <c r="KA59" s="108"/>
-      <c r="KB59" s="108"/>
-      <c r="KC59" s="108"/>
-      <c r="KD59" s="108"/>
-      <c r="KE59" s="108"/>
-      <c r="KF59" s="108"/>
-      <c r="KG59" s="108"/>
-      <c r="KH59" s="108"/>
-      <c r="KI59" s="108"/>
-      <c r="KJ59" s="108"/>
-      <c r="KK59" s="108"/>
-      <c r="KL59" s="108"/>
-      <c r="KM59" s="108"/>
-      <c r="KN59" s="108"/>
-      <c r="KO59" s="108"/>
-      <c r="KP59" s="108"/>
+      <c r="AT59" s="88"/>
+      <c r="AU59" s="88"/>
+      <c r="AV59" s="88"/>
+      <c r="AW59" s="88"/>
+      <c r="AX59" s="88"/>
+      <c r="AY59" s="88"/>
+      <c r="AZ59" s="88"/>
+      <c r="BA59" s="88"/>
+      <c r="BB59" s="88"/>
+      <c r="BC59" s="88"/>
+      <c r="BD59" s="88"/>
+      <c r="BE59" s="88"/>
+      <c r="BF59" s="88"/>
+      <c r="BG59" s="88"/>
+      <c r="BH59" s="88"/>
+      <c r="BI59" s="88"/>
+      <c r="BJ59" s="88"/>
+      <c r="BK59" s="88"/>
+      <c r="BL59" s="88"/>
+      <c r="BM59" s="88"/>
+      <c r="BN59" s="88"/>
+      <c r="BO59" s="88"/>
+      <c r="BP59" s="88"/>
+      <c r="BQ59" s="88"/>
+      <c r="BR59" s="88"/>
+      <c r="BS59" s="88"/>
+      <c r="BT59" s="88"/>
+      <c r="BU59" s="88"/>
+      <c r="BV59" s="88"/>
+      <c r="BW59" s="88"/>
+      <c r="BX59" s="88"/>
+      <c r="BY59" s="88"/>
+      <c r="BZ59" s="88"/>
+      <c r="CA59" s="88"/>
+      <c r="CB59" s="88"/>
+      <c r="CC59" s="88"/>
+      <c r="CD59" s="88"/>
+      <c r="CE59" s="88"/>
+      <c r="CF59" s="88"/>
+      <c r="CG59" s="88"/>
+      <c r="CH59" s="88"/>
+      <c r="CI59" s="88"/>
+      <c r="CJ59" s="88"/>
+      <c r="CK59" s="88"/>
+      <c r="CL59" s="88"/>
+      <c r="CM59" s="88"/>
+      <c r="CN59" s="88"/>
+      <c r="CO59" s="88"/>
+      <c r="CP59" s="88"/>
+      <c r="CQ59" s="88"/>
+      <c r="CR59" s="88"/>
+      <c r="CS59" s="88"/>
+      <c r="CT59" s="88"/>
+      <c r="CU59" s="88"/>
+      <c r="CV59" s="88"/>
+      <c r="CW59" s="88"/>
+      <c r="CX59" s="88"/>
+      <c r="CY59" s="88"/>
+      <c r="CZ59" s="88"/>
+      <c r="DA59" s="88"/>
+      <c r="DB59" s="88"/>
+      <c r="DC59" s="88"/>
+      <c r="DD59" s="88"/>
+      <c r="DE59" s="88"/>
+      <c r="DF59" s="88"/>
+      <c r="DG59" s="88"/>
+      <c r="DH59" s="88"/>
+      <c r="DI59" s="88"/>
+      <c r="DJ59" s="88"/>
+      <c r="DK59" s="88"/>
+      <c r="DL59" s="88"/>
+      <c r="DM59" s="88"/>
+      <c r="DN59" s="88"/>
+      <c r="DO59" s="88"/>
+      <c r="DP59" s="88"/>
+      <c r="DQ59" s="88"/>
+      <c r="DR59" s="88"/>
+      <c r="DS59" s="88"/>
+      <c r="DT59" s="88"/>
+      <c r="DU59" s="88"/>
+      <c r="DV59" s="88"/>
+      <c r="DW59" s="88"/>
+      <c r="DX59" s="88"/>
+      <c r="DY59" s="88"/>
+      <c r="DZ59" s="88"/>
+      <c r="EA59" s="88"/>
+      <c r="EB59" s="88"/>
+      <c r="EC59" s="88"/>
+      <c r="ED59" s="88"/>
+      <c r="EE59" s="88"/>
+      <c r="EF59" s="88"/>
+      <c r="EG59" s="88"/>
+      <c r="EH59" s="88"/>
+      <c r="EI59" s="88"/>
+      <c r="EJ59" s="88"/>
+      <c r="EK59" s="88"/>
+      <c r="EL59" s="88"/>
+      <c r="EM59" s="88"/>
+      <c r="EN59" s="88"/>
+      <c r="EO59" s="88"/>
+      <c r="EP59" s="88"/>
+      <c r="EQ59" s="88"/>
+      <c r="ER59" s="88"/>
+      <c r="ES59" s="88"/>
+      <c r="ET59" s="88"/>
+      <c r="EU59" s="88"/>
+      <c r="EV59" s="88"/>
+      <c r="EW59" s="88"/>
+      <c r="EX59" s="88"/>
+      <c r="EY59" s="88"/>
+      <c r="EZ59" s="88"/>
+      <c r="FA59" s="88"/>
+      <c r="FB59" s="88"/>
+      <c r="FC59" s="88"/>
+      <c r="FD59" s="88"/>
+      <c r="FE59" s="88"/>
+      <c r="FF59" s="88"/>
+      <c r="FG59" s="88"/>
+      <c r="FH59" s="88"/>
+      <c r="FI59" s="88"/>
+      <c r="FJ59" s="88"/>
+      <c r="FK59" s="88"/>
+      <c r="FL59" s="88"/>
+      <c r="FM59" s="88"/>
+      <c r="FN59" s="88"/>
+      <c r="FO59" s="88"/>
+      <c r="FP59" s="88"/>
+      <c r="FQ59" s="88"/>
+      <c r="FR59" s="88"/>
+      <c r="FS59" s="88"/>
+      <c r="FT59" s="88"/>
+      <c r="FU59" s="88"/>
+      <c r="FV59" s="88"/>
+      <c r="FW59" s="88"/>
+      <c r="FX59" s="88"/>
+      <c r="FY59" s="88"/>
+      <c r="FZ59" s="88"/>
+      <c r="GA59" s="88"/>
+      <c r="GB59" s="88"/>
+      <c r="GC59" s="88"/>
+      <c r="GD59" s="88"/>
+      <c r="GE59" s="88"/>
+      <c r="GF59" s="88"/>
+      <c r="GG59" s="88"/>
+      <c r="GH59" s="88"/>
+      <c r="GI59" s="88"/>
+      <c r="GJ59" s="88"/>
+      <c r="GK59" s="88"/>
+      <c r="GL59" s="88"/>
+      <c r="GM59" s="88"/>
+      <c r="GN59" s="88"/>
+      <c r="GO59" s="88"/>
+      <c r="GP59" s="88"/>
+      <c r="GQ59" s="88"/>
+      <c r="GR59" s="88"/>
+      <c r="GS59" s="88"/>
+      <c r="GT59" s="88"/>
+      <c r="GU59" s="88"/>
+      <c r="GV59" s="88"/>
+      <c r="GW59" s="88"/>
+      <c r="GX59" s="88"/>
+      <c r="GY59" s="88"/>
+      <c r="GZ59" s="88"/>
+      <c r="HA59" s="88"/>
+      <c r="HB59" s="88"/>
+      <c r="HC59" s="88"/>
+      <c r="HD59" s="88"/>
+      <c r="HE59" s="88"/>
+      <c r="HF59" s="88"/>
+      <c r="HG59" s="88"/>
+      <c r="HH59" s="88"/>
+      <c r="HI59" s="88"/>
+      <c r="HJ59" s="88"/>
+      <c r="HK59" s="88"/>
+      <c r="HL59" s="88"/>
+      <c r="HM59" s="88"/>
+      <c r="HN59" s="88"/>
+      <c r="HO59" s="88"/>
+      <c r="HP59" s="88"/>
+      <c r="HQ59" s="88"/>
+      <c r="HR59" s="88"/>
+      <c r="HS59" s="88"/>
+      <c r="HT59" s="88"/>
+      <c r="HU59" s="88"/>
+      <c r="HV59" s="88"/>
+      <c r="HW59" s="88"/>
+      <c r="HX59" s="88"/>
+      <c r="HY59" s="88"/>
+      <c r="HZ59" s="88"/>
+      <c r="IA59" s="88"/>
+      <c r="IB59" s="88"/>
+      <c r="IC59" s="88"/>
+      <c r="ID59" s="88"/>
+      <c r="IE59" s="88"/>
+      <c r="IF59" s="88"/>
+      <c r="IG59" s="88"/>
+      <c r="IH59" s="88"/>
+      <c r="II59" s="88"/>
+      <c r="IJ59" s="88"/>
+      <c r="IK59" s="88"/>
+      <c r="IL59" s="88"/>
+      <c r="IM59" s="88"/>
+      <c r="IN59" s="88"/>
+      <c r="IO59" s="88"/>
+      <c r="IP59" s="88"/>
+      <c r="IQ59" s="88"/>
+      <c r="IR59" s="88"/>
+      <c r="IS59" s="88"/>
+      <c r="IT59" s="88"/>
+      <c r="IU59" s="88"/>
+      <c r="IV59" s="88"/>
+      <c r="IW59" s="88"/>
+      <c r="IX59" s="88"/>
+      <c r="IY59" s="88"/>
+      <c r="IZ59" s="88"/>
+      <c r="JA59" s="88"/>
+      <c r="JB59" s="88"/>
+      <c r="JC59" s="88"/>
+      <c r="JD59" s="88"/>
+      <c r="JE59" s="88"/>
+      <c r="JF59" s="88"/>
+      <c r="JG59" s="88"/>
+      <c r="JH59" s="88"/>
+      <c r="JI59" s="88"/>
+      <c r="JJ59" s="88"/>
+      <c r="JK59" s="88"/>
+      <c r="JL59" s="88"/>
+      <c r="JM59" s="88"/>
+      <c r="JN59" s="88"/>
+      <c r="JO59" s="88"/>
+      <c r="JP59" s="88"/>
+      <c r="JQ59" s="88"/>
+      <c r="JR59" s="88"/>
+      <c r="JS59" s="88"/>
+      <c r="JT59" s="88"/>
+      <c r="JU59" s="88"/>
+      <c r="JV59" s="88"/>
+      <c r="JW59" s="88"/>
+      <c r="JX59" s="88"/>
+      <c r="JY59" s="88"/>
+      <c r="JZ59" s="88"/>
+      <c r="KA59" s="88"/>
+      <c r="KB59" s="88"/>
+      <c r="KC59" s="88"/>
+      <c r="KD59" s="88"/>
+      <c r="KE59" s="88"/>
+      <c r="KF59" s="88"/>
+      <c r="KG59" s="88"/>
+      <c r="KH59" s="88"/>
+      <c r="KI59" s="88"/>
+      <c r="KJ59" s="88"/>
+      <c r="KK59" s="88"/>
+      <c r="KL59" s="88"/>
+      <c r="KM59" s="88"/>
+      <c r="KN59" s="88"/>
+      <c r="KO59" s="88"/>
+      <c r="KP59" s="88"/>
     </row>
-    <row r="60" spans="1:302" s="109" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="110"/>
-      <c r="B60" s="111">
+    <row r="60" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="A60" s="41"/>
+      <c r="B60" s="18">
         <v>5</v>
       </c>
-      <c r="C60" s="111">
-        <v>3</v>
-      </c>
-      <c r="D60" s="111">
-        <v>3</v>
-      </c>
-      <c r="E60" s="111">
-        <v>3</v>
-      </c>
-      <c r="F60" s="112"/>
-      <c r="G60" s="111"/>
-      <c r="H60" s="111"/>
-      <c r="I60" s="113"/>
-      <c r="J60" s="112"/>
-      <c r="K60" s="111"/>
-      <c r="L60" s="111"/>
-      <c r="M60" s="113"/>
-      <c r="N60" s="111"/>
-      <c r="O60" s="111"/>
-      <c r="P60" s="111"/>
-      <c r="Q60" s="112"/>
-      <c r="R60" s="113"/>
-      <c r="S60" s="114"/>
-      <c r="T60" s="114"/>
-      <c r="U60" s="114"/>
-      <c r="V60" s="114"/>
-      <c r="W60" s="114"/>
-      <c r="X60" s="114"/>
-      <c r="Y60" s="114"/>
-      <c r="Z60" s="114"/>
-      <c r="AA60" s="114"/>
-      <c r="AB60" s="114"/>
-      <c r="AC60" s="114"/>
-      <c r="AD60" s="114"/>
-      <c r="AE60" s="114"/>
-      <c r="AF60" s="114"/>
-      <c r="AG60" s="115"/>
-      <c r="AH60" s="111">
+      <c r="C60" s="18">
+        <v>3</v>
+      </c>
+      <c r="D60" s="18">
+        <v>3</v>
+      </c>
+      <c r="E60" s="18">
+        <v>3</v>
+      </c>
+      <c r="F60" s="19"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="18"/>
+      <c r="Q60" s="19"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="57"/>
+      <c r="T60" s="57"/>
+      <c r="U60" s="57"/>
+      <c r="V60" s="57"/>
+      <c r="W60" s="57"/>
+      <c r="X60" s="57"/>
+      <c r="Y60" s="57"/>
+      <c r="Z60" s="57"/>
+      <c r="AA60" s="57"/>
+      <c r="AB60" s="57"/>
+      <c r="AC60" s="57"/>
+      <c r="AD60" s="57"/>
+      <c r="AE60" s="57"/>
+      <c r="AF60" s="57"/>
+      <c r="AG60" s="58"/>
+      <c r="AH60" s="18">
         <v>5</v>
       </c>
-      <c r="AI60" s="111">
-        <v>3</v>
-      </c>
-      <c r="AJ60" s="111">
-        <v>3</v>
-      </c>
-      <c r="AK60" s="111">
-        <v>3</v>
-      </c>
-      <c r="AL60" s="111"/>
-      <c r="AM60" s="111"/>
-      <c r="AN60" s="111"/>
-      <c r="AO60" s="111"/>
-      <c r="AP60" s="111"/>
-      <c r="AQ60" s="111"/>
-      <c r="AR60" s="116"/>
-      <c r="AS60" s="117"/>
-      <c r="AT60" s="108"/>
-      <c r="AU60" s="108"/>
-      <c r="AV60" s="108"/>
-      <c r="AW60" s="108"/>
-      <c r="AX60" s="108"/>
-      <c r="AY60" s="108"/>
-      <c r="AZ60" s="108"/>
-      <c r="BA60" s="108"/>
-      <c r="BB60" s="108"/>
-      <c r="BC60" s="108"/>
-      <c r="BD60" s="108"/>
-      <c r="BE60" s="108"/>
-      <c r="BF60" s="108"/>
-      <c r="BG60" s="108"/>
-      <c r="BH60" s="108"/>
-      <c r="BI60" s="108"/>
-      <c r="BJ60" s="108"/>
-      <c r="BK60" s="108"/>
-      <c r="BL60" s="108"/>
-      <c r="BM60" s="108"/>
-      <c r="BN60" s="108"/>
-      <c r="BO60" s="108"/>
-      <c r="BP60" s="108"/>
-      <c r="BQ60" s="108"/>
-      <c r="BR60" s="108"/>
-      <c r="BS60" s="108"/>
-      <c r="BT60" s="108"/>
-      <c r="BU60" s="108"/>
-      <c r="BV60" s="108"/>
-      <c r="BW60" s="108"/>
-      <c r="BX60" s="108"/>
-      <c r="BY60" s="108"/>
-      <c r="BZ60" s="108"/>
-      <c r="CA60" s="108"/>
-      <c r="CB60" s="108"/>
-      <c r="CC60" s="108"/>
-      <c r="CD60" s="108"/>
-      <c r="CE60" s="108"/>
-      <c r="CF60" s="108"/>
-      <c r="CG60" s="108"/>
-      <c r="CH60" s="108"/>
-      <c r="CI60" s="108"/>
-      <c r="CJ60" s="108"/>
-      <c r="CK60" s="108"/>
-      <c r="CL60" s="108"/>
-      <c r="CM60" s="108"/>
-      <c r="CN60" s="108"/>
-      <c r="CO60" s="108"/>
-      <c r="CP60" s="108"/>
-      <c r="CQ60" s="108"/>
-      <c r="CR60" s="108"/>
-      <c r="CS60" s="108"/>
-      <c r="CT60" s="108"/>
-      <c r="CU60" s="108"/>
-      <c r="CV60" s="108"/>
-      <c r="CW60" s="108"/>
-      <c r="CX60" s="108"/>
-      <c r="CY60" s="108"/>
-      <c r="CZ60" s="108"/>
-      <c r="DA60" s="108"/>
-      <c r="DB60" s="108"/>
-      <c r="DC60" s="108"/>
-      <c r="DD60" s="108"/>
-      <c r="DE60" s="108"/>
-      <c r="DF60" s="108"/>
-      <c r="DG60" s="108"/>
-      <c r="DH60" s="108"/>
-      <c r="DI60" s="108"/>
-      <c r="DJ60" s="108"/>
-      <c r="DK60" s="108"/>
-      <c r="DL60" s="108"/>
-      <c r="DM60" s="108"/>
-      <c r="DN60" s="108"/>
-      <c r="DO60" s="108"/>
-      <c r="DP60" s="108"/>
-      <c r="DQ60" s="108"/>
-      <c r="DR60" s="108"/>
-      <c r="DS60" s="108"/>
-      <c r="DT60" s="108"/>
-      <c r="DU60" s="108"/>
-      <c r="DV60" s="108"/>
-      <c r="DW60" s="108"/>
-      <c r="DX60" s="108"/>
-      <c r="DY60" s="108"/>
-      <c r="DZ60" s="108"/>
-      <c r="EA60" s="108"/>
-      <c r="EB60" s="108"/>
-      <c r="EC60" s="108"/>
-      <c r="ED60" s="108"/>
-      <c r="EE60" s="108"/>
-      <c r="EF60" s="108"/>
-      <c r="EG60" s="108"/>
-      <c r="EH60" s="108"/>
-      <c r="EI60" s="108"/>
-      <c r="EJ60" s="108"/>
-      <c r="EK60" s="108"/>
-      <c r="EL60" s="108"/>
-      <c r="EM60" s="108"/>
-      <c r="EN60" s="108"/>
-      <c r="EO60" s="108"/>
-      <c r="EP60" s="108"/>
-      <c r="EQ60" s="108"/>
-      <c r="ER60" s="108"/>
-      <c r="ES60" s="108"/>
-      <c r="ET60" s="108"/>
-      <c r="EU60" s="108"/>
-      <c r="EV60" s="108"/>
-      <c r="EW60" s="108"/>
-      <c r="EX60" s="108"/>
-      <c r="EY60" s="108"/>
-      <c r="EZ60" s="108"/>
-      <c r="FA60" s="108"/>
-      <c r="FB60" s="108"/>
-      <c r="FC60" s="108"/>
-      <c r="FD60" s="108"/>
-      <c r="FE60" s="108"/>
-      <c r="FF60" s="108"/>
-      <c r="FG60" s="108"/>
-      <c r="FH60" s="108"/>
-      <c r="FI60" s="108"/>
-      <c r="FJ60" s="108"/>
-      <c r="FK60" s="108"/>
-      <c r="FL60" s="108"/>
-      <c r="FM60" s="108"/>
-      <c r="FN60" s="108"/>
-      <c r="FO60" s="108"/>
-      <c r="FP60" s="108"/>
-      <c r="FQ60" s="108"/>
-      <c r="FR60" s="108"/>
-      <c r="FS60" s="108"/>
-      <c r="FT60" s="108"/>
-      <c r="FU60" s="108"/>
-      <c r="FV60" s="108"/>
-      <c r="FW60" s="108"/>
-      <c r="FX60" s="108"/>
-      <c r="FY60" s="108"/>
-      <c r="FZ60" s="108"/>
-      <c r="GA60" s="108"/>
-      <c r="GB60" s="108"/>
-      <c r="GC60" s="108"/>
-      <c r="GD60" s="108"/>
-      <c r="GE60" s="108"/>
-      <c r="GF60" s="108"/>
-      <c r="GG60" s="108"/>
-      <c r="GH60" s="108"/>
-      <c r="GI60" s="108"/>
-      <c r="GJ60" s="108"/>
-      <c r="GK60" s="108"/>
-      <c r="GL60" s="108"/>
-      <c r="GM60" s="108"/>
-      <c r="GN60" s="108"/>
-      <c r="GO60" s="108"/>
-      <c r="GP60" s="108"/>
-      <c r="GQ60" s="108"/>
-      <c r="GR60" s="108"/>
-      <c r="GS60" s="108"/>
-      <c r="GT60" s="108"/>
-      <c r="GU60" s="108"/>
-      <c r="GV60" s="108"/>
-      <c r="GW60" s="108"/>
-      <c r="GX60" s="108"/>
-      <c r="GY60" s="108"/>
-      <c r="GZ60" s="108"/>
-      <c r="HA60" s="108"/>
-      <c r="HB60" s="108"/>
-      <c r="HC60" s="108"/>
-      <c r="HD60" s="108"/>
-      <c r="HE60" s="108"/>
-      <c r="HF60" s="108"/>
-      <c r="HG60" s="108"/>
-      <c r="HH60" s="108"/>
-      <c r="HI60" s="108"/>
-      <c r="HJ60" s="108"/>
-      <c r="HK60" s="108"/>
-      <c r="HL60" s="108"/>
-      <c r="HM60" s="108"/>
-      <c r="HN60" s="108"/>
-      <c r="HO60" s="108"/>
-      <c r="HP60" s="108"/>
-      <c r="HQ60" s="108"/>
-      <c r="HR60" s="108"/>
-      <c r="HS60" s="108"/>
-      <c r="HT60" s="108"/>
-      <c r="HU60" s="108"/>
-      <c r="HV60" s="108"/>
-      <c r="HW60" s="108"/>
-      <c r="HX60" s="108"/>
-      <c r="HY60" s="108"/>
-      <c r="HZ60" s="108"/>
-      <c r="IA60" s="108"/>
-      <c r="IB60" s="108"/>
-      <c r="IC60" s="108"/>
-      <c r="ID60" s="108"/>
-      <c r="IE60" s="108"/>
-      <c r="IF60" s="108"/>
-      <c r="IG60" s="108"/>
-      <c r="IH60" s="108"/>
-      <c r="II60" s="108"/>
-      <c r="IJ60" s="108"/>
-      <c r="IK60" s="108"/>
-      <c r="IL60" s="108"/>
-      <c r="IM60" s="108"/>
-      <c r="IN60" s="108"/>
-      <c r="IO60" s="108"/>
-      <c r="IP60" s="108"/>
-      <c r="IQ60" s="108"/>
-      <c r="IR60" s="108"/>
-      <c r="IS60" s="108"/>
-      <c r="IT60" s="108"/>
-      <c r="IU60" s="108"/>
-      <c r="IV60" s="108"/>
-      <c r="IW60" s="108"/>
-      <c r="IX60" s="108"/>
-      <c r="IY60" s="108"/>
-      <c r="IZ60" s="108"/>
-      <c r="JA60" s="108"/>
-      <c r="JB60" s="108"/>
-      <c r="JC60" s="108"/>
-      <c r="JD60" s="108"/>
-      <c r="JE60" s="108"/>
-      <c r="JF60" s="108"/>
-      <c r="JG60" s="108"/>
-      <c r="JH60" s="108"/>
-      <c r="JI60" s="108"/>
-      <c r="JJ60" s="108"/>
-      <c r="JK60" s="108"/>
-      <c r="JL60" s="108"/>
-      <c r="JM60" s="108"/>
-      <c r="JN60" s="108"/>
-      <c r="JO60" s="108"/>
-      <c r="JP60" s="108"/>
-      <c r="JQ60" s="108"/>
-      <c r="JR60" s="108"/>
-      <c r="JS60" s="108"/>
-      <c r="JT60" s="108"/>
-      <c r="JU60" s="108"/>
-      <c r="JV60" s="108"/>
-      <c r="JW60" s="108"/>
-      <c r="JX60" s="108"/>
-      <c r="JY60" s="108"/>
-      <c r="JZ60" s="108"/>
-      <c r="KA60" s="108"/>
-      <c r="KB60" s="108"/>
-      <c r="KC60" s="108"/>
-      <c r="KD60" s="108"/>
-      <c r="KE60" s="108"/>
-      <c r="KF60" s="108"/>
-      <c r="KG60" s="108"/>
-      <c r="KH60" s="108"/>
-      <c r="KI60" s="108"/>
-      <c r="KJ60" s="108"/>
-      <c r="KK60" s="108"/>
-      <c r="KL60" s="108"/>
-      <c r="KM60" s="108"/>
-      <c r="KN60" s="108"/>
-      <c r="KO60" s="108"/>
-      <c r="KP60" s="108"/>
+      <c r="AI60" s="18">
+        <v>3</v>
+      </c>
+      <c r="AJ60" s="18">
+        <v>3</v>
+      </c>
+      <c r="AK60" s="18">
+        <v>3</v>
+      </c>
+      <c r="AL60" s="18"/>
+      <c r="AM60" s="18"/>
+      <c r="AN60" s="18"/>
+      <c r="AO60" s="18"/>
+      <c r="AP60" s="18"/>
+      <c r="AQ60" s="18"/>
+      <c r="AR60" s="78"/>
+      <c r="AS60" s="21"/>
+      <c r="AT60" s="88"/>
+      <c r="AU60" s="88"/>
+      <c r="AV60" s="88"/>
+      <c r="AW60" s="88"/>
+      <c r="AX60" s="88"/>
+      <c r="AY60" s="88"/>
+      <c r="AZ60" s="88"/>
+      <c r="BA60" s="88"/>
+      <c r="BB60" s="88"/>
+      <c r="BC60" s="88"/>
+      <c r="BD60" s="88"/>
+      <c r="BE60" s="88"/>
+      <c r="BF60" s="88"/>
+      <c r="BG60" s="88"/>
+      <c r="BH60" s="88"/>
+      <c r="BI60" s="88"/>
+      <c r="BJ60" s="88"/>
+      <c r="BK60" s="88"/>
+      <c r="BL60" s="88"/>
+      <c r="BM60" s="88"/>
+      <c r="BN60" s="88"/>
+      <c r="BO60" s="88"/>
+      <c r="BP60" s="88"/>
+      <c r="BQ60" s="88"/>
+      <c r="BR60" s="88"/>
+      <c r="BS60" s="88"/>
+      <c r="BT60" s="88"/>
+      <c r="BU60" s="88"/>
+      <c r="BV60" s="88"/>
+      <c r="BW60" s="88"/>
+      <c r="BX60" s="88"/>
+      <c r="BY60" s="88"/>
+      <c r="BZ60" s="88"/>
+      <c r="CA60" s="88"/>
+      <c r="CB60" s="88"/>
+      <c r="CC60" s="88"/>
+      <c r="CD60" s="88"/>
+      <c r="CE60" s="88"/>
+      <c r="CF60" s="88"/>
+      <c r="CG60" s="88"/>
+      <c r="CH60" s="88"/>
+      <c r="CI60" s="88"/>
+      <c r="CJ60" s="88"/>
+      <c r="CK60" s="88"/>
+      <c r="CL60" s="88"/>
+      <c r="CM60" s="88"/>
+      <c r="CN60" s="88"/>
+      <c r="CO60" s="88"/>
+      <c r="CP60" s="88"/>
+      <c r="CQ60" s="88"/>
+      <c r="CR60" s="88"/>
+      <c r="CS60" s="88"/>
+      <c r="CT60" s="88"/>
+      <c r="CU60" s="88"/>
+      <c r="CV60" s="88"/>
+      <c r="CW60" s="88"/>
+      <c r="CX60" s="88"/>
+      <c r="CY60" s="88"/>
+      <c r="CZ60" s="88"/>
+      <c r="DA60" s="88"/>
+      <c r="DB60" s="88"/>
+      <c r="DC60" s="88"/>
+      <c r="DD60" s="88"/>
+      <c r="DE60" s="88"/>
+      <c r="DF60" s="88"/>
+      <c r="DG60" s="88"/>
+      <c r="DH60" s="88"/>
+      <c r="DI60" s="88"/>
+      <c r="DJ60" s="88"/>
+      <c r="DK60" s="88"/>
+      <c r="DL60" s="88"/>
+      <c r="DM60" s="88"/>
+      <c r="DN60" s="88"/>
+      <c r="DO60" s="88"/>
+      <c r="DP60" s="88"/>
+      <c r="DQ60" s="88"/>
+      <c r="DR60" s="88"/>
+      <c r="DS60" s="88"/>
+      <c r="DT60" s="88"/>
+      <c r="DU60" s="88"/>
+      <c r="DV60" s="88"/>
+      <c r="DW60" s="88"/>
+      <c r="DX60" s="88"/>
+      <c r="DY60" s="88"/>
+      <c r="DZ60" s="88"/>
+      <c r="EA60" s="88"/>
+      <c r="EB60" s="88"/>
+      <c r="EC60" s="88"/>
+      <c r="ED60" s="88"/>
+      <c r="EE60" s="88"/>
+      <c r="EF60" s="88"/>
+      <c r="EG60" s="88"/>
+      <c r="EH60" s="88"/>
+      <c r="EI60" s="88"/>
+      <c r="EJ60" s="88"/>
+      <c r="EK60" s="88"/>
+      <c r="EL60" s="88"/>
+      <c r="EM60" s="88"/>
+      <c r="EN60" s="88"/>
+      <c r="EO60" s="88"/>
+      <c r="EP60" s="88"/>
+      <c r="EQ60" s="88"/>
+      <c r="ER60" s="88"/>
+      <c r="ES60" s="88"/>
+      <c r="ET60" s="88"/>
+      <c r="EU60" s="88"/>
+      <c r="EV60" s="88"/>
+      <c r="EW60" s="88"/>
+      <c r="EX60" s="88"/>
+      <c r="EY60" s="88"/>
+      <c r="EZ60" s="88"/>
+      <c r="FA60" s="88"/>
+      <c r="FB60" s="88"/>
+      <c r="FC60" s="88"/>
+      <c r="FD60" s="88"/>
+      <c r="FE60" s="88"/>
+      <c r="FF60" s="88"/>
+      <c r="FG60" s="88"/>
+      <c r="FH60" s="88"/>
+      <c r="FI60" s="88"/>
+      <c r="FJ60" s="88"/>
+      <c r="FK60" s="88"/>
+      <c r="FL60" s="88"/>
+      <c r="FM60" s="88"/>
+      <c r="FN60" s="88"/>
+      <c r="FO60" s="88"/>
+      <c r="FP60" s="88"/>
+      <c r="FQ60" s="88"/>
+      <c r="FR60" s="88"/>
+      <c r="FS60" s="88"/>
+      <c r="FT60" s="88"/>
+      <c r="FU60" s="88"/>
+      <c r="FV60" s="88"/>
+      <c r="FW60" s="88"/>
+      <c r="FX60" s="88"/>
+      <c r="FY60" s="88"/>
+      <c r="FZ60" s="88"/>
+      <c r="GA60" s="88"/>
+      <c r="GB60" s="88"/>
+      <c r="GC60" s="88"/>
+      <c r="GD60" s="88"/>
+      <c r="GE60" s="88"/>
+      <c r="GF60" s="88"/>
+      <c r="GG60" s="88"/>
+      <c r="GH60" s="88"/>
+      <c r="GI60" s="88"/>
+      <c r="GJ60" s="88"/>
+      <c r="GK60" s="88"/>
+      <c r="GL60" s="88"/>
+      <c r="GM60" s="88"/>
+      <c r="GN60" s="88"/>
+      <c r="GO60" s="88"/>
+      <c r="GP60" s="88"/>
+      <c r="GQ60" s="88"/>
+      <c r="GR60" s="88"/>
+      <c r="GS60" s="88"/>
+      <c r="GT60" s="88"/>
+      <c r="GU60" s="88"/>
+      <c r="GV60" s="88"/>
+      <c r="GW60" s="88"/>
+      <c r="GX60" s="88"/>
+      <c r="GY60" s="88"/>
+      <c r="GZ60" s="88"/>
+      <c r="HA60" s="88"/>
+      <c r="HB60" s="88"/>
+      <c r="HC60" s="88"/>
+      <c r="HD60" s="88"/>
+      <c r="HE60" s="88"/>
+      <c r="HF60" s="88"/>
+      <c r="HG60" s="88"/>
+      <c r="HH60" s="88"/>
+      <c r="HI60" s="88"/>
+      <c r="HJ60" s="88"/>
+      <c r="HK60" s="88"/>
+      <c r="HL60" s="88"/>
+      <c r="HM60" s="88"/>
+      <c r="HN60" s="88"/>
+      <c r="HO60" s="88"/>
+      <c r="HP60" s="88"/>
+      <c r="HQ60" s="88"/>
+      <c r="HR60" s="88"/>
+      <c r="HS60" s="88"/>
+      <c r="HT60" s="88"/>
+      <c r="HU60" s="88"/>
+      <c r="HV60" s="88"/>
+      <c r="HW60" s="88"/>
+      <c r="HX60" s="88"/>
+      <c r="HY60" s="88"/>
+      <c r="HZ60" s="88"/>
+      <c r="IA60" s="88"/>
+      <c r="IB60" s="88"/>
+      <c r="IC60" s="88"/>
+      <c r="ID60" s="88"/>
+      <c r="IE60" s="88"/>
+      <c r="IF60" s="88"/>
+      <c r="IG60" s="88"/>
+      <c r="IH60" s="88"/>
+      <c r="II60" s="88"/>
+      <c r="IJ60" s="88"/>
+      <c r="IK60" s="88"/>
+      <c r="IL60" s="88"/>
+      <c r="IM60" s="88"/>
+      <c r="IN60" s="88"/>
+      <c r="IO60" s="88"/>
+      <c r="IP60" s="88"/>
+      <c r="IQ60" s="88"/>
+      <c r="IR60" s="88"/>
+      <c r="IS60" s="88"/>
+      <c r="IT60" s="88"/>
+      <c r="IU60" s="88"/>
+      <c r="IV60" s="88"/>
+      <c r="IW60" s="88"/>
+      <c r="IX60" s="88"/>
+      <c r="IY60" s="88"/>
+      <c r="IZ60" s="88"/>
+      <c r="JA60" s="88"/>
+      <c r="JB60" s="88"/>
+      <c r="JC60" s="88"/>
+      <c r="JD60" s="88"/>
+      <c r="JE60" s="88"/>
+      <c r="JF60" s="88"/>
+      <c r="JG60" s="88"/>
+      <c r="JH60" s="88"/>
+      <c r="JI60" s="88"/>
+      <c r="JJ60" s="88"/>
+      <c r="JK60" s="88"/>
+      <c r="JL60" s="88"/>
+      <c r="JM60" s="88"/>
+      <c r="JN60" s="88"/>
+      <c r="JO60" s="88"/>
+      <c r="JP60" s="88"/>
+      <c r="JQ60" s="88"/>
+      <c r="JR60" s="88"/>
+      <c r="JS60" s="88"/>
+      <c r="JT60" s="88"/>
+      <c r="JU60" s="88"/>
+      <c r="JV60" s="88"/>
+      <c r="JW60" s="88"/>
+      <c r="JX60" s="88"/>
+      <c r="JY60" s="88"/>
+      <c r="JZ60" s="88"/>
+      <c r="KA60" s="88"/>
+      <c r="KB60" s="88"/>
+      <c r="KC60" s="88"/>
+      <c r="KD60" s="88"/>
+      <c r="KE60" s="88"/>
+      <c r="KF60" s="88"/>
+      <c r="KG60" s="88"/>
+      <c r="KH60" s="88"/>
+      <c r="KI60" s="88"/>
+      <c r="KJ60" s="88"/>
+      <c r="KK60" s="88"/>
+      <c r="KL60" s="88"/>
+      <c r="KM60" s="88"/>
+      <c r="KN60" s="88"/>
+      <c r="KO60" s="88"/>
+      <c r="KP60" s="88"/>
     </row>
     <row r="61" spans="1:302" x14ac:dyDescent="0.2">
       <c r="A61" s="40">
@@ -56041,8 +56011,357 @@
       <c r="KO296" s="84"/>
       <c r="KP296" s="84"/>
     </row>
+    <row r="297" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A297" s="46">
+        <v>137</v>
+      </c>
+      <c r="B297" s="29">
+        <v>3</v>
+      </c>
+      <c r="C297" s="97">
+        <v>1</v>
+      </c>
+      <c r="D297" s="29">
+        <v>4</v>
+      </c>
+      <c r="E297" s="29">
+        <v>4</v>
+      </c>
+      <c r="F297" s="28"/>
+      <c r="I297" s="30"/>
+      <c r="J297" s="28"/>
+      <c r="M297" s="30"/>
+      <c r="N297" s="29">
+        <v>0</v>
+      </c>
+      <c r="O297" s="29">
+        <v>0</v>
+      </c>
+      <c r="P297" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q297" s="28">
+        <v>6</v>
+      </c>
+      <c r="R297" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S297" s="65"/>
+      <c r="T297" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="U297" s="65">
+        <v>-1</v>
+      </c>
+      <c r="V297" s="65">
+        <v>1</v>
+      </c>
+      <c r="W297" s="65"/>
+      <c r="X297" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="Y297" s="65"/>
+      <c r="Z297" s="65"/>
+      <c r="AA297" s="65"/>
+      <c r="AB297" s="65"/>
+      <c r="AC297" s="65"/>
+      <c r="AD297" s="65"/>
+      <c r="AE297" s="65"/>
+      <c r="AF297" s="65"/>
+      <c r="AG297" s="91"/>
+      <c r="AH297" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI297" s="29">
+        <v>1</v>
+      </c>
+      <c r="AJ297" s="29">
+        <v>4</v>
+      </c>
+      <c r="AK297" s="29">
+        <v>4</v>
+      </c>
+      <c r="AP297" s="29">
+        <v>0</v>
+      </c>
+      <c r="AQ297" s="29">
+        <v>9</v>
+      </c>
+      <c r="AR297" s="92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AT297" s="93"/>
+      <c r="AU297" s="93"/>
+      <c r="AV297" s="93"/>
+      <c r="AW297" s="93"/>
+      <c r="AX297" s="93"/>
+      <c r="AY297" s="93"/>
+      <c r="AZ297" s="93"/>
+      <c r="BA297" s="93"/>
+      <c r="BB297" s="93"/>
+      <c r="BC297" s="93"/>
+      <c r="BD297" s="93"/>
+      <c r="BE297" s="93"/>
+      <c r="BF297" s="93"/>
+      <c r="BG297" s="93"/>
+      <c r="BH297" s="93"/>
+      <c r="BI297" s="93"/>
+      <c r="BJ297" s="93"/>
+      <c r="BK297" s="93"/>
+      <c r="BL297" s="93"/>
+      <c r="BM297" s="93"/>
+      <c r="BN297" s="93"/>
+      <c r="BO297" s="93"/>
+      <c r="BP297" s="93"/>
+      <c r="BQ297" s="93"/>
+      <c r="BR297" s="93"/>
+      <c r="BS297" s="93"/>
+      <c r="BT297" s="93"/>
+      <c r="BU297" s="93"/>
+      <c r="BV297" s="93"/>
+      <c r="BW297" s="93"/>
+      <c r="BX297" s="93"/>
+      <c r="BY297" s="93"/>
+      <c r="BZ297" s="93"/>
+      <c r="CA297" s="93"/>
+      <c r="CB297" s="93"/>
+      <c r="CC297" s="93"/>
+      <c r="CD297" s="93"/>
+      <c r="CE297" s="93"/>
+      <c r="CF297" s="93"/>
+      <c r="CG297" s="93"/>
+      <c r="CH297" s="93"/>
+      <c r="CI297" s="93"/>
+      <c r="CJ297" s="93"/>
+      <c r="CK297" s="93"/>
+      <c r="CL297" s="93"/>
+      <c r="CM297" s="93"/>
+      <c r="CN297" s="93"/>
+      <c r="CO297" s="93"/>
+      <c r="CP297" s="93"/>
+      <c r="CQ297" s="93"/>
+      <c r="CR297" s="93"/>
+      <c r="CS297" s="93"/>
+      <c r="CT297" s="93"/>
+      <c r="CU297" s="93"/>
+      <c r="CV297" s="93"/>
+      <c r="CW297" s="93"/>
+      <c r="CX297" s="93"/>
+      <c r="CY297" s="93"/>
+      <c r="CZ297" s="93"/>
+      <c r="DA297" s="93"/>
+      <c r="DB297" s="93"/>
+      <c r="DC297" s="93"/>
+      <c r="DD297" s="93"/>
+      <c r="DE297" s="93"/>
+      <c r="DF297" s="93"/>
+      <c r="DG297" s="93"/>
+      <c r="DH297" s="93"/>
+      <c r="DI297" s="93"/>
+      <c r="DJ297" s="93"/>
+      <c r="DK297" s="93"/>
+      <c r="DL297" s="93"/>
+      <c r="DM297" s="93"/>
+      <c r="DN297" s="93"/>
+      <c r="DO297" s="93"/>
+      <c r="DP297" s="93"/>
+      <c r="DQ297" s="93"/>
+      <c r="DR297" s="93"/>
+      <c r="DS297" s="93"/>
+      <c r="DT297" s="93"/>
+      <c r="DU297" s="93"/>
+      <c r="DV297" s="93"/>
+      <c r="DW297" s="93"/>
+      <c r="DX297" s="93"/>
+      <c r="DY297" s="93"/>
+      <c r="DZ297" s="93"/>
+      <c r="EA297" s="93"/>
+      <c r="EB297" s="93"/>
+      <c r="EC297" s="93"/>
+      <c r="ED297" s="93"/>
+      <c r="EE297" s="93"/>
+      <c r="EF297" s="93"/>
+      <c r="EG297" s="93"/>
+      <c r="EH297" s="93"/>
+      <c r="EI297" s="93"/>
+      <c r="EJ297" s="93"/>
+      <c r="EK297" s="93"/>
+      <c r="EL297" s="93"/>
+      <c r="EM297" s="93"/>
+      <c r="EN297" s="93"/>
+      <c r="EO297" s="93"/>
+      <c r="EP297" s="93"/>
+      <c r="EQ297" s="93"/>
+      <c r="ER297" s="93"/>
+      <c r="ES297" s="93"/>
+      <c r="ET297" s="93"/>
+      <c r="EU297" s="93"/>
+      <c r="EV297" s="93"/>
+      <c r="EW297" s="93"/>
+      <c r="EX297" s="93"/>
+      <c r="EY297" s="93"/>
+      <c r="EZ297" s="93"/>
+      <c r="FA297" s="93"/>
+      <c r="FB297" s="93"/>
+      <c r="FC297" s="93"/>
+      <c r="FD297" s="93"/>
+      <c r="FE297" s="93"/>
+      <c r="FF297" s="93"/>
+      <c r="FG297" s="93"/>
+      <c r="FH297" s="93"/>
+      <c r="FI297" s="93"/>
+      <c r="FJ297" s="93"/>
+      <c r="FK297" s="93"/>
+      <c r="FL297" s="93"/>
+      <c r="FM297" s="93"/>
+      <c r="FN297" s="93"/>
+      <c r="FO297" s="93"/>
+      <c r="FP297" s="93"/>
+      <c r="FQ297" s="93"/>
+      <c r="FR297" s="93"/>
+      <c r="FS297" s="93"/>
+      <c r="FT297" s="93"/>
+      <c r="FU297" s="93"/>
+      <c r="FV297" s="93"/>
+      <c r="FW297" s="93"/>
+      <c r="FX297" s="93"/>
+      <c r="FY297" s="93"/>
+      <c r="FZ297" s="93"/>
+      <c r="GA297" s="93"/>
+      <c r="GB297" s="93"/>
+      <c r="GC297" s="93"/>
+      <c r="GD297" s="93"/>
+      <c r="GE297" s="93"/>
+      <c r="GF297" s="93"/>
+      <c r="GG297" s="93"/>
+      <c r="GH297" s="93"/>
+      <c r="GI297" s="93"/>
+      <c r="GJ297" s="93"/>
+      <c r="GK297" s="93"/>
+      <c r="GL297" s="93"/>
+      <c r="GM297" s="93"/>
+      <c r="GN297" s="93"/>
+      <c r="GO297" s="93"/>
+      <c r="GP297" s="93"/>
+      <c r="GQ297" s="93"/>
+      <c r="GR297" s="93"/>
+      <c r="GS297" s="93"/>
+      <c r="GT297" s="93"/>
+      <c r="GU297" s="93"/>
+      <c r="GV297" s="93"/>
+      <c r="GW297" s="93"/>
+      <c r="GX297" s="93"/>
+      <c r="GY297" s="93"/>
+      <c r="GZ297" s="93"/>
+      <c r="HA297" s="93"/>
+      <c r="HB297" s="93"/>
+      <c r="HC297" s="93"/>
+      <c r="HD297" s="93"/>
+      <c r="HE297" s="93"/>
+      <c r="HF297" s="93"/>
+      <c r="HG297" s="93"/>
+      <c r="HH297" s="93"/>
+      <c r="HI297" s="93"/>
+      <c r="HJ297" s="93"/>
+      <c r="HK297" s="93"/>
+      <c r="HL297" s="93"/>
+      <c r="HM297" s="93"/>
+      <c r="HN297" s="93"/>
+      <c r="HO297" s="93"/>
+      <c r="HP297" s="93"/>
+      <c r="HQ297" s="93"/>
+      <c r="HR297" s="93"/>
+      <c r="HS297" s="93"/>
+      <c r="HT297" s="93"/>
+      <c r="HU297" s="93"/>
+      <c r="HV297" s="93"/>
+      <c r="HW297" s="93"/>
+      <c r="HX297" s="93"/>
+      <c r="HY297" s="93"/>
+      <c r="HZ297" s="93"/>
+      <c r="IA297" s="93"/>
+      <c r="IB297" s="93"/>
+      <c r="IC297" s="93"/>
+      <c r="ID297" s="93"/>
+      <c r="IE297" s="93"/>
+      <c r="IF297" s="93"/>
+      <c r="IG297" s="93"/>
+      <c r="IH297" s="93"/>
+      <c r="II297" s="93"/>
+      <c r="IJ297" s="93"/>
+      <c r="IK297" s="93"/>
+      <c r="IL297" s="93"/>
+      <c r="IM297" s="93"/>
+      <c r="IN297" s="93"/>
+      <c r="IO297" s="93"/>
+      <c r="IP297" s="93"/>
+      <c r="IQ297" s="93"/>
+      <c r="IR297" s="93"/>
+      <c r="IS297" s="93"/>
+      <c r="IT297" s="93"/>
+      <c r="IU297" s="93"/>
+      <c r="IV297" s="93"/>
+      <c r="IW297" s="93"/>
+      <c r="IX297" s="93"/>
+      <c r="IY297" s="93"/>
+      <c r="IZ297" s="93"/>
+      <c r="JA297" s="93"/>
+      <c r="JB297" s="93"/>
+      <c r="JC297" s="93"/>
+      <c r="JD297" s="93"/>
+      <c r="JE297" s="93"/>
+      <c r="JF297" s="93"/>
+      <c r="JG297" s="93"/>
+      <c r="JH297" s="93"/>
+      <c r="JI297" s="93"/>
+      <c r="JJ297" s="93"/>
+      <c r="JK297" s="93"/>
+      <c r="JL297" s="93"/>
+      <c r="JM297" s="93"/>
+      <c r="JN297" s="93"/>
+      <c r="JO297" s="93"/>
+      <c r="JP297" s="93"/>
+      <c r="JQ297" s="93"/>
+      <c r="JR297" s="93"/>
+      <c r="JS297" s="93"/>
+      <c r="JT297" s="93"/>
+      <c r="JU297" s="93"/>
+      <c r="JV297" s="93"/>
+      <c r="JW297" s="93"/>
+      <c r="JX297" s="93"/>
+      <c r="JY297" s="93"/>
+      <c r="JZ297" s="93"/>
+      <c r="KA297" s="93"/>
+      <c r="KB297" s="93"/>
+      <c r="KC297" s="93"/>
+      <c r="KD297" s="93"/>
+      <c r="KE297" s="93"/>
+      <c r="KF297" s="93"/>
+      <c r="KG297" s="93"/>
+      <c r="KH297" s="93"/>
+      <c r="KI297" s="93"/>
+      <c r="KJ297" s="93"/>
+      <c r="KK297" s="93"/>
+      <c r="KL297" s="93"/>
+      <c r="KM297" s="93"/>
+      <c r="KN297" s="93"/>
+      <c r="KO297" s="93"/>
+      <c r="KP297" s="93"/>
+    </row>
     <row r="298" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A298" s="41"/>
+      <c r="B298" s="33">
+        <v>3</v>
+      </c>
+      <c r="C298" s="33">
+        <v>3</v>
+      </c>
+      <c r="D298" s="33">
+        <v>3</v>
+      </c>
+      <c r="E298" s="33">
+        <v>3</v>
+      </c>
       <c r="F298" s="32"/>
       <c r="I298" s="34"/>
       <c r="J298" s="32"/>
@@ -56064,6 +56383,18 @@
       <c r="AE298" s="67"/>
       <c r="AF298" s="67"/>
       <c r="AG298" s="68"/>
+      <c r="AH298" s="33">
+        <v>3</v>
+      </c>
+      <c r="AI298" s="33">
+        <v>0</v>
+      </c>
+      <c r="AJ298" s="33">
+        <v>0</v>
+      </c>
+      <c r="AK298" s="33">
+        <v>0</v>
+      </c>
       <c r="AR298" s="83"/>
       <c r="AT298" s="84"/>
       <c r="AU298" s="84"/>
@@ -56323,8 +56654,357 @@
       <c r="KO298" s="84"/>
       <c r="KP298" s="84"/>
     </row>
+    <row r="299" spans="1:302" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="46">
+        <v>138</v>
+      </c>
+      <c r="B299" s="29">
+        <v>3</v>
+      </c>
+      <c r="C299" s="97">
+        <v>4</v>
+      </c>
+      <c r="D299" s="29">
+        <v>4</v>
+      </c>
+      <c r="E299" s="29">
+        <v>4</v>
+      </c>
+      <c r="F299" s="28"/>
+      <c r="I299" s="30"/>
+      <c r="J299" s="28"/>
+      <c r="M299" s="30"/>
+      <c r="N299" s="29">
+        <v>0</v>
+      </c>
+      <c r="O299" s="29">
+        <v>0</v>
+      </c>
+      <c r="P299" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q299" s="28">
+        <v>6</v>
+      </c>
+      <c r="R299" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S299" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="T299" s="65"/>
+      <c r="U299" s="65">
+        <v>-1</v>
+      </c>
+      <c r="V299" s="65">
+        <v>1</v>
+      </c>
+      <c r="W299" s="65"/>
+      <c r="X299" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="Y299" s="65"/>
+      <c r="Z299" s="65"/>
+      <c r="AA299" s="65"/>
+      <c r="AB299" s="65"/>
+      <c r="AC299" s="65"/>
+      <c r="AD299" s="65"/>
+      <c r="AE299" s="65"/>
+      <c r="AF299" s="65"/>
+      <c r="AG299" s="91"/>
+      <c r="AH299" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI299" s="29">
+        <v>4</v>
+      </c>
+      <c r="AJ299" s="29">
+        <v>4</v>
+      </c>
+      <c r="AK299" s="29">
+        <v>4</v>
+      </c>
+      <c r="AP299" s="29">
+        <v>0</v>
+      </c>
+      <c r="AQ299" s="29">
+        <v>0</v>
+      </c>
+      <c r="AR299" s="92" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT299" s="93"/>
+      <c r="AU299" s="93"/>
+      <c r="AV299" s="93"/>
+      <c r="AW299" s="93"/>
+      <c r="AX299" s="93"/>
+      <c r="AY299" s="93"/>
+      <c r="AZ299" s="93"/>
+      <c r="BA299" s="93"/>
+      <c r="BB299" s="93"/>
+      <c r="BC299" s="93"/>
+      <c r="BD299" s="93"/>
+      <c r="BE299" s="93"/>
+      <c r="BF299" s="93"/>
+      <c r="BG299" s="93"/>
+      <c r="BH299" s="93"/>
+      <c r="BI299" s="93"/>
+      <c r="BJ299" s="93"/>
+      <c r="BK299" s="93"/>
+      <c r="BL299" s="93"/>
+      <c r="BM299" s="93"/>
+      <c r="BN299" s="93"/>
+      <c r="BO299" s="93"/>
+      <c r="BP299" s="93"/>
+      <c r="BQ299" s="93"/>
+      <c r="BR299" s="93"/>
+      <c r="BS299" s="93"/>
+      <c r="BT299" s="93"/>
+      <c r="BU299" s="93"/>
+      <c r="BV299" s="93"/>
+      <c r="BW299" s="93"/>
+      <c r="BX299" s="93"/>
+      <c r="BY299" s="93"/>
+      <c r="BZ299" s="93"/>
+      <c r="CA299" s="93"/>
+      <c r="CB299" s="93"/>
+      <c r="CC299" s="93"/>
+      <c r="CD299" s="93"/>
+      <c r="CE299" s="93"/>
+      <c r="CF299" s="93"/>
+      <c r="CG299" s="93"/>
+      <c r="CH299" s="93"/>
+      <c r="CI299" s="93"/>
+      <c r="CJ299" s="93"/>
+      <c r="CK299" s="93"/>
+      <c r="CL299" s="93"/>
+      <c r="CM299" s="93"/>
+      <c r="CN299" s="93"/>
+      <c r="CO299" s="93"/>
+      <c r="CP299" s="93"/>
+      <c r="CQ299" s="93"/>
+      <c r="CR299" s="93"/>
+      <c r="CS299" s="93"/>
+      <c r="CT299" s="93"/>
+      <c r="CU299" s="93"/>
+      <c r="CV299" s="93"/>
+      <c r="CW299" s="93"/>
+      <c r="CX299" s="93"/>
+      <c r="CY299" s="93"/>
+      <c r="CZ299" s="93"/>
+      <c r="DA299" s="93"/>
+      <c r="DB299" s="93"/>
+      <c r="DC299" s="93"/>
+      <c r="DD299" s="93"/>
+      <c r="DE299" s="93"/>
+      <c r="DF299" s="93"/>
+      <c r="DG299" s="93"/>
+      <c r="DH299" s="93"/>
+      <c r="DI299" s="93"/>
+      <c r="DJ299" s="93"/>
+      <c r="DK299" s="93"/>
+      <c r="DL299" s="93"/>
+      <c r="DM299" s="93"/>
+      <c r="DN299" s="93"/>
+      <c r="DO299" s="93"/>
+      <c r="DP299" s="93"/>
+      <c r="DQ299" s="93"/>
+      <c r="DR299" s="93"/>
+      <c r="DS299" s="93"/>
+      <c r="DT299" s="93"/>
+      <c r="DU299" s="93"/>
+      <c r="DV299" s="93"/>
+      <c r="DW299" s="93"/>
+      <c r="DX299" s="93"/>
+      <c r="DY299" s="93"/>
+      <c r="DZ299" s="93"/>
+      <c r="EA299" s="93"/>
+      <c r="EB299" s="93"/>
+      <c r="EC299" s="93"/>
+      <c r="ED299" s="93"/>
+      <c r="EE299" s="93"/>
+      <c r="EF299" s="93"/>
+      <c r="EG299" s="93"/>
+      <c r="EH299" s="93"/>
+      <c r="EI299" s="93"/>
+      <c r="EJ299" s="93"/>
+      <c r="EK299" s="93"/>
+      <c r="EL299" s="93"/>
+      <c r="EM299" s="93"/>
+      <c r="EN299" s="93"/>
+      <c r="EO299" s="93"/>
+      <c r="EP299" s="93"/>
+      <c r="EQ299" s="93"/>
+      <c r="ER299" s="93"/>
+      <c r="ES299" s="93"/>
+      <c r="ET299" s="93"/>
+      <c r="EU299" s="93"/>
+      <c r="EV299" s="93"/>
+      <c r="EW299" s="93"/>
+      <c r="EX299" s="93"/>
+      <c r="EY299" s="93"/>
+      <c r="EZ299" s="93"/>
+      <c r="FA299" s="93"/>
+      <c r="FB299" s="93"/>
+      <c r="FC299" s="93"/>
+      <c r="FD299" s="93"/>
+      <c r="FE299" s="93"/>
+      <c r="FF299" s="93"/>
+      <c r="FG299" s="93"/>
+      <c r="FH299" s="93"/>
+      <c r="FI299" s="93"/>
+      <c r="FJ299" s="93"/>
+      <c r="FK299" s="93"/>
+      <c r="FL299" s="93"/>
+      <c r="FM299" s="93"/>
+      <c r="FN299" s="93"/>
+      <c r="FO299" s="93"/>
+      <c r="FP299" s="93"/>
+      <c r="FQ299" s="93"/>
+      <c r="FR299" s="93"/>
+      <c r="FS299" s="93"/>
+      <c r="FT299" s="93"/>
+      <c r="FU299" s="93"/>
+      <c r="FV299" s="93"/>
+      <c r="FW299" s="93"/>
+      <c r="FX299" s="93"/>
+      <c r="FY299" s="93"/>
+      <c r="FZ299" s="93"/>
+      <c r="GA299" s="93"/>
+      <c r="GB299" s="93"/>
+      <c r="GC299" s="93"/>
+      <c r="GD299" s="93"/>
+      <c r="GE299" s="93"/>
+      <c r="GF299" s="93"/>
+      <c r="GG299" s="93"/>
+      <c r="GH299" s="93"/>
+      <c r="GI299" s="93"/>
+      <c r="GJ299" s="93"/>
+      <c r="GK299" s="93"/>
+      <c r="GL299" s="93"/>
+      <c r="GM299" s="93"/>
+      <c r="GN299" s="93"/>
+      <c r="GO299" s="93"/>
+      <c r="GP299" s="93"/>
+      <c r="GQ299" s="93"/>
+      <c r="GR299" s="93"/>
+      <c r="GS299" s="93"/>
+      <c r="GT299" s="93"/>
+      <c r="GU299" s="93"/>
+      <c r="GV299" s="93"/>
+      <c r="GW299" s="93"/>
+      <c r="GX299" s="93"/>
+      <c r="GY299" s="93"/>
+      <c r="GZ299" s="93"/>
+      <c r="HA299" s="93"/>
+      <c r="HB299" s="93"/>
+      <c r="HC299" s="93"/>
+      <c r="HD299" s="93"/>
+      <c r="HE299" s="93"/>
+      <c r="HF299" s="93"/>
+      <c r="HG299" s="93"/>
+      <c r="HH299" s="93"/>
+      <c r="HI299" s="93"/>
+      <c r="HJ299" s="93"/>
+      <c r="HK299" s="93"/>
+      <c r="HL299" s="93"/>
+      <c r="HM299" s="93"/>
+      <c r="HN299" s="93"/>
+      <c r="HO299" s="93"/>
+      <c r="HP299" s="93"/>
+      <c r="HQ299" s="93"/>
+      <c r="HR299" s="93"/>
+      <c r="HS299" s="93"/>
+      <c r="HT299" s="93"/>
+      <c r="HU299" s="93"/>
+      <c r="HV299" s="93"/>
+      <c r="HW299" s="93"/>
+      <c r="HX299" s="93"/>
+      <c r="HY299" s="93"/>
+      <c r="HZ299" s="93"/>
+      <c r="IA299" s="93"/>
+      <c r="IB299" s="93"/>
+      <c r="IC299" s="93"/>
+      <c r="ID299" s="93"/>
+      <c r="IE299" s="93"/>
+      <c r="IF299" s="93"/>
+      <c r="IG299" s="93"/>
+      <c r="IH299" s="93"/>
+      <c r="II299" s="93"/>
+      <c r="IJ299" s="93"/>
+      <c r="IK299" s="93"/>
+      <c r="IL299" s="93"/>
+      <c r="IM299" s="93"/>
+      <c r="IN299" s="93"/>
+      <c r="IO299" s="93"/>
+      <c r="IP299" s="93"/>
+      <c r="IQ299" s="93"/>
+      <c r="IR299" s="93"/>
+      <c r="IS299" s="93"/>
+      <c r="IT299" s="93"/>
+      <c r="IU299" s="93"/>
+      <c r="IV299" s="93"/>
+      <c r="IW299" s="93"/>
+      <c r="IX299" s="93"/>
+      <c r="IY299" s="93"/>
+      <c r="IZ299" s="93"/>
+      <c r="JA299" s="93"/>
+      <c r="JB299" s="93"/>
+      <c r="JC299" s="93"/>
+      <c r="JD299" s="93"/>
+      <c r="JE299" s="93"/>
+      <c r="JF299" s="93"/>
+      <c r="JG299" s="93"/>
+      <c r="JH299" s="93"/>
+      <c r="JI299" s="93"/>
+      <c r="JJ299" s="93"/>
+      <c r="JK299" s="93"/>
+      <c r="JL299" s="93"/>
+      <c r="JM299" s="93"/>
+      <c r="JN299" s="93"/>
+      <c r="JO299" s="93"/>
+      <c r="JP299" s="93"/>
+      <c r="JQ299" s="93"/>
+      <c r="JR299" s="93"/>
+      <c r="JS299" s="93"/>
+      <c r="JT299" s="93"/>
+      <c r="JU299" s="93"/>
+      <c r="JV299" s="93"/>
+      <c r="JW299" s="93"/>
+      <c r="JX299" s="93"/>
+      <c r="JY299" s="93"/>
+      <c r="JZ299" s="93"/>
+      <c r="KA299" s="93"/>
+      <c r="KB299" s="93"/>
+      <c r="KC299" s="93"/>
+      <c r="KD299" s="93"/>
+      <c r="KE299" s="93"/>
+      <c r="KF299" s="93"/>
+      <c r="KG299" s="93"/>
+      <c r="KH299" s="93"/>
+      <c r="KI299" s="93"/>
+      <c r="KJ299" s="93"/>
+      <c r="KK299" s="93"/>
+      <c r="KL299" s="93"/>
+      <c r="KM299" s="93"/>
+      <c r="KN299" s="93"/>
+      <c r="KO299" s="93"/>
+      <c r="KP299" s="93"/>
+    </row>
     <row r="300" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A300" s="41"/>
+      <c r="B300" s="33">
+        <v>3</v>
+      </c>
+      <c r="C300" s="33">
+        <v>3</v>
+      </c>
+      <c r="D300" s="33">
+        <v>3</v>
+      </c>
+      <c r="E300" s="33">
+        <v>0</v>
+      </c>
       <c r="F300" s="32"/>
       <c r="I300" s="34"/>
       <c r="J300" s="32"/>
@@ -56346,6 +57026,18 @@
       <c r="AE300" s="67"/>
       <c r="AF300" s="67"/>
       <c r="AG300" s="68"/>
+      <c r="AH300" s="33">
+        <v>3</v>
+      </c>
+      <c r="AI300" s="33">
+        <v>3</v>
+      </c>
+      <c r="AJ300" s="33">
+        <v>3</v>
+      </c>
+      <c r="AK300" s="33">
+        <v>0</v>
+      </c>
       <c r="AR300" s="83"/>
       <c r="AT300" s="84"/>
       <c r="AU300" s="84"/>

</xml_diff>

<commit_message>
Added sandwich capture which is used as an variation for Dakon.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73979B4B-5B34-4033-8FDA-5A1413B46B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549FBD18-2301-4CDA-8F38-3A4A59290758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="210">
   <si>
     <t>setup</t>
   </si>
@@ -649,6 +649,21 @@
   <si>
     <t>1_ANY</t>
   </si>
+  <si>
+    <t>SAND</t>
+  </si>
+  <si>
+    <t>not single seed</t>
+  </si>
+  <si>
+    <t>not match</t>
+  </si>
+  <si>
+    <t>not opp holes</t>
+  </si>
+  <si>
+    <t>capture</t>
+  </si>
 </sst>
 </file>
 
@@ -1153,7 +1168,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1337,6 +1352,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1670,12 +1690,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AMK312"/>
+  <dimension ref="A1:AMK324"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AQ298" sqref="AQ298"/>
+      <selection pane="bottomLeft" activeCell="AJ308" sqref="AJ308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -57297,8 +57317,79 @@
       <c r="KO300" s="84"/>
       <c r="KP300" s="84"/>
     </row>
+    <row r="301" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="A301" s="40">
+        <v>139</v>
+      </c>
+      <c r="B301" s="29">
+        <v>3</v>
+      </c>
+      <c r="C301" s="29">
+        <v>3</v>
+      </c>
+      <c r="D301" s="87">
+        <v>2</v>
+      </c>
+      <c r="E301" s="29">
+        <v>3</v>
+      </c>
+      <c r="N301">
+        <v>3</v>
+      </c>
+      <c r="O301">
+        <v>3</v>
+      </c>
+      <c r="P301" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q301" s="23">
+        <v>5</v>
+      </c>
+      <c r="R301" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB301" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH301" s="99">
+        <v>3</v>
+      </c>
+      <c r="AI301" s="99">
+        <v>3</v>
+      </c>
+      <c r="AJ301" s="99">
+        <v>2</v>
+      </c>
+      <c r="AK301" s="99">
+        <v>3</v>
+      </c>
+      <c r="AP301">
+        <v>3</v>
+      </c>
+      <c r="AQ301">
+        <v>3</v>
+      </c>
+      <c r="AR301" s="80" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS301" t="s">
+        <v>206</v>
+      </c>
+    </row>
     <row r="302" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A302" s="41"/>
+      <c r="B302" s="98">
+        <v>3</v>
+      </c>
+      <c r="C302" s="33">
+        <v>1</v>
+      </c>
+      <c r="D302" s="33">
+        <v>3</v>
+      </c>
+      <c r="E302" s="34">
+        <v>0</v>
+      </c>
       <c r="F302" s="32"/>
       <c r="I302" s="34"/>
       <c r="J302" s="32"/>
@@ -57320,6 +57411,18 @@
       <c r="AE302" s="67"/>
       <c r="AF302" s="67"/>
       <c r="AG302" s="68"/>
+      <c r="AH302" s="100">
+        <v>3</v>
+      </c>
+      <c r="AI302" s="101">
+        <v>1</v>
+      </c>
+      <c r="AJ302" s="101">
+        <v>3</v>
+      </c>
+      <c r="AK302" s="102">
+        <v>0</v>
+      </c>
       <c r="AR302" s="83"/>
       <c r="AT302" s="84"/>
       <c r="AU302" s="84"/>
@@ -57579,8 +57682,79 @@
       <c r="KO302" s="84"/>
       <c r="KP302" s="84"/>
     </row>
+    <row r="303" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="A303" s="40">
+        <v>140</v>
+      </c>
+      <c r="B303" s="29">
+        <v>3</v>
+      </c>
+      <c r="C303" s="29">
+        <v>3</v>
+      </c>
+      <c r="D303" s="87">
+        <v>1</v>
+      </c>
+      <c r="E303" s="29">
+        <v>4</v>
+      </c>
+      <c r="N303">
+        <v>3</v>
+      </c>
+      <c r="O303">
+        <v>3</v>
+      </c>
+      <c r="P303" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q303" s="23">
+        <v>5</v>
+      </c>
+      <c r="R303" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB303" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH303" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI303" s="29">
+        <v>3</v>
+      </c>
+      <c r="AJ303" s="99">
+        <v>1</v>
+      </c>
+      <c r="AK303" s="46">
+        <v>4</v>
+      </c>
+      <c r="AP303">
+        <v>3</v>
+      </c>
+      <c r="AQ303">
+        <v>3</v>
+      </c>
+      <c r="AR303" s="80" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS303" t="s">
+        <v>207</v>
+      </c>
+    </row>
     <row r="304" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A304" s="41"/>
+      <c r="B304" s="98">
+        <v>3</v>
+      </c>
+      <c r="C304" s="33">
+        <v>1</v>
+      </c>
+      <c r="D304" s="33">
+        <v>3</v>
+      </c>
+      <c r="E304" s="34">
+        <v>0</v>
+      </c>
       <c r="F304" s="32"/>
       <c r="I304" s="34"/>
       <c r="J304" s="32"/>
@@ -57602,6 +57776,18 @@
       <c r="AE304" s="67"/>
       <c r="AF304" s="67"/>
       <c r="AG304" s="68"/>
+      <c r="AH304" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI304" s="33">
+        <v>1</v>
+      </c>
+      <c r="AJ304" s="33">
+        <v>3</v>
+      </c>
+      <c r="AK304" s="41">
+        <v>0</v>
+      </c>
       <c r="AR304" s="83"/>
       <c r="AT304" s="84"/>
       <c r="AU304" s="84"/>
@@ -57861,8 +58047,79 @@
       <c r="KO304" s="84"/>
       <c r="KP304" s="84"/>
     </row>
+    <row r="305" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="A305" s="40">
+        <v>141</v>
+      </c>
+      <c r="B305" s="29">
+        <v>3</v>
+      </c>
+      <c r="C305" s="29">
+        <v>3</v>
+      </c>
+      <c r="D305" s="99">
+        <v>3</v>
+      </c>
+      <c r="E305" s="87">
+        <v>1</v>
+      </c>
+      <c r="N305">
+        <v>3</v>
+      </c>
+      <c r="O305">
+        <v>4</v>
+      </c>
+      <c r="P305" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q305" s="23">
+        <v>4</v>
+      </c>
+      <c r="R305" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB305" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH305" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI305" s="29">
+        <v>3</v>
+      </c>
+      <c r="AJ305" s="99">
+        <v>3</v>
+      </c>
+      <c r="AK305" s="103">
+        <v>1</v>
+      </c>
+      <c r="AP305">
+        <v>3</v>
+      </c>
+      <c r="AQ305">
+        <v>4</v>
+      </c>
+      <c r="AR305" s="80" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS305" t="s">
+        <v>208</v>
+      </c>
+    </row>
     <row r="306" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A306" s="41"/>
+      <c r="B306" s="98">
+        <v>3</v>
+      </c>
+      <c r="C306" s="33">
+        <v>1</v>
+      </c>
+      <c r="D306" s="33">
+        <v>0</v>
+      </c>
+      <c r="E306" s="34">
+        <v>3</v>
+      </c>
       <c r="F306" s="32"/>
       <c r="I306" s="34"/>
       <c r="J306" s="32"/>
@@ -57884,6 +58141,18 @@
       <c r="AE306" s="67"/>
       <c r="AF306" s="67"/>
       <c r="AG306" s="68"/>
+      <c r="AH306" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI306" s="33">
+        <v>1</v>
+      </c>
+      <c r="AJ306" s="33">
+        <v>0</v>
+      </c>
+      <c r="AK306" s="41">
+        <v>3</v>
+      </c>
       <c r="AR306" s="83"/>
       <c r="AT306" s="84"/>
       <c r="AU306" s="84"/>
@@ -58143,8 +58412,79 @@
       <c r="KO306" s="84"/>
       <c r="KP306" s="84"/>
     </row>
+    <row r="307" spans="1:302" x14ac:dyDescent="0.2">
+      <c r="A307" s="40">
+        <v>142</v>
+      </c>
+      <c r="B307" s="29">
+        <v>3</v>
+      </c>
+      <c r="C307" s="29">
+        <v>3</v>
+      </c>
+      <c r="D307" s="87">
+        <v>1</v>
+      </c>
+      <c r="E307" s="29">
+        <v>3</v>
+      </c>
+      <c r="N307">
+        <v>3</v>
+      </c>
+      <c r="O307">
+        <v>4</v>
+      </c>
+      <c r="P307" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q307" s="23">
+        <v>5</v>
+      </c>
+      <c r="R307" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB307" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH307">
+        <v>3</v>
+      </c>
+      <c r="AI307">
+        <v>0</v>
+      </c>
+      <c r="AJ307">
+        <v>0</v>
+      </c>
+      <c r="AK307" s="40">
+        <v>0</v>
+      </c>
+      <c r="AP307">
+        <v>10</v>
+      </c>
+      <c r="AQ307">
+        <v>4</v>
+      </c>
+      <c r="AR307" s="80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS307" t="s">
+        <v>209</v>
+      </c>
+    </row>
     <row r="308" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A308" s="41"/>
+      <c r="B308" s="98">
+        <v>3</v>
+      </c>
+      <c r="C308" s="33">
+        <v>1</v>
+      </c>
+      <c r="D308" s="33">
+        <v>1</v>
+      </c>
+      <c r="E308" s="34">
+        <v>2</v>
+      </c>
       <c r="F308" s="32"/>
       <c r="I308" s="34"/>
       <c r="J308" s="32"/>
@@ -58166,6 +58506,18 @@
       <c r="AE308" s="67"/>
       <c r="AF308" s="67"/>
       <c r="AG308" s="68"/>
+      <c r="AH308" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI308" s="33">
+        <v>1</v>
+      </c>
+      <c r="AJ308" s="33">
+        <v>1</v>
+      </c>
+      <c r="AK308" s="34">
+        <v>2</v>
+      </c>
       <c r="AR308" s="83"/>
       <c r="AT308" s="84"/>
       <c r="AU308" s="84"/>
@@ -58989,6 +59341,1698 @@
       <c r="KO312" s="84"/>
       <c r="KP312" s="84"/>
     </row>
+    <row r="314" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A314" s="41"/>
+      <c r="F314" s="32"/>
+      <c r="I314" s="34"/>
+      <c r="J314" s="32"/>
+      <c r="M314" s="34"/>
+      <c r="Q314" s="32"/>
+      <c r="R314" s="34"/>
+      <c r="S314" s="67"/>
+      <c r="T314" s="67"/>
+      <c r="U314" s="67"/>
+      <c r="V314" s="67"/>
+      <c r="W314" s="67"/>
+      <c r="X314" s="67"/>
+      <c r="Y314" s="67"/>
+      <c r="Z314" s="67"/>
+      <c r="AA314" s="67"/>
+      <c r="AB314" s="67"/>
+      <c r="AC314" s="67"/>
+      <c r="AD314" s="67"/>
+      <c r="AE314" s="67"/>
+      <c r="AF314" s="67"/>
+      <c r="AG314" s="68"/>
+      <c r="AR314" s="83"/>
+      <c r="AT314" s="84"/>
+      <c r="AU314" s="84"/>
+      <c r="AV314" s="84"/>
+      <c r="AW314" s="84"/>
+      <c r="AX314" s="84"/>
+      <c r="AY314" s="84"/>
+      <c r="AZ314" s="84"/>
+      <c r="BA314" s="84"/>
+      <c r="BB314" s="84"/>
+      <c r="BC314" s="84"/>
+      <c r="BD314" s="84"/>
+      <c r="BE314" s="84"/>
+      <c r="BF314" s="84"/>
+      <c r="BG314" s="84"/>
+      <c r="BH314" s="84"/>
+      <c r="BI314" s="84"/>
+      <c r="BJ314" s="84"/>
+      <c r="BK314" s="84"/>
+      <c r="BL314" s="84"/>
+      <c r="BM314" s="84"/>
+      <c r="BN314" s="84"/>
+      <c r="BO314" s="84"/>
+      <c r="BP314" s="84"/>
+      <c r="BQ314" s="84"/>
+      <c r="BR314" s="84"/>
+      <c r="BS314" s="84"/>
+      <c r="BT314" s="84"/>
+      <c r="BU314" s="84"/>
+      <c r="BV314" s="84"/>
+      <c r="BW314" s="84"/>
+      <c r="BX314" s="84"/>
+      <c r="BY314" s="84"/>
+      <c r="BZ314" s="84"/>
+      <c r="CA314" s="84"/>
+      <c r="CB314" s="84"/>
+      <c r="CC314" s="84"/>
+      <c r="CD314" s="84"/>
+      <c r="CE314" s="84"/>
+      <c r="CF314" s="84"/>
+      <c r="CG314" s="84"/>
+      <c r="CH314" s="84"/>
+      <c r="CI314" s="84"/>
+      <c r="CJ314" s="84"/>
+      <c r="CK314" s="84"/>
+      <c r="CL314" s="84"/>
+      <c r="CM314" s="84"/>
+      <c r="CN314" s="84"/>
+      <c r="CO314" s="84"/>
+      <c r="CP314" s="84"/>
+      <c r="CQ314" s="84"/>
+      <c r="CR314" s="84"/>
+      <c r="CS314" s="84"/>
+      <c r="CT314" s="84"/>
+      <c r="CU314" s="84"/>
+      <c r="CV314" s="84"/>
+      <c r="CW314" s="84"/>
+      <c r="CX314" s="84"/>
+      <c r="CY314" s="84"/>
+      <c r="CZ314" s="84"/>
+      <c r="DA314" s="84"/>
+      <c r="DB314" s="84"/>
+      <c r="DC314" s="84"/>
+      <c r="DD314" s="84"/>
+      <c r="DE314" s="84"/>
+      <c r="DF314" s="84"/>
+      <c r="DG314" s="84"/>
+      <c r="DH314" s="84"/>
+      <c r="DI314" s="84"/>
+      <c r="DJ314" s="84"/>
+      <c r="DK314" s="84"/>
+      <c r="DL314" s="84"/>
+      <c r="DM314" s="84"/>
+      <c r="DN314" s="84"/>
+      <c r="DO314" s="84"/>
+      <c r="DP314" s="84"/>
+      <c r="DQ314" s="84"/>
+      <c r="DR314" s="84"/>
+      <c r="DS314" s="84"/>
+      <c r="DT314" s="84"/>
+      <c r="DU314" s="84"/>
+      <c r="DV314" s="84"/>
+      <c r="DW314" s="84"/>
+      <c r="DX314" s="84"/>
+      <c r="DY314" s="84"/>
+      <c r="DZ314" s="84"/>
+      <c r="EA314" s="84"/>
+      <c r="EB314" s="84"/>
+      <c r="EC314" s="84"/>
+      <c r="ED314" s="84"/>
+      <c r="EE314" s="84"/>
+      <c r="EF314" s="84"/>
+      <c r="EG314" s="84"/>
+      <c r="EH314" s="84"/>
+      <c r="EI314" s="84"/>
+      <c r="EJ314" s="84"/>
+      <c r="EK314" s="84"/>
+      <c r="EL314" s="84"/>
+      <c r="EM314" s="84"/>
+      <c r="EN314" s="84"/>
+      <c r="EO314" s="84"/>
+      <c r="EP314" s="84"/>
+      <c r="EQ314" s="84"/>
+      <c r="ER314" s="84"/>
+      <c r="ES314" s="84"/>
+      <c r="ET314" s="84"/>
+      <c r="EU314" s="84"/>
+      <c r="EV314" s="84"/>
+      <c r="EW314" s="84"/>
+      <c r="EX314" s="84"/>
+      <c r="EY314" s="84"/>
+      <c r="EZ314" s="84"/>
+      <c r="FA314" s="84"/>
+      <c r="FB314" s="84"/>
+      <c r="FC314" s="84"/>
+      <c r="FD314" s="84"/>
+      <c r="FE314" s="84"/>
+      <c r="FF314" s="84"/>
+      <c r="FG314" s="84"/>
+      <c r="FH314" s="84"/>
+      <c r="FI314" s="84"/>
+      <c r="FJ314" s="84"/>
+      <c r="FK314" s="84"/>
+      <c r="FL314" s="84"/>
+      <c r="FM314" s="84"/>
+      <c r="FN314" s="84"/>
+      <c r="FO314" s="84"/>
+      <c r="FP314" s="84"/>
+      <c r="FQ314" s="84"/>
+      <c r="FR314" s="84"/>
+      <c r="FS314" s="84"/>
+      <c r="FT314" s="84"/>
+      <c r="FU314" s="84"/>
+      <c r="FV314" s="84"/>
+      <c r="FW314" s="84"/>
+      <c r="FX314" s="84"/>
+      <c r="FY314" s="84"/>
+      <c r="FZ314" s="84"/>
+      <c r="GA314" s="84"/>
+      <c r="GB314" s="84"/>
+      <c r="GC314" s="84"/>
+      <c r="GD314" s="84"/>
+      <c r="GE314" s="84"/>
+      <c r="GF314" s="84"/>
+      <c r="GG314" s="84"/>
+      <c r="GH314" s="84"/>
+      <c r="GI314" s="84"/>
+      <c r="GJ314" s="84"/>
+      <c r="GK314" s="84"/>
+      <c r="GL314" s="84"/>
+      <c r="GM314" s="84"/>
+      <c r="GN314" s="84"/>
+      <c r="GO314" s="84"/>
+      <c r="GP314" s="84"/>
+      <c r="GQ314" s="84"/>
+      <c r="GR314" s="84"/>
+      <c r="GS314" s="84"/>
+      <c r="GT314" s="84"/>
+      <c r="GU314" s="84"/>
+      <c r="GV314" s="84"/>
+      <c r="GW314" s="84"/>
+      <c r="GX314" s="84"/>
+      <c r="GY314" s="84"/>
+      <c r="GZ314" s="84"/>
+      <c r="HA314" s="84"/>
+      <c r="HB314" s="84"/>
+      <c r="HC314" s="84"/>
+      <c r="HD314" s="84"/>
+      <c r="HE314" s="84"/>
+      <c r="HF314" s="84"/>
+      <c r="HG314" s="84"/>
+      <c r="HH314" s="84"/>
+      <c r="HI314" s="84"/>
+      <c r="HJ314" s="84"/>
+      <c r="HK314" s="84"/>
+      <c r="HL314" s="84"/>
+      <c r="HM314" s="84"/>
+      <c r="HN314" s="84"/>
+      <c r="HO314" s="84"/>
+      <c r="HP314" s="84"/>
+      <c r="HQ314" s="84"/>
+      <c r="HR314" s="84"/>
+      <c r="HS314" s="84"/>
+      <c r="HT314" s="84"/>
+      <c r="HU314" s="84"/>
+      <c r="HV314" s="84"/>
+      <c r="HW314" s="84"/>
+      <c r="HX314" s="84"/>
+      <c r="HY314" s="84"/>
+      <c r="HZ314" s="84"/>
+      <c r="IA314" s="84"/>
+      <c r="IB314" s="84"/>
+      <c r="IC314" s="84"/>
+      <c r="ID314" s="84"/>
+      <c r="IE314" s="84"/>
+      <c r="IF314" s="84"/>
+      <c r="IG314" s="84"/>
+      <c r="IH314" s="84"/>
+      <c r="II314" s="84"/>
+      <c r="IJ314" s="84"/>
+      <c r="IK314" s="84"/>
+      <c r="IL314" s="84"/>
+      <c r="IM314" s="84"/>
+      <c r="IN314" s="84"/>
+      <c r="IO314" s="84"/>
+      <c r="IP314" s="84"/>
+      <c r="IQ314" s="84"/>
+      <c r="IR314" s="84"/>
+      <c r="IS314" s="84"/>
+      <c r="IT314" s="84"/>
+      <c r="IU314" s="84"/>
+      <c r="IV314" s="84"/>
+      <c r="IW314" s="84"/>
+      <c r="IX314" s="84"/>
+      <c r="IY314" s="84"/>
+      <c r="IZ314" s="84"/>
+      <c r="JA314" s="84"/>
+      <c r="JB314" s="84"/>
+      <c r="JC314" s="84"/>
+      <c r="JD314" s="84"/>
+      <c r="JE314" s="84"/>
+      <c r="JF314" s="84"/>
+      <c r="JG314" s="84"/>
+      <c r="JH314" s="84"/>
+      <c r="JI314" s="84"/>
+      <c r="JJ314" s="84"/>
+      <c r="JK314" s="84"/>
+      <c r="JL314" s="84"/>
+      <c r="JM314" s="84"/>
+      <c r="JN314" s="84"/>
+      <c r="JO314" s="84"/>
+      <c r="JP314" s="84"/>
+      <c r="JQ314" s="84"/>
+      <c r="JR314" s="84"/>
+      <c r="JS314" s="84"/>
+      <c r="JT314" s="84"/>
+      <c r="JU314" s="84"/>
+      <c r="JV314" s="84"/>
+      <c r="JW314" s="84"/>
+      <c r="JX314" s="84"/>
+      <c r="JY314" s="84"/>
+      <c r="JZ314" s="84"/>
+      <c r="KA314" s="84"/>
+      <c r="KB314" s="84"/>
+      <c r="KC314" s="84"/>
+      <c r="KD314" s="84"/>
+      <c r="KE314" s="84"/>
+      <c r="KF314" s="84"/>
+      <c r="KG314" s="84"/>
+      <c r="KH314" s="84"/>
+      <c r="KI314" s="84"/>
+      <c r="KJ314" s="84"/>
+      <c r="KK314" s="84"/>
+      <c r="KL314" s="84"/>
+      <c r="KM314" s="84"/>
+      <c r="KN314" s="84"/>
+      <c r="KO314" s="84"/>
+      <c r="KP314" s="84"/>
+    </row>
+    <row r="316" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A316" s="41"/>
+      <c r="F316" s="32"/>
+      <c r="I316" s="34"/>
+      <c r="J316" s="32"/>
+      <c r="M316" s="34"/>
+      <c r="Q316" s="32"/>
+      <c r="R316" s="34"/>
+      <c r="S316" s="67"/>
+      <c r="T316" s="67"/>
+      <c r="U316" s="67"/>
+      <c r="V316" s="67"/>
+      <c r="W316" s="67"/>
+      <c r="X316" s="67"/>
+      <c r="Y316" s="67"/>
+      <c r="Z316" s="67"/>
+      <c r="AA316" s="67"/>
+      <c r="AB316" s="67"/>
+      <c r="AC316" s="67"/>
+      <c r="AD316" s="67"/>
+      <c r="AE316" s="67"/>
+      <c r="AF316" s="67"/>
+      <c r="AG316" s="68"/>
+      <c r="AR316" s="83"/>
+      <c r="AT316" s="84"/>
+      <c r="AU316" s="84"/>
+      <c r="AV316" s="84"/>
+      <c r="AW316" s="84"/>
+      <c r="AX316" s="84"/>
+      <c r="AY316" s="84"/>
+      <c r="AZ316" s="84"/>
+      <c r="BA316" s="84"/>
+      <c r="BB316" s="84"/>
+      <c r="BC316" s="84"/>
+      <c r="BD316" s="84"/>
+      <c r="BE316" s="84"/>
+      <c r="BF316" s="84"/>
+      <c r="BG316" s="84"/>
+      <c r="BH316" s="84"/>
+      <c r="BI316" s="84"/>
+      <c r="BJ316" s="84"/>
+      <c r="BK316" s="84"/>
+      <c r="BL316" s="84"/>
+      <c r="BM316" s="84"/>
+      <c r="BN316" s="84"/>
+      <c r="BO316" s="84"/>
+      <c r="BP316" s="84"/>
+      <c r="BQ316" s="84"/>
+      <c r="BR316" s="84"/>
+      <c r="BS316" s="84"/>
+      <c r="BT316" s="84"/>
+      <c r="BU316" s="84"/>
+      <c r="BV316" s="84"/>
+      <c r="BW316" s="84"/>
+      <c r="BX316" s="84"/>
+      <c r="BY316" s="84"/>
+      <c r="BZ316" s="84"/>
+      <c r="CA316" s="84"/>
+      <c r="CB316" s="84"/>
+      <c r="CC316" s="84"/>
+      <c r="CD316" s="84"/>
+      <c r="CE316" s="84"/>
+      <c r="CF316" s="84"/>
+      <c r="CG316" s="84"/>
+      <c r="CH316" s="84"/>
+      <c r="CI316" s="84"/>
+      <c r="CJ316" s="84"/>
+      <c r="CK316" s="84"/>
+      <c r="CL316" s="84"/>
+      <c r="CM316" s="84"/>
+      <c r="CN316" s="84"/>
+      <c r="CO316" s="84"/>
+      <c r="CP316" s="84"/>
+      <c r="CQ316" s="84"/>
+      <c r="CR316" s="84"/>
+      <c r="CS316" s="84"/>
+      <c r="CT316" s="84"/>
+      <c r="CU316" s="84"/>
+      <c r="CV316" s="84"/>
+      <c r="CW316" s="84"/>
+      <c r="CX316" s="84"/>
+      <c r="CY316" s="84"/>
+      <c r="CZ316" s="84"/>
+      <c r="DA316" s="84"/>
+      <c r="DB316" s="84"/>
+      <c r="DC316" s="84"/>
+      <c r="DD316" s="84"/>
+      <c r="DE316" s="84"/>
+      <c r="DF316" s="84"/>
+      <c r="DG316" s="84"/>
+      <c r="DH316" s="84"/>
+      <c r="DI316" s="84"/>
+      <c r="DJ316" s="84"/>
+      <c r="DK316" s="84"/>
+      <c r="DL316" s="84"/>
+      <c r="DM316" s="84"/>
+      <c r="DN316" s="84"/>
+      <c r="DO316" s="84"/>
+      <c r="DP316" s="84"/>
+      <c r="DQ316" s="84"/>
+      <c r="DR316" s="84"/>
+      <c r="DS316" s="84"/>
+      <c r="DT316" s="84"/>
+      <c r="DU316" s="84"/>
+      <c r="DV316" s="84"/>
+      <c r="DW316" s="84"/>
+      <c r="DX316" s="84"/>
+      <c r="DY316" s="84"/>
+      <c r="DZ316" s="84"/>
+      <c r="EA316" s="84"/>
+      <c r="EB316" s="84"/>
+      <c r="EC316" s="84"/>
+      <c r="ED316" s="84"/>
+      <c r="EE316" s="84"/>
+      <c r="EF316" s="84"/>
+      <c r="EG316" s="84"/>
+      <c r="EH316" s="84"/>
+      <c r="EI316" s="84"/>
+      <c r="EJ316" s="84"/>
+      <c r="EK316" s="84"/>
+      <c r="EL316" s="84"/>
+      <c r="EM316" s="84"/>
+      <c r="EN316" s="84"/>
+      <c r="EO316" s="84"/>
+      <c r="EP316" s="84"/>
+      <c r="EQ316" s="84"/>
+      <c r="ER316" s="84"/>
+      <c r="ES316" s="84"/>
+      <c r="ET316" s="84"/>
+      <c r="EU316" s="84"/>
+      <c r="EV316" s="84"/>
+      <c r="EW316" s="84"/>
+      <c r="EX316" s="84"/>
+      <c r="EY316" s="84"/>
+      <c r="EZ316" s="84"/>
+      <c r="FA316" s="84"/>
+      <c r="FB316" s="84"/>
+      <c r="FC316" s="84"/>
+      <c r="FD316" s="84"/>
+      <c r="FE316" s="84"/>
+      <c r="FF316" s="84"/>
+      <c r="FG316" s="84"/>
+      <c r="FH316" s="84"/>
+      <c r="FI316" s="84"/>
+      <c r="FJ316" s="84"/>
+      <c r="FK316" s="84"/>
+      <c r="FL316" s="84"/>
+      <c r="FM316" s="84"/>
+      <c r="FN316" s="84"/>
+      <c r="FO316" s="84"/>
+      <c r="FP316" s="84"/>
+      <c r="FQ316" s="84"/>
+      <c r="FR316" s="84"/>
+      <c r="FS316" s="84"/>
+      <c r="FT316" s="84"/>
+      <c r="FU316" s="84"/>
+      <c r="FV316" s="84"/>
+      <c r="FW316" s="84"/>
+      <c r="FX316" s="84"/>
+      <c r="FY316" s="84"/>
+      <c r="FZ316" s="84"/>
+      <c r="GA316" s="84"/>
+      <c r="GB316" s="84"/>
+      <c r="GC316" s="84"/>
+      <c r="GD316" s="84"/>
+      <c r="GE316" s="84"/>
+      <c r="GF316" s="84"/>
+      <c r="GG316" s="84"/>
+      <c r="GH316" s="84"/>
+      <c r="GI316" s="84"/>
+      <c r="GJ316" s="84"/>
+      <c r="GK316" s="84"/>
+      <c r="GL316" s="84"/>
+      <c r="GM316" s="84"/>
+      <c r="GN316" s="84"/>
+      <c r="GO316" s="84"/>
+      <c r="GP316" s="84"/>
+      <c r="GQ316" s="84"/>
+      <c r="GR316" s="84"/>
+      <c r="GS316" s="84"/>
+      <c r="GT316" s="84"/>
+      <c r="GU316" s="84"/>
+      <c r="GV316" s="84"/>
+      <c r="GW316" s="84"/>
+      <c r="GX316" s="84"/>
+      <c r="GY316" s="84"/>
+      <c r="GZ316" s="84"/>
+      <c r="HA316" s="84"/>
+      <c r="HB316" s="84"/>
+      <c r="HC316" s="84"/>
+      <c r="HD316" s="84"/>
+      <c r="HE316" s="84"/>
+      <c r="HF316" s="84"/>
+      <c r="HG316" s="84"/>
+      <c r="HH316" s="84"/>
+      <c r="HI316" s="84"/>
+      <c r="HJ316" s="84"/>
+      <c r="HK316" s="84"/>
+      <c r="HL316" s="84"/>
+      <c r="HM316" s="84"/>
+      <c r="HN316" s="84"/>
+      <c r="HO316" s="84"/>
+      <c r="HP316" s="84"/>
+      <c r="HQ316" s="84"/>
+      <c r="HR316" s="84"/>
+      <c r="HS316" s="84"/>
+      <c r="HT316" s="84"/>
+      <c r="HU316" s="84"/>
+      <c r="HV316" s="84"/>
+      <c r="HW316" s="84"/>
+      <c r="HX316" s="84"/>
+      <c r="HY316" s="84"/>
+      <c r="HZ316" s="84"/>
+      <c r="IA316" s="84"/>
+      <c r="IB316" s="84"/>
+      <c r="IC316" s="84"/>
+      <c r="ID316" s="84"/>
+      <c r="IE316" s="84"/>
+      <c r="IF316" s="84"/>
+      <c r="IG316" s="84"/>
+      <c r="IH316" s="84"/>
+      <c r="II316" s="84"/>
+      <c r="IJ316" s="84"/>
+      <c r="IK316" s="84"/>
+      <c r="IL316" s="84"/>
+      <c r="IM316" s="84"/>
+      <c r="IN316" s="84"/>
+      <c r="IO316" s="84"/>
+      <c r="IP316" s="84"/>
+      <c r="IQ316" s="84"/>
+      <c r="IR316" s="84"/>
+      <c r="IS316" s="84"/>
+      <c r="IT316" s="84"/>
+      <c r="IU316" s="84"/>
+      <c r="IV316" s="84"/>
+      <c r="IW316" s="84"/>
+      <c r="IX316" s="84"/>
+      <c r="IY316" s="84"/>
+      <c r="IZ316" s="84"/>
+      <c r="JA316" s="84"/>
+      <c r="JB316" s="84"/>
+      <c r="JC316" s="84"/>
+      <c r="JD316" s="84"/>
+      <c r="JE316" s="84"/>
+      <c r="JF316" s="84"/>
+      <c r="JG316" s="84"/>
+      <c r="JH316" s="84"/>
+      <c r="JI316" s="84"/>
+      <c r="JJ316" s="84"/>
+      <c r="JK316" s="84"/>
+      <c r="JL316" s="84"/>
+      <c r="JM316" s="84"/>
+      <c r="JN316" s="84"/>
+      <c r="JO316" s="84"/>
+      <c r="JP316" s="84"/>
+      <c r="JQ316" s="84"/>
+      <c r="JR316" s="84"/>
+      <c r="JS316" s="84"/>
+      <c r="JT316" s="84"/>
+      <c r="JU316" s="84"/>
+      <c r="JV316" s="84"/>
+      <c r="JW316" s="84"/>
+      <c r="JX316" s="84"/>
+      <c r="JY316" s="84"/>
+      <c r="JZ316" s="84"/>
+      <c r="KA316" s="84"/>
+      <c r="KB316" s="84"/>
+      <c r="KC316" s="84"/>
+      <c r="KD316" s="84"/>
+      <c r="KE316" s="84"/>
+      <c r="KF316" s="84"/>
+      <c r="KG316" s="84"/>
+      <c r="KH316" s="84"/>
+      <c r="KI316" s="84"/>
+      <c r="KJ316" s="84"/>
+      <c r="KK316" s="84"/>
+      <c r="KL316" s="84"/>
+      <c r="KM316" s="84"/>
+      <c r="KN316" s="84"/>
+      <c r="KO316" s="84"/>
+      <c r="KP316" s="84"/>
+    </row>
+    <row r="318" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A318" s="41"/>
+      <c r="F318" s="32"/>
+      <c r="I318" s="34"/>
+      <c r="J318" s="32"/>
+      <c r="M318" s="34"/>
+      <c r="Q318" s="32"/>
+      <c r="R318" s="34"/>
+      <c r="S318" s="67"/>
+      <c r="T318" s="67"/>
+      <c r="U318" s="67"/>
+      <c r="V318" s="67"/>
+      <c r="W318" s="67"/>
+      <c r="X318" s="67"/>
+      <c r="Y318" s="67"/>
+      <c r="Z318" s="67"/>
+      <c r="AA318" s="67"/>
+      <c r="AB318" s="67"/>
+      <c r="AC318" s="67"/>
+      <c r="AD318" s="67"/>
+      <c r="AE318" s="67"/>
+      <c r="AF318" s="67"/>
+      <c r="AG318" s="68"/>
+      <c r="AR318" s="83"/>
+      <c r="AT318" s="84"/>
+      <c r="AU318" s="84"/>
+      <c r="AV318" s="84"/>
+      <c r="AW318" s="84"/>
+      <c r="AX318" s="84"/>
+      <c r="AY318" s="84"/>
+      <c r="AZ318" s="84"/>
+      <c r="BA318" s="84"/>
+      <c r="BB318" s="84"/>
+      <c r="BC318" s="84"/>
+      <c r="BD318" s="84"/>
+      <c r="BE318" s="84"/>
+      <c r="BF318" s="84"/>
+      <c r="BG318" s="84"/>
+      <c r="BH318" s="84"/>
+      <c r="BI318" s="84"/>
+      <c r="BJ318" s="84"/>
+      <c r="BK318" s="84"/>
+      <c r="BL318" s="84"/>
+      <c r="BM318" s="84"/>
+      <c r="BN318" s="84"/>
+      <c r="BO318" s="84"/>
+      <c r="BP318" s="84"/>
+      <c r="BQ318" s="84"/>
+      <c r="BR318" s="84"/>
+      <c r="BS318" s="84"/>
+      <c r="BT318" s="84"/>
+      <c r="BU318" s="84"/>
+      <c r="BV318" s="84"/>
+      <c r="BW318" s="84"/>
+      <c r="BX318" s="84"/>
+      <c r="BY318" s="84"/>
+      <c r="BZ318" s="84"/>
+      <c r="CA318" s="84"/>
+      <c r="CB318" s="84"/>
+      <c r="CC318" s="84"/>
+      <c r="CD318" s="84"/>
+      <c r="CE318" s="84"/>
+      <c r="CF318" s="84"/>
+      <c r="CG318" s="84"/>
+      <c r="CH318" s="84"/>
+      <c r="CI318" s="84"/>
+      <c r="CJ318" s="84"/>
+      <c r="CK318" s="84"/>
+      <c r="CL318" s="84"/>
+      <c r="CM318" s="84"/>
+      <c r="CN318" s="84"/>
+      <c r="CO318" s="84"/>
+      <c r="CP318" s="84"/>
+      <c r="CQ318" s="84"/>
+      <c r="CR318" s="84"/>
+      <c r="CS318" s="84"/>
+      <c r="CT318" s="84"/>
+      <c r="CU318" s="84"/>
+      <c r="CV318" s="84"/>
+      <c r="CW318" s="84"/>
+      <c r="CX318" s="84"/>
+      <c r="CY318" s="84"/>
+      <c r="CZ318" s="84"/>
+      <c r="DA318" s="84"/>
+      <c r="DB318" s="84"/>
+      <c r="DC318" s="84"/>
+      <c r="DD318" s="84"/>
+      <c r="DE318" s="84"/>
+      <c r="DF318" s="84"/>
+      <c r="DG318" s="84"/>
+      <c r="DH318" s="84"/>
+      <c r="DI318" s="84"/>
+      <c r="DJ318" s="84"/>
+      <c r="DK318" s="84"/>
+      <c r="DL318" s="84"/>
+      <c r="DM318" s="84"/>
+      <c r="DN318" s="84"/>
+      <c r="DO318" s="84"/>
+      <c r="DP318" s="84"/>
+      <c r="DQ318" s="84"/>
+      <c r="DR318" s="84"/>
+      <c r="DS318" s="84"/>
+      <c r="DT318" s="84"/>
+      <c r="DU318" s="84"/>
+      <c r="DV318" s="84"/>
+      <c r="DW318" s="84"/>
+      <c r="DX318" s="84"/>
+      <c r="DY318" s="84"/>
+      <c r="DZ318" s="84"/>
+      <c r="EA318" s="84"/>
+      <c r="EB318" s="84"/>
+      <c r="EC318" s="84"/>
+      <c r="ED318" s="84"/>
+      <c r="EE318" s="84"/>
+      <c r="EF318" s="84"/>
+      <c r="EG318" s="84"/>
+      <c r="EH318" s="84"/>
+      <c r="EI318" s="84"/>
+      <c r="EJ318" s="84"/>
+      <c r="EK318" s="84"/>
+      <c r="EL318" s="84"/>
+      <c r="EM318" s="84"/>
+      <c r="EN318" s="84"/>
+      <c r="EO318" s="84"/>
+      <c r="EP318" s="84"/>
+      <c r="EQ318" s="84"/>
+      <c r="ER318" s="84"/>
+      <c r="ES318" s="84"/>
+      <c r="ET318" s="84"/>
+      <c r="EU318" s="84"/>
+      <c r="EV318" s="84"/>
+      <c r="EW318" s="84"/>
+      <c r="EX318" s="84"/>
+      <c r="EY318" s="84"/>
+      <c r="EZ318" s="84"/>
+      <c r="FA318" s="84"/>
+      <c r="FB318" s="84"/>
+      <c r="FC318" s="84"/>
+      <c r="FD318" s="84"/>
+      <c r="FE318" s="84"/>
+      <c r="FF318" s="84"/>
+      <c r="FG318" s="84"/>
+      <c r="FH318" s="84"/>
+      <c r="FI318" s="84"/>
+      <c r="FJ318" s="84"/>
+      <c r="FK318" s="84"/>
+      <c r="FL318" s="84"/>
+      <c r="FM318" s="84"/>
+      <c r="FN318" s="84"/>
+      <c r="FO318" s="84"/>
+      <c r="FP318" s="84"/>
+      <c r="FQ318" s="84"/>
+      <c r="FR318" s="84"/>
+      <c r="FS318" s="84"/>
+      <c r="FT318" s="84"/>
+      <c r="FU318" s="84"/>
+      <c r="FV318" s="84"/>
+      <c r="FW318" s="84"/>
+      <c r="FX318" s="84"/>
+      <c r="FY318" s="84"/>
+      <c r="FZ318" s="84"/>
+      <c r="GA318" s="84"/>
+      <c r="GB318" s="84"/>
+      <c r="GC318" s="84"/>
+      <c r="GD318" s="84"/>
+      <c r="GE318" s="84"/>
+      <c r="GF318" s="84"/>
+      <c r="GG318" s="84"/>
+      <c r="GH318" s="84"/>
+      <c r="GI318" s="84"/>
+      <c r="GJ318" s="84"/>
+      <c r="GK318" s="84"/>
+      <c r="GL318" s="84"/>
+      <c r="GM318" s="84"/>
+      <c r="GN318" s="84"/>
+      <c r="GO318" s="84"/>
+      <c r="GP318" s="84"/>
+      <c r="GQ318" s="84"/>
+      <c r="GR318" s="84"/>
+      <c r="GS318" s="84"/>
+      <c r="GT318" s="84"/>
+      <c r="GU318" s="84"/>
+      <c r="GV318" s="84"/>
+      <c r="GW318" s="84"/>
+      <c r="GX318" s="84"/>
+      <c r="GY318" s="84"/>
+      <c r="GZ318" s="84"/>
+      <c r="HA318" s="84"/>
+      <c r="HB318" s="84"/>
+      <c r="HC318" s="84"/>
+      <c r="HD318" s="84"/>
+      <c r="HE318" s="84"/>
+      <c r="HF318" s="84"/>
+      <c r="HG318" s="84"/>
+      <c r="HH318" s="84"/>
+      <c r="HI318" s="84"/>
+      <c r="HJ318" s="84"/>
+      <c r="HK318" s="84"/>
+      <c r="HL318" s="84"/>
+      <c r="HM318" s="84"/>
+      <c r="HN318" s="84"/>
+      <c r="HO318" s="84"/>
+      <c r="HP318" s="84"/>
+      <c r="HQ318" s="84"/>
+      <c r="HR318" s="84"/>
+      <c r="HS318" s="84"/>
+      <c r="HT318" s="84"/>
+      <c r="HU318" s="84"/>
+      <c r="HV318" s="84"/>
+      <c r="HW318" s="84"/>
+      <c r="HX318" s="84"/>
+      <c r="HY318" s="84"/>
+      <c r="HZ318" s="84"/>
+      <c r="IA318" s="84"/>
+      <c r="IB318" s="84"/>
+      <c r="IC318" s="84"/>
+      <c r="ID318" s="84"/>
+      <c r="IE318" s="84"/>
+      <c r="IF318" s="84"/>
+      <c r="IG318" s="84"/>
+      <c r="IH318" s="84"/>
+      <c r="II318" s="84"/>
+      <c r="IJ318" s="84"/>
+      <c r="IK318" s="84"/>
+      <c r="IL318" s="84"/>
+      <c r="IM318" s="84"/>
+      <c r="IN318" s="84"/>
+      <c r="IO318" s="84"/>
+      <c r="IP318" s="84"/>
+      <c r="IQ318" s="84"/>
+      <c r="IR318" s="84"/>
+      <c r="IS318" s="84"/>
+      <c r="IT318" s="84"/>
+      <c r="IU318" s="84"/>
+      <c r="IV318" s="84"/>
+      <c r="IW318" s="84"/>
+      <c r="IX318" s="84"/>
+      <c r="IY318" s="84"/>
+      <c r="IZ318" s="84"/>
+      <c r="JA318" s="84"/>
+      <c r="JB318" s="84"/>
+      <c r="JC318" s="84"/>
+      <c r="JD318" s="84"/>
+      <c r="JE318" s="84"/>
+      <c r="JF318" s="84"/>
+      <c r="JG318" s="84"/>
+      <c r="JH318" s="84"/>
+      <c r="JI318" s="84"/>
+      <c r="JJ318" s="84"/>
+      <c r="JK318" s="84"/>
+      <c r="JL318" s="84"/>
+      <c r="JM318" s="84"/>
+      <c r="JN318" s="84"/>
+      <c r="JO318" s="84"/>
+      <c r="JP318" s="84"/>
+      <c r="JQ318" s="84"/>
+      <c r="JR318" s="84"/>
+      <c r="JS318" s="84"/>
+      <c r="JT318" s="84"/>
+      <c r="JU318" s="84"/>
+      <c r="JV318" s="84"/>
+      <c r="JW318" s="84"/>
+      <c r="JX318" s="84"/>
+      <c r="JY318" s="84"/>
+      <c r="JZ318" s="84"/>
+      <c r="KA318" s="84"/>
+      <c r="KB318" s="84"/>
+      <c r="KC318" s="84"/>
+      <c r="KD318" s="84"/>
+      <c r="KE318" s="84"/>
+      <c r="KF318" s="84"/>
+      <c r="KG318" s="84"/>
+      <c r="KH318" s="84"/>
+      <c r="KI318" s="84"/>
+      <c r="KJ318" s="84"/>
+      <c r="KK318" s="84"/>
+      <c r="KL318" s="84"/>
+      <c r="KM318" s="84"/>
+      <c r="KN318" s="84"/>
+      <c r="KO318" s="84"/>
+      <c r="KP318" s="84"/>
+    </row>
+    <row r="320" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A320" s="41"/>
+      <c r="F320" s="32"/>
+      <c r="I320" s="34"/>
+      <c r="J320" s="32"/>
+      <c r="M320" s="34"/>
+      <c r="Q320" s="32"/>
+      <c r="R320" s="34"/>
+      <c r="S320" s="67"/>
+      <c r="T320" s="67"/>
+      <c r="U320" s="67"/>
+      <c r="V320" s="67"/>
+      <c r="W320" s="67"/>
+      <c r="X320" s="67"/>
+      <c r="Y320" s="67"/>
+      <c r="Z320" s="67"/>
+      <c r="AA320" s="67"/>
+      <c r="AB320" s="67"/>
+      <c r="AC320" s="67"/>
+      <c r="AD320" s="67"/>
+      <c r="AE320" s="67"/>
+      <c r="AF320" s="67"/>
+      <c r="AG320" s="68"/>
+      <c r="AR320" s="83"/>
+      <c r="AT320" s="84"/>
+      <c r="AU320" s="84"/>
+      <c r="AV320" s="84"/>
+      <c r="AW320" s="84"/>
+      <c r="AX320" s="84"/>
+      <c r="AY320" s="84"/>
+      <c r="AZ320" s="84"/>
+      <c r="BA320" s="84"/>
+      <c r="BB320" s="84"/>
+      <c r="BC320" s="84"/>
+      <c r="BD320" s="84"/>
+      <c r="BE320" s="84"/>
+      <c r="BF320" s="84"/>
+      <c r="BG320" s="84"/>
+      <c r="BH320" s="84"/>
+      <c r="BI320" s="84"/>
+      <c r="BJ320" s="84"/>
+      <c r="BK320" s="84"/>
+      <c r="BL320" s="84"/>
+      <c r="BM320" s="84"/>
+      <c r="BN320" s="84"/>
+      <c r="BO320" s="84"/>
+      <c r="BP320" s="84"/>
+      <c r="BQ320" s="84"/>
+      <c r="BR320" s="84"/>
+      <c r="BS320" s="84"/>
+      <c r="BT320" s="84"/>
+      <c r="BU320" s="84"/>
+      <c r="BV320" s="84"/>
+      <c r="BW320" s="84"/>
+      <c r="BX320" s="84"/>
+      <c r="BY320" s="84"/>
+      <c r="BZ320" s="84"/>
+      <c r="CA320" s="84"/>
+      <c r="CB320" s="84"/>
+      <c r="CC320" s="84"/>
+      <c r="CD320" s="84"/>
+      <c r="CE320" s="84"/>
+      <c r="CF320" s="84"/>
+      <c r="CG320" s="84"/>
+      <c r="CH320" s="84"/>
+      <c r="CI320" s="84"/>
+      <c r="CJ320" s="84"/>
+      <c r="CK320" s="84"/>
+      <c r="CL320" s="84"/>
+      <c r="CM320" s="84"/>
+      <c r="CN320" s="84"/>
+      <c r="CO320" s="84"/>
+      <c r="CP320" s="84"/>
+      <c r="CQ320" s="84"/>
+      <c r="CR320" s="84"/>
+      <c r="CS320" s="84"/>
+      <c r="CT320" s="84"/>
+      <c r="CU320" s="84"/>
+      <c r="CV320" s="84"/>
+      <c r="CW320" s="84"/>
+      <c r="CX320" s="84"/>
+      <c r="CY320" s="84"/>
+      <c r="CZ320" s="84"/>
+      <c r="DA320" s="84"/>
+      <c r="DB320" s="84"/>
+      <c r="DC320" s="84"/>
+      <c r="DD320" s="84"/>
+      <c r="DE320" s="84"/>
+      <c r="DF320" s="84"/>
+      <c r="DG320" s="84"/>
+      <c r="DH320" s="84"/>
+      <c r="DI320" s="84"/>
+      <c r="DJ320" s="84"/>
+      <c r="DK320" s="84"/>
+      <c r="DL320" s="84"/>
+      <c r="DM320" s="84"/>
+      <c r="DN320" s="84"/>
+      <c r="DO320" s="84"/>
+      <c r="DP320" s="84"/>
+      <c r="DQ320" s="84"/>
+      <c r="DR320" s="84"/>
+      <c r="DS320" s="84"/>
+      <c r="DT320" s="84"/>
+      <c r="DU320" s="84"/>
+      <c r="DV320" s="84"/>
+      <c r="DW320" s="84"/>
+      <c r="DX320" s="84"/>
+      <c r="DY320" s="84"/>
+      <c r="DZ320" s="84"/>
+      <c r="EA320" s="84"/>
+      <c r="EB320" s="84"/>
+      <c r="EC320" s="84"/>
+      <c r="ED320" s="84"/>
+      <c r="EE320" s="84"/>
+      <c r="EF320" s="84"/>
+      <c r="EG320" s="84"/>
+      <c r="EH320" s="84"/>
+      <c r="EI320" s="84"/>
+      <c r="EJ320" s="84"/>
+      <c r="EK320" s="84"/>
+      <c r="EL320" s="84"/>
+      <c r="EM320" s="84"/>
+      <c r="EN320" s="84"/>
+      <c r="EO320" s="84"/>
+      <c r="EP320" s="84"/>
+      <c r="EQ320" s="84"/>
+      <c r="ER320" s="84"/>
+      <c r="ES320" s="84"/>
+      <c r="ET320" s="84"/>
+      <c r="EU320" s="84"/>
+      <c r="EV320" s="84"/>
+      <c r="EW320" s="84"/>
+      <c r="EX320" s="84"/>
+      <c r="EY320" s="84"/>
+      <c r="EZ320" s="84"/>
+      <c r="FA320" s="84"/>
+      <c r="FB320" s="84"/>
+      <c r="FC320" s="84"/>
+      <c r="FD320" s="84"/>
+      <c r="FE320" s="84"/>
+      <c r="FF320" s="84"/>
+      <c r="FG320" s="84"/>
+      <c r="FH320" s="84"/>
+      <c r="FI320" s="84"/>
+      <c r="FJ320" s="84"/>
+      <c r="FK320" s="84"/>
+      <c r="FL320" s="84"/>
+      <c r="FM320" s="84"/>
+      <c r="FN320" s="84"/>
+      <c r="FO320" s="84"/>
+      <c r="FP320" s="84"/>
+      <c r="FQ320" s="84"/>
+      <c r="FR320" s="84"/>
+      <c r="FS320" s="84"/>
+      <c r="FT320" s="84"/>
+      <c r="FU320" s="84"/>
+      <c r="FV320" s="84"/>
+      <c r="FW320" s="84"/>
+      <c r="FX320" s="84"/>
+      <c r="FY320" s="84"/>
+      <c r="FZ320" s="84"/>
+      <c r="GA320" s="84"/>
+      <c r="GB320" s="84"/>
+      <c r="GC320" s="84"/>
+      <c r="GD320" s="84"/>
+      <c r="GE320" s="84"/>
+      <c r="GF320" s="84"/>
+      <c r="GG320" s="84"/>
+      <c r="GH320" s="84"/>
+      <c r="GI320" s="84"/>
+      <c r="GJ320" s="84"/>
+      <c r="GK320" s="84"/>
+      <c r="GL320" s="84"/>
+      <c r="GM320" s="84"/>
+      <c r="GN320" s="84"/>
+      <c r="GO320" s="84"/>
+      <c r="GP320" s="84"/>
+      <c r="GQ320" s="84"/>
+      <c r="GR320" s="84"/>
+      <c r="GS320" s="84"/>
+      <c r="GT320" s="84"/>
+      <c r="GU320" s="84"/>
+      <c r="GV320" s="84"/>
+      <c r="GW320" s="84"/>
+      <c r="GX320" s="84"/>
+      <c r="GY320" s="84"/>
+      <c r="GZ320" s="84"/>
+      <c r="HA320" s="84"/>
+      <c r="HB320" s="84"/>
+      <c r="HC320" s="84"/>
+      <c r="HD320" s="84"/>
+      <c r="HE320" s="84"/>
+      <c r="HF320" s="84"/>
+      <c r="HG320" s="84"/>
+      <c r="HH320" s="84"/>
+      <c r="HI320" s="84"/>
+      <c r="HJ320" s="84"/>
+      <c r="HK320" s="84"/>
+      <c r="HL320" s="84"/>
+      <c r="HM320" s="84"/>
+      <c r="HN320" s="84"/>
+      <c r="HO320" s="84"/>
+      <c r="HP320" s="84"/>
+      <c r="HQ320" s="84"/>
+      <c r="HR320" s="84"/>
+      <c r="HS320" s="84"/>
+      <c r="HT320" s="84"/>
+      <c r="HU320" s="84"/>
+      <c r="HV320" s="84"/>
+      <c r="HW320" s="84"/>
+      <c r="HX320" s="84"/>
+      <c r="HY320" s="84"/>
+      <c r="HZ320" s="84"/>
+      <c r="IA320" s="84"/>
+      <c r="IB320" s="84"/>
+      <c r="IC320" s="84"/>
+      <c r="ID320" s="84"/>
+      <c r="IE320" s="84"/>
+      <c r="IF320" s="84"/>
+      <c r="IG320" s="84"/>
+      <c r="IH320" s="84"/>
+      <c r="II320" s="84"/>
+      <c r="IJ320" s="84"/>
+      <c r="IK320" s="84"/>
+      <c r="IL320" s="84"/>
+      <c r="IM320" s="84"/>
+      <c r="IN320" s="84"/>
+      <c r="IO320" s="84"/>
+      <c r="IP320" s="84"/>
+      <c r="IQ320" s="84"/>
+      <c r="IR320" s="84"/>
+      <c r="IS320" s="84"/>
+      <c r="IT320" s="84"/>
+      <c r="IU320" s="84"/>
+      <c r="IV320" s="84"/>
+      <c r="IW320" s="84"/>
+      <c r="IX320" s="84"/>
+      <c r="IY320" s="84"/>
+      <c r="IZ320" s="84"/>
+      <c r="JA320" s="84"/>
+      <c r="JB320" s="84"/>
+      <c r="JC320" s="84"/>
+      <c r="JD320" s="84"/>
+      <c r="JE320" s="84"/>
+      <c r="JF320" s="84"/>
+      <c r="JG320" s="84"/>
+      <c r="JH320" s="84"/>
+      <c r="JI320" s="84"/>
+      <c r="JJ320" s="84"/>
+      <c r="JK320" s="84"/>
+      <c r="JL320" s="84"/>
+      <c r="JM320" s="84"/>
+      <c r="JN320" s="84"/>
+      <c r="JO320" s="84"/>
+      <c r="JP320" s="84"/>
+      <c r="JQ320" s="84"/>
+      <c r="JR320" s="84"/>
+      <c r="JS320" s="84"/>
+      <c r="JT320" s="84"/>
+      <c r="JU320" s="84"/>
+      <c r="JV320" s="84"/>
+      <c r="JW320" s="84"/>
+      <c r="JX320" s="84"/>
+      <c r="JY320" s="84"/>
+      <c r="JZ320" s="84"/>
+      <c r="KA320" s="84"/>
+      <c r="KB320" s="84"/>
+      <c r="KC320" s="84"/>
+      <c r="KD320" s="84"/>
+      <c r="KE320" s="84"/>
+      <c r="KF320" s="84"/>
+      <c r="KG320" s="84"/>
+      <c r="KH320" s="84"/>
+      <c r="KI320" s="84"/>
+      <c r="KJ320" s="84"/>
+      <c r="KK320" s="84"/>
+      <c r="KL320" s="84"/>
+      <c r="KM320" s="84"/>
+      <c r="KN320" s="84"/>
+      <c r="KO320" s="84"/>
+      <c r="KP320" s="84"/>
+    </row>
+    <row r="322" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A322" s="41"/>
+      <c r="F322" s="32"/>
+      <c r="I322" s="34"/>
+      <c r="J322" s="32"/>
+      <c r="M322" s="34"/>
+      <c r="Q322" s="32"/>
+      <c r="R322" s="34"/>
+      <c r="S322" s="67"/>
+      <c r="T322" s="67"/>
+      <c r="U322" s="67"/>
+      <c r="V322" s="67"/>
+      <c r="W322" s="67"/>
+      <c r="X322" s="67"/>
+      <c r="Y322" s="67"/>
+      <c r="Z322" s="67"/>
+      <c r="AA322" s="67"/>
+      <c r="AB322" s="67"/>
+      <c r="AC322" s="67"/>
+      <c r="AD322" s="67"/>
+      <c r="AE322" s="67"/>
+      <c r="AF322" s="67"/>
+      <c r="AG322" s="68"/>
+      <c r="AR322" s="83"/>
+      <c r="AT322" s="84"/>
+      <c r="AU322" s="84"/>
+      <c r="AV322" s="84"/>
+      <c r="AW322" s="84"/>
+      <c r="AX322" s="84"/>
+      <c r="AY322" s="84"/>
+      <c r="AZ322" s="84"/>
+      <c r="BA322" s="84"/>
+      <c r="BB322" s="84"/>
+      <c r="BC322" s="84"/>
+      <c r="BD322" s="84"/>
+      <c r="BE322" s="84"/>
+      <c r="BF322" s="84"/>
+      <c r="BG322" s="84"/>
+      <c r="BH322" s="84"/>
+      <c r="BI322" s="84"/>
+      <c r="BJ322" s="84"/>
+      <c r="BK322" s="84"/>
+      <c r="BL322" s="84"/>
+      <c r="BM322" s="84"/>
+      <c r="BN322" s="84"/>
+      <c r="BO322" s="84"/>
+      <c r="BP322" s="84"/>
+      <c r="BQ322" s="84"/>
+      <c r="BR322" s="84"/>
+      <c r="BS322" s="84"/>
+      <c r="BT322" s="84"/>
+      <c r="BU322" s="84"/>
+      <c r="BV322" s="84"/>
+      <c r="BW322" s="84"/>
+      <c r="BX322" s="84"/>
+      <c r="BY322" s="84"/>
+      <c r="BZ322" s="84"/>
+      <c r="CA322" s="84"/>
+      <c r="CB322" s="84"/>
+      <c r="CC322" s="84"/>
+      <c r="CD322" s="84"/>
+      <c r="CE322" s="84"/>
+      <c r="CF322" s="84"/>
+      <c r="CG322" s="84"/>
+      <c r="CH322" s="84"/>
+      <c r="CI322" s="84"/>
+      <c r="CJ322" s="84"/>
+      <c r="CK322" s="84"/>
+      <c r="CL322" s="84"/>
+      <c r="CM322" s="84"/>
+      <c r="CN322" s="84"/>
+      <c r="CO322" s="84"/>
+      <c r="CP322" s="84"/>
+      <c r="CQ322" s="84"/>
+      <c r="CR322" s="84"/>
+      <c r="CS322" s="84"/>
+      <c r="CT322" s="84"/>
+      <c r="CU322" s="84"/>
+      <c r="CV322" s="84"/>
+      <c r="CW322" s="84"/>
+      <c r="CX322" s="84"/>
+      <c r="CY322" s="84"/>
+      <c r="CZ322" s="84"/>
+      <c r="DA322" s="84"/>
+      <c r="DB322" s="84"/>
+      <c r="DC322" s="84"/>
+      <c r="DD322" s="84"/>
+      <c r="DE322" s="84"/>
+      <c r="DF322" s="84"/>
+      <c r="DG322" s="84"/>
+      <c r="DH322" s="84"/>
+      <c r="DI322" s="84"/>
+      <c r="DJ322" s="84"/>
+      <c r="DK322" s="84"/>
+      <c r="DL322" s="84"/>
+      <c r="DM322" s="84"/>
+      <c r="DN322" s="84"/>
+      <c r="DO322" s="84"/>
+      <c r="DP322" s="84"/>
+      <c r="DQ322" s="84"/>
+      <c r="DR322" s="84"/>
+      <c r="DS322" s="84"/>
+      <c r="DT322" s="84"/>
+      <c r="DU322" s="84"/>
+      <c r="DV322" s="84"/>
+      <c r="DW322" s="84"/>
+      <c r="DX322" s="84"/>
+      <c r="DY322" s="84"/>
+      <c r="DZ322" s="84"/>
+      <c r="EA322" s="84"/>
+      <c r="EB322" s="84"/>
+      <c r="EC322" s="84"/>
+      <c r="ED322" s="84"/>
+      <c r="EE322" s="84"/>
+      <c r="EF322" s="84"/>
+      <c r="EG322" s="84"/>
+      <c r="EH322" s="84"/>
+      <c r="EI322" s="84"/>
+      <c r="EJ322" s="84"/>
+      <c r="EK322" s="84"/>
+      <c r="EL322" s="84"/>
+      <c r="EM322" s="84"/>
+      <c r="EN322" s="84"/>
+      <c r="EO322" s="84"/>
+      <c r="EP322" s="84"/>
+      <c r="EQ322" s="84"/>
+      <c r="ER322" s="84"/>
+      <c r="ES322" s="84"/>
+      <c r="ET322" s="84"/>
+      <c r="EU322" s="84"/>
+      <c r="EV322" s="84"/>
+      <c r="EW322" s="84"/>
+      <c r="EX322" s="84"/>
+      <c r="EY322" s="84"/>
+      <c r="EZ322" s="84"/>
+      <c r="FA322" s="84"/>
+      <c r="FB322" s="84"/>
+      <c r="FC322" s="84"/>
+      <c r="FD322" s="84"/>
+      <c r="FE322" s="84"/>
+      <c r="FF322" s="84"/>
+      <c r="FG322" s="84"/>
+      <c r="FH322" s="84"/>
+      <c r="FI322" s="84"/>
+      <c r="FJ322" s="84"/>
+      <c r="FK322" s="84"/>
+      <c r="FL322" s="84"/>
+      <c r="FM322" s="84"/>
+      <c r="FN322" s="84"/>
+      <c r="FO322" s="84"/>
+      <c r="FP322" s="84"/>
+      <c r="FQ322" s="84"/>
+      <c r="FR322" s="84"/>
+      <c r="FS322" s="84"/>
+      <c r="FT322" s="84"/>
+      <c r="FU322" s="84"/>
+      <c r="FV322" s="84"/>
+      <c r="FW322" s="84"/>
+      <c r="FX322" s="84"/>
+      <c r="FY322" s="84"/>
+      <c r="FZ322" s="84"/>
+      <c r="GA322" s="84"/>
+      <c r="GB322" s="84"/>
+      <c r="GC322" s="84"/>
+      <c r="GD322" s="84"/>
+      <c r="GE322" s="84"/>
+      <c r="GF322" s="84"/>
+      <c r="GG322" s="84"/>
+      <c r="GH322" s="84"/>
+      <c r="GI322" s="84"/>
+      <c r="GJ322" s="84"/>
+      <c r="GK322" s="84"/>
+      <c r="GL322" s="84"/>
+      <c r="GM322" s="84"/>
+      <c r="GN322" s="84"/>
+      <c r="GO322" s="84"/>
+      <c r="GP322" s="84"/>
+      <c r="GQ322" s="84"/>
+      <c r="GR322" s="84"/>
+      <c r="GS322" s="84"/>
+      <c r="GT322" s="84"/>
+      <c r="GU322" s="84"/>
+      <c r="GV322" s="84"/>
+      <c r="GW322" s="84"/>
+      <c r="GX322" s="84"/>
+      <c r="GY322" s="84"/>
+      <c r="GZ322" s="84"/>
+      <c r="HA322" s="84"/>
+      <c r="HB322" s="84"/>
+      <c r="HC322" s="84"/>
+      <c r="HD322" s="84"/>
+      <c r="HE322" s="84"/>
+      <c r="HF322" s="84"/>
+      <c r="HG322" s="84"/>
+      <c r="HH322" s="84"/>
+      <c r="HI322" s="84"/>
+      <c r="HJ322" s="84"/>
+      <c r="HK322" s="84"/>
+      <c r="HL322" s="84"/>
+      <c r="HM322" s="84"/>
+      <c r="HN322" s="84"/>
+      <c r="HO322" s="84"/>
+      <c r="HP322" s="84"/>
+      <c r="HQ322" s="84"/>
+      <c r="HR322" s="84"/>
+      <c r="HS322" s="84"/>
+      <c r="HT322" s="84"/>
+      <c r="HU322" s="84"/>
+      <c r="HV322" s="84"/>
+      <c r="HW322" s="84"/>
+      <c r="HX322" s="84"/>
+      <c r="HY322" s="84"/>
+      <c r="HZ322" s="84"/>
+      <c r="IA322" s="84"/>
+      <c r="IB322" s="84"/>
+      <c r="IC322" s="84"/>
+      <c r="ID322" s="84"/>
+      <c r="IE322" s="84"/>
+      <c r="IF322" s="84"/>
+      <c r="IG322" s="84"/>
+      <c r="IH322" s="84"/>
+      <c r="II322" s="84"/>
+      <c r="IJ322" s="84"/>
+      <c r="IK322" s="84"/>
+      <c r="IL322" s="84"/>
+      <c r="IM322" s="84"/>
+      <c r="IN322" s="84"/>
+      <c r="IO322" s="84"/>
+      <c r="IP322" s="84"/>
+      <c r="IQ322" s="84"/>
+      <c r="IR322" s="84"/>
+      <c r="IS322" s="84"/>
+      <c r="IT322" s="84"/>
+      <c r="IU322" s="84"/>
+      <c r="IV322" s="84"/>
+      <c r="IW322" s="84"/>
+      <c r="IX322" s="84"/>
+      <c r="IY322" s="84"/>
+      <c r="IZ322" s="84"/>
+      <c r="JA322" s="84"/>
+      <c r="JB322" s="84"/>
+      <c r="JC322" s="84"/>
+      <c r="JD322" s="84"/>
+      <c r="JE322" s="84"/>
+      <c r="JF322" s="84"/>
+      <c r="JG322" s="84"/>
+      <c r="JH322" s="84"/>
+      <c r="JI322" s="84"/>
+      <c r="JJ322" s="84"/>
+      <c r="JK322" s="84"/>
+      <c r="JL322" s="84"/>
+      <c r="JM322" s="84"/>
+      <c r="JN322" s="84"/>
+      <c r="JO322" s="84"/>
+      <c r="JP322" s="84"/>
+      <c r="JQ322" s="84"/>
+      <c r="JR322" s="84"/>
+      <c r="JS322" s="84"/>
+      <c r="JT322" s="84"/>
+      <c r="JU322" s="84"/>
+      <c r="JV322" s="84"/>
+      <c r="JW322" s="84"/>
+      <c r="JX322" s="84"/>
+      <c r="JY322" s="84"/>
+      <c r="JZ322" s="84"/>
+      <c r="KA322" s="84"/>
+      <c r="KB322" s="84"/>
+      <c r="KC322" s="84"/>
+      <c r="KD322" s="84"/>
+      <c r="KE322" s="84"/>
+      <c r="KF322" s="84"/>
+      <c r="KG322" s="84"/>
+      <c r="KH322" s="84"/>
+      <c r="KI322" s="84"/>
+      <c r="KJ322" s="84"/>
+      <c r="KK322" s="84"/>
+      <c r="KL322" s="84"/>
+      <c r="KM322" s="84"/>
+      <c r="KN322" s="84"/>
+      <c r="KO322" s="84"/>
+      <c r="KP322" s="84"/>
+    </row>
+    <row r="324" spans="1:302" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A324" s="41"/>
+      <c r="F324" s="32"/>
+      <c r="I324" s="34"/>
+      <c r="J324" s="32"/>
+      <c r="M324" s="34"/>
+      <c r="Q324" s="32"/>
+      <c r="R324" s="34"/>
+      <c r="S324" s="67"/>
+      <c r="T324" s="67"/>
+      <c r="U324" s="67"/>
+      <c r="V324" s="67"/>
+      <c r="W324" s="67"/>
+      <c r="X324" s="67"/>
+      <c r="Y324" s="67"/>
+      <c r="Z324" s="67"/>
+      <c r="AA324" s="67"/>
+      <c r="AB324" s="67"/>
+      <c r="AC324" s="67"/>
+      <c r="AD324" s="67"/>
+      <c r="AE324" s="67"/>
+      <c r="AF324" s="67"/>
+      <c r="AG324" s="68"/>
+      <c r="AR324" s="83"/>
+      <c r="AT324" s="84"/>
+      <c r="AU324" s="84"/>
+      <c r="AV324" s="84"/>
+      <c r="AW324" s="84"/>
+      <c r="AX324" s="84"/>
+      <c r="AY324" s="84"/>
+      <c r="AZ324" s="84"/>
+      <c r="BA324" s="84"/>
+      <c r="BB324" s="84"/>
+      <c r="BC324" s="84"/>
+      <c r="BD324" s="84"/>
+      <c r="BE324" s="84"/>
+      <c r="BF324" s="84"/>
+      <c r="BG324" s="84"/>
+      <c r="BH324" s="84"/>
+      <c r="BI324" s="84"/>
+      <c r="BJ324" s="84"/>
+      <c r="BK324" s="84"/>
+      <c r="BL324" s="84"/>
+      <c r="BM324" s="84"/>
+      <c r="BN324" s="84"/>
+      <c r="BO324" s="84"/>
+      <c r="BP324" s="84"/>
+      <c r="BQ324" s="84"/>
+      <c r="BR324" s="84"/>
+      <c r="BS324" s="84"/>
+      <c r="BT324" s="84"/>
+      <c r="BU324" s="84"/>
+      <c r="BV324" s="84"/>
+      <c r="BW324" s="84"/>
+      <c r="BX324" s="84"/>
+      <c r="BY324" s="84"/>
+      <c r="BZ324" s="84"/>
+      <c r="CA324" s="84"/>
+      <c r="CB324" s="84"/>
+      <c r="CC324" s="84"/>
+      <c r="CD324" s="84"/>
+      <c r="CE324" s="84"/>
+      <c r="CF324" s="84"/>
+      <c r="CG324" s="84"/>
+      <c r="CH324" s="84"/>
+      <c r="CI324" s="84"/>
+      <c r="CJ324" s="84"/>
+      <c r="CK324" s="84"/>
+      <c r="CL324" s="84"/>
+      <c r="CM324" s="84"/>
+      <c r="CN324" s="84"/>
+      <c r="CO324" s="84"/>
+      <c r="CP324" s="84"/>
+      <c r="CQ324" s="84"/>
+      <c r="CR324" s="84"/>
+      <c r="CS324" s="84"/>
+      <c r="CT324" s="84"/>
+      <c r="CU324" s="84"/>
+      <c r="CV324" s="84"/>
+      <c r="CW324" s="84"/>
+      <c r="CX324" s="84"/>
+      <c r="CY324" s="84"/>
+      <c r="CZ324" s="84"/>
+      <c r="DA324" s="84"/>
+      <c r="DB324" s="84"/>
+      <c r="DC324" s="84"/>
+      <c r="DD324" s="84"/>
+      <c r="DE324" s="84"/>
+      <c r="DF324" s="84"/>
+      <c r="DG324" s="84"/>
+      <c r="DH324" s="84"/>
+      <c r="DI324" s="84"/>
+      <c r="DJ324" s="84"/>
+      <c r="DK324" s="84"/>
+      <c r="DL324" s="84"/>
+      <c r="DM324" s="84"/>
+      <c r="DN324" s="84"/>
+      <c r="DO324" s="84"/>
+      <c r="DP324" s="84"/>
+      <c r="DQ324" s="84"/>
+      <c r="DR324" s="84"/>
+      <c r="DS324" s="84"/>
+      <c r="DT324" s="84"/>
+      <c r="DU324" s="84"/>
+      <c r="DV324" s="84"/>
+      <c r="DW324" s="84"/>
+      <c r="DX324" s="84"/>
+      <c r="DY324" s="84"/>
+      <c r="DZ324" s="84"/>
+      <c r="EA324" s="84"/>
+      <c r="EB324" s="84"/>
+      <c r="EC324" s="84"/>
+      <c r="ED324" s="84"/>
+      <c r="EE324" s="84"/>
+      <c r="EF324" s="84"/>
+      <c r="EG324" s="84"/>
+      <c r="EH324" s="84"/>
+      <c r="EI324" s="84"/>
+      <c r="EJ324" s="84"/>
+      <c r="EK324" s="84"/>
+      <c r="EL324" s="84"/>
+      <c r="EM324" s="84"/>
+      <c r="EN324" s="84"/>
+      <c r="EO324" s="84"/>
+      <c r="EP324" s="84"/>
+      <c r="EQ324" s="84"/>
+      <c r="ER324" s="84"/>
+      <c r="ES324" s="84"/>
+      <c r="ET324" s="84"/>
+      <c r="EU324" s="84"/>
+      <c r="EV324" s="84"/>
+      <c r="EW324" s="84"/>
+      <c r="EX324" s="84"/>
+      <c r="EY324" s="84"/>
+      <c r="EZ324" s="84"/>
+      <c r="FA324" s="84"/>
+      <c r="FB324" s="84"/>
+      <c r="FC324" s="84"/>
+      <c r="FD324" s="84"/>
+      <c r="FE324" s="84"/>
+      <c r="FF324" s="84"/>
+      <c r="FG324" s="84"/>
+      <c r="FH324" s="84"/>
+      <c r="FI324" s="84"/>
+      <c r="FJ324" s="84"/>
+      <c r="FK324" s="84"/>
+      <c r="FL324" s="84"/>
+      <c r="FM324" s="84"/>
+      <c r="FN324" s="84"/>
+      <c r="FO324" s="84"/>
+      <c r="FP324" s="84"/>
+      <c r="FQ324" s="84"/>
+      <c r="FR324" s="84"/>
+      <c r="FS324" s="84"/>
+      <c r="FT324" s="84"/>
+      <c r="FU324" s="84"/>
+      <c r="FV324" s="84"/>
+      <c r="FW324" s="84"/>
+      <c r="FX324" s="84"/>
+      <c r="FY324" s="84"/>
+      <c r="FZ324" s="84"/>
+      <c r="GA324" s="84"/>
+      <c r="GB324" s="84"/>
+      <c r="GC324" s="84"/>
+      <c r="GD324" s="84"/>
+      <c r="GE324" s="84"/>
+      <c r="GF324" s="84"/>
+      <c r="GG324" s="84"/>
+      <c r="GH324" s="84"/>
+      <c r="GI324" s="84"/>
+      <c r="GJ324" s="84"/>
+      <c r="GK324" s="84"/>
+      <c r="GL324" s="84"/>
+      <c r="GM324" s="84"/>
+      <c r="GN324" s="84"/>
+      <c r="GO324" s="84"/>
+      <c r="GP324" s="84"/>
+      <c r="GQ324" s="84"/>
+      <c r="GR324" s="84"/>
+      <c r="GS324" s="84"/>
+      <c r="GT324" s="84"/>
+      <c r="GU324" s="84"/>
+      <c r="GV324" s="84"/>
+      <c r="GW324" s="84"/>
+      <c r="GX324" s="84"/>
+      <c r="GY324" s="84"/>
+      <c r="GZ324" s="84"/>
+      <c r="HA324" s="84"/>
+      <c r="HB324" s="84"/>
+      <c r="HC324" s="84"/>
+      <c r="HD324" s="84"/>
+      <c r="HE324" s="84"/>
+      <c r="HF324" s="84"/>
+      <c r="HG324" s="84"/>
+      <c r="HH324" s="84"/>
+      <c r="HI324" s="84"/>
+      <c r="HJ324" s="84"/>
+      <c r="HK324" s="84"/>
+      <c r="HL324" s="84"/>
+      <c r="HM324" s="84"/>
+      <c r="HN324" s="84"/>
+      <c r="HO324" s="84"/>
+      <c r="HP324" s="84"/>
+      <c r="HQ324" s="84"/>
+      <c r="HR324" s="84"/>
+      <c r="HS324" s="84"/>
+      <c r="HT324" s="84"/>
+      <c r="HU324" s="84"/>
+      <c r="HV324" s="84"/>
+      <c r="HW324" s="84"/>
+      <c r="HX324" s="84"/>
+      <c r="HY324" s="84"/>
+      <c r="HZ324" s="84"/>
+      <c r="IA324" s="84"/>
+      <c r="IB324" s="84"/>
+      <c r="IC324" s="84"/>
+      <c r="ID324" s="84"/>
+      <c r="IE324" s="84"/>
+      <c r="IF324" s="84"/>
+      <c r="IG324" s="84"/>
+      <c r="IH324" s="84"/>
+      <c r="II324" s="84"/>
+      <c r="IJ324" s="84"/>
+      <c r="IK324" s="84"/>
+      <c r="IL324" s="84"/>
+      <c r="IM324" s="84"/>
+      <c r="IN324" s="84"/>
+      <c r="IO324" s="84"/>
+      <c r="IP324" s="84"/>
+      <c r="IQ324" s="84"/>
+      <c r="IR324" s="84"/>
+      <c r="IS324" s="84"/>
+      <c r="IT324" s="84"/>
+      <c r="IU324" s="84"/>
+      <c r="IV324" s="84"/>
+      <c r="IW324" s="84"/>
+      <c r="IX324" s="84"/>
+      <c r="IY324" s="84"/>
+      <c r="IZ324" s="84"/>
+      <c r="JA324" s="84"/>
+      <c r="JB324" s="84"/>
+      <c r="JC324" s="84"/>
+      <c r="JD324" s="84"/>
+      <c r="JE324" s="84"/>
+      <c r="JF324" s="84"/>
+      <c r="JG324" s="84"/>
+      <c r="JH324" s="84"/>
+      <c r="JI324" s="84"/>
+      <c r="JJ324" s="84"/>
+      <c r="JK324" s="84"/>
+      <c r="JL324" s="84"/>
+      <c r="JM324" s="84"/>
+      <c r="JN324" s="84"/>
+      <c r="JO324" s="84"/>
+      <c r="JP324" s="84"/>
+      <c r="JQ324" s="84"/>
+      <c r="JR324" s="84"/>
+      <c r="JS324" s="84"/>
+      <c r="JT324" s="84"/>
+      <c r="JU324" s="84"/>
+      <c r="JV324" s="84"/>
+      <c r="JW324" s="84"/>
+      <c r="JX324" s="84"/>
+      <c r="JY324" s="84"/>
+      <c r="JZ324" s="84"/>
+      <c r="KA324" s="84"/>
+      <c r="KB324" s="84"/>
+      <c r="KC324" s="84"/>
+      <c r="KD324" s="84"/>
+      <c r="KE324" s="84"/>
+      <c r="KF324" s="84"/>
+      <c r="KG324" s="84"/>
+      <c r="KH324" s="84"/>
+      <c r="KI324" s="84"/>
+      <c r="KJ324" s="84"/>
+      <c r="KK324" s="84"/>
+      <c r="KL324" s="84"/>
+      <c r="KM324" s="84"/>
+      <c r="KN324" s="84"/>
+      <c r="KO324" s="84"/>
+      <c r="KP324" s="84"/>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
Corrected the LapContinue deco chain for all the capture types. Moved StopSingleSeed in the deco chain to be more logical. Changed PassStoreCapture to use a local deco of capt_ok to check side. Added the missing capture_ok checks to SandwichCapt. Added CaptSideOk to the capt_check deco chain. Added en passant captures, corrected a few tests for above changes, and added a test for the sowing stopping when it shouldn't with en passant captures. Unit test coverage 100%.
</commit_message>
<xml_diff>
--- a/test/capture_test_data.xlsx
+++ b/test/capture_test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549FBD18-2301-4CDA-8F38-3A4A59290758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDAB671-66C3-464C-95AF-2FD2DAF9527D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capture_test_data" sheetId="1" r:id="rId1"/>
@@ -1168,7 +1168,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1352,11 +1352,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1693,9 +1688,9 @@
   <dimension ref="A1:AMK324"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AJ308" sqref="AJ308"/>
+      <selection pane="bottomLeft" activeCell="V306" sqref="V306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -44277,9 +44272,7 @@
         <v>32</v>
       </c>
       <c r="S243" s="65"/>
-      <c r="T243" s="65">
-        <v>3</v>
-      </c>
+      <c r="T243" s="65"/>
       <c r="U243" s="65">
         <v>3</v>
       </c>
@@ -57351,16 +57344,16 @@
       <c r="AB301" s="60" t="s">
         <v>205</v>
       </c>
-      <c r="AH301" s="99">
-        <v>3</v>
-      </c>
-      <c r="AI301" s="99">
-        <v>3</v>
-      </c>
-      <c r="AJ301" s="99">
+      <c r="AH301" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI301" s="29">
+        <v>3</v>
+      </c>
+      <c r="AJ301" s="29">
         <v>2</v>
       </c>
-      <c r="AK301" s="99">
+      <c r="AK301" s="29">
         <v>3</v>
       </c>
       <c r="AP301">
@@ -57411,16 +57404,16 @@
       <c r="AE302" s="67"/>
       <c r="AF302" s="67"/>
       <c r="AG302" s="68"/>
-      <c r="AH302" s="100">
-        <v>3</v>
-      </c>
-      <c r="AI302" s="101">
+      <c r="AH302" s="98">
+        <v>3</v>
+      </c>
+      <c r="AI302" s="33">
         <v>1</v>
       </c>
-      <c r="AJ302" s="101">
-        <v>3</v>
-      </c>
-      <c r="AK302" s="102">
+      <c r="AJ302" s="33">
+        <v>3</v>
+      </c>
+      <c r="AK302" s="41">
         <v>0</v>
       </c>
       <c r="AR302" s="83"/>
@@ -57722,7 +57715,7 @@
       <c r="AI303" s="29">
         <v>3</v>
       </c>
-      <c r="AJ303" s="99">
+      <c r="AJ303" s="29">
         <v>1</v>
       </c>
       <c r="AK303" s="46">
@@ -58057,7 +58050,7 @@
       <c r="C305" s="29">
         <v>3</v>
       </c>
-      <c r="D305" s="99">
+      <c r="D305" s="29">
         <v>3</v>
       </c>
       <c r="E305" s="87">
@@ -58078,6 +58071,9 @@
       <c r="R305" s="24" t="s">
         <v>44</v>
       </c>
+      <c r="V305" s="60">
+        <v>1</v>
+      </c>
       <c r="AB305" s="60" t="s">
         <v>205</v>
       </c>
@@ -58087,10 +58083,10 @@
       <c r="AI305" s="29">
         <v>3</v>
       </c>
-      <c r="AJ305" s="99">
-        <v>3</v>
-      </c>
-      <c r="AK305" s="103">
+      <c r="AJ305" s="29">
+        <v>3</v>
+      </c>
+      <c r="AK305" s="46">
         <v>1</v>
       </c>
       <c r="AP305">

</xml_diff>